<commit_message>
clear encoder loss + some lookup table refinement
</commit_message>
<xml_diff>
--- a/startup/lookup_table/Modes.xlsx
+++ b/startup/lookup_table/Modes.xlsx
@@ -11117,7 +11117,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="148">
+  <cellXfs count="150">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -11374,6 +11374,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -11383,6 +11391,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11658,10 +11670,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -11790,14 +11798,14 @@
   <dimension ref="A1:AMJ66"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="E28" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="H28" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topRight" activeCell="H1" activeCellId="0" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
-      <selection pane="bottomRight" activeCell="F46" activeCellId="0" sqref="F46:F47"/>
+      <selection pane="bottomRight" activeCell="O59" activeCellId="0" sqref="O59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.04"/>
@@ -14922,19 +14930,19 @@
       <c r="J56" s="23" t="n">
         <v>6151303</v>
       </c>
-      <c r="K56" s="61" t="n">
-        <v>125.596</v>
+      <c r="K56" s="64" t="n">
+        <v>124.496</v>
       </c>
       <c r="L56" s="23" t="n">
         <v>9901395</v>
       </c>
-      <c r="M56" s="61" t="n">
-        <v>126.051</v>
+      <c r="M56" s="65" t="n">
+        <v>124.496</v>
       </c>
       <c r="N56" s="23" t="n">
         <v>9901395</v>
       </c>
-      <c r="O56" s="61" t="n">
+      <c r="O56" s="65" t="n">
         <v>97.709</v>
       </c>
       <c r="P56" s="23" t="n">
@@ -14966,38 +14974,38 @@
       <c r="D57" s="0" t="s">
         <v>192</v>
       </c>
-      <c r="E57" s="64" t="n">
+      <c r="E57" s="66" t="n">
         <v>116.993</v>
       </c>
       <c r="F57" s="32" t="n">
         <v>6972005</v>
       </c>
-      <c r="G57" s="65" t="n">
+      <c r="G57" s="67" t="n">
         <v>12.81</v>
       </c>
-      <c r="H57" s="66" t="n">
+      <c r="H57" s="68" t="n">
         <v>1551088</v>
       </c>
-      <c r="I57" s="64" t="n">
+      <c r="I57" s="66" t="n">
         <v>47.758</v>
       </c>
       <c r="J57" s="32" t="n">
         <v>3351899</v>
       </c>
       <c r="K57" s="64" t="n">
-        <v>129.041</v>
+        <v>129.341</v>
       </c>
       <c r="L57" s="32" t="n">
         <v>7552437</v>
       </c>
-      <c r="M57" s="64" t="n">
-        <v>129.496</v>
+      <c r="M57" s="69" t="n">
+        <v>129.841</v>
       </c>
       <c r="N57" s="32" t="n">
         <v>7552437</v>
       </c>
-      <c r="O57" s="64" t="n">
-        <v>96.404</v>
+      <c r="O57" s="69" t="n">
+        <v>96.004</v>
       </c>
       <c r="P57" s="32" t="n">
         <v>5879304</v>
@@ -15020,40 +15028,40 @@
       <c r="D58" s="26" t="s">
         <v>195</v>
       </c>
-      <c r="E58" s="64" t="n">
+      <c r="E58" s="66" t="n">
         <v>116.993</v>
       </c>
       <c r="F58" s="28" t="n">
         <v>5572330</v>
       </c>
-      <c r="G58" s="65" t="n">
+      <c r="G58" s="67" t="n">
         <v>12.81</v>
       </c>
-      <c r="H58" s="66" t="n">
+      <c r="H58" s="68" t="n">
         <v>354340</v>
       </c>
-      <c r="I58" s="64" t="n">
+      <c r="I58" s="66" t="n">
         <v>47.758</v>
       </c>
       <c r="J58" s="32" t="n">
         <v>1952224</v>
       </c>
       <c r="K58" s="64" t="n">
-        <v>129.041</v>
+        <v>129.341</v>
       </c>
       <c r="L58" s="32" t="n">
         <v>6355689</v>
       </c>
-      <c r="M58" s="64" t="n">
-        <v>129.496</v>
+      <c r="M58" s="69" t="n">
+        <v>129.841</v>
       </c>
       <c r="N58" s="32" t="n">
         <v>6355689</v>
       </c>
-      <c r="O58" s="64" t="n">
-        <v>96.404</v>
-      </c>
-      <c r="P58" s="67" t="n">
+      <c r="O58" s="69" t="n">
+        <v>96.004</v>
+      </c>
+      <c r="P58" s="70" t="n">
         <v>4479629</v>
       </c>
       <c r="T58" s="27" t="n">
@@ -15079,43 +15087,43 @@
       <c r="D59" s="26" t="s">
         <v>198</v>
       </c>
-      <c r="E59" s="64" t="n">
+      <c r="E59" s="66" t="n">
         <v>-9.0621</v>
       </c>
       <c r="F59" s="28" t="n">
         <v>-242758</v>
       </c>
-      <c r="G59" s="65" t="n">
+      <c r="G59" s="67" t="n">
         <v>-9.0621</v>
       </c>
-      <c r="H59" s="68" t="n">
+      <c r="H59" s="71" t="n">
         <v>-242758</v>
       </c>
-      <c r="I59" s="64" t="n">
+      <c r="I59" s="66" t="n">
         <v>-9.0621</v>
       </c>
       <c r="J59" s="28" t="n">
         <v>-242758</v>
       </c>
-      <c r="K59" s="64" t="n">
+      <c r="K59" s="66" t="n">
         <v>-9.0621</v>
       </c>
       <c r="L59" s="28" t="n">
         <v>-242758</v>
       </c>
-      <c r="M59" s="64" t="n">
+      <c r="M59" s="66" t="n">
         <v>-9.0621</v>
       </c>
       <c r="N59" s="28" t="n">
         <v>-242758</v>
       </c>
-      <c r="O59" s="64" t="n">
+      <c r="O59" s="66" t="n">
         <v>-9.0621</v>
       </c>
       <c r="P59" s="28" t="n">
         <v>-242758</v>
       </c>
-      <c r="T59" s="64" t="n">
+      <c r="T59" s="66" t="n">
         <v>-0.6</v>
       </c>
       <c r="U59" s="28" t="n">
@@ -15133,46 +15141,46 @@
       <c r="D60" s="35" t="s">
         <v>201</v>
       </c>
-      <c r="E60" s="69" t="n">
+      <c r="E60" s="72" t="n">
         <v>15.3898</v>
       </c>
       <c r="F60" s="47" t="n">
         <v>160203</v>
       </c>
-      <c r="G60" s="70" t="n">
+      <c r="G60" s="73" t="n">
         <v>15.3898</v>
       </c>
-      <c r="H60" s="71" t="n">
+      <c r="H60" s="74" t="n">
         <v>160203</v>
       </c>
-      <c r="I60" s="69" t="n">
+      <c r="I60" s="72" t="n">
         <v>15.3898</v>
       </c>
       <c r="J60" s="47" t="n">
         <v>160203</v>
       </c>
-      <c r="K60" s="69" t="n">
+      <c r="K60" s="72" t="n">
         <v>15.3898</v>
       </c>
       <c r="L60" s="47" t="n">
         <v>160203</v>
       </c>
-      <c r="M60" s="69" t="n">
+      <c r="M60" s="72" t="n">
         <v>15.3898</v>
       </c>
       <c r="N60" s="47" t="n">
         <v>160203</v>
       </c>
-      <c r="O60" s="69" t="n">
+      <c r="O60" s="72" t="n">
         <v>15.3898</v>
       </c>
       <c r="P60" s="47" t="n">
         <v>160203</v>
       </c>
-      <c r="Q60" s="72"/>
-      <c r="R60" s="72"/>
-      <c r="S60" s="72"/>
-      <c r="T60" s="69" t="n">
+      <c r="Q60" s="75"/>
+      <c r="R60" s="75"/>
+      <c r="S60" s="75"/>
+      <c r="T60" s="72" t="n">
         <v>33.3721</v>
       </c>
       <c r="U60" s="47" t="n">
@@ -15185,52 +15193,52 @@
       <c r="Z60" s="0"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="73" t="s">
+      <c r="A61" s="76" t="s">
         <v>202</v>
       </c>
-      <c r="B61" s="74" t="s">
+      <c r="B61" s="77" t="s">
         <v>203</v>
       </c>
-      <c r="C61" s="75" t="s">
+      <c r="C61" s="78" t="s">
         <v>204</v>
       </c>
-      <c r="D61" s="75" t="s">
+      <c r="D61" s="78" t="s">
         <v>205</v>
       </c>
-      <c r="E61" s="76" t="n">
-        <v>0</v>
-      </c>
-      <c r="F61" s="77" t="n">
-        <v>0</v>
-      </c>
-      <c r="G61" s="76" t="n">
-        <v>0</v>
-      </c>
-      <c r="H61" s="77" t="n">
-        <v>0</v>
-      </c>
-      <c r="I61" s="76" t="n">
-        <v>0</v>
-      </c>
-      <c r="J61" s="77" t="n">
-        <v>0</v>
-      </c>
-      <c r="K61" s="76" t="n">
-        <v>0</v>
-      </c>
-      <c r="L61" s="77" t="n">
-        <v>0</v>
-      </c>
-      <c r="M61" s="76" t="n">
-        <v>0</v>
-      </c>
-      <c r="N61" s="77" t="n">
-        <v>0</v>
-      </c>
-      <c r="O61" s="76" t="n">
-        <v>0</v>
-      </c>
-      <c r="P61" s="77" t="n">
+      <c r="E61" s="79" t="n">
+        <v>0</v>
+      </c>
+      <c r="F61" s="80" t="n">
+        <v>0</v>
+      </c>
+      <c r="G61" s="79" t="n">
+        <v>0</v>
+      </c>
+      <c r="H61" s="80" t="n">
+        <v>0</v>
+      </c>
+      <c r="I61" s="79" t="n">
+        <v>0</v>
+      </c>
+      <c r="J61" s="80" t="n">
+        <v>0</v>
+      </c>
+      <c r="K61" s="79" t="n">
+        <v>0</v>
+      </c>
+      <c r="L61" s="80" t="n">
+        <v>0</v>
+      </c>
+      <c r="M61" s="79" t="n">
+        <v>0</v>
+      </c>
+      <c r="N61" s="80" t="n">
+        <v>0</v>
+      </c>
+      <c r="O61" s="79" t="n">
+        <v>0</v>
+      </c>
+      <c r="P61" s="80" t="n">
         <v>0</v>
       </c>
       <c r="T61" s="30" t="n">
@@ -15241,8 +15249,8 @@
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="73"/>
-      <c r="B62" s="78" t="s">
+      <c r="A62" s="76"/>
+      <c r="B62" s="81" t="s">
         <v>206</v>
       </c>
       <c r="C62" s="0" t="s">
@@ -15295,8 +15303,8 @@
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="73"/>
-      <c r="B63" s="78" t="s">
+      <c r="A63" s="76"/>
+      <c r="B63" s="81" t="s">
         <v>209</v>
       </c>
       <c r="C63" s="0" t="s">
@@ -15349,8 +15357,8 @@
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="73"/>
-      <c r="B64" s="78" t="s">
+      <c r="A64" s="76"/>
+      <c r="B64" s="81" t="s">
         <v>212</v>
       </c>
       <c r="C64" s="0" t="s">
@@ -15403,8 +15411,8 @@
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="73"/>
-      <c r="B65" s="78" t="s">
+      <c r="A65" s="76"/>
+      <c r="B65" s="81" t="s">
         <v>215</v>
       </c>
       <c r="C65" s="0" t="s">
@@ -15457,53 +15465,53 @@
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="73"/>
-      <c r="B66" s="79" t="s">
+      <c r="A66" s="76"/>
+      <c r="B66" s="82" t="s">
         <v>218</v>
       </c>
-      <c r="C66" s="80" t="s">
+      <c r="C66" s="83" t="s">
         <v>219</v>
       </c>
-      <c r="D66" s="80" t="s">
+      <c r="D66" s="83" t="s">
         <v>220</v>
       </c>
-      <c r="E66" s="81" t="n">
-        <v>0</v>
-      </c>
-      <c r="F66" s="82" t="n">
-        <v>0</v>
-      </c>
-      <c r="G66" s="81" t="n">
-        <v>0</v>
-      </c>
-      <c r="H66" s="82" t="n">
-        <v>0</v>
-      </c>
-      <c r="I66" s="81" t="n">
-        <v>0</v>
-      </c>
-      <c r="J66" s="82" t="n">
-        <v>0</v>
-      </c>
-      <c r="K66" s="81" t="n">
-        <v>0</v>
-      </c>
-      <c r="L66" s="82" t="n">
-        <v>0</v>
-      </c>
-      <c r="M66" s="81" t="n">
-        <v>0</v>
-      </c>
-      <c r="N66" s="82" t="n">
-        <v>0</v>
-      </c>
-      <c r="O66" s="81" t="n">
-        <v>0</v>
-      </c>
-      <c r="P66" s="82" t="n">
-        <v>0</v>
-      </c>
-      <c r="T66" s="69" t="n">
+      <c r="E66" s="84" t="n">
+        <v>0</v>
+      </c>
+      <c r="F66" s="85" t="n">
+        <v>0</v>
+      </c>
+      <c r="G66" s="84" t="n">
+        <v>0</v>
+      </c>
+      <c r="H66" s="85" t="n">
+        <v>0</v>
+      </c>
+      <c r="I66" s="84" t="n">
+        <v>0</v>
+      </c>
+      <c r="J66" s="85" t="n">
+        <v>0</v>
+      </c>
+      <c r="K66" s="84" t="n">
+        <v>0</v>
+      </c>
+      <c r="L66" s="85" t="n">
+        <v>0</v>
+      </c>
+      <c r="M66" s="84" t="n">
+        <v>0</v>
+      </c>
+      <c r="N66" s="85" t="n">
+        <v>0</v>
+      </c>
+      <c r="O66" s="84" t="n">
+        <v>0</v>
+      </c>
+      <c r="P66" s="85" t="n">
+        <v>0</v>
+      </c>
+      <c r="T66" s="72" t="n">
         <v>0</v>
       </c>
       <c r="U66" s="47" t="n">
@@ -15558,39 +15566,39 @@
   <dimension ref="A1:AMJ31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D28" activeCellId="1" sqref="F46:F47 D28"/>
+      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="83" width="3.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="2" style="83" width="13.26"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="10" style="83" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="86" width="3.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="2" style="86" width="13.26"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="10" style="86" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" s="84" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="83"/>
+    <row r="1" s="87" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="86"/>
       <c r="B1" s="0"/>
       <c r="C1" s="0"/>
       <c r="D1" s="0"/>
       <c r="E1" s="0"/>
-      <c r="F1" s="83"/>
-      <c r="G1" s="83"/>
-      <c r="H1" s="83"/>
-      <c r="I1" s="83"/>
-      <c r="J1" s="83"/>
-      <c r="K1" s="83"/>
-      <c r="L1" s="83"/>
-      <c r="AMJ1" s="83"/>
+      <c r="F1" s="86"/>
+      <c r="G1" s="86"/>
+      <c r="H1" s="86"/>
+      <c r="I1" s="86"/>
+      <c r="J1" s="86"/>
+      <c r="K1" s="86"/>
+      <c r="L1" s="86"/>
+      <c r="AMJ1" s="86"/>
     </row>
     <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0"/>
-      <c r="B2" s="85" t="s">
+      <c r="B2" s="88" t="s">
         <v>221</v>
       </c>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
       <c r="F2" s="0"/>
       <c r="G2" s="0"/>
       <c r="H2" s="0"/>
@@ -16611,168 +16619,168 @@
       <c r="AMI2" s="0"/>
       <c r="AMJ2" s="0"/>
     </row>
-    <row r="3" s="90" customFormat="true" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="86"/>
-      <c r="B3" s="87"/>
-      <c r="C3" s="88" t="s">
+    <row r="3" s="93" customFormat="true" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="89"/>
+      <c r="B3" s="90"/>
+      <c r="C3" s="91" t="s">
         <v>222</v>
       </c>
-      <c r="D3" s="88" t="s">
+      <c r="D3" s="91" t="s">
         <v>223</v>
       </c>
-      <c r="E3" s="89" t="s">
+      <c r="E3" s="92" t="s">
         <v>224</v>
       </c>
-      <c r="F3" s="86"/>
-      <c r="G3" s="86"/>
-      <c r="H3" s="86"/>
-      <c r="I3" s="86"/>
-      <c r="J3" s="86"/>
-      <c r="K3" s="86"/>
-      <c r="L3" s="86"/>
-      <c r="AMJ3" s="86"/>
-    </row>
-    <row r="4" s="84" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="83"/>
-      <c r="B4" s="87" t="s">
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="89"/>
+      <c r="L3" s="89"/>
+      <c r="AMJ3" s="89"/>
+    </row>
+    <row r="4" s="87" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="86"/>
+      <c r="B4" s="90" t="s">
         <v>225</v>
       </c>
-      <c r="C4" s="83"/>
-      <c r="D4" s="83" t="n">
+      <c r="C4" s="86"/>
+      <c r="D4" s="86" t="n">
         <v>55</v>
       </c>
-      <c r="E4" s="91" t="n">
+      <c r="E4" s="94" t="n">
         <v>55</v>
       </c>
-      <c r="F4" s="83"/>
-      <c r="G4" s="83"/>
-      <c r="H4" s="83"/>
-      <c r="I4" s="83"/>
-      <c r="J4" s="83"/>
-      <c r="K4" s="83"/>
-      <c r="L4" s="83"/>
-      <c r="AMJ4" s="83"/>
-    </row>
-    <row r="5" s="84" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="83"/>
-      <c r="B5" s="87" t="s">
+      <c r="F4" s="86"/>
+      <c r="G4" s="86"/>
+      <c r="H4" s="86"/>
+      <c r="I4" s="86"/>
+      <c r="J4" s="86"/>
+      <c r="K4" s="86"/>
+      <c r="L4" s="86"/>
+      <c r="AMJ4" s="86"/>
+    </row>
+    <row r="5" s="87" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="86"/>
+      <c r="B5" s="90" t="s">
         <v>226</v>
       </c>
-      <c r="C5" s="83" t="s">
+      <c r="C5" s="86" t="s">
         <v>227</v>
       </c>
-      <c r="D5" s="83" t="n">
+      <c r="D5" s="86" t="n">
         <v>-46.5</v>
       </c>
-      <c r="E5" s="91"/>
-      <c r="F5" s="83"/>
-      <c r="G5" s="83"/>
-      <c r="H5" s="83"/>
-      <c r="I5" s="83"/>
-      <c r="J5" s="83"/>
-      <c r="K5" s="83"/>
-      <c r="L5" s="83"/>
-      <c r="AMJ5" s="83"/>
-    </row>
-    <row r="6" s="84" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="83"/>
-      <c r="B6" s="87" t="s">
+      <c r="E5" s="94"/>
+      <c r="F5" s="86"/>
+      <c r="G5" s="86"/>
+      <c r="H5" s="86"/>
+      <c r="I5" s="86"/>
+      <c r="J5" s="86"/>
+      <c r="K5" s="86"/>
+      <c r="L5" s="86"/>
+      <c r="AMJ5" s="86"/>
+    </row>
+    <row r="6" s="87" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="86"/>
+      <c r="B6" s="90" t="s">
         <v>228</v>
       </c>
-      <c r="C6" s="83" t="s">
+      <c r="C6" s="86" t="s">
         <v>229</v>
       </c>
-      <c r="D6" s="83" t="n">
+      <c r="D6" s="86" t="n">
         <v>-20.5</v>
       </c>
-      <c r="E6" s="91"/>
-      <c r="F6" s="83"/>
-      <c r="G6" s="83"/>
-      <c r="H6" s="83"/>
-      <c r="I6" s="83"/>
-      <c r="J6" s="83"/>
-      <c r="K6" s="83"/>
-      <c r="L6" s="83"/>
-      <c r="AMJ6" s="83"/>
-    </row>
-    <row r="7" s="84" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="83"/>
-      <c r="B7" s="87" t="s">
+      <c r="E6" s="94"/>
+      <c r="F6" s="86"/>
+      <c r="G6" s="86"/>
+      <c r="H6" s="86"/>
+      <c r="I6" s="86"/>
+      <c r="J6" s="86"/>
+      <c r="K6" s="86"/>
+      <c r="L6" s="86"/>
+      <c r="AMJ6" s="86"/>
+    </row>
+    <row r="7" s="87" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="86"/>
+      <c r="B7" s="90" t="s">
         <v>230</v>
       </c>
-      <c r="C7" s="83" t="s">
+      <c r="C7" s="86" t="s">
         <v>231</v>
       </c>
-      <c r="D7" s="83" t="n">
+      <c r="D7" s="86" t="n">
         <v>5.5</v>
       </c>
-      <c r="E7" s="91"/>
-      <c r="F7" s="83"/>
-      <c r="G7" s="83"/>
-      <c r="H7" s="83"/>
-      <c r="I7" s="83"/>
-      <c r="J7" s="83"/>
-      <c r="K7" s="83"/>
-      <c r="L7" s="83"/>
-      <c r="AMJ7" s="83"/>
-    </row>
-    <row r="8" s="84" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="83"/>
-      <c r="B8" s="87" t="s">
+      <c r="E7" s="94"/>
+      <c r="F7" s="86"/>
+      <c r="G7" s="86"/>
+      <c r="H7" s="86"/>
+      <c r="I7" s="86"/>
+      <c r="J7" s="86"/>
+      <c r="K7" s="86"/>
+      <c r="L7" s="86"/>
+      <c r="AMJ7" s="86"/>
+    </row>
+    <row r="8" s="87" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="86"/>
+      <c r="B8" s="90" t="s">
         <v>232</v>
       </c>
-      <c r="C8" s="83" t="s">
+      <c r="C8" s="86" t="s">
         <v>233</v>
       </c>
-      <c r="D8" s="83" t="n">
+      <c r="D8" s="86" t="n">
         <v>31</v>
       </c>
-      <c r="E8" s="91"/>
-      <c r="F8" s="83"/>
-      <c r="G8" s="83"/>
-      <c r="H8" s="83"/>
-      <c r="I8" s="83"/>
-      <c r="J8" s="83"/>
-      <c r="K8" s="83"/>
-      <c r="L8" s="83"/>
-      <c r="AMJ8" s="83"/>
-    </row>
-    <row r="9" s="84" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="83"/>
-      <c r="B9" s="87" t="s">
+      <c r="E8" s="94"/>
+      <c r="F8" s="86"/>
+      <c r="G8" s="86"/>
+      <c r="H8" s="86"/>
+      <c r="I8" s="86"/>
+      <c r="J8" s="86"/>
+      <c r="K8" s="86"/>
+      <c r="L8" s="86"/>
+      <c r="AMJ8" s="86"/>
+    </row>
+    <row r="9" s="87" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="86"/>
+      <c r="B9" s="90" t="s">
         <v>234</v>
       </c>
-      <c r="C9" s="83"/>
-      <c r="D9" s="83" t="n">
+      <c r="C9" s="86"/>
+      <c r="D9" s="86" t="n">
         <v>-52.6</v>
       </c>
-      <c r="E9" s="91"/>
-      <c r="F9" s="83"/>
-      <c r="G9" s="83"/>
-      <c r="H9" s="83"/>
-      <c r="I9" s="83"/>
-      <c r="J9" s="83"/>
-      <c r="K9" s="83"/>
-      <c r="L9" s="83"/>
-      <c r="AMJ9" s="83"/>
+      <c r="E9" s="94"/>
+      <c r="F9" s="86"/>
+      <c r="G9" s="86"/>
+      <c r="H9" s="86"/>
+      <c r="I9" s="86"/>
+      <c r="J9" s="86"/>
+      <c r="K9" s="86"/>
+      <c r="L9" s="86"/>
+      <c r="AMJ9" s="86"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="92" t="s">
+      <c r="B10" s="95" t="s">
         <v>235</v>
       </c>
-      <c r="C10" s="93"/>
-      <c r="D10" s="93" t="n">
+      <c r="C10" s="96"/>
+      <c r="D10" s="96" t="n">
         <v>-52</v>
       </c>
-      <c r="E10" s="94"/>
+      <c r="E10" s="97"/>
       <c r="F10" s="0"/>
       <c r="G10" s="0"/>
       <c r="H10" s="0"/>
       <c r="I10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="95"/>
-      <c r="C11" s="96"/>
+      <c r="B11" s="98"/>
+      <c r="C11" s="99"/>
       <c r="D11" s="0"/>
       <c r="E11" s="0"/>
       <c r="F11" s="0"/>
@@ -16781,8 +16789,8 @@
       <c r="I11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="95"/>
-      <c r="C12" s="96"/>
+      <c r="B12" s="98"/>
+      <c r="C12" s="99"/>
       <c r="D12" s="0"/>
       <c r="E12" s="0"/>
       <c r="F12" s="0"/>
@@ -16791,82 +16799,82 @@
       <c r="I12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="97" t="s">
+      <c r="B13" s="100" t="s">
         <v>236</v>
       </c>
-      <c r="C13" s="97"/>
-      <c r="D13" s="97"/>
-      <c r="E13" s="97"/>
+      <c r="C13" s="100"/>
+      <c r="D13" s="100"/>
+      <c r="E13" s="100"/>
       <c r="F13" s="0"/>
       <c r="G13" s="0"/>
       <c r="H13" s="0"/>
       <c r="I13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="98" t="s">
+      <c r="B14" s="101" t="s">
         <v>237</v>
       </c>
-      <c r="C14" s="99" t="s">
+      <c r="C14" s="102" t="s">
         <v>238</v>
       </c>
       <c r="D14" s="0"/>
-      <c r="E14" s="91"/>
+      <c r="E14" s="94"/>
       <c r="F14" s="0"/>
       <c r="G14" s="0"/>
       <c r="H14" s="0"/>
       <c r="I14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="87" t="s">
+      <c r="B15" s="90" t="s">
         <v>225</v>
       </c>
-      <c r="C15" s="83" t="n">
+      <c r="C15" s="86" t="n">
         <v>67</v>
       </c>
       <c r="D15" s="0"/>
-      <c r="E15" s="91"/>
+      <c r="E15" s="94"/>
       <c r="F15" s="0"/>
       <c r="G15" s="0"/>
       <c r="H15" s="0"/>
       <c r="I15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="87" t="s">
+      <c r="B16" s="90" t="s">
         <v>239</v>
       </c>
-      <c r="C16" s="100" t="n">
+      <c r="C16" s="103" t="n">
         <v>-1.5</v>
       </c>
       <c r="D16" s="0"/>
-      <c r="E16" s="91"/>
+      <c r="E16" s="94"/>
       <c r="F16" s="0"/>
       <c r="G16" s="0"/>
       <c r="H16" s="0"/>
       <c r="I16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="87" t="s">
+      <c r="B17" s="90" t="s">
         <v>240</v>
       </c>
-      <c r="C17" s="83" t="n">
+      <c r="C17" s="86" t="n">
         <v>33</v>
       </c>
       <c r="D17" s="0"/>
-      <c r="E17" s="91"/>
+      <c r="E17" s="94"/>
       <c r="F17" s="0"/>
       <c r="G17" s="0"/>
       <c r="H17" s="0"/>
       <c r="I17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="92" t="s">
+      <c r="B18" s="95" t="s">
         <v>241</v>
       </c>
-      <c r="C18" s="93" t="n">
+      <c r="C18" s="96" t="n">
         <v>53</v>
       </c>
-      <c r="D18" s="93"/>
-      <c r="E18" s="94"/>
+      <c r="D18" s="96"/>
+      <c r="E18" s="97"/>
       <c r="F18" s="0"/>
       <c r="G18" s="0"/>
       <c r="H18" s="0"/>
@@ -16893,213 +16901,213 @@
       <c r="I20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="97" t="s">
+      <c r="B21" s="100" t="s">
         <v>176</v>
       </c>
-      <c r="C21" s="97"/>
-      <c r="D21" s="97"/>
-      <c r="E21" s="97"/>
-      <c r="F21" s="97"/>
-      <c r="G21" s="97"/>
-      <c r="H21" s="97"/>
-      <c r="I21" s="97"/>
+      <c r="C21" s="100"/>
+      <c r="D21" s="100"/>
+      <c r="E21" s="100"/>
+      <c r="F21" s="100"/>
+      <c r="G21" s="100"/>
+      <c r="H21" s="100"/>
+      <c r="I21" s="100"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="101" t="s">
+      <c r="B22" s="104" t="s">
         <v>242</v>
       </c>
-      <c r="C22" s="101"/>
-      <c r="D22" s="84"/>
-      <c r="E22" s="95" t="s">
+      <c r="C22" s="104"/>
+      <c r="D22" s="87"/>
+      <c r="E22" s="98" t="s">
         <v>243</v>
       </c>
-      <c r="F22" s="95"/>
-      <c r="G22" s="84"/>
-      <c r="H22" s="102" t="s">
+      <c r="F22" s="98"/>
+      <c r="G22" s="87"/>
+      <c r="H22" s="105" t="s">
         <v>244</v>
       </c>
-      <c r="I22" s="102"/>
+      <c r="I22" s="105"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="98" t="s">
+      <c r="B23" s="101" t="s">
         <v>245</v>
       </c>
-      <c r="C23" s="99" t="s">
+      <c r="C23" s="102" t="s">
         <v>238</v>
       </c>
       <c r="D23" s="0"/>
-      <c r="E23" s="84" t="s">
+      <c r="E23" s="87" t="s">
         <v>245</v>
       </c>
-      <c r="F23" s="99" t="s">
+      <c r="F23" s="102" t="s">
         <v>238</v>
       </c>
       <c r="G23" s="0"/>
-      <c r="H23" s="84" t="s">
+      <c r="H23" s="87" t="s">
         <v>246</v>
       </c>
-      <c r="I23" s="103" t="s">
+      <c r="I23" s="106" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="87" t="s">
+      <c r="B24" s="90" t="s">
         <v>247</v>
       </c>
       <c r="C24" s="0" t="n">
         <v>33</v>
       </c>
       <c r="D24" s="0"/>
-      <c r="E24" s="83" t="s">
+      <c r="E24" s="86" t="s">
         <v>247</v>
       </c>
-      <c r="F24" s="104" t="n">
+      <c r="F24" s="107" t="n">
         <f aca="false">'Modes A-F'!E54</f>
         <v>31.259</v>
       </c>
       <c r="G24" s="0"/>
-      <c r="H24" s="83" t="s">
+      <c r="H24" s="86" t="s">
         <v>248</v>
       </c>
-      <c r="I24" s="91" t="n">
+      <c r="I24" s="94" t="n">
         <v>40</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="87" t="s">
+      <c r="B25" s="90" t="s">
         <v>249</v>
       </c>
       <c r="C25" s="0" t="n">
         <v>-66.743</v>
       </c>
       <c r="D25" s="0"/>
-      <c r="E25" s="83" t="s">
+      <c r="E25" s="86" t="s">
         <v>249</v>
       </c>
-      <c r="F25" s="104" t="n">
+      <c r="F25" s="107" t="n">
         <f aca="false">'Modes A-F'!G54</f>
         <v>-55.188</v>
       </c>
       <c r="G25" s="0"/>
-      <c r="H25" s="83" t="s">
+      <c r="H25" s="86" t="s">
         <v>250</v>
       </c>
-      <c r="I25" s="91" t="n">
+      <c r="I25" s="94" t="n">
         <v>-17.5</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="87" t="s">
+      <c r="B26" s="90" t="s">
         <v>251</v>
       </c>
       <c r="C26" s="0" t="n">
         <v>-48.1824</v>
       </c>
       <c r="D26" s="0"/>
-      <c r="E26" s="83" t="s">
+      <c r="E26" s="86" t="s">
         <v>251</v>
       </c>
-      <c r="F26" s="104" t="n">
+      <c r="F26" s="107" t="n">
         <f aca="false">'Modes A-F'!I54</f>
         <v>-23.247</v>
       </c>
       <c r="G26" s="0"/>
-      <c r="H26" s="83" t="s">
+      <c r="H26" s="86" t="s">
         <v>252</v>
       </c>
-      <c r="I26" s="91" t="n">
+      <c r="I26" s="94" t="n">
         <v>6.5</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="87" t="s">
+      <c r="B27" s="90" t="s">
         <v>253</v>
       </c>
-      <c r="C27" s="83" t="n">
+      <c r="C27" s="86" t="n">
         <v>27.1</v>
       </c>
       <c r="D27" s="0"/>
-      <c r="E27" s="83" t="s">
+      <c r="E27" s="86" t="s">
         <v>253</v>
       </c>
-      <c r="F27" s="104" t="n">
+      <c r="F27" s="107" t="n">
         <f aca="false">'Modes A-F'!K54</f>
         <v>42.66</v>
       </c>
       <c r="G27" s="0"/>
       <c r="H27" s="0"/>
-      <c r="I27" s="91"/>
+      <c r="I27" s="94"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="87" t="s">
+      <c r="B28" s="90" t="s">
         <v>254</v>
       </c>
-      <c r="C28" s="83" t="n">
+      <c r="C28" s="86" t="n">
         <v>27.1</v>
       </c>
       <c r="D28" s="0"/>
-      <c r="E28" s="83" t="s">
+      <c r="E28" s="86" t="s">
         <v>254</v>
       </c>
-      <c r="F28" s="104" t="n">
+      <c r="F28" s="107" t="n">
         <f aca="false">'Modes A-F'!M54</f>
         <v>43.0474</v>
       </c>
       <c r="G28" s="0"/>
       <c r="H28" s="0"/>
-      <c r="I28" s="91"/>
+      <c r="I28" s="94"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="87" t="s">
+      <c r="B29" s="90" t="s">
         <v>255</v>
       </c>
-      <c r="C29" s="83" t="n">
+      <c r="C29" s="86" t="n">
         <v>2.8</v>
       </c>
       <c r="D29" s="0"/>
-      <c r="E29" s="83" t="s">
+      <c r="E29" s="86" t="s">
         <v>255</v>
       </c>
-      <c r="F29" s="104" t="n">
+      <c r="F29" s="107" t="n">
         <f aca="false">'Modes A-F'!O54</f>
         <v>17.066</v>
       </c>
       <c r="G29" s="0"/>
       <c r="H29" s="0"/>
-      <c r="I29" s="91"/>
+      <c r="I29" s="94"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="87" t="s">
+      <c r="B30" s="90" t="s">
         <v>256</v>
       </c>
-      <c r="C30" s="83" t="n">
+      <c r="C30" s="86" t="n">
         <v>15</v>
       </c>
       <c r="D30" s="0"/>
-      <c r="E30" s="83" t="s">
+      <c r="E30" s="86" t="s">
         <v>256</v>
       </c>
-      <c r="F30" s="104" t="n">
+      <c r="F30" s="107" t="n">
         <f aca="false">'Modes A-F'!T54</f>
         <v>53.33</v>
       </c>
       <c r="G30" s="0"/>
       <c r="H30" s="0"/>
-      <c r="I30" s="91"/>
+      <c r="I30" s="94"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="92" t="s">
+      <c r="B31" s="95" t="s">
         <v>248</v>
       </c>
-      <c r="C31" s="93" t="n">
+      <c r="C31" s="96" t="n">
         <v>55</v>
       </c>
-      <c r="D31" s="93"/>
-      <c r="E31" s="93"/>
-      <c r="F31" s="93"/>
-      <c r="G31" s="93"/>
-      <c r="H31" s="93"/>
-      <c r="I31" s="94"/>
+      <c r="D31" s="96"/>
+      <c r="E31" s="96"/>
+      <c r="F31" s="96"/>
+      <c r="G31" s="96"/>
+      <c r="H31" s="96"/>
+      <c r="I31" s="97"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -17132,10 +17140,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G11" activeCellId="1" sqref="F46:F47 G11"/>
+      <selection pane="bottomRight" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33"/>
@@ -17155,14 +17163,14 @@
       <c r="D1" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="105" t="s">
+      <c r="E1" s="108" t="s">
         <v>257</v>
       </c>
-      <c r="F1" s="105"/>
-      <c r="G1" s="106" t="s">
+      <c r="F1" s="108"/>
+      <c r="G1" s="109" t="s">
         <v>258</v>
       </c>
-      <c r="H1" s="106"/>
+      <c r="H1" s="109"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="44" t="s">
@@ -17188,25 +17196,25 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="107" t="s">
+      <c r="B3" s="110" t="s">
         <v>92</v>
       </c>
-      <c r="C3" s="108" t="s">
+      <c r="C3" s="111" t="s">
         <v>93</v>
       </c>
-      <c r="D3" s="108" t="s">
+      <c r="D3" s="111" t="s">
         <v>259</v>
       </c>
-      <c r="E3" s="108" t="n">
+      <c r="E3" s="111" t="n">
         <v>8.77968</v>
       </c>
-      <c r="F3" s="108" t="n">
+      <c r="F3" s="111" t="n">
         <v>-2703</v>
       </c>
-      <c r="G3" s="109" t="n">
+      <c r="G3" s="112" t="n">
         <v>7.16226</v>
       </c>
-      <c r="H3" s="110" t="n">
+      <c r="H3" s="113" t="n">
         <v>-6620</v>
       </c>
     </row>
@@ -17269,11 +17277,11 @@
       <c r="G6" s="1" t="n">
         <v>15.99439325</v>
       </c>
-      <c r="I6" s="111" t="s">
+      <c r="I6" s="114" t="s">
         <v>262</v>
       </c>
-      <c r="J6" s="111"/>
-      <c r="K6" s="111"/>
+      <c r="J6" s="114"/>
+      <c r="K6" s="114"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D7" s="0" t="s">
@@ -17285,9 +17293,9 @@
       <c r="G7" s="1" t="n">
         <v>1.63763854</v>
       </c>
-      <c r="I7" s="111"/>
-      <c r="J7" s="111"/>
-      <c r="K7" s="111"/>
+      <c r="I7" s="114"/>
+      <c r="J7" s="114"/>
+      <c r="K7" s="114"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -17314,10 +17322,10 @@
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="1" sqref="F46:F47 E4"/>
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.36"/>
@@ -17327,26 +17335,26 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="112"/>
-      <c r="B1" s="113"/>
-      <c r="C1" s="113"/>
-      <c r="D1" s="113"/>
-      <c r="E1" s="114" t="s">
+      <c r="A1" s="115"/>
+      <c r="B1" s="116"/>
+      <c r="C1" s="116"/>
+      <c r="D1" s="116"/>
+      <c r="E1" s="117" t="s">
         <v>264</v>
       </c>
-      <c r="F1" s="114" t="s">
+      <c r="F1" s="117" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="115" t="s">
+      <c r="G1" s="118" t="s">
         <v>265</v>
       </c>
-      <c r="H1" s="116" t="s">
+      <c r="H1" s="119" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="117"/>
-      <c r="D2" s="118" t="s">
+      <c r="A2" s="120"/>
+      <c r="D2" s="121" t="s">
         <v>267</v>
       </c>
       <c r="E2" s="0" t="n">
@@ -17355,514 +17363,514 @@
       <c r="F2" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="G2" s="119"/>
+      <c r="G2" s="122"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="120" t="s">
+      <c r="A3" s="123" t="s">
         <v>268</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>9002</v>
       </c>
-      <c r="D3" s="118" t="s">
+      <c r="D3" s="121" t="s">
         <v>269</v>
       </c>
-      <c r="E3" s="121" t="n">
+      <c r="E3" s="124" t="n">
         <v>46.1092</v>
       </c>
-      <c r="F3" s="104" t="n">
+      <c r="F3" s="107" t="n">
         <f aca="false">E3-B3*TAN(2*(F2-E2)/1000)</f>
         <v>19.1031189817083</v>
       </c>
-      <c r="G3" s="122" t="n">
+      <c r="G3" s="125" t="n">
         <f aca="false">'Modes A-F'!O54</f>
         <v>17.066</v>
       </c>
-      <c r="H3" s="123" t="n">
+      <c r="H3" s="126" t="n">
         <f aca="false">G3-F3</f>
         <v>-2.0371189817083</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="120" t="s">
+      <c r="A4" s="123" t="s">
         <v>270</v>
       </c>
       <c r="B4" s="0" t="n">
         <f aca="false">B3+635</f>
         <v>9637</v>
       </c>
-      <c r="D4" s="118" t="s">
+      <c r="D4" s="121" t="s">
         <v>271</v>
       </c>
-      <c r="E4" s="104" t="n">
+      <c r="E4" s="107" t="n">
         <f aca="false">'Modes A-F'!K56</f>
-        <v>125.596</v>
-      </c>
-      <c r="F4" s="104" t="n">
+        <v>124.496</v>
+      </c>
+      <c r="F4" s="107" t="n">
         <f aca="false">E4-B4*TAN(2*(F2-E2)/1000)</f>
-        <v>96.6849132666878</v>
-      </c>
-      <c r="G4" s="122" t="n">
+        <v>95.5849132666878</v>
+      </c>
+      <c r="G4" s="125" t="n">
         <f aca="false">'Modes A-F'!O56</f>
         <v>97.709</v>
       </c>
-      <c r="H4" s="123" t="n">
+      <c r="H4" s="126" t="n">
         <f aca="false">G4-F4</f>
-        <v>1.02408673331225</v>
+        <v>2.12408673331225</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="124" t="s">
+      <c r="A5" s="127" t="s">
         <v>272</v>
       </c>
-      <c r="B5" s="125" t="n">
+      <c r="B5" s="128" t="n">
         <f aca="false">B3+1790</f>
         <v>10792</v>
       </c>
-      <c r="C5" s="125"/>
-      <c r="D5" s="126" t="s">
+      <c r="C5" s="128"/>
+      <c r="D5" s="129" t="s">
         <v>273</v>
       </c>
-      <c r="E5" s="127" t="n">
+      <c r="E5" s="130" t="n">
         <f aca="false">'Modes A-F'!K57</f>
-        <v>129.041</v>
-      </c>
-      <c r="F5" s="127" t="n">
+        <v>129.341</v>
+      </c>
+      <c r="F5" s="130" t="n">
         <f aca="false">E5-B5*TAN(2*(F2-E2)/1000)</f>
-        <v>96.6649028716503</v>
-      </c>
-      <c r="G5" s="128" t="n">
+        <v>96.9649028716503</v>
+      </c>
+      <c r="G5" s="131" t="n">
         <f aca="false">'Modes A-F'!O57</f>
-        <v>96.404</v>
-      </c>
-      <c r="H5" s="123" t="n">
+        <v>96.004</v>
+      </c>
+      <c r="H5" s="126" t="n">
         <f aca="false">G5-F5</f>
-        <v>-0.26090287165033</v>
+        <v>-0.960902871650333</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H6" s="123" t="n">
+      <c r="H6" s="126" t="n">
         <f aca="false">AVERAGE(H3,H4,H5)</f>
-        <v>-0.42464504001546</v>
+        <v>-0.291311706682126</v>
       </c>
       <c r="I6" s="0" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="129" t="s">
+      <c r="A8" s="132" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="129"/>
-      <c r="C8" s="129"/>
-      <c r="D8" s="113"/>
-      <c r="E8" s="113"/>
-      <c r="F8" s="130" t="s">
+      <c r="B8" s="132"/>
+      <c r="C8" s="132"/>
+      <c r="D8" s="116"/>
+      <c r="E8" s="116"/>
+      <c r="F8" s="133" t="s">
         <v>275</v>
       </c>
-      <c r="G8" s="131" t="n">
+      <c r="G8" s="134" t="n">
         <v>-0.1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="117"/>
-      <c r="D9" s="118" t="s">
+      <c r="A9" s="120"/>
+      <c r="D9" s="121" t="s">
         <v>267</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>3.5</v>
       </c>
-      <c r="G9" s="119" t="n">
+      <c r="G9" s="122" t="n">
         <f aca="false">E9+G8</f>
         <v>3.4</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="120" t="s">
+      <c r="A10" s="123" t="s">
         <v>276</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>10907</v>
       </c>
-      <c r="D10" s="118" t="s">
+      <c r="D10" s="121" t="s">
         <v>269</v>
       </c>
-      <c r="E10" s="123" t="n">
+      <c r="E10" s="126" t="n">
         <f aca="false">'Modes A-F'!E54</f>
         <v>31.259</v>
       </c>
-      <c r="F10" s="123"/>
-      <c r="G10" s="132" t="n">
+      <c r="F10" s="126"/>
+      <c r="G10" s="135" t="n">
         <f aca="false">E10-B10*TAN(2*(G9-E9)/1000)</f>
         <v>33.4404000290853</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="120" t="s">
+      <c r="A11" s="123" t="s">
         <v>277</v>
       </c>
       <c r="B11" s="0" t="n">
         <f aca="false">B10+635</f>
         <v>11542</v>
       </c>
-      <c r="D11" s="118" t="s">
+      <c r="D11" s="121" t="s">
         <v>271</v>
       </c>
-      <c r="E11" s="123" t="n">
+      <c r="E11" s="126" t="n">
         <f aca="false">'Modes A-F'!E57</f>
         <v>116.993</v>
       </c>
-      <c r="F11" s="123"/>
-      <c r="G11" s="132" t="n">
+      <c r="F11" s="126"/>
+      <c r="G11" s="135" t="n">
         <f aca="false">E11-B11*TAN(2*(G9-E9)/1000)</f>
         <v>119.301400030779</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="124" t="s">
+      <c r="A12" s="127" t="s">
         <v>278</v>
       </c>
-      <c r="B12" s="125" t="n">
+      <c r="B12" s="128" t="n">
         <f aca="false">B10+1790</f>
         <v>12697</v>
       </c>
-      <c r="C12" s="125"/>
-      <c r="D12" s="126" t="s">
+      <c r="C12" s="128"/>
+      <c r="D12" s="129" t="s">
         <v>273</v>
       </c>
-      <c r="E12" s="133" t="n">
+      <c r="E12" s="136" t="n">
         <f aca="false">'Modes A-F'!E58</f>
         <v>116.993</v>
       </c>
-      <c r="F12" s="133"/>
-      <c r="G12" s="134" t="n">
+      <c r="F12" s="136"/>
+      <c r="G12" s="137" t="n">
         <f aca="false">E12-B12*TAN(2*(G9-E9)/1000)</f>
         <v>119.532400033859</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="129" t="s">
+      <c r="A16" s="132" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="129"/>
-      <c r="C16" s="129"/>
-      <c r="D16" s="113"/>
-      <c r="E16" s="113"/>
-      <c r="F16" s="130" t="s">
+      <c r="B16" s="132"/>
+      <c r="C16" s="132"/>
+      <c r="D16" s="116"/>
+      <c r="E16" s="116"/>
+      <c r="F16" s="133" t="s">
         <v>275</v>
       </c>
-      <c r="G16" s="113" t="n">
+      <c r="G16" s="116" t="n">
         <v>0.275</v>
       </c>
-      <c r="H16" s="113"/>
-      <c r="I16" s="131"/>
+      <c r="H16" s="116"/>
+      <c r="I16" s="134"/>
     </row>
     <row r="17" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="117"/>
-      <c r="D17" s="118" t="s">
+      <c r="A17" s="120"/>
+      <c r="D17" s="121" t="s">
         <v>267</v>
       </c>
       <c r="E17" s="0" t="n">
         <v>3.225</v>
       </c>
-      <c r="G17" s="72" t="n">
+      <c r="G17" s="75" t="n">
         <f aca="false">E17+G16</f>
         <v>3.5</v>
       </c>
-      <c r="H17" s="135" t="s">
+      <c r="H17" s="64" t="s">
         <v>279</v>
       </c>
-      <c r="I17" s="119" t="n">
+      <c r="I17" s="122" t="n">
         <f aca="false">B18*TAN(2*(E9-G17)/1000)</f>
         <v>0</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="120" t="s">
+      <c r="A18" s="123" t="s">
         <v>280</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>1908</v>
       </c>
-      <c r="D18" s="118" t="s">
+      <c r="D18" s="121" t="s">
         <v>281</v>
       </c>
       <c r="E18" s="0" t="n">
         <v>-7.25</v>
       </c>
-      <c r="G18" s="136" t="n">
+      <c r="G18" s="138" t="n">
         <f aca="false">E18+B18*TAN(2*(G17-E17)/1000)</f>
         <v>-6.20059989418549</v>
       </c>
-      <c r="I18" s="119"/>
+      <c r="I18" s="122"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="117"/>
-      <c r="D19" s="118" t="s">
+      <c r="A19" s="120"/>
+      <c r="D19" s="121" t="s">
         <v>282</v>
       </c>
       <c r="E19" s="0" t="n">
         <f aca="false">3.5 + (3.5-E17)</f>
         <v>3.775</v>
       </c>
-      <c r="G19" s="72" t="n">
+      <c r="G19" s="75" t="n">
         <f aca="false">E19-G16</f>
         <v>3.5</v>
       </c>
-      <c r="I19" s="119"/>
+      <c r="I19" s="122"/>
     </row>
     <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="117"/>
-      <c r="D20" s="118"/>
-      <c r="G20" s="137" t="s">
+      <c r="A20" s="120"/>
+      <c r="D20" s="121"/>
+      <c r="G20" s="139" t="s">
         <v>283</v>
       </c>
-      <c r="I20" s="119"/>
+      <c r="I20" s="122"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="117"/>
-      <c r="F21" s="138" t="s">
+      <c r="A21" s="120"/>
+      <c r="F21" s="140" t="s">
         <v>265</v>
       </c>
-      <c r="I21" s="119"/>
+      <c r="I21" s="122"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="120" t="s">
+      <c r="A22" s="123" t="s">
         <v>268</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>9002</v>
       </c>
-      <c r="D22" s="118" t="s">
+      <c r="D22" s="121" t="s">
         <v>269</v>
       </c>
-      <c r="E22" s="123" t="n">
+      <c r="E22" s="126" t="n">
         <f aca="false">E10-B22*TAN(2*(E19)/1000)+I17</f>
         <v>-36.7073914229833</v>
       </c>
-      <c r="F22" s="139" t="n">
+      <c r="F22" s="141" t="n">
         <f aca="false">'Modes A-F'!I54</f>
         <v>-23.247</v>
       </c>
-      <c r="G22" s="123" t="n">
+      <c r="G22" s="126" t="n">
         <f aca="false">E10-B22*TAN(2*(G19)/1000)+I17</f>
         <v>-31.75602924884</v>
       </c>
-      <c r="I22" s="119"/>
+      <c r="I22" s="122"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="120" t="s">
+      <c r="A23" s="123" t="s">
         <v>270</v>
       </c>
       <c r="B23" s="0" t="n">
         <f aca="false">B22+635</f>
         <v>9637</v>
       </c>
-      <c r="D23" s="118" t="s">
+      <c r="D23" s="121" t="s">
         <v>271</v>
       </c>
-      <c r="E23" s="123" t="n">
+      <c r="E23" s="126" t="n">
         <f aca="false">E11-B23*TAN(2*(E19)/1000)+I17</f>
         <v>44.2322674801944</v>
       </c>
-      <c r="F23" s="139" t="n">
+      <c r="F23" s="141" t="n">
         <f aca="false">'Modes A-F'!I56</f>
         <v>54.559</v>
       </c>
-      <c r="G23" s="123" t="n">
+      <c r="G23" s="126" t="n">
         <f aca="false">E11-B23*TAN(2*(G19)/1000)+I17</f>
         <v>49.5328981480704</v>
       </c>
-      <c r="I23" s="119"/>
+      <c r="I23" s="122"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="124" t="s">
+      <c r="A24" s="127" t="s">
         <v>272</v>
       </c>
-      <c r="B24" s="125" t="n">
+      <c r="B24" s="128" t="n">
         <f aca="false">B22+1790</f>
         <v>10792</v>
       </c>
-      <c r="C24" s="125"/>
-      <c r="D24" s="126" t="s">
+      <c r="C24" s="128"/>
+      <c r="D24" s="129" t="s">
         <v>273</v>
       </c>
-      <c r="E24" s="133" t="n">
+      <c r="E24" s="136" t="n">
         <f aca="false">E12-B24*TAN(2*(E19)/1000)+I17</f>
         <v>35.5118517843995</v>
       </c>
-      <c r="F24" s="140" t="n">
+      <c r="F24" s="142" t="n">
         <f aca="false">'Modes A-F'!I57</f>
         <v>47.758</v>
       </c>
-      <c r="G24" s="141" t="n">
+      <c r="G24" s="143" t="n">
         <f aca="false">E12-B24*TAN(2*(G19)/1000)+I17</f>
         <v>41.447766090482</v>
       </c>
-      <c r="H24" s="125"/>
-      <c r="I24" s="142"/>
+      <c r="H24" s="128"/>
+      <c r="I24" s="144"/>
     </row>
     <row r="28" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="143" t="s">
+      <c r="A28" s="145" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="143"/>
-      <c r="C28" s="143"/>
-      <c r="D28" s="113"/>
-      <c r="E28" s="113"/>
-      <c r="F28" s="130" t="s">
+      <c r="B28" s="145"/>
+      <c r="C28" s="145"/>
+      <c r="D28" s="116"/>
+      <c r="E28" s="116"/>
+      <c r="F28" s="133" t="s">
         <v>275</v>
       </c>
-      <c r="G28" s="113" t="n">
+      <c r="G28" s="116" t="n">
         <v>0.275</v>
       </c>
-      <c r="H28" s="113"/>
-      <c r="I28" s="131"/>
+      <c r="H28" s="116"/>
+      <c r="I28" s="134"/>
     </row>
     <row r="29" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="117"/>
-      <c r="D29" s="118" t="s">
+      <c r="A29" s="120"/>
+      <c r="D29" s="121" t="s">
         <v>267</v>
       </c>
       <c r="E29" s="0" t="n">
         <v>3.225</v>
       </c>
-      <c r="G29" s="72" t="n">
+      <c r="G29" s="75" t="n">
         <f aca="false">E29+G28</f>
         <v>3.5</v>
       </c>
-      <c r="H29" s="135" t="s">
+      <c r="H29" s="64" t="s">
         <v>279</v>
       </c>
-      <c r="I29" s="119" t="n">
+      <c r="I29" s="122" t="n">
         <f aca="false">B30*TAN(2*(E9-G29)/1000)</f>
         <v>0</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="120" t="s">
+      <c r="A30" s="123" t="s">
         <v>280</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>1908</v>
       </c>
-      <c r="D30" s="118" t="s">
+      <c r="D30" s="121" t="s">
         <v>281</v>
       </c>
       <c r="E30" s="0" t="n">
         <v>-6.583</v>
       </c>
-      <c r="G30" s="136" t="n">
+      <c r="G30" s="138" t="n">
         <f aca="false">E30+B30*TAN(2*(G29-E29)/1000)</f>
         <v>-5.53359989418549</v>
       </c>
-      <c r="I30" s="119"/>
+      <c r="I30" s="122"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="117"/>
-      <c r="D31" s="118" t="s">
+      <c r="A31" s="120"/>
+      <c r="D31" s="121" t="s">
         <v>282</v>
       </c>
       <c r="E31" s="0" t="n">
         <f aca="false">5+(3.5-E29)</f>
         <v>5.275</v>
       </c>
-      <c r="G31" s="72" t="n">
+      <c r="G31" s="75" t="n">
         <f aca="false">E31-G28</f>
         <v>5</v>
       </c>
-      <c r="I31" s="119"/>
+      <c r="I31" s="122"/>
     </row>
     <row r="32" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="117"/>
-      <c r="D32" s="118"/>
-      <c r="G32" s="137" t="s">
+      <c r="A32" s="120"/>
+      <c r="D32" s="121"/>
+      <c r="G32" s="139" t="s">
         <v>283</v>
       </c>
-      <c r="I32" s="119"/>
+      <c r="I32" s="122"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="117"/>
-      <c r="F33" s="138" t="s">
+      <c r="A33" s="120"/>
+      <c r="F33" s="140" t="s">
         <v>265</v>
       </c>
-      <c r="I33" s="119"/>
+      <c r="I33" s="122"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="120" t="s">
+      <c r="A34" s="123" t="s">
         <v>268</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>9002</v>
       </c>
-      <c r="D34" s="118" t="s">
+      <c r="D34" s="121" t="s">
         <v>269</v>
       </c>
-      <c r="E34" s="123" t="n">
+      <c r="E34" s="126" t="n">
         <f aca="false">E10-B34*TAN(2*(E31)/1000)</f>
         <v>-63.7156236638297</v>
       </c>
-      <c r="F34" s="139" t="n">
+      <c r="F34" s="141" t="n">
         <f aca="false">'Modes A-F'!G54</f>
         <v>-55.188</v>
       </c>
-      <c r="G34" s="123" t="n">
+      <c r="G34" s="126" t="n">
         <f aca="false">E10-B34*TAN(2*(G31)/1000)+I29</f>
         <v>-58.7640007866982</v>
       </c>
-      <c r="I34" s="119"/>
+      <c r="I34" s="122"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="120" t="s">
+      <c r="A35" s="123" t="s">
         <v>270</v>
       </c>
       <c r="B35" s="0" t="n">
         <f aca="false">B34+635</f>
         <v>9637</v>
       </c>
-      <c r="D35" s="118" t="s">
+      <c r="D35" s="121" t="s">
         <v>271</v>
       </c>
-      <c r="E35" s="123" t="n">
+      <c r="E35" s="126" t="n">
         <f aca="false">E11-B35*TAN(2*(E31)/1000)</f>
         <v>15.3188777773465</v>
       </c>
-      <c r="F35" s="139" t="n">
+      <c r="F35" s="141" t="n">
         <f aca="false">'Modes A-F'!G56</f>
         <v>24.4104</v>
       </c>
-      <c r="G35" s="123" t="n">
+      <c r="G35" s="126" t="n">
         <f aca="false">E11-B35*TAN(2*(G31)/1000)+I29</f>
         <v>20.6197875381681</v>
       </c>
-      <c r="I35" s="119"/>
+      <c r="I35" s="122"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="124" t="s">
+      <c r="A36" s="127" t="s">
         <v>272</v>
       </c>
-      <c r="B36" s="125" t="n">
+      <c r="B36" s="128" t="n">
         <f aca="false">B34+1790</f>
         <v>10792</v>
       </c>
-      <c r="C36" s="125"/>
-      <c r="D36" s="126" t="s">
+      <c r="C36" s="128"/>
+      <c r="D36" s="129" t="s">
         <v>273</v>
       </c>
-      <c r="E36" s="133" t="n">
+      <c r="E36" s="136" t="n">
         <f aca="false">E12-B36*TAN(2*(E31)/1000)</f>
         <v>3.13317567428902</v>
       </c>
-      <c r="F36" s="140" t="n">
+      <c r="F36" s="142" t="n">
         <f aca="false">'Modes A-F'!G57</f>
         <v>12.81</v>
       </c>
-      <c r="G36" s="133" t="n">
+      <c r="G36" s="136" t="n">
         <f aca="false">E12-B36*TAN(2*(G31)/1000)+I29</f>
         <v>9.06940252276749</v>
       </c>
-      <c r="H36" s="125"/>
-      <c r="I36" s="142"/>
+      <c r="H36" s="128"/>
+      <c r="I36" s="144"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -17888,10 +17896,10 @@
   <dimension ref="A1:CX484"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="F46:F47 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.26"/>
   </cols>
@@ -17964,7 +17972,7 @@
       <c r="A9" s="0" t="s">
         <v>292</v>
       </c>
-      <c r="B9" s="144" t="n">
+      <c r="B9" s="146" t="n">
         <v>1E-006</v>
       </c>
     </row>
@@ -17988,7 +17996,7 @@
       <c r="A12" s="0" t="s">
         <v>295</v>
       </c>
-      <c r="B12" s="144" t="n">
+      <c r="B12" s="146" t="n">
         <v>1E-005</v>
       </c>
     </row>
@@ -18084,7 +18092,7 @@
       <c r="A24" s="0" t="s">
         <v>307</v>
       </c>
-      <c r="B24" s="144" t="n">
+      <c r="B24" s="146" t="n">
         <v>1E-006</v>
       </c>
     </row>
@@ -18108,7 +18116,7 @@
       <c r="A27" s="0" t="s">
         <v>310</v>
       </c>
-      <c r="B27" s="144" t="n">
+      <c r="B27" s="146" t="n">
         <v>1E-005</v>
       </c>
     </row>
@@ -18204,7 +18212,7 @@
       <c r="A39" s="0" t="s">
         <v>322</v>
       </c>
-      <c r="B39" s="144" t="n">
+      <c r="B39" s="146" t="n">
         <v>1E-006</v>
       </c>
     </row>
@@ -18228,7 +18236,7 @@
       <c r="A42" s="0" t="s">
         <v>325</v>
       </c>
-      <c r="B42" s="144" t="n">
+      <c r="B42" s="146" t="n">
         <v>1E-005</v>
       </c>
     </row>
@@ -18324,7 +18332,7 @@
       <c r="A54" s="0" t="s">
         <v>337</v>
       </c>
-      <c r="B54" s="144" t="n">
+      <c r="B54" s="146" t="n">
         <v>1E-006</v>
       </c>
     </row>
@@ -18348,7 +18356,7 @@
       <c r="A57" s="0" t="s">
         <v>340</v>
       </c>
-      <c r="B57" s="144" t="n">
+      <c r="B57" s="146" t="n">
         <v>1E-005</v>
       </c>
     </row>
@@ -18412,7 +18420,7 @@
       <c r="A65" s="0" t="s">
         <v>348</v>
       </c>
-      <c r="B65" s="144" t="n">
+      <c r="B65" s="146" t="n">
         <v>8.1921E-011</v>
       </c>
     </row>
@@ -18420,7 +18428,7 @@
       <c r="A66" s="0" t="s">
         <v>349</v>
       </c>
-      <c r="B66" s="144" t="n">
+      <c r="B66" s="146" t="n">
         <v>6.1817E-009</v>
       </c>
     </row>
@@ -18428,7 +18436,7 @@
       <c r="A67" s="0" t="s">
         <v>350</v>
       </c>
-      <c r="B67" s="144" t="n">
+      <c r="B67" s="146" t="n">
         <v>-8.139E-009</v>
       </c>
     </row>
@@ -18436,7 +18444,7 @@
       <c r="A68" s="0" t="s">
         <v>351</v>
       </c>
-      <c r="B68" s="144" t="n">
+      <c r="B68" s="146" t="n">
         <v>4.2612E-009</v>
       </c>
     </row>
@@ -18756,7 +18764,7 @@
       <c r="A108" s="0" t="s">
         <v>391</v>
       </c>
-      <c r="B108" s="144" t="n">
+      <c r="B108" s="146" t="n">
         <v>1E-006</v>
       </c>
     </row>
@@ -18780,7 +18788,7 @@
       <c r="A111" s="0" t="s">
         <v>394</v>
       </c>
-      <c r="B111" s="144" t="n">
+      <c r="B111" s="146" t="n">
         <v>1E-005</v>
       </c>
     </row>
@@ -18876,7 +18884,7 @@
       <c r="A123" s="0" t="s">
         <v>406</v>
       </c>
-      <c r="B123" s="144" t="n">
+      <c r="B123" s="146" t="n">
         <v>1E-006</v>
       </c>
     </row>
@@ -18900,7 +18908,7 @@
       <c r="A126" s="0" t="s">
         <v>409</v>
       </c>
-      <c r="B126" s="144" t="n">
+      <c r="B126" s="146" t="n">
         <v>1E-005</v>
       </c>
     </row>
@@ -18996,7 +19004,7 @@
       <c r="A138" s="0" t="s">
         <v>421</v>
       </c>
-      <c r="B138" s="144" t="n">
+      <c r="B138" s="146" t="n">
         <v>1E-006</v>
       </c>
     </row>
@@ -19020,7 +19028,7 @@
       <c r="A141" s="0" t="s">
         <v>424</v>
       </c>
-      <c r="B141" s="144" t="n">
+      <c r="B141" s="146" t="n">
         <v>1E-005</v>
       </c>
     </row>
@@ -19116,7 +19124,7 @@
       <c r="A153" s="0" t="s">
         <v>436</v>
       </c>
-      <c r="B153" s="144" t="n">
+      <c r="B153" s="146" t="n">
         <v>1E-006</v>
       </c>
     </row>
@@ -19140,7 +19148,7 @@
       <c r="A156" s="0" t="s">
         <v>439</v>
       </c>
-      <c r="B156" s="144" t="n">
+      <c r="B156" s="146" t="n">
         <v>1E-005</v>
       </c>
     </row>
@@ -19204,7 +19212,7 @@
       <c r="A164" s="0" t="s">
         <v>447</v>
       </c>
-      <c r="B164" s="144" t="n">
+      <c r="B164" s="146" t="n">
         <v>1.9024E-008</v>
       </c>
     </row>
@@ -19212,7 +19220,7 @@
       <c r="A165" s="0" t="s">
         <v>448</v>
       </c>
-      <c r="B165" s="144" t="n">
+      <c r="B165" s="146" t="n">
         <v>-9.5679E-009</v>
       </c>
     </row>
@@ -19220,7 +19228,7 @@
       <c r="A166" s="0" t="s">
         <v>449</v>
       </c>
-      <c r="B166" s="144" t="n">
+      <c r="B166" s="146" t="n">
         <v>-1.1631E-009</v>
       </c>
     </row>
@@ -19228,7 +19236,7 @@
       <c r="A167" s="0" t="s">
         <v>450</v>
       </c>
-      <c r="B167" s="144" t="n">
+      <c r="B167" s="146" t="n">
         <v>1.027E-008</v>
       </c>
     </row>
@@ -19364,7 +19372,7 @@
       <c r="A184" s="0" t="s">
         <v>467</v>
       </c>
-      <c r="B184" s="144" t="n">
+      <c r="B184" s="146" t="n">
         <v>2.8833E-008</v>
       </c>
     </row>
@@ -19372,7 +19380,7 @@
       <c r="A185" s="0" t="s">
         <v>468</v>
       </c>
-      <c r="B185" s="144" t="n">
+      <c r="B185" s="146" t="n">
         <v>2.8833E-008</v>
       </c>
     </row>
@@ -19404,7 +19412,7 @@
       <c r="A189" s="0" t="s">
         <v>472</v>
       </c>
-      <c r="B189" s="144" t="n">
+      <c r="B189" s="146" t="n">
         <v>4761600</v>
       </c>
     </row>
@@ -19428,7 +19436,7 @@
       <c r="A192" s="0" t="s">
         <v>475</v>
       </c>
-      <c r="B192" s="144" t="n">
+      <c r="B192" s="146" t="n">
         <v>2.8343E-008</v>
       </c>
     </row>
@@ -19436,7 +19444,7 @@
       <c r="A193" s="0" t="s">
         <v>476</v>
       </c>
-      <c r="B193" s="144" t="n">
+      <c r="B193" s="146" t="n">
         <v>-7.401E-010</v>
       </c>
     </row>
@@ -19444,7 +19452,7 @@
       <c r="A194" s="0" t="s">
         <v>477</v>
       </c>
-      <c r="B194" s="144" t="n">
+      <c r="B194" s="146" t="n">
         <v>-1.4084E-009</v>
       </c>
     </row>
@@ -19452,7 +19460,7 @@
       <c r="A195" s="0" t="s">
         <v>478</v>
       </c>
-      <c r="B195" s="144" t="n">
+      <c r="B195" s="146" t="n">
         <v>2.0325E-008</v>
       </c>
     </row>
@@ -20876,40 +20884,40 @@
       <c r="B337" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C337" s="144" t="n">
+      <c r="C337" s="146" t="n">
         <v>8.3006E-011</v>
       </c>
-      <c r="D337" s="144" t="n">
+      <c r="D337" s="146" t="n">
         <v>8.2839E-011</v>
       </c>
-      <c r="E337" s="144" t="n">
+      <c r="E337" s="146" t="n">
         <v>8.2777E-011</v>
       </c>
-      <c r="F337" s="144" t="n">
+      <c r="F337" s="146" t="n">
         <v>8.1528E-011</v>
       </c>
-      <c r="G337" s="144" t="n">
+      <c r="G337" s="146" t="n">
         <v>8.2662E-011</v>
       </c>
-      <c r="H337" s="144" t="n">
+      <c r="H337" s="146" t="n">
         <v>8.3572E-011</v>
       </c>
-      <c r="I337" s="144" t="n">
+      <c r="I337" s="146" t="n">
         <v>8.489E-011</v>
       </c>
-      <c r="J337" s="144" t="n">
+      <c r="J337" s="146" t="n">
         <v>8.3896E-011</v>
       </c>
-      <c r="K337" s="144" t="n">
+      <c r="K337" s="146" t="n">
         <v>8.2012E-011</v>
       </c>
-      <c r="L337" s="144" t="n">
+      <c r="L337" s="146" t="n">
         <v>8.0897E-011</v>
       </c>
-      <c r="M337" s="144" t="n">
+      <c r="M337" s="146" t="n">
         <v>8.29E-011</v>
       </c>
-      <c r="N337" s="144" t="n">
+      <c r="N337" s="146" t="n">
         <v>8.0797E-011</v>
       </c>
     </row>
@@ -20920,40 +20928,40 @@
       <c r="B338" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C338" s="144" t="n">
+      <c r="C338" s="146" t="n">
         <v>6.3068E-009</v>
       </c>
-      <c r="D338" s="144" t="n">
+      <c r="D338" s="146" t="n">
         <v>6.0737E-009</v>
       </c>
-      <c r="E338" s="144" t="n">
+      <c r="E338" s="146" t="n">
         <v>6.6921E-009</v>
       </c>
-      <c r="F338" s="144" t="n">
+      <c r="F338" s="146" t="n">
         <v>5.7007E-009</v>
       </c>
-      <c r="G338" s="144" t="n">
+      <c r="G338" s="146" t="n">
         <v>5.6393E-009</v>
       </c>
-      <c r="H338" s="144" t="n">
+      <c r="H338" s="146" t="n">
         <v>6.6627E-009</v>
       </c>
-      <c r="I338" s="144" t="n">
+      <c r="I338" s="146" t="n">
         <v>6.6038E-009</v>
       </c>
-      <c r="J338" s="144" t="n">
+      <c r="J338" s="146" t="n">
         <v>5.87E-009</v>
       </c>
-      <c r="K338" s="144" t="n">
+      <c r="K338" s="146" t="n">
         <v>6.1792E-009</v>
       </c>
-      <c r="L338" s="144" t="n">
+      <c r="L338" s="146" t="n">
         <v>5.3276E-009</v>
       </c>
-      <c r="M338" s="144" t="n">
+      <c r="M338" s="146" t="n">
         <v>6.513E-009</v>
       </c>
-      <c r="N338" s="144" t="n">
+      <c r="N338" s="146" t="n">
         <v>5.9829E-009</v>
       </c>
     </row>
@@ -20964,40 +20972,40 @@
       <c r="B339" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C339" s="144" t="n">
+      <c r="C339" s="146" t="n">
         <v>-7.2948E-009</v>
       </c>
-      <c r="D339" s="144" t="n">
+      <c r="D339" s="146" t="n">
         <v>-7.6015E-009</v>
       </c>
-      <c r="E339" s="144" t="n">
+      <c r="E339" s="146" t="n">
         <v>-7.4862E-009</v>
       </c>
-      <c r="F339" s="144" t="n">
+      <c r="F339" s="146" t="n">
         <v>-8.5513E-009</v>
       </c>
-      <c r="G339" s="144" t="n">
+      <c r="G339" s="146" t="n">
         <v>-8.3206E-009</v>
       </c>
-      <c r="H339" s="144" t="n">
+      <c r="H339" s="146" t="n">
         <v>-7.5942E-009</v>
       </c>
-      <c r="I339" s="144" t="n">
+      <c r="I339" s="146" t="n">
         <v>-7.5377E-009</v>
       </c>
-      <c r="J339" s="144" t="n">
+      <c r="J339" s="146" t="n">
         <v>-8.5415E-009</v>
       </c>
-      <c r="K339" s="144" t="n">
+      <c r="K339" s="146" t="n">
         <v>-7.7635E-009</v>
       </c>
-      <c r="L339" s="144" t="n">
+      <c r="L339" s="146" t="n">
         <v>-8.0482E-009</v>
       </c>
-      <c r="M339" s="144" t="n">
+      <c r="M339" s="146" t="n">
         <v>-8.2175E-009</v>
       </c>
-      <c r="N339" s="144" t="n">
+      <c r="N339" s="146" t="n">
         <v>-7.9966E-009</v>
       </c>
     </row>
@@ -21008,40 +21016,40 @@
       <c r="B340" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C340" s="144" t="n">
+      <c r="C340" s="146" t="n">
         <v>4.8625E-009</v>
       </c>
-      <c r="D340" s="144" t="n">
+      <c r="D340" s="146" t="n">
         <v>4.433E-009</v>
       </c>
-      <c r="E340" s="144" t="n">
+      <c r="E340" s="146" t="n">
         <v>3.4611E-009</v>
       </c>
-      <c r="F340" s="144" t="n">
+      <c r="F340" s="146" t="n">
         <v>3.9372E-009</v>
       </c>
-      <c r="G340" s="144" t="n">
+      <c r="G340" s="146" t="n">
         <v>4.8526E-009</v>
       </c>
-      <c r="H340" s="144" t="n">
+      <c r="H340" s="146" t="n">
         <v>4.5041E-009</v>
       </c>
-      <c r="I340" s="144" t="n">
+      <c r="I340" s="146" t="n">
         <v>4.5311E-009</v>
       </c>
-      <c r="J340" s="144" t="n">
+      <c r="J340" s="146" t="n">
         <v>4.2882E-009</v>
       </c>
-      <c r="K340" s="144" t="n">
+      <c r="K340" s="146" t="n">
         <v>4.4551E-009</v>
       </c>
-      <c r="L340" s="144" t="n">
+      <c r="L340" s="146" t="n">
         <v>4.136E-009</v>
       </c>
-      <c r="M340" s="144" t="n">
+      <c r="M340" s="146" t="n">
         <v>3.9078E-009</v>
       </c>
-      <c r="N340" s="144" t="n">
+      <c r="N340" s="146" t="n">
         <v>3.9593E-009</v>
       </c>
     </row>
@@ -21756,40 +21764,40 @@
       <c r="B357" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C357" s="144" t="n">
+      <c r="C357" s="146" t="n">
         <v>2.1231E-008</v>
       </c>
-      <c r="D357" s="144" t="n">
+      <c r="D357" s="146" t="n">
         <v>1.9514E-008</v>
       </c>
-      <c r="E357" s="144" t="n">
+      <c r="E357" s="146" t="n">
         <v>1.8533E-008</v>
       </c>
-      <c r="F357" s="144" t="n">
+      <c r="F357" s="146" t="n">
         <v>2.1231E-008</v>
       </c>
-      <c r="G357" s="144" t="n">
+      <c r="G357" s="146" t="n">
         <v>2.4174E-008</v>
       </c>
-      <c r="H357" s="144" t="n">
+      <c r="H357" s="146" t="n">
         <v>1.9024E-008</v>
       </c>
-      <c r="I357" s="144" t="n">
+      <c r="I357" s="146" t="n">
         <v>2.8588E-008</v>
       </c>
-      <c r="J357" s="144" t="n">
+      <c r="J357" s="146" t="n">
         <v>1.9024E-008</v>
       </c>
-      <c r="K357" s="144" t="n">
+      <c r="K357" s="146" t="n">
         <v>3.2757E-008</v>
       </c>
-      <c r="L357" s="144" t="n">
+      <c r="L357" s="146" t="n">
         <v>3.5455E-008</v>
       </c>
-      <c r="M357" s="144" t="n">
+      <c r="M357" s="146" t="n">
         <v>2.025E-008</v>
       </c>
-      <c r="N357" s="144" t="n">
+      <c r="N357" s="146" t="n">
         <v>2.1231E-008</v>
       </c>
     </row>
@@ -21800,40 +21808,40 @@
       <c r="B358" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C358" s="144" t="n">
+      <c r="C358" s="146" t="n">
         <v>-1.766E-008</v>
       </c>
-      <c r="D358" s="144" t="n">
+      <c r="D358" s="146" t="n">
         <v>-4.4184E-009</v>
       </c>
-      <c r="E358" s="144" t="n">
+      <c r="E358" s="146" t="n">
         <v>-1.1284E-008</v>
       </c>
-      <c r="F358" s="144" t="n">
+      <c r="F358" s="146" t="n">
         <v>-1.1039E-008</v>
       </c>
-      <c r="G358" s="144" t="n">
+      <c r="G358" s="146" t="n">
         <v>-9.5679E-009</v>
       </c>
-      <c r="H358" s="144" t="n">
+      <c r="H358" s="146" t="n">
         <v>-1.1284E-008</v>
       </c>
-      <c r="I358" s="144" t="n">
+      <c r="I358" s="146" t="n">
         <v>-2.2114E-009</v>
       </c>
-      <c r="J358" s="144" t="n">
+      <c r="J358" s="146" t="n">
         <v>-5.3992E-009</v>
       </c>
-      <c r="K358" s="144" t="n">
+      <c r="K358" s="146" t="n">
         <v>9.7642E-010</v>
       </c>
-      <c r="L358" s="144" t="n">
+      <c r="L358" s="146" t="n">
         <v>6.3712E-009</v>
       </c>
-      <c r="M358" s="144" t="n">
+      <c r="M358" s="146" t="n">
         <v>-1.153E-008</v>
       </c>
-      <c r="N358" s="144" t="n">
+      <c r="N358" s="146" t="n">
         <v>-9.8131E-009</v>
       </c>
     </row>
@@ -21844,40 +21852,40 @@
       <c r="B359" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C359" s="144" t="n">
+      <c r="C359" s="146" t="n">
         <v>-9.0112E-009</v>
       </c>
-      <c r="D359" s="144" t="n">
+      <c r="D359" s="146" t="n">
         <v>-4.3514E-009</v>
       </c>
-      <c r="E359" s="144" t="n">
+      <c r="E359" s="146" t="n">
         <v>-6.0682E-009</v>
       </c>
-      <c r="F359" s="144" t="n">
+      <c r="F359" s="146" t="n">
         <v>-9.0112E-009</v>
       </c>
-      <c r="G359" s="144" t="n">
+      <c r="G359" s="146" t="n">
         <v>-4.5967E-009</v>
       </c>
-      <c r="H359" s="144" t="n">
+      <c r="H359" s="146" t="n">
         <v>-1.0483E-008</v>
       </c>
-      <c r="I359" s="144" t="n">
+      <c r="I359" s="146" t="n">
         <v>7.6659E-009</v>
       </c>
-      <c r="J359" s="144" t="n">
+      <c r="J359" s="146" t="n">
         <v>-3.3704E-009</v>
       </c>
-      <c r="K359" s="144" t="n">
+      <c r="K359" s="146" t="n">
         <v>6.6849E-009</v>
       </c>
-      <c r="L359" s="144" t="n">
+      <c r="L359" s="146" t="n">
         <v>5.2134E-009</v>
       </c>
-      <c r="M359" s="144" t="n">
+      <c r="M359" s="146" t="n">
         <v>-1.6536E-009</v>
       </c>
-      <c r="N359" s="144" t="n">
+      <c r="N359" s="146" t="n">
         <v>-5.5777E-009</v>
       </c>
     </row>
@@ -21888,40 +21896,40 @@
       <c r="B360" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C360" s="144" t="n">
+      <c r="C360" s="146" t="n">
         <v>7.8174E-009</v>
       </c>
-      <c r="D360" s="144" t="n">
+      <c r="D360" s="146" t="n">
         <v>2.3513E-008</v>
       </c>
-      <c r="E360" s="144" t="n">
+      <c r="E360" s="146" t="n">
         <v>1.7382E-008</v>
       </c>
-      <c r="F360" s="144" t="n">
+      <c r="F360" s="146" t="n">
         <v>1.1006E-008</v>
       </c>
-      <c r="G360" s="144" t="n">
+      <c r="G360" s="146" t="n">
         <v>1.5665E-008</v>
       </c>
-      <c r="H360" s="144" t="n">
+      <c r="H360" s="146" t="n">
         <v>1.2477E-008</v>
       </c>
-      <c r="I360" s="144" t="n">
+      <c r="I360" s="146" t="n">
         <v>2.057E-008</v>
       </c>
-      <c r="J360" s="144" t="n">
+      <c r="J360" s="146" t="n">
         <v>1.9835E-008</v>
       </c>
-      <c r="K360" s="144" t="n">
+      <c r="K360" s="146" t="n">
         <v>2.5721E-008</v>
       </c>
-      <c r="L360" s="144" t="n">
+      <c r="L360" s="146" t="n">
         <v>2.5475E-008</v>
       </c>
-      <c r="M360" s="144" t="n">
+      <c r="M360" s="146" t="n">
         <v>1.076E-008</v>
       </c>
-      <c r="N360" s="144" t="n">
+      <c r="N360" s="146" t="n">
         <v>1.3213E-008</v>
       </c>
     </row>
@@ -22064,7 +22072,7 @@
       <c r="B364" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C364" s="144" t="n">
+      <c r="C364" s="146" t="n">
         <v>2.8343E-008</v>
       </c>
       <c r="D364" s="0" t="n">
@@ -22108,7 +22116,7 @@
       <c r="B365" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C365" s="144" t="n">
+      <c r="C365" s="146" t="n">
         <v>-7.401E-010</v>
       </c>
       <c r="D365" s="0" t="n">
@@ -22152,7 +22160,7 @@
       <c r="B366" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C366" s="144" t="n">
+      <c r="C366" s="146" t="n">
         <v>-1.4084E-009</v>
       </c>
       <c r="D366" s="0" t="n">
@@ -22196,7 +22204,7 @@
       <c r="B367" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C367" s="144" t="n">
+      <c r="C367" s="146" t="n">
         <v>2.0325E-008</v>
       </c>
       <c r="D367" s="0" t="n">
@@ -23959,10 +23967,10 @@
   <dimension ref="A1:G2383"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A44" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="1" sqref="F46:F47 B4"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="56.14"/>
@@ -23972,13 +23980,13 @@
       <c r="A1" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B1" s="145" t="s">
+      <c r="B1" s="147" t="s">
         <v>814</v>
       </c>
-      <c r="C1" s="145" t="n">
+      <c r="C1" s="147" t="n">
         <v>350</v>
       </c>
-      <c r="D1" s="145" t="s">
+      <c r="D1" s="147" t="s">
         <v>815</v>
       </c>
     </row>
@@ -23986,10 +23994,10 @@
       <c r="A2" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B2" s="145" t="s">
+      <c r="B2" s="147" t="s">
         <v>816</v>
       </c>
-      <c r="C2" s="145" t="n">
+      <c r="C2" s="147" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -23997,10 +24005,10 @@
       <c r="A3" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="145" t="s">
+      <c r="B3" s="147" t="s">
         <v>817</v>
       </c>
-      <c r="C3" s="145" t="n">
+      <c r="C3" s="147" t="n">
         <v>0.0004</v>
       </c>
     </row>
@@ -24104,7 +24112,7 @@
       <c r="B16" s="0" t="s">
         <v>832</v>
       </c>
-      <c r="C16" s="144" t="n">
+      <c r="C16" s="146" t="n">
         <v>3.71179E-009</v>
       </c>
     </row>
@@ -24112,7 +24120,7 @@
       <c r="B17" s="0" t="s">
         <v>833</v>
       </c>
-      <c r="C17" s="144" t="n">
+      <c r="C17" s="146" t="n">
         <v>3.71272E-009</v>
       </c>
     </row>
@@ -24120,7 +24128,7 @@
       <c r="B18" s="0" t="s">
         <v>834</v>
       </c>
-      <c r="C18" s="144" t="n">
+      <c r="C18" s="146" t="n">
         <v>3.71425E-009</v>
       </c>
     </row>
@@ -24128,7 +24136,7 @@
       <c r="B19" s="0" t="s">
         <v>835</v>
       </c>
-      <c r="C19" s="144" t="n">
+      <c r="C19" s="146" t="n">
         <v>3.71562E-009</v>
       </c>
     </row>
@@ -24616,7 +24624,7 @@
       <c r="B80" s="0" t="s">
         <v>903</v>
       </c>
-      <c r="C80" s="144" t="n">
+      <c r="C80" s="146" t="n">
         <v>1.58855E-007</v>
       </c>
     </row>
@@ -24664,7 +24672,7 @@
       <c r="B86" s="0" t="s">
         <v>909</v>
       </c>
-      <c r="C86" s="144" t="n">
+      <c r="C86" s="146" t="n">
         <v>1.58316E-007</v>
       </c>
     </row>
@@ -24696,7 +24704,7 @@
       <c r="B90" s="0" t="s">
         <v>913</v>
       </c>
-      <c r="C90" s="144" t="n">
+      <c r="C90" s="146" t="n">
         <v>1.57838E-007</v>
       </c>
     </row>
@@ -24784,7 +24792,7 @@
       <c r="B101" s="0" t="s">
         <v>925</v>
       </c>
-      <c r="C101" s="144" t="n">
+      <c r="C101" s="146" t="n">
         <v>2.397E-009</v>
       </c>
     </row>
@@ -24960,7 +24968,7 @@
       <c r="B123" s="0" t="s">
         <v>949</v>
       </c>
-      <c r="C123" s="144" t="n">
+      <c r="C123" s="146" t="n">
         <v>2.37898E-010</v>
       </c>
     </row>
@@ -25024,7 +25032,7 @@
       <c r="B131" s="0" t="s">
         <v>957</v>
       </c>
-      <c r="C131" s="144" t="n">
+      <c r="C131" s="146" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -25040,7 +25048,7 @@
       <c r="B133" s="0" t="s">
         <v>959</v>
       </c>
-      <c r="C133" s="144" t="n">
+      <c r="C133" s="146" t="n">
         <v>1.97895E-005</v>
       </c>
     </row>
@@ -25560,7 +25568,7 @@
       <c r="B198" s="0" t="s">
         <v>1026</v>
       </c>
-      <c r="C198" s="144" t="n">
+      <c r="C198" s="146" t="n">
         <v>2.78422E-007</v>
       </c>
     </row>
@@ -25608,7 +25616,7 @@
       <c r="B204" s="0" t="s">
         <v>1032</v>
       </c>
-      <c r="C204" s="144" t="n">
+      <c r="C204" s="146" t="n">
         <v>2.77565E-007</v>
       </c>
     </row>
@@ -25640,7 +25648,7 @@
       <c r="B208" s="0" t="s">
         <v>1036</v>
       </c>
-      <c r="C208" s="144" t="n">
+      <c r="C208" s="146" t="n">
         <v>2.76716E-007</v>
       </c>
     </row>
@@ -25728,7 +25736,7 @@
       <c r="B219" s="0" t="s">
         <v>1047</v>
       </c>
-      <c r="C219" s="144" t="n">
+      <c r="C219" s="146" t="n">
         <v>5.98328E-009</v>
       </c>
     </row>
@@ -25904,7 +25912,7 @@
       <c r="B241" s="0" t="s">
         <v>1070</v>
       </c>
-      <c r="C241" s="144" t="n">
+      <c r="C241" s="146" t="n">
         <v>4.11728E-010</v>
       </c>
     </row>
@@ -25968,7 +25976,7 @@
       <c r="B249" s="0" t="s">
         <v>1078</v>
       </c>
-      <c r="C249" s="144" t="n">
+      <c r="C249" s="146" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -25984,7 +25992,7 @@
       <c r="B251" s="0" t="s">
         <v>1080</v>
       </c>
-      <c r="C251" s="144" t="n">
+      <c r="C251" s="146" t="n">
         <v>3.46956E-005</v>
       </c>
     </row>
@@ -26504,7 +26512,7 @@
       <c r="B316" s="0" t="s">
         <v>1145</v>
       </c>
-      <c r="C316" s="144" t="n">
+      <c r="C316" s="146" t="n">
         <v>5.45673E-012</v>
       </c>
     </row>
@@ -26552,7 +26560,7 @@
       <c r="B322" s="0" t="s">
         <v>1151</v>
       </c>
-      <c r="C322" s="144" t="n">
+      <c r="C322" s="146" t="n">
         <v>7.71713E-013</v>
       </c>
     </row>
@@ -26584,7 +26592,7 @@
       <c r="B326" s="0" t="s">
         <v>1155</v>
       </c>
-      <c r="C326" s="144" t="n">
+      <c r="C326" s="146" t="n">
         <v>-7.72781E-012</v>
       </c>
     </row>
@@ -26672,7 +26680,7 @@
       <c r="B337" s="0" t="s">
         <v>1166</v>
       </c>
-      <c r="C337" s="144" t="n">
+      <c r="C337" s="146" t="n">
         <v>5.61762E-010</v>
       </c>
     </row>
@@ -26848,7 +26856,7 @@
       <c r="B359" s="0" t="s">
         <v>1189</v>
       </c>
-      <c r="C359" s="144" t="n">
+      <c r="C359" s="146" t="n">
         <v>2.605E-012</v>
       </c>
     </row>
@@ -26912,7 +26920,7 @@
       <c r="B367" s="0" t="s">
         <v>1197</v>
       </c>
-      <c r="C367" s="144" t="n">
+      <c r="C367" s="146" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -26928,7 +26936,7 @@
       <c r="B369" s="0" t="s">
         <v>1199</v>
       </c>
-      <c r="C369" s="144" t="n">
+      <c r="C369" s="146" t="n">
         <v>9.64642E-011</v>
       </c>
     </row>
@@ -27448,7 +27456,7 @@
       <c r="B434" s="0" t="s">
         <v>1264</v>
       </c>
-      <c r="C434" s="144" t="n">
+      <c r="C434" s="146" t="n">
         <v>5.42202E-012</v>
       </c>
     </row>
@@ -27496,7 +27504,7 @@
       <c r="B440" s="0" t="s">
         <v>1270</v>
       </c>
-      <c r="C440" s="144" t="n">
+      <c r="C440" s="146" t="n">
         <v>5.83458E-013</v>
       </c>
     </row>
@@ -27528,7 +27536,7 @@
       <c r="B444" s="0" t="s">
         <v>1274</v>
       </c>
-      <c r="C444" s="144" t="n">
+      <c r="C444" s="146" t="n">
         <v>-5.09224E-012</v>
       </c>
     </row>
@@ -27616,7 +27624,7 @@
       <c r="B455" s="0" t="s">
         <v>1285</v>
       </c>
-      <c r="C455" s="144" t="n">
+      <c r="C455" s="146" t="n">
         <v>2.08783E-010</v>
       </c>
     </row>
@@ -27792,7 +27800,7 @@
       <c r="B477" s="0" t="s">
         <v>1308</v>
       </c>
-      <c r="C477" s="144" t="n">
+      <c r="C477" s="146" t="n">
         <v>2.32565E-012</v>
       </c>
     </row>
@@ -27856,7 +27864,7 @@
       <c r="B485" s="0" t="s">
         <v>1316</v>
       </c>
-      <c r="C485" s="144" t="n">
+      <c r="C485" s="146" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -27872,7 +27880,7 @@
       <c r="B487" s="0" t="s">
         <v>1318</v>
       </c>
-      <c r="C487" s="144" t="n">
+      <c r="C487" s="146" t="n">
         <v>7.29322E-011</v>
       </c>
     </row>
@@ -27960,7 +27968,7 @@
       <c r="B498" s="0" t="s">
         <v>1329</v>
       </c>
-      <c r="C498" s="144" t="n">
+      <c r="C498" s="146" t="n">
         <v>3.71179E-009</v>
       </c>
     </row>
@@ -27968,7 +27976,7 @@
       <c r="B499" s="0" t="s">
         <v>1330</v>
       </c>
-      <c r="C499" s="144" t="n">
+      <c r="C499" s="146" t="n">
         <v>3.71272E-009</v>
       </c>
     </row>
@@ -27976,7 +27984,7 @@
       <c r="B500" s="0" t="s">
         <v>1331</v>
       </c>
-      <c r="C500" s="144" t="n">
+      <c r="C500" s="146" t="n">
         <v>3.71425E-009</v>
       </c>
     </row>
@@ -27984,7 +27992,7 @@
       <c r="B501" s="0" t="s">
         <v>1332</v>
       </c>
-      <c r="C501" s="144" t="n">
+      <c r="C501" s="146" t="n">
         <v>3.71562E-009</v>
       </c>
     </row>
@@ -28552,7 +28560,7 @@
       <c r="B572" s="0" t="s">
         <v>1403</v>
       </c>
-      <c r="C572" s="144" t="n">
+      <c r="C572" s="146" t="n">
         <v>1.19678E-007</v>
       </c>
     </row>
@@ -28600,7 +28608,7 @@
       <c r="B578" s="0" t="s">
         <v>1409</v>
       </c>
-      <c r="C578" s="144" t="n">
+      <c r="C578" s="146" t="n">
         <v>1.19249E-007</v>
       </c>
     </row>
@@ -28632,7 +28640,7 @@
       <c r="B582" s="0" t="s">
         <v>1413</v>
       </c>
-      <c r="C582" s="144" t="n">
+      <c r="C582" s="146" t="n">
         <v>1.18808E-007</v>
       </c>
     </row>
@@ -28720,7 +28728,7 @@
       <c r="B593" s="0" t="s">
         <v>1424</v>
       </c>
-      <c r="C593" s="144" t="n">
+      <c r="C593" s="146" t="n">
         <v>3.58628E-009</v>
       </c>
     </row>
@@ -28896,7 +28904,7 @@
       <c r="B615" s="0" t="s">
         <v>1447</v>
       </c>
-      <c r="C615" s="144" t="n">
+      <c r="C615" s="146" t="n">
         <v>1.9029E-010</v>
       </c>
     </row>
@@ -28960,7 +28968,7 @@
       <c r="B623" s="0" t="s">
         <v>1455</v>
       </c>
-      <c r="C623" s="144" t="n">
+      <c r="C623" s="146" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -28976,7 +28984,7 @@
       <c r="B625" s="0" t="s">
         <v>1457</v>
       </c>
-      <c r="C625" s="144" t="n">
+      <c r="C625" s="146" t="n">
         <v>1.49062E-005</v>
       </c>
     </row>
@@ -29496,7 +29504,7 @@
       <c r="B690" s="0" t="s">
         <v>1522</v>
       </c>
-      <c r="C690" s="144" t="n">
+      <c r="C690" s="146" t="n">
         <v>5.80654E-012</v>
       </c>
     </row>
@@ -29544,7 +29552,7 @@
       <c r="B696" s="0" t="s">
         <v>1528</v>
       </c>
-      <c r="C696" s="144" t="n">
+      <c r="C696" s="146" t="n">
         <v>-1.88255E-013</v>
       </c>
     </row>
@@ -29576,7 +29584,7 @@
       <c r="B700" s="0" t="s">
         <v>1532</v>
       </c>
-      <c r="C700" s="144" t="n">
+      <c r="C700" s="146" t="n">
         <v>-6.71043E-012</v>
       </c>
     </row>
@@ -29664,7 +29672,7 @@
       <c r="B711" s="0" t="s">
         <v>1543</v>
       </c>
-      <c r="C711" s="144" t="n">
+      <c r="C711" s="146" t="n">
         <v>-3.52979E-010</v>
       </c>
     </row>
@@ -29840,7 +29848,7 @@
       <c r="B733" s="0" t="s">
         <v>1566</v>
       </c>
-      <c r="C733" s="144" t="n">
+      <c r="C733" s="146" t="n">
         <v>2.64443E-012</v>
       </c>
     </row>
@@ -29904,7 +29912,7 @@
       <c r="B741" s="0" t="s">
         <v>1574</v>
       </c>
-      <c r="C741" s="144" t="n">
+      <c r="C741" s="146" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -29920,7 +29928,7 @@
       <c r="B743" s="0" t="s">
         <v>1576</v>
       </c>
-      <c r="C743" s="144" t="n">
+      <c r="C743" s="146" t="n">
         <v>-2.35319E-011</v>
       </c>
     </row>
@@ -30476,7 +30484,7 @@
       <c r="B811" s="0" t="s">
         <v>1652</v>
       </c>
-      <c r="C811" s="144" t="n">
+      <c r="C811" s="146" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -30992,7 +31000,7 @@
       <c r="B874" s="0" t="s">
         <v>1717</v>
       </c>
-      <c r="C874" s="144" t="n">
+      <c r="C874" s="146" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -31508,7 +31516,7 @@
       <c r="B937" s="0" t="s">
         <v>1782</v>
       </c>
-      <c r="C937" s="144" t="n">
+      <c r="C937" s="146" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -32024,7 +32032,7 @@
       <c r="B1000" s="0" t="s">
         <v>1847</v>
       </c>
-      <c r="C1000" s="144" t="n">
+      <c r="C1000" s="146" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -32540,7 +32548,7 @@
       <c r="B1063" s="0" t="s">
         <v>1912</v>
       </c>
-      <c r="C1063" s="144" t="n">
+      <c r="C1063" s="146" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -33056,7 +33064,7 @@
       <c r="B1126" s="0" t="s">
         <v>1977</v>
       </c>
-      <c r="C1126" s="144" t="n">
+      <c r="C1126" s="146" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -33572,7 +33580,7 @@
       <c r="B1189" s="0" t="s">
         <v>2042</v>
       </c>
-      <c r="C1189" s="144" t="n">
+      <c r="C1189" s="146" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -34088,7 +34096,7 @@
       <c r="B1252" s="0" t="s">
         <v>2107</v>
       </c>
-      <c r="C1252" s="144" t="n">
+      <c r="C1252" s="146" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -34604,7 +34612,7 @@
       <c r="B1315" s="0" t="s">
         <v>2172</v>
       </c>
-      <c r="C1315" s="144" t="n">
+      <c r="C1315" s="146" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -35120,7 +35128,7 @@
       <c r="B1378" s="0" t="s">
         <v>2237</v>
       </c>
-      <c r="C1378" s="144" t="n">
+      <c r="C1378" s="146" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -35636,7 +35644,7 @@
       <c r="B1441" s="0" t="s">
         <v>2302</v>
       </c>
-      <c r="C1441" s="144" t="n">
+      <c r="C1441" s="146" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -36084,7 +36092,7 @@
       <c r="B1497" s="0" t="s">
         <v>2361</v>
       </c>
-      <c r="C1497" s="144" t="n">
+      <c r="C1497" s="146" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -36710,7 +36718,7 @@
       <c r="B1576" s="0" t="s">
         <v>2445</v>
       </c>
-      <c r="C1576" s="144" t="n">
+      <c r="C1576" s="146" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -36879,7 +36887,7 @@
       <c r="B1596" s="0" t="s">
         <v>2467</v>
       </c>
-      <c r="C1596" s="144" t="n">
+      <c r="C1596" s="146" t="n">
         <v>1000000</v>
       </c>
     </row>
@@ -36887,7 +36895,7 @@
       <c r="B1597" s="0" t="s">
         <v>2468</v>
       </c>
-      <c r="C1597" s="144" t="n">
+      <c r="C1597" s="146" t="n">
         <v>1000000</v>
       </c>
     </row>
@@ -37767,7 +37775,7 @@
       <c r="B1707" s="0" t="s">
         <v>2579</v>
       </c>
-      <c r="C1707" s="144" t="n">
+      <c r="C1707" s="146" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -37783,7 +37791,7 @@
       <c r="B1709" s="0" t="s">
         <v>2581</v>
       </c>
-      <c r="C1709" s="144" t="n">
+      <c r="C1709" s="146" t="n">
         <v>34197800</v>
       </c>
     </row>
@@ -38303,7 +38311,7 @@
       <c r="B1774" s="0" t="s">
         <v>2646</v>
       </c>
-      <c r="C1774" s="144" t="n">
+      <c r="C1774" s="146" t="n">
         <v>12147700</v>
       </c>
     </row>
@@ -38383,7 +38391,7 @@
       <c r="B1784" s="0" t="s">
         <v>2656</v>
       </c>
-      <c r="C1784" s="144" t="n">
+      <c r="C1784" s="146" t="n">
         <v>-7098040</v>
       </c>
     </row>
@@ -38471,7 +38479,7 @@
       <c r="B1795" s="0" t="s">
         <v>2667</v>
       </c>
-      <c r="C1795" s="144" t="n">
+      <c r="C1795" s="146" t="n">
         <v>4465690</v>
       </c>
     </row>
@@ -38647,7 +38655,7 @@
       <c r="B1817" s="0" t="s">
         <v>2690</v>
       </c>
-      <c r="C1817" s="144" t="n">
+      <c r="C1817" s="146" t="n">
         <v>1999640</v>
       </c>
     </row>
@@ -38711,7 +38719,7 @@
       <c r="B1825" s="0" t="s">
         <v>2698</v>
       </c>
-      <c r="C1825" s="144" t="n">
+      <c r="C1825" s="146" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -38727,7 +38735,7 @@
       <c r="B1827" s="0" t="s">
         <v>2700</v>
       </c>
-      <c r="C1827" s="144" t="n">
+      <c r="C1827" s="146" t="n">
         <v>-13532400</v>
       </c>
     </row>
@@ -39330,7 +39338,7 @@
       <c r="B1902" s="0" t="s">
         <v>2777</v>
       </c>
-      <c r="C1902" s="144" t="n">
+      <c r="C1902" s="146" t="n">
         <v>4.37265E-007</v>
       </c>
     </row>
@@ -39378,7 +39386,7 @@
       <c r="B1908" s="0" t="s">
         <v>2783</v>
       </c>
-      <c r="C1908" s="144" t="n">
+      <c r="C1908" s="146" t="n">
         <v>4.35882E-007</v>
       </c>
     </row>
@@ -39410,7 +39418,7 @@
       <c r="B1912" s="0" t="s">
         <v>2787</v>
       </c>
-      <c r="C1912" s="144" t="n">
+      <c r="C1912" s="146" t="n">
         <v>4.34577E-007</v>
       </c>
     </row>
@@ -39498,7 +39506,7 @@
       <c r="B1923" s="0" t="s">
         <v>2798</v>
       </c>
-      <c r="C1923" s="144" t="n">
+      <c r="C1923" s="146" t="n">
         <v>9.15083E-009</v>
       </c>
     </row>
@@ -39674,7 +39682,7 @@
       <c r="B1945" s="0" t="s">
         <v>2821</v>
       </c>
-      <c r="C1945" s="144" t="n">
+      <c r="C1945" s="146" t="n">
         <v>6.45121E-010</v>
       </c>
     </row>
@@ -39738,7 +39746,7 @@
       <c r="B1953" s="0" t="s">
         <v>2829</v>
       </c>
-      <c r="C1953" s="144" t="n">
+      <c r="C1953" s="146" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -39754,7 +39762,7 @@
       <c r="B1955" s="0" t="s">
         <v>2831</v>
       </c>
-      <c r="C1955" s="144" t="n">
+      <c r="C1955" s="146" t="n">
         <v>5.44853E-005</v>
       </c>
     </row>
@@ -40274,7 +40282,7 @@
       <c r="B2020" s="0" t="s">
         <v>2896</v>
       </c>
-      <c r="C2020" s="144" t="n">
+      <c r="C2020" s="146" t="n">
         <v>4.37266E-007</v>
       </c>
     </row>
@@ -40322,7 +40330,7 @@
       <c r="B2026" s="0" t="s">
         <v>2902</v>
       </c>
-      <c r="C2026" s="144" t="n">
+      <c r="C2026" s="146" t="n">
         <v>4.35881E-007</v>
       </c>
     </row>
@@ -40354,7 +40362,7 @@
       <c r="B2030" s="0" t="s">
         <v>2906</v>
       </c>
-      <c r="C2030" s="144" t="n">
+      <c r="C2030" s="146" t="n">
         <v>4.34576E-007</v>
       </c>
     </row>
@@ -40442,7 +40450,7 @@
       <c r="B2041" s="0" t="s">
         <v>2917</v>
       </c>
-      <c r="C2041" s="144" t="n">
+      <c r="C2041" s="146" t="n">
         <v>8.38028E-009</v>
       </c>
     </row>
@@ -40618,7 +40626,7 @@
       <c r="B2063" s="0" t="s">
         <v>2940</v>
       </c>
-      <c r="C2063" s="144" t="n">
+      <c r="C2063" s="146" t="n">
         <v>6.44996E-010</v>
       </c>
     </row>
@@ -40682,7 +40690,7 @@
       <c r="B2071" s="0" t="s">
         <v>2948</v>
       </c>
-      <c r="C2071" s="144" t="n">
+      <c r="C2071" s="146" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -40698,7 +40706,7 @@
       <c r="B2073" s="0" t="s">
         <v>2950</v>
       </c>
-      <c r="C2073" s="144" t="n">
+      <c r="C2073" s="146" t="n">
         <v>5.44851E-005</v>
       </c>
     </row>
@@ -41218,7 +41226,7 @@
       <c r="B2138" s="0" t="s">
         <v>3015</v>
       </c>
-      <c r="C2138" s="144" t="n">
+      <c r="C2138" s="146" t="n">
         <v>1.0545E-011</v>
       </c>
     </row>
@@ -41266,7 +41274,7 @@
       <c r="B2144" s="0" t="s">
         <v>3021</v>
       </c>
-      <c r="C2144" s="144" t="n">
+      <c r="C2144" s="146" t="n">
         <v>1.35517E-012</v>
       </c>
     </row>
@@ -41298,7 +41306,7 @@
       <c r="B2148" s="0" t="s">
         <v>3025</v>
       </c>
-      <c r="C2148" s="144" t="n">
+      <c r="C2148" s="146" t="n">
         <v>-1.06504E-011</v>
       </c>
     </row>
@@ -41386,7 +41394,7 @@
       <c r="B2159" s="0" t="s">
         <v>3036</v>
       </c>
-      <c r="C2159" s="144" t="n">
+      <c r="C2159" s="146" t="n">
         <v>7.70545E-010</v>
       </c>
     </row>
@@ -41562,7 +41570,7 @@
       <c r="B2181" s="0" t="s">
         <v>3059</v>
       </c>
-      <c r="C2181" s="144" t="n">
+      <c r="C2181" s="146" t="n">
         <v>4.1709E-012</v>
       </c>
     </row>
@@ -41626,7 +41634,7 @@
       <c r="B2189" s="0" t="s">
         <v>3067</v>
       </c>
-      <c r="C2189" s="144" t="n">
+      <c r="C2189" s="146" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -41642,7 +41650,7 @@
       <c r="B2191" s="0" t="s">
         <v>3069</v>
       </c>
-      <c r="C2191" s="144" t="n">
+      <c r="C2191" s="146" t="n">
         <v>1.69396E-010</v>
       </c>
     </row>
@@ -42218,7 +42226,7 @@
       <c r="B2263" s="0" t="s">
         <v>3144</v>
       </c>
-      <c r="C2263" s="144" t="n">
+      <c r="C2263" s="146" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -42505,7 +42513,7 @@
       <c r="F2297" s="0" t="s">
         <v>3189</v>
       </c>
-      <c r="G2297" s="146" t="n">
+      <c r="G2297" s="148" t="n">
         <v>41244</v>
       </c>
     </row>
@@ -42597,7 +42605,7 @@
       <c r="B2307" s="0" t="s">
         <v>3203</v>
       </c>
-      <c r="C2307" s="144" t="n">
+      <c r="C2307" s="146" t="n">
         <v>878236000</v>
       </c>
     </row>
@@ -42683,7 +42691,7 @@
       <c r="B2317" s="0" t="s">
         <v>3219</v>
       </c>
-      <c r="C2317" s="144" t="n">
+      <c r="C2317" s="146" t="n">
         <v>32640100000</v>
       </c>
     </row>
@@ -42691,7 +42699,7 @@
       <c r="B2318" s="0" t="s">
         <v>3220</v>
       </c>
-      <c r="C2318" s="144" t="n">
+      <c r="C2318" s="146" t="n">
         <v>33683000000</v>
       </c>
     </row>
@@ -42707,7 +42715,7 @@
       <c r="B2320" s="0" t="s">
         <v>3222</v>
       </c>
-      <c r="C2320" s="144" t="n">
+      <c r="C2320" s="146" t="n">
         <v>30883800</v>
       </c>
     </row>
@@ -42755,7 +42763,7 @@
       <c r="C2326" s="0" t="s">
         <v>3230</v>
       </c>
-      <c r="D2326" s="147" t="n">
+      <c r="D2326" s="149" t="n">
         <v>0.443159722222222</v>
       </c>
     </row>
@@ -42806,7 +42814,7 @@
       <c r="C2332" s="0" t="s">
         <v>3238</v>
       </c>
-      <c r="D2332" s="147" t="n">
+      <c r="D2332" s="149" t="n">
         <v>0.600474537037037</v>
       </c>
     </row>
@@ -42825,7 +42833,7 @@
       <c r="D2334" s="0" t="s">
         <v>3241</v>
       </c>
-      <c r="E2334" s="147" t="n">
+      <c r="E2334" s="149" t="n">
         <v>0.157314814814815</v>
       </c>
     </row>
@@ -42883,7 +42891,7 @@
       <c r="E2339" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="F2339" s="147" t="n">
+      <c r="F2339" s="149" t="n">
         <v>0.596990740740741</v>
       </c>
     </row>
@@ -43355,7 +43363,7 @@
       <c r="E2380" s="0" t="n">
         <v>26</v>
       </c>
-      <c r="F2380" s="147" t="n">
+      <c r="F2380" s="149" t="n">
         <v>0.443159722222222</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new xafs_table values in lookup table
</commit_message>
<xml_diff>
--- a/startup/lookup_table/Modes.xlsx
+++ b/startup/lookup_table/Modes.xlsx
@@ -108,29 +108,6 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Rh/Pt stripe</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E56" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Vertical = 110.75
-Pitch = -1.465</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">These values obtained by seeing spot on phosphor screen at upstream end of I0 and downstream end of Ir</t>
         </r>
       </text>
     </comment>
@@ -11117,7 +11094,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="150">
+  <cellXfs count="147">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -11362,8 +11339,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="7" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -11371,18 +11348,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11394,11 +11359,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11798,14 +11763,14 @@
   <dimension ref="A1:AMJ66"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="L17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="E32" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="L1" activeCellId="0" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="M54" activeCellId="0" sqref="M54"/>
+      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
+      <selection pane="bottomRight" activeCell="K56" activeCellId="0" sqref="K56:K58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.04"/>
@@ -14913,7 +14878,7 @@
         <v>189</v>
       </c>
       <c r="E56" s="61" t="n">
-        <v>113.811</v>
+        <v>113.887</v>
       </c>
       <c r="F56" s="25" t="n">
         <v>9251952</v>
@@ -14925,25 +14890,25 @@
         <v>4600216</v>
       </c>
       <c r="I56" s="61" t="n">
-        <v>54.559</v>
+        <v>54.059</v>
       </c>
       <c r="J56" s="23" t="n">
         <v>6151303</v>
       </c>
-      <c r="K56" s="64" t="n">
-        <v>124.496</v>
+      <c r="K56" s="61" t="n">
+        <v>125.144</v>
       </c>
       <c r="L56" s="23" t="n">
         <v>9901395</v>
       </c>
-      <c r="M56" s="65" t="n">
-        <v>124.496</v>
+      <c r="M56" s="61" t="n">
+        <v>124.985</v>
       </c>
       <c r="N56" s="23" t="n">
         <v>9901395</v>
       </c>
-      <c r="O56" s="65" t="n">
-        <v>97.709</v>
+      <c r="O56" s="61" t="n">
+        <v>96.516</v>
       </c>
       <c r="P56" s="23" t="n">
         <v>8392750</v>
@@ -14974,38 +14939,38 @@
       <c r="D57" s="0" t="s">
         <v>192</v>
       </c>
-      <c r="E57" s="66" t="n">
-        <v>116.993</v>
+      <c r="E57" s="61" t="n">
+        <v>119.819</v>
       </c>
       <c r="F57" s="32" t="n">
         <v>6972005</v>
       </c>
-      <c r="G57" s="67" t="n">
+      <c r="G57" s="64" t="n">
         <v>12.81</v>
       </c>
-      <c r="H57" s="68" t="n">
+      <c r="H57" s="65" t="n">
         <v>1551088</v>
       </c>
-      <c r="I57" s="66" t="n">
-        <v>47.758</v>
+      <c r="I57" s="61" t="n">
+        <v>52.458</v>
       </c>
       <c r="J57" s="32" t="n">
         <v>3351899</v>
       </c>
-      <c r="K57" s="64" t="n">
-        <v>129.341</v>
+      <c r="K57" s="61" t="n">
+        <v>130.739</v>
       </c>
       <c r="L57" s="32" t="n">
         <v>7552437</v>
       </c>
-      <c r="M57" s="69" t="n">
-        <v>129.841</v>
+      <c r="M57" s="61" t="n">
+        <v>130.33</v>
       </c>
       <c r="N57" s="32" t="n">
         <v>7552437</v>
       </c>
-      <c r="O57" s="69" t="n">
-        <v>96.004</v>
+      <c r="O57" s="61" t="n">
+        <v>98.811</v>
       </c>
       <c r="P57" s="32" t="n">
         <v>5879304</v>
@@ -15028,40 +14993,40 @@
       <c r="D58" s="26" t="s">
         <v>195</v>
       </c>
-      <c r="E58" s="66" t="n">
-        <v>116.993</v>
+      <c r="E58" s="61" t="n">
+        <v>119.819</v>
       </c>
       <c r="F58" s="28" t="n">
         <v>5572330</v>
       </c>
-      <c r="G58" s="67" t="n">
+      <c r="G58" s="64" t="n">
         <v>12.81</v>
       </c>
-      <c r="H58" s="68" t="n">
+      <c r="H58" s="65" t="n">
         <v>354340</v>
       </c>
-      <c r="I58" s="66" t="n">
-        <v>47.758</v>
+      <c r="I58" s="61" t="n">
+        <v>52.458</v>
       </c>
       <c r="J58" s="32" t="n">
         <v>1952224</v>
       </c>
-      <c r="K58" s="64" t="n">
-        <v>129.341</v>
+      <c r="K58" s="61" t="n">
+        <v>130.739</v>
       </c>
       <c r="L58" s="32" t="n">
         <v>6355689</v>
       </c>
-      <c r="M58" s="69" t="n">
-        <v>129.841</v>
+      <c r="M58" s="61" t="n">
+        <v>130.33</v>
       </c>
       <c r="N58" s="32" t="n">
         <v>6355689</v>
       </c>
-      <c r="O58" s="69" t="n">
-        <v>96.004</v>
-      </c>
-      <c r="P58" s="70" t="n">
+      <c r="O58" s="61" t="n">
+        <v>98.811</v>
+      </c>
+      <c r="P58" s="66" t="n">
         <v>4479629</v>
       </c>
       <c r="T58" s="27" t="n">
@@ -15087,43 +15052,43 @@
       <c r="D59" s="26" t="s">
         <v>198</v>
       </c>
-      <c r="E59" s="66" t="n">
+      <c r="E59" s="67" t="n">
         <v>-9.0621</v>
       </c>
       <c r="F59" s="28" t="n">
         <v>-242758</v>
       </c>
-      <c r="G59" s="67" t="n">
+      <c r="G59" s="64" t="n">
         <v>-9.0621</v>
       </c>
-      <c r="H59" s="71" t="n">
+      <c r="H59" s="68" t="n">
         <v>-242758</v>
       </c>
-      <c r="I59" s="66" t="n">
+      <c r="I59" s="67" t="n">
         <v>-9.0621</v>
       </c>
       <c r="J59" s="28" t="n">
         <v>-242758</v>
       </c>
-      <c r="K59" s="66" t="n">
+      <c r="K59" s="67" t="n">
         <v>-9.0621</v>
       </c>
       <c r="L59" s="28" t="n">
         <v>-242758</v>
       </c>
-      <c r="M59" s="66" t="n">
+      <c r="M59" s="67" t="n">
         <v>-9.0621</v>
       </c>
       <c r="N59" s="28" t="n">
         <v>-242758</v>
       </c>
-      <c r="O59" s="66" t="n">
+      <c r="O59" s="67" t="n">
         <v>-9.0621</v>
       </c>
       <c r="P59" s="28" t="n">
         <v>-242758</v>
       </c>
-      <c r="T59" s="66" t="n">
+      <c r="T59" s="67" t="n">
         <v>-0.6</v>
       </c>
       <c r="U59" s="28" t="n">
@@ -15141,46 +15106,46 @@
       <c r="D60" s="35" t="s">
         <v>201</v>
       </c>
-      <c r="E60" s="72" t="n">
+      <c r="E60" s="69" t="n">
         <v>15.3898</v>
       </c>
       <c r="F60" s="47" t="n">
         <v>160203</v>
       </c>
-      <c r="G60" s="73" t="n">
+      <c r="G60" s="70" t="n">
         <v>15.3898</v>
       </c>
-      <c r="H60" s="74" t="n">
+      <c r="H60" s="71" t="n">
         <v>160203</v>
       </c>
-      <c r="I60" s="72" t="n">
+      <c r="I60" s="69" t="n">
         <v>15.3898</v>
       </c>
       <c r="J60" s="47" t="n">
         <v>160203</v>
       </c>
-      <c r="K60" s="72" t="n">
+      <c r="K60" s="69" t="n">
         <v>15.3898</v>
       </c>
       <c r="L60" s="47" t="n">
         <v>160203</v>
       </c>
-      <c r="M60" s="72" t="n">
+      <c r="M60" s="69" t="n">
         <v>15.3898</v>
       </c>
       <c r="N60" s="47" t="n">
         <v>160203</v>
       </c>
-      <c r="O60" s="72" t="n">
+      <c r="O60" s="69" t="n">
         <v>15.3898</v>
       </c>
       <c r="P60" s="47" t="n">
         <v>160203</v>
       </c>
-      <c r="Q60" s="75"/>
-      <c r="R60" s="75"/>
-      <c r="S60" s="75"/>
-      <c r="T60" s="72" t="n">
+      <c r="Q60" s="72"/>
+      <c r="R60" s="72"/>
+      <c r="S60" s="72"/>
+      <c r="T60" s="69" t="n">
         <v>33.3721</v>
       </c>
       <c r="U60" s="47" t="n">
@@ -15193,52 +15158,52 @@
       <c r="Z60" s="0"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="76" t="s">
+      <c r="A61" s="73" t="s">
         <v>202</v>
       </c>
-      <c r="B61" s="77" t="s">
+      <c r="B61" s="74" t="s">
         <v>203</v>
       </c>
-      <c r="C61" s="78" t="s">
+      <c r="C61" s="75" t="s">
         <v>204</v>
       </c>
-      <c r="D61" s="78" t="s">
+      <c r="D61" s="75" t="s">
         <v>205</v>
       </c>
-      <c r="E61" s="79" t="n">
-        <v>0</v>
-      </c>
-      <c r="F61" s="80" t="n">
-        <v>0</v>
-      </c>
-      <c r="G61" s="79" t="n">
-        <v>0</v>
-      </c>
-      <c r="H61" s="80" t="n">
-        <v>0</v>
-      </c>
-      <c r="I61" s="79" t="n">
-        <v>0</v>
-      </c>
-      <c r="J61" s="80" t="n">
-        <v>0</v>
-      </c>
-      <c r="K61" s="79" t="n">
-        <v>0</v>
-      </c>
-      <c r="L61" s="80" t="n">
-        <v>0</v>
-      </c>
-      <c r="M61" s="79" t="n">
-        <v>0</v>
-      </c>
-      <c r="N61" s="80" t="n">
-        <v>0</v>
-      </c>
-      <c r="O61" s="79" t="n">
-        <v>0</v>
-      </c>
-      <c r="P61" s="80" t="n">
+      <c r="E61" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="F61" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="G61" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="H61" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="I61" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="J61" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="K61" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="L61" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="M61" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="N61" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="O61" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="P61" s="77" t="n">
         <v>0</v>
       </c>
       <c r="T61" s="30" t="n">
@@ -15249,8 +15214,8 @@
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="76"/>
-      <c r="B62" s="81" t="s">
+      <c r="A62" s="73"/>
+      <c r="B62" s="78" t="s">
         <v>206</v>
       </c>
       <c r="C62" s="0" t="s">
@@ -15303,8 +15268,8 @@
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="76"/>
-      <c r="B63" s="81" t="s">
+      <c r="A63" s="73"/>
+      <c r="B63" s="78" t="s">
         <v>209</v>
       </c>
       <c r="C63" s="0" t="s">
@@ -15357,8 +15322,8 @@
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="76"/>
-      <c r="B64" s="81" t="s">
+      <c r="A64" s="73"/>
+      <c r="B64" s="78" t="s">
         <v>212</v>
       </c>
       <c r="C64" s="0" t="s">
@@ -15411,8 +15376,8 @@
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="76"/>
-      <c r="B65" s="81" t="s">
+      <c r="A65" s="73"/>
+      <c r="B65" s="78" t="s">
         <v>215</v>
       </c>
       <c r="C65" s="0" t="s">
@@ -15465,53 +15430,53 @@
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="76"/>
-      <c r="B66" s="82" t="s">
+      <c r="A66" s="73"/>
+      <c r="B66" s="79" t="s">
         <v>218</v>
       </c>
-      <c r="C66" s="83" t="s">
+      <c r="C66" s="80" t="s">
         <v>219</v>
       </c>
-      <c r="D66" s="83" t="s">
+      <c r="D66" s="80" t="s">
         <v>220</v>
       </c>
-      <c r="E66" s="84" t="n">
-        <v>0</v>
-      </c>
-      <c r="F66" s="85" t="n">
-        <v>0</v>
-      </c>
-      <c r="G66" s="84" t="n">
-        <v>0</v>
-      </c>
-      <c r="H66" s="85" t="n">
-        <v>0</v>
-      </c>
-      <c r="I66" s="84" t="n">
-        <v>0</v>
-      </c>
-      <c r="J66" s="85" t="n">
-        <v>0</v>
-      </c>
-      <c r="K66" s="84" t="n">
-        <v>0</v>
-      </c>
-      <c r="L66" s="85" t="n">
-        <v>0</v>
-      </c>
-      <c r="M66" s="84" t="n">
-        <v>0</v>
-      </c>
-      <c r="N66" s="85" t="n">
-        <v>0</v>
-      </c>
-      <c r="O66" s="84" t="n">
-        <v>0</v>
-      </c>
-      <c r="P66" s="85" t="n">
-        <v>0</v>
-      </c>
-      <c r="T66" s="72" t="n">
+      <c r="E66" s="81" t="n">
+        <v>0</v>
+      </c>
+      <c r="F66" s="82" t="n">
+        <v>0</v>
+      </c>
+      <c r="G66" s="81" t="n">
+        <v>0</v>
+      </c>
+      <c r="H66" s="82" t="n">
+        <v>0</v>
+      </c>
+      <c r="I66" s="81" t="n">
+        <v>0</v>
+      </c>
+      <c r="J66" s="82" t="n">
+        <v>0</v>
+      </c>
+      <c r="K66" s="81" t="n">
+        <v>0</v>
+      </c>
+      <c r="L66" s="82" t="n">
+        <v>0</v>
+      </c>
+      <c r="M66" s="81" t="n">
+        <v>0</v>
+      </c>
+      <c r="N66" s="82" t="n">
+        <v>0</v>
+      </c>
+      <c r="O66" s="81" t="n">
+        <v>0</v>
+      </c>
+      <c r="P66" s="82" t="n">
+        <v>0</v>
+      </c>
+      <c r="T66" s="69" t="n">
         <v>0</v>
       </c>
       <c r="U66" s="47" t="n">
@@ -15566,39 +15531,39 @@
   <dimension ref="A1:AMJ31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
+      <selection pane="topLeft" activeCell="D28" activeCellId="1" sqref="K56:K58 D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="86" width="3.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="2" style="86" width="13.26"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="10" style="86" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="83" width="3.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="2" style="83" width="13.26"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="10" style="83" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" s="87" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="86"/>
+    <row r="1" s="84" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="83"/>
       <c r="B1" s="0"/>
       <c r="C1" s="0"/>
       <c r="D1" s="0"/>
       <c r="E1" s="0"/>
-      <c r="F1" s="86"/>
-      <c r="G1" s="86"/>
-      <c r="H1" s="86"/>
-      <c r="I1" s="86"/>
-      <c r="J1" s="86"/>
-      <c r="K1" s="86"/>
-      <c r="L1" s="86"/>
-      <c r="AMJ1" s="86"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
+      <c r="H1" s="83"/>
+      <c r="I1" s="83"/>
+      <c r="J1" s="83"/>
+      <c r="K1" s="83"/>
+      <c r="L1" s="83"/>
+      <c r="AMJ1" s="83"/>
     </row>
     <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0"/>
-      <c r="B2" s="88" t="s">
+      <c r="B2" s="85" t="s">
         <v>221</v>
       </c>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
       <c r="F2" s="0"/>
       <c r="G2" s="0"/>
       <c r="H2" s="0"/>
@@ -16619,168 +16584,168 @@
       <c r="AMI2" s="0"/>
       <c r="AMJ2" s="0"/>
     </row>
-    <row r="3" s="93" customFormat="true" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="89"/>
-      <c r="B3" s="90"/>
-      <c r="C3" s="91" t="s">
+    <row r="3" s="90" customFormat="true" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="86"/>
+      <c r="B3" s="87"/>
+      <c r="C3" s="88" t="s">
         <v>222</v>
       </c>
-      <c r="D3" s="91" t="s">
+      <c r="D3" s="88" t="s">
         <v>223</v>
       </c>
-      <c r="E3" s="92" t="s">
+      <c r="E3" s="89" t="s">
         <v>224</v>
       </c>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
-      <c r="AMJ3" s="89"/>
-    </row>
-    <row r="4" s="87" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="86"/>
-      <c r="B4" s="90" t="s">
+      <c r="F3" s="86"/>
+      <c r="G3" s="86"/>
+      <c r="H3" s="86"/>
+      <c r="I3" s="86"/>
+      <c r="J3" s="86"/>
+      <c r="K3" s="86"/>
+      <c r="L3" s="86"/>
+      <c r="AMJ3" s="86"/>
+    </row>
+    <row r="4" s="84" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="83"/>
+      <c r="B4" s="87" t="s">
         <v>225</v>
       </c>
-      <c r="C4" s="86"/>
-      <c r="D4" s="86" t="n">
+      <c r="C4" s="83"/>
+      <c r="D4" s="83" t="n">
         <v>55</v>
       </c>
-      <c r="E4" s="94" t="n">
+      <c r="E4" s="91" t="n">
         <v>55</v>
       </c>
-      <c r="F4" s="86"/>
-      <c r="G4" s="86"/>
-      <c r="H4" s="86"/>
-      <c r="I4" s="86"/>
-      <c r="J4" s="86"/>
-      <c r="K4" s="86"/>
-      <c r="L4" s="86"/>
-      <c r="AMJ4" s="86"/>
-    </row>
-    <row r="5" s="87" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="86"/>
-      <c r="B5" s="90" t="s">
+      <c r="F4" s="83"/>
+      <c r="G4" s="83"/>
+      <c r="H4" s="83"/>
+      <c r="I4" s="83"/>
+      <c r="J4" s="83"/>
+      <c r="K4" s="83"/>
+      <c r="L4" s="83"/>
+      <c r="AMJ4" s="83"/>
+    </row>
+    <row r="5" s="84" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="83"/>
+      <c r="B5" s="87" t="s">
         <v>226</v>
       </c>
-      <c r="C5" s="86" t="s">
+      <c r="C5" s="83" t="s">
         <v>227</v>
       </c>
-      <c r="D5" s="86" t="n">
+      <c r="D5" s="83" t="n">
         <v>-46.5</v>
       </c>
-      <c r="E5" s="94"/>
-      <c r="F5" s="86"/>
-      <c r="G5" s="86"/>
-      <c r="H5" s="86"/>
-      <c r="I5" s="86"/>
-      <c r="J5" s="86"/>
-      <c r="K5" s="86"/>
-      <c r="L5" s="86"/>
-      <c r="AMJ5" s="86"/>
-    </row>
-    <row r="6" s="87" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="86"/>
-      <c r="B6" s="90" t="s">
+      <c r="E5" s="91"/>
+      <c r="F5" s="83"/>
+      <c r="G5" s="83"/>
+      <c r="H5" s="83"/>
+      <c r="I5" s="83"/>
+      <c r="J5" s="83"/>
+      <c r="K5" s="83"/>
+      <c r="L5" s="83"/>
+      <c r="AMJ5" s="83"/>
+    </row>
+    <row r="6" s="84" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="83"/>
+      <c r="B6" s="87" t="s">
         <v>228</v>
       </c>
-      <c r="C6" s="86" t="s">
+      <c r="C6" s="83" t="s">
         <v>229</v>
       </c>
-      <c r="D6" s="86" t="n">
+      <c r="D6" s="83" t="n">
         <v>-20.5</v>
       </c>
-      <c r="E6" s="94"/>
-      <c r="F6" s="86"/>
-      <c r="G6" s="86"/>
-      <c r="H6" s="86"/>
-      <c r="I6" s="86"/>
-      <c r="J6" s="86"/>
-      <c r="K6" s="86"/>
-      <c r="L6" s="86"/>
-      <c r="AMJ6" s="86"/>
-    </row>
-    <row r="7" s="87" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="86"/>
-      <c r="B7" s="90" t="s">
+      <c r="E6" s="91"/>
+      <c r="F6" s="83"/>
+      <c r="G6" s="83"/>
+      <c r="H6" s="83"/>
+      <c r="I6" s="83"/>
+      <c r="J6" s="83"/>
+      <c r="K6" s="83"/>
+      <c r="L6" s="83"/>
+      <c r="AMJ6" s="83"/>
+    </row>
+    <row r="7" s="84" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="83"/>
+      <c r="B7" s="87" t="s">
         <v>230</v>
       </c>
-      <c r="C7" s="86" t="s">
+      <c r="C7" s="83" t="s">
         <v>231</v>
       </c>
-      <c r="D7" s="86" t="n">
+      <c r="D7" s="83" t="n">
         <v>5.5</v>
       </c>
-      <c r="E7" s="94"/>
-      <c r="F7" s="86"/>
-      <c r="G7" s="86"/>
-      <c r="H7" s="86"/>
-      <c r="I7" s="86"/>
-      <c r="J7" s="86"/>
-      <c r="K7" s="86"/>
-      <c r="L7" s="86"/>
-      <c r="AMJ7" s="86"/>
-    </row>
-    <row r="8" s="87" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="86"/>
-      <c r="B8" s="90" t="s">
+      <c r="E7" s="91"/>
+      <c r="F7" s="83"/>
+      <c r="G7" s="83"/>
+      <c r="H7" s="83"/>
+      <c r="I7" s="83"/>
+      <c r="J7" s="83"/>
+      <c r="K7" s="83"/>
+      <c r="L7" s="83"/>
+      <c r="AMJ7" s="83"/>
+    </row>
+    <row r="8" s="84" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="83"/>
+      <c r="B8" s="87" t="s">
         <v>232</v>
       </c>
-      <c r="C8" s="86" t="s">
+      <c r="C8" s="83" t="s">
         <v>233</v>
       </c>
-      <c r="D8" s="86" t="n">
+      <c r="D8" s="83" t="n">
         <v>31</v>
       </c>
-      <c r="E8" s="94"/>
-      <c r="F8" s="86"/>
-      <c r="G8" s="86"/>
-      <c r="H8" s="86"/>
-      <c r="I8" s="86"/>
-      <c r="J8" s="86"/>
-      <c r="K8" s="86"/>
-      <c r="L8" s="86"/>
-      <c r="AMJ8" s="86"/>
-    </row>
-    <row r="9" s="87" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="86"/>
-      <c r="B9" s="90" t="s">
+      <c r="E8" s="91"/>
+      <c r="F8" s="83"/>
+      <c r="G8" s="83"/>
+      <c r="H8" s="83"/>
+      <c r="I8" s="83"/>
+      <c r="J8" s="83"/>
+      <c r="K8" s="83"/>
+      <c r="L8" s="83"/>
+      <c r="AMJ8" s="83"/>
+    </row>
+    <row r="9" s="84" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="83"/>
+      <c r="B9" s="87" t="s">
         <v>234</v>
       </c>
-      <c r="C9" s="86"/>
-      <c r="D9" s="86" t="n">
+      <c r="C9" s="83"/>
+      <c r="D9" s="83" t="n">
         <v>-52.6</v>
       </c>
-      <c r="E9" s="94"/>
-      <c r="F9" s="86"/>
-      <c r="G9" s="86"/>
-      <c r="H9" s="86"/>
-      <c r="I9" s="86"/>
-      <c r="J9" s="86"/>
-      <c r="K9" s="86"/>
-      <c r="L9" s="86"/>
-      <c r="AMJ9" s="86"/>
+      <c r="E9" s="91"/>
+      <c r="F9" s="83"/>
+      <c r="G9" s="83"/>
+      <c r="H9" s="83"/>
+      <c r="I9" s="83"/>
+      <c r="J9" s="83"/>
+      <c r="K9" s="83"/>
+      <c r="L9" s="83"/>
+      <c r="AMJ9" s="83"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="95" t="s">
+      <c r="B10" s="92" t="s">
         <v>235</v>
       </c>
-      <c r="C10" s="96"/>
-      <c r="D10" s="96" t="n">
+      <c r="C10" s="93"/>
+      <c r="D10" s="93" t="n">
         <v>-52</v>
       </c>
-      <c r="E10" s="97"/>
+      <c r="E10" s="94"/>
       <c r="F10" s="0"/>
       <c r="G10" s="0"/>
       <c r="H10" s="0"/>
       <c r="I10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="98"/>
-      <c r="C11" s="99"/>
+      <c r="B11" s="95"/>
+      <c r="C11" s="96"/>
       <c r="D11" s="0"/>
       <c r="E11" s="0"/>
       <c r="F11" s="0"/>
@@ -16789,8 +16754,8 @@
       <c r="I11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="98"/>
-      <c r="C12" s="99"/>
+      <c r="B12" s="95"/>
+      <c r="C12" s="96"/>
       <c r="D12" s="0"/>
       <c r="E12" s="0"/>
       <c r="F12" s="0"/>
@@ -16799,82 +16764,82 @@
       <c r="I12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="100" t="s">
+      <c r="B13" s="97" t="s">
         <v>236</v>
       </c>
-      <c r="C13" s="100"/>
-      <c r="D13" s="100"/>
-      <c r="E13" s="100"/>
+      <c r="C13" s="97"/>
+      <c r="D13" s="97"/>
+      <c r="E13" s="97"/>
       <c r="F13" s="0"/>
       <c r="G13" s="0"/>
       <c r="H13" s="0"/>
       <c r="I13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="101" t="s">
+      <c r="B14" s="98" t="s">
         <v>237</v>
       </c>
-      <c r="C14" s="102" t="s">
+      <c r="C14" s="99" t="s">
         <v>238</v>
       </c>
       <c r="D14" s="0"/>
-      <c r="E14" s="94"/>
+      <c r="E14" s="91"/>
       <c r="F14" s="0"/>
       <c r="G14" s="0"/>
       <c r="H14" s="0"/>
       <c r="I14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="90" t="s">
+      <c r="B15" s="87" t="s">
         <v>225</v>
       </c>
-      <c r="C15" s="86" t="n">
+      <c r="C15" s="83" t="n">
         <v>67</v>
       </c>
       <c r="D15" s="0"/>
-      <c r="E15" s="94"/>
+      <c r="E15" s="91"/>
       <c r="F15" s="0"/>
       <c r="G15" s="0"/>
       <c r="H15" s="0"/>
       <c r="I15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="90" t="s">
+      <c r="B16" s="87" t="s">
         <v>239</v>
       </c>
-      <c r="C16" s="103" t="n">
+      <c r="C16" s="100" t="n">
         <v>-1.5</v>
       </c>
       <c r="D16" s="0"/>
-      <c r="E16" s="94"/>
+      <c r="E16" s="91"/>
       <c r="F16" s="0"/>
       <c r="G16" s="0"/>
       <c r="H16" s="0"/>
       <c r="I16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="90" t="s">
+      <c r="B17" s="87" t="s">
         <v>240</v>
       </c>
-      <c r="C17" s="86" t="n">
+      <c r="C17" s="83" t="n">
         <v>33</v>
       </c>
       <c r="D17" s="0"/>
-      <c r="E17" s="94"/>
+      <c r="E17" s="91"/>
       <c r="F17" s="0"/>
       <c r="G17" s="0"/>
       <c r="H17" s="0"/>
       <c r="I17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="95" t="s">
+      <c r="B18" s="92" t="s">
         <v>241</v>
       </c>
-      <c r="C18" s="96" t="n">
+      <c r="C18" s="93" t="n">
         <v>53</v>
       </c>
-      <c r="D18" s="96"/>
-      <c r="E18" s="97"/>
+      <c r="D18" s="93"/>
+      <c r="E18" s="94"/>
       <c r="F18" s="0"/>
       <c r="G18" s="0"/>
       <c r="H18" s="0"/>
@@ -16901,213 +16866,213 @@
       <c r="I20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="100" t="s">
+      <c r="B21" s="97" t="s">
         <v>176</v>
       </c>
-      <c r="C21" s="100"/>
-      <c r="D21" s="100"/>
-      <c r="E21" s="100"/>
-      <c r="F21" s="100"/>
-      <c r="G21" s="100"/>
-      <c r="H21" s="100"/>
-      <c r="I21" s="100"/>
+      <c r="C21" s="97"/>
+      <c r="D21" s="97"/>
+      <c r="E21" s="97"/>
+      <c r="F21" s="97"/>
+      <c r="G21" s="97"/>
+      <c r="H21" s="97"/>
+      <c r="I21" s="97"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="104" t="s">
+      <c r="B22" s="101" t="s">
         <v>242</v>
       </c>
-      <c r="C22" s="104"/>
-      <c r="D22" s="87"/>
-      <c r="E22" s="98" t="s">
+      <c r="C22" s="101"/>
+      <c r="D22" s="84"/>
+      <c r="E22" s="95" t="s">
         <v>243</v>
       </c>
-      <c r="F22" s="98"/>
-      <c r="G22" s="87"/>
-      <c r="H22" s="105" t="s">
+      <c r="F22" s="95"/>
+      <c r="G22" s="84"/>
+      <c r="H22" s="102" t="s">
         <v>244</v>
       </c>
-      <c r="I22" s="105"/>
+      <c r="I22" s="102"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="101" t="s">
+      <c r="B23" s="98" t="s">
         <v>245</v>
       </c>
-      <c r="C23" s="102" t="s">
+      <c r="C23" s="99" t="s">
         <v>238</v>
       </c>
       <c r="D23" s="0"/>
-      <c r="E23" s="87" t="s">
+      <c r="E23" s="84" t="s">
         <v>245</v>
       </c>
-      <c r="F23" s="102" t="s">
+      <c r="F23" s="99" t="s">
         <v>238</v>
       </c>
       <c r="G23" s="0"/>
-      <c r="H23" s="87" t="s">
+      <c r="H23" s="84" t="s">
         <v>246</v>
       </c>
-      <c r="I23" s="106" t="s">
+      <c r="I23" s="103" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="90" t="s">
+      <c r="B24" s="87" t="s">
         <v>247</v>
       </c>
       <c r="C24" s="0" t="n">
         <v>33</v>
       </c>
       <c r="D24" s="0"/>
-      <c r="E24" s="86" t="s">
+      <c r="E24" s="83" t="s">
         <v>247</v>
       </c>
-      <c r="F24" s="107" t="n">
+      <c r="F24" s="104" t="n">
         <f aca="false">'Modes A-F'!E54</f>
         <v>31.259</v>
       </c>
       <c r="G24" s="0"/>
-      <c r="H24" s="86" t="s">
+      <c r="H24" s="83" t="s">
         <v>248</v>
       </c>
-      <c r="I24" s="94" t="n">
+      <c r="I24" s="91" t="n">
         <v>40</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="90" t="s">
+      <c r="B25" s="87" t="s">
         <v>249</v>
       </c>
       <c r="C25" s="0" t="n">
         <v>-66.743</v>
       </c>
       <c r="D25" s="0"/>
-      <c r="E25" s="86" t="s">
+      <c r="E25" s="83" t="s">
         <v>249</v>
       </c>
-      <c r="F25" s="107" t="n">
+      <c r="F25" s="104" t="n">
         <f aca="false">'Modes A-F'!G54</f>
         <v>-55.188</v>
       </c>
       <c r="G25" s="0"/>
-      <c r="H25" s="86" t="s">
+      <c r="H25" s="83" t="s">
         <v>250</v>
       </c>
-      <c r="I25" s="94" t="n">
+      <c r="I25" s="91" t="n">
         <v>-17.5</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="90" t="s">
+      <c r="B26" s="87" t="s">
         <v>251</v>
       </c>
       <c r="C26" s="0" t="n">
         <v>-48.1824</v>
       </c>
       <c r="D26" s="0"/>
-      <c r="E26" s="86" t="s">
+      <c r="E26" s="83" t="s">
         <v>251</v>
       </c>
-      <c r="F26" s="107" t="n">
+      <c r="F26" s="104" t="n">
         <f aca="false">'Modes A-F'!I54</f>
         <v>-23.247</v>
       </c>
       <c r="G26" s="0"/>
-      <c r="H26" s="86" t="s">
+      <c r="H26" s="83" t="s">
         <v>252</v>
       </c>
-      <c r="I26" s="94" t="n">
+      <c r="I26" s="91" t="n">
         <v>6.5</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="90" t="s">
+      <c r="B27" s="87" t="s">
         <v>253</v>
       </c>
-      <c r="C27" s="86" t="n">
+      <c r="C27" s="83" t="n">
         <v>27.1</v>
       </c>
       <c r="D27" s="0"/>
-      <c r="E27" s="86" t="s">
+      <c r="E27" s="83" t="s">
         <v>253</v>
       </c>
-      <c r="F27" s="107" t="n">
+      <c r="F27" s="104" t="n">
         <f aca="false">'Modes A-F'!K54</f>
         <v>42.66</v>
       </c>
       <c r="G27" s="0"/>
       <c r="H27" s="0"/>
-      <c r="I27" s="94"/>
+      <c r="I27" s="91"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="90" t="s">
+      <c r="B28" s="87" t="s">
         <v>254</v>
       </c>
-      <c r="C28" s="86" t="n">
+      <c r="C28" s="83" t="n">
         <v>27.1</v>
       </c>
       <c r="D28" s="0"/>
-      <c r="E28" s="86" t="s">
+      <c r="E28" s="83" t="s">
         <v>254</v>
       </c>
-      <c r="F28" s="107" t="n">
+      <c r="F28" s="104" t="n">
         <f aca="false">'Modes A-F'!M54</f>
         <v>43.0474</v>
       </c>
       <c r="G28" s="0"/>
       <c r="H28" s="0"/>
-      <c r="I28" s="94"/>
+      <c r="I28" s="91"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="90" t="s">
+      <c r="B29" s="87" t="s">
         <v>255</v>
       </c>
-      <c r="C29" s="86" t="n">
+      <c r="C29" s="83" t="n">
         <v>2.8</v>
       </c>
       <c r="D29" s="0"/>
-      <c r="E29" s="86" t="s">
+      <c r="E29" s="83" t="s">
         <v>255</v>
       </c>
-      <c r="F29" s="107" t="n">
+      <c r="F29" s="104" t="n">
         <f aca="false">'Modes A-F'!O54</f>
         <v>17.066</v>
       </c>
       <c r="G29" s="0"/>
       <c r="H29" s="0"/>
-      <c r="I29" s="94"/>
+      <c r="I29" s="91"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="90" t="s">
+      <c r="B30" s="87" t="s">
         <v>256</v>
       </c>
-      <c r="C30" s="86" t="n">
+      <c r="C30" s="83" t="n">
         <v>15</v>
       </c>
       <c r="D30" s="0"/>
-      <c r="E30" s="86" t="s">
+      <c r="E30" s="83" t="s">
         <v>256</v>
       </c>
-      <c r="F30" s="107" t="n">
+      <c r="F30" s="104" t="n">
         <f aca="false">'Modes A-F'!T54</f>
         <v>53.33</v>
       </c>
       <c r="G30" s="0"/>
       <c r="H30" s="0"/>
-      <c r="I30" s="94"/>
+      <c r="I30" s="91"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="95" t="s">
+      <c r="B31" s="92" t="s">
         <v>248</v>
       </c>
-      <c r="C31" s="96" t="n">
+      <c r="C31" s="93" t="n">
         <v>55</v>
       </c>
-      <c r="D31" s="96"/>
-      <c r="E31" s="96"/>
-      <c r="F31" s="96"/>
-      <c r="G31" s="96"/>
-      <c r="H31" s="96"/>
-      <c r="I31" s="97"/>
+      <c r="D31" s="93"/>
+      <c r="E31" s="93"/>
+      <c r="F31" s="93"/>
+      <c r="G31" s="93"/>
+      <c r="H31" s="93"/>
+      <c r="I31" s="94"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -17140,10 +17105,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G11" activeCellId="0" sqref="G11"/>
+      <selection pane="bottomRight" activeCell="G11" activeCellId="1" sqref="K56:K58 G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33"/>
@@ -17163,14 +17128,14 @@
       <c r="D1" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="108" t="s">
+      <c r="E1" s="105" t="s">
         <v>257</v>
       </c>
-      <c r="F1" s="108"/>
-      <c r="G1" s="109" t="s">
+      <c r="F1" s="105"/>
+      <c r="G1" s="106" t="s">
         <v>258</v>
       </c>
-      <c r="H1" s="109"/>
+      <c r="H1" s="106"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="44" t="s">
@@ -17196,25 +17161,25 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="110" t="s">
+      <c r="B3" s="107" t="s">
         <v>92</v>
       </c>
-      <c r="C3" s="111" t="s">
+      <c r="C3" s="108" t="s">
         <v>93</v>
       </c>
-      <c r="D3" s="111" t="s">
+      <c r="D3" s="108" t="s">
         <v>259</v>
       </c>
-      <c r="E3" s="111" t="n">
+      <c r="E3" s="108" t="n">
         <v>8.77968</v>
       </c>
-      <c r="F3" s="111" t="n">
+      <c r="F3" s="108" t="n">
         <v>-2703</v>
       </c>
-      <c r="G3" s="112" t="n">
+      <c r="G3" s="109" t="n">
         <v>7.16226</v>
       </c>
-      <c r="H3" s="113" t="n">
+      <c r="H3" s="110" t="n">
         <v>-6620</v>
       </c>
     </row>
@@ -17277,11 +17242,11 @@
       <c r="G6" s="1" t="n">
         <v>15.99439325</v>
       </c>
-      <c r="I6" s="114" t="s">
+      <c r="I6" s="111" t="s">
         <v>262</v>
       </c>
-      <c r="J6" s="114"/>
-      <c r="K6" s="114"/>
+      <c r="J6" s="111"/>
+      <c r="K6" s="111"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D7" s="0" t="s">
@@ -17293,9 +17258,9 @@
       <c r="G7" s="1" t="n">
         <v>1.63763854</v>
       </c>
-      <c r="I7" s="114"/>
-      <c r="J7" s="114"/>
-      <c r="K7" s="114"/>
+      <c r="I7" s="111"/>
+      <c r="J7" s="111"/>
+      <c r="K7" s="111"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -17322,10 +17287,10 @@
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+      <selection pane="topLeft" activeCell="E4" activeCellId="1" sqref="K56:K58 E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.36"/>
@@ -17335,26 +17300,26 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="115"/>
-      <c r="B1" s="116"/>
-      <c r="C1" s="116"/>
-      <c r="D1" s="116"/>
-      <c r="E1" s="117" t="s">
+      <c r="A1" s="112"/>
+      <c r="B1" s="113"/>
+      <c r="C1" s="113"/>
+      <c r="D1" s="113"/>
+      <c r="E1" s="114" t="s">
         <v>264</v>
       </c>
-      <c r="F1" s="117" t="s">
+      <c r="F1" s="114" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="118" t="s">
+      <c r="G1" s="115" t="s">
         <v>265</v>
       </c>
-      <c r="H1" s="119" t="s">
+      <c r="H1" s="116" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="120"/>
-      <c r="D2" s="121" t="s">
+      <c r="A2" s="117"/>
+      <c r="D2" s="118" t="s">
         <v>267</v>
       </c>
       <c r="E2" s="0" t="n">
@@ -17363,514 +17328,514 @@
       <c r="F2" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="G2" s="122"/>
+      <c r="G2" s="119"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="123" t="s">
+      <c r="A3" s="120" t="s">
         <v>268</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>9002</v>
       </c>
-      <c r="D3" s="121" t="s">
+      <c r="D3" s="118" t="s">
         <v>269</v>
       </c>
-      <c r="E3" s="124" t="n">
+      <c r="E3" s="121" t="n">
         <v>46.1092</v>
       </c>
-      <c r="F3" s="107" t="n">
+      <c r="F3" s="104" t="n">
         <f aca="false">E3-B3*TAN(2*(F2-E2)/1000)</f>
         <v>19.1031189817083</v>
       </c>
-      <c r="G3" s="125" t="n">
+      <c r="G3" s="122" t="n">
         <f aca="false">'Modes A-F'!O54</f>
         <v>17.066</v>
       </c>
-      <c r="H3" s="126" t="n">
+      <c r="H3" s="123" t="n">
         <f aca="false">G3-F3</f>
         <v>-2.0371189817083</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="123" t="s">
+      <c r="A4" s="120" t="s">
         <v>270</v>
       </c>
       <c r="B4" s="0" t="n">
         <f aca="false">B3+635</f>
         <v>9637</v>
       </c>
-      <c r="D4" s="121" t="s">
+      <c r="D4" s="118" t="s">
         <v>271</v>
       </c>
-      <c r="E4" s="107" t="n">
+      <c r="E4" s="104" t="n">
         <f aca="false">'Modes A-F'!K56</f>
-        <v>124.496</v>
-      </c>
-      <c r="F4" s="107" t="n">
+        <v>125.144</v>
+      </c>
+      <c r="F4" s="104" t="n">
         <f aca="false">E4-B4*TAN(2*(F2-E2)/1000)</f>
-        <v>95.5849132666878</v>
-      </c>
-      <c r="G4" s="125" t="n">
+        <v>96.2329132666878</v>
+      </c>
+      <c r="G4" s="122" t="n">
         <f aca="false">'Modes A-F'!O56</f>
-        <v>97.709</v>
-      </c>
-      <c r="H4" s="126" t="n">
+        <v>96.516</v>
+      </c>
+      <c r="H4" s="123" t="n">
         <f aca="false">G4-F4</f>
-        <v>2.12408673331225</v>
+        <v>0.283086733312246</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="127" t="s">
+      <c r="A5" s="124" t="s">
         <v>272</v>
       </c>
-      <c r="B5" s="128" t="n">
+      <c r="B5" s="125" t="n">
         <f aca="false">B3+1790</f>
         <v>10792</v>
       </c>
-      <c r="C5" s="128"/>
-      <c r="D5" s="129" t="s">
+      <c r="C5" s="125"/>
+      <c r="D5" s="126" t="s">
         <v>273</v>
       </c>
-      <c r="E5" s="130" t="n">
+      <c r="E5" s="127" t="n">
         <f aca="false">'Modes A-F'!K57</f>
-        <v>129.341</v>
-      </c>
-      <c r="F5" s="130" t="n">
+        <v>130.739</v>
+      </c>
+      <c r="F5" s="127" t="n">
         <f aca="false">E5-B5*TAN(2*(F2-E2)/1000)</f>
-        <v>96.9649028716503</v>
-      </c>
-      <c r="G5" s="131" t="n">
+        <v>98.3629028716503</v>
+      </c>
+      <c r="G5" s="128" t="n">
         <f aca="false">'Modes A-F'!O57</f>
-        <v>96.004</v>
-      </c>
-      <c r="H5" s="126" t="n">
+        <v>98.811</v>
+      </c>
+      <c r="H5" s="123" t="n">
         <f aca="false">G5-F5</f>
-        <v>-0.960902871650333</v>
+        <v>0.448097128349673</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H6" s="126" t="n">
+      <c r="H6" s="123" t="n">
         <f aca="false">AVERAGE(H3,H4,H5)</f>
-        <v>-0.291311706682126</v>
+        <v>-0.435311706682127</v>
       </c>
       <c r="I6" s="0" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="132" t="s">
+      <c r="A8" s="129" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="132"/>
-      <c r="C8" s="132"/>
-      <c r="D8" s="116"/>
-      <c r="E8" s="116"/>
-      <c r="F8" s="133" t="s">
+      <c r="B8" s="129"/>
+      <c r="C8" s="129"/>
+      <c r="D8" s="113"/>
+      <c r="E8" s="113"/>
+      <c r="F8" s="130" t="s">
         <v>275</v>
       </c>
-      <c r="G8" s="134" t="n">
+      <c r="G8" s="131" t="n">
         <v>-0.1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="120"/>
-      <c r="D9" s="121" t="s">
+      <c r="A9" s="117"/>
+      <c r="D9" s="118" t="s">
         <v>267</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>3.5</v>
       </c>
-      <c r="G9" s="122" t="n">
+      <c r="G9" s="119" t="n">
         <f aca="false">E9+G8</f>
         <v>3.4</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="123" t="s">
+      <c r="A10" s="120" t="s">
         <v>276</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>10907</v>
       </c>
-      <c r="D10" s="121" t="s">
+      <c r="D10" s="118" t="s">
         <v>269</v>
       </c>
-      <c r="E10" s="126" t="n">
+      <c r="E10" s="123" t="n">
         <f aca="false">'Modes A-F'!E54</f>
         <v>31.259</v>
       </c>
-      <c r="F10" s="126"/>
-      <c r="G10" s="135" t="n">
+      <c r="F10" s="123"/>
+      <c r="G10" s="132" t="n">
         <f aca="false">E10-B10*TAN(2*(G9-E9)/1000)</f>
         <v>33.4404000290853</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="123" t="s">
+      <c r="A11" s="120" t="s">
         <v>277</v>
       </c>
       <c r="B11" s="0" t="n">
         <f aca="false">B10+635</f>
         <v>11542</v>
       </c>
-      <c r="D11" s="121" t="s">
+      <c r="D11" s="118" t="s">
         <v>271</v>
       </c>
-      <c r="E11" s="126" t="n">
+      <c r="E11" s="123" t="n">
         <f aca="false">'Modes A-F'!E57</f>
-        <v>116.993</v>
-      </c>
-      <c r="F11" s="126"/>
-      <c r="G11" s="135" t="n">
+        <v>119.819</v>
+      </c>
+      <c r="F11" s="123"/>
+      <c r="G11" s="132" t="n">
         <f aca="false">E11-B11*TAN(2*(G9-E9)/1000)</f>
-        <v>119.301400030779</v>
+        <v>122.127400030779</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="127" t="s">
+      <c r="A12" s="124" t="s">
         <v>278</v>
       </c>
-      <c r="B12" s="128" t="n">
+      <c r="B12" s="125" t="n">
         <f aca="false">B10+1790</f>
         <v>12697</v>
       </c>
-      <c r="C12" s="128"/>
-      <c r="D12" s="129" t="s">
+      <c r="C12" s="125"/>
+      <c r="D12" s="126" t="s">
         <v>273</v>
       </c>
-      <c r="E12" s="136" t="n">
+      <c r="E12" s="133" t="n">
         <f aca="false">'Modes A-F'!E58</f>
-        <v>116.993</v>
-      </c>
-      <c r="F12" s="136"/>
-      <c r="G12" s="137" t="n">
+        <v>119.819</v>
+      </c>
+      <c r="F12" s="133"/>
+      <c r="G12" s="134" t="n">
         <f aca="false">E12-B12*TAN(2*(G9-E9)/1000)</f>
-        <v>119.532400033859</v>
+        <v>122.358400033859</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="132" t="s">
+      <c r="A16" s="129" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="132"/>
-      <c r="C16" s="132"/>
-      <c r="D16" s="116"/>
-      <c r="E16" s="116"/>
-      <c r="F16" s="133" t="s">
+      <c r="B16" s="129"/>
+      <c r="C16" s="129"/>
+      <c r="D16" s="113"/>
+      <c r="E16" s="113"/>
+      <c r="F16" s="130" t="s">
         <v>275</v>
       </c>
-      <c r="G16" s="116" t="n">
+      <c r="G16" s="113" t="n">
         <v>0.275</v>
       </c>
-      <c r="H16" s="116"/>
-      <c r="I16" s="134"/>
+      <c r="H16" s="113"/>
+      <c r="I16" s="131"/>
     </row>
     <row r="17" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="120"/>
-      <c r="D17" s="121" t="s">
+      <c r="A17" s="117"/>
+      <c r="D17" s="118" t="s">
         <v>267</v>
       </c>
       <c r="E17" s="0" t="n">
         <v>3.225</v>
       </c>
-      <c r="G17" s="75" t="n">
+      <c r="G17" s="72" t="n">
         <f aca="false">E17+G16</f>
         <v>3.5</v>
       </c>
-      <c r="H17" s="64" t="s">
+      <c r="H17" s="61" t="s">
         <v>279</v>
       </c>
-      <c r="I17" s="122" t="n">
+      <c r="I17" s="119" t="n">
         <f aca="false">B18*TAN(2*(E9-G17)/1000)</f>
         <v>0</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="123" t="s">
+      <c r="A18" s="120" t="s">
         <v>280</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>1908</v>
       </c>
-      <c r="D18" s="121" t="s">
+      <c r="D18" s="118" t="s">
         <v>281</v>
       </c>
       <c r="E18" s="0" t="n">
         <v>-7.25</v>
       </c>
-      <c r="G18" s="138" t="n">
+      <c r="G18" s="135" t="n">
         <f aca="false">E18+B18*TAN(2*(G17-E17)/1000)</f>
         <v>-6.20059989418549</v>
       </c>
-      <c r="I18" s="122"/>
+      <c r="I18" s="119"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="120"/>
-      <c r="D19" s="121" t="s">
+      <c r="A19" s="117"/>
+      <c r="D19" s="118" t="s">
         <v>282</v>
       </c>
       <c r="E19" s="0" t="n">
         <f aca="false">3.5 + (3.5-E17)</f>
         <v>3.775</v>
       </c>
-      <c r="G19" s="75" t="n">
+      <c r="G19" s="72" t="n">
         <f aca="false">E19-G16</f>
         <v>3.5</v>
       </c>
-      <c r="I19" s="122"/>
+      <c r="I19" s="119"/>
     </row>
     <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="120"/>
-      <c r="D20" s="121"/>
-      <c r="G20" s="139" t="s">
+      <c r="A20" s="117"/>
+      <c r="D20" s="118"/>
+      <c r="G20" s="136" t="s">
         <v>283</v>
       </c>
-      <c r="I20" s="122"/>
+      <c r="I20" s="119"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="120"/>
-      <c r="F21" s="140" t="s">
+      <c r="A21" s="117"/>
+      <c r="F21" s="137" t="s">
         <v>265</v>
       </c>
-      <c r="I21" s="122"/>
+      <c r="I21" s="119"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="123" t="s">
+      <c r="A22" s="120" t="s">
         <v>268</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>9002</v>
       </c>
-      <c r="D22" s="121" t="s">
+      <c r="D22" s="118" t="s">
         <v>269</v>
       </c>
-      <c r="E22" s="126" t="n">
+      <c r="E22" s="123" t="n">
         <f aca="false">E10-B22*TAN(2*(E19)/1000)+I17</f>
         <v>-36.7073914229833</v>
       </c>
-      <c r="F22" s="141" t="n">
+      <c r="F22" s="138" t="n">
         <f aca="false">'Modes A-F'!I54</f>
         <v>-23.247</v>
       </c>
-      <c r="G22" s="126" t="n">
+      <c r="G22" s="123" t="n">
         <f aca="false">E10-B22*TAN(2*(G19)/1000)+I17</f>
         <v>-31.75602924884</v>
       </c>
-      <c r="I22" s="122"/>
+      <c r="I22" s="119"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="123" t="s">
+      <c r="A23" s="120" t="s">
         <v>270</v>
       </c>
       <c r="B23" s="0" t="n">
         <f aca="false">B22+635</f>
         <v>9637</v>
       </c>
-      <c r="D23" s="121" t="s">
+      <c r="D23" s="118" t="s">
         <v>271</v>
       </c>
-      <c r="E23" s="126" t="n">
+      <c r="E23" s="123" t="n">
         <f aca="false">E11-B23*TAN(2*(E19)/1000)+I17</f>
-        <v>44.2322674801944</v>
-      </c>
-      <c r="F23" s="141" t="n">
+        <v>47.0582674801944</v>
+      </c>
+      <c r="F23" s="138" t="n">
         <f aca="false">'Modes A-F'!I56</f>
-        <v>54.559</v>
-      </c>
-      <c r="G23" s="126" t="n">
+        <v>54.059</v>
+      </c>
+      <c r="G23" s="123" t="n">
         <f aca="false">E11-B23*TAN(2*(G19)/1000)+I17</f>
-        <v>49.5328981480704</v>
-      </c>
-      <c r="I23" s="122"/>
+        <v>52.3588981480704</v>
+      </c>
+      <c r="I23" s="119"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="127" t="s">
+      <c r="A24" s="124" t="s">
         <v>272</v>
       </c>
-      <c r="B24" s="128" t="n">
+      <c r="B24" s="125" t="n">
         <f aca="false">B22+1790</f>
         <v>10792</v>
       </c>
-      <c r="C24" s="128"/>
-      <c r="D24" s="129" t="s">
+      <c r="C24" s="125"/>
+      <c r="D24" s="126" t="s">
         <v>273</v>
       </c>
-      <c r="E24" s="136" t="n">
+      <c r="E24" s="133" t="n">
         <f aca="false">E12-B24*TAN(2*(E19)/1000)+I17</f>
-        <v>35.5118517843995</v>
-      </c>
-      <c r="F24" s="142" t="n">
+        <v>38.3378517843995</v>
+      </c>
+      <c r="F24" s="139" t="n">
         <f aca="false">'Modes A-F'!I57</f>
-        <v>47.758</v>
-      </c>
-      <c r="G24" s="143" t="n">
+        <v>52.458</v>
+      </c>
+      <c r="G24" s="140" t="n">
         <f aca="false">E12-B24*TAN(2*(G19)/1000)+I17</f>
-        <v>41.447766090482</v>
-      </c>
-      <c r="H24" s="128"/>
-      <c r="I24" s="144"/>
+        <v>44.273766090482</v>
+      </c>
+      <c r="H24" s="125"/>
+      <c r="I24" s="141"/>
     </row>
     <row r="28" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="145" t="s">
+      <c r="A28" s="142" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="145"/>
-      <c r="C28" s="145"/>
-      <c r="D28" s="116"/>
-      <c r="E28" s="116"/>
-      <c r="F28" s="133" t="s">
+      <c r="B28" s="142"/>
+      <c r="C28" s="142"/>
+      <c r="D28" s="113"/>
+      <c r="E28" s="113"/>
+      <c r="F28" s="130" t="s">
         <v>275</v>
       </c>
-      <c r="G28" s="116" t="n">
+      <c r="G28" s="113" t="n">
         <v>0.275</v>
       </c>
-      <c r="H28" s="116"/>
-      <c r="I28" s="134"/>
+      <c r="H28" s="113"/>
+      <c r="I28" s="131"/>
     </row>
     <row r="29" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="120"/>
-      <c r="D29" s="121" t="s">
+      <c r="A29" s="117"/>
+      <c r="D29" s="118" t="s">
         <v>267</v>
       </c>
       <c r="E29" s="0" t="n">
         <v>3.225</v>
       </c>
-      <c r="G29" s="75" t="n">
+      <c r="G29" s="72" t="n">
         <f aca="false">E29+G28</f>
         <v>3.5</v>
       </c>
-      <c r="H29" s="64" t="s">
+      <c r="H29" s="61" t="s">
         <v>279</v>
       </c>
-      <c r="I29" s="122" t="n">
+      <c r="I29" s="119" t="n">
         <f aca="false">B30*TAN(2*(E9-G29)/1000)</f>
         <v>0</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="123" t="s">
+      <c r="A30" s="120" t="s">
         <v>280</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>1908</v>
       </c>
-      <c r="D30" s="121" t="s">
+      <c r="D30" s="118" t="s">
         <v>281</v>
       </c>
       <c r="E30" s="0" t="n">
         <v>-6.583</v>
       </c>
-      <c r="G30" s="138" t="n">
+      <c r="G30" s="135" t="n">
         <f aca="false">E30+B30*TAN(2*(G29-E29)/1000)</f>
         <v>-5.53359989418549</v>
       </c>
-      <c r="I30" s="122"/>
+      <c r="I30" s="119"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="120"/>
-      <c r="D31" s="121" t="s">
+      <c r="A31" s="117"/>
+      <c r="D31" s="118" t="s">
         <v>282</v>
       </c>
       <c r="E31" s="0" t="n">
         <f aca="false">5+(3.5-E29)</f>
         <v>5.275</v>
       </c>
-      <c r="G31" s="75" t="n">
+      <c r="G31" s="72" t="n">
         <f aca="false">E31-G28</f>
         <v>5</v>
       </c>
-      <c r="I31" s="122"/>
+      <c r="I31" s="119"/>
     </row>
     <row r="32" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="120"/>
-      <c r="D32" s="121"/>
-      <c r="G32" s="139" t="s">
+      <c r="A32" s="117"/>
+      <c r="D32" s="118"/>
+      <c r="G32" s="136" t="s">
         <v>283</v>
       </c>
-      <c r="I32" s="122"/>
+      <c r="I32" s="119"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="120"/>
-      <c r="F33" s="140" t="s">
+      <c r="A33" s="117"/>
+      <c r="F33" s="137" t="s">
         <v>265</v>
       </c>
-      <c r="I33" s="122"/>
+      <c r="I33" s="119"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="123" t="s">
+      <c r="A34" s="120" t="s">
         <v>268</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>9002</v>
       </c>
-      <c r="D34" s="121" t="s">
+      <c r="D34" s="118" t="s">
         <v>269</v>
       </c>
-      <c r="E34" s="126" t="n">
+      <c r="E34" s="123" t="n">
         <f aca="false">E10-B34*TAN(2*(E31)/1000)</f>
         <v>-63.7156236638297</v>
       </c>
-      <c r="F34" s="141" t="n">
+      <c r="F34" s="138" t="n">
         <f aca="false">'Modes A-F'!G54</f>
         <v>-55.188</v>
       </c>
-      <c r="G34" s="126" t="n">
+      <c r="G34" s="123" t="n">
         <f aca="false">E10-B34*TAN(2*(G31)/1000)+I29</f>
         <v>-58.7640007866982</v>
       </c>
-      <c r="I34" s="122"/>
+      <c r="I34" s="119"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="123" t="s">
+      <c r="A35" s="120" t="s">
         <v>270</v>
       </c>
       <c r="B35" s="0" t="n">
         <f aca="false">B34+635</f>
         <v>9637</v>
       </c>
-      <c r="D35" s="121" t="s">
+      <c r="D35" s="118" t="s">
         <v>271</v>
       </c>
-      <c r="E35" s="126" t="n">
+      <c r="E35" s="123" t="n">
         <f aca="false">E11-B35*TAN(2*(E31)/1000)</f>
-        <v>15.3188777773465</v>
-      </c>
-      <c r="F35" s="141" t="n">
+        <v>18.1448777773465</v>
+      </c>
+      <c r="F35" s="138" t="n">
         <f aca="false">'Modes A-F'!G56</f>
         <v>24.4104</v>
       </c>
-      <c r="G35" s="126" t="n">
+      <c r="G35" s="123" t="n">
         <f aca="false">E11-B35*TAN(2*(G31)/1000)+I29</f>
-        <v>20.6197875381681</v>
-      </c>
-      <c r="I35" s="122"/>
+        <v>23.4457875381681</v>
+      </c>
+      <c r="I35" s="119"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="127" t="s">
+      <c r="A36" s="124" t="s">
         <v>272</v>
       </c>
-      <c r="B36" s="128" t="n">
+      <c r="B36" s="125" t="n">
         <f aca="false">B34+1790</f>
         <v>10792</v>
       </c>
-      <c r="C36" s="128"/>
-      <c r="D36" s="129" t="s">
+      <c r="C36" s="125"/>
+      <c r="D36" s="126" t="s">
         <v>273</v>
       </c>
-      <c r="E36" s="136" t="n">
+      <c r="E36" s="133" t="n">
         <f aca="false">E12-B36*TAN(2*(E31)/1000)</f>
-        <v>3.13317567428902</v>
-      </c>
-      <c r="F36" s="142" t="n">
+        <v>5.95917567428903</v>
+      </c>
+      <c r="F36" s="139" t="n">
         <f aca="false">'Modes A-F'!G57</f>
         <v>12.81</v>
       </c>
-      <c r="G36" s="136" t="n">
+      <c r="G36" s="133" t="n">
         <f aca="false">E12-B36*TAN(2*(G31)/1000)+I29</f>
-        <v>9.06940252276749</v>
-      </c>
-      <c r="H36" s="128"/>
-      <c r="I36" s="144"/>
+        <v>11.8954025227675</v>
+      </c>
+      <c r="H36" s="125"/>
+      <c r="I36" s="141"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -17896,10 +17861,10 @@
   <dimension ref="A1:CX484"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="K56:K58 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.26"/>
   </cols>
@@ -17972,7 +17937,7 @@
       <c r="A9" s="0" t="s">
         <v>292</v>
       </c>
-      <c r="B9" s="146" t="n">
+      <c r="B9" s="143" t="n">
         <v>1E-006</v>
       </c>
     </row>
@@ -17996,7 +17961,7 @@
       <c r="A12" s="0" t="s">
         <v>295</v>
       </c>
-      <c r="B12" s="146" t="n">
+      <c r="B12" s="143" t="n">
         <v>1E-005</v>
       </c>
     </row>
@@ -18092,7 +18057,7 @@
       <c r="A24" s="0" t="s">
         <v>307</v>
       </c>
-      <c r="B24" s="146" t="n">
+      <c r="B24" s="143" t="n">
         <v>1E-006</v>
       </c>
     </row>
@@ -18116,7 +18081,7 @@
       <c r="A27" s="0" t="s">
         <v>310</v>
       </c>
-      <c r="B27" s="146" t="n">
+      <c r="B27" s="143" t="n">
         <v>1E-005</v>
       </c>
     </row>
@@ -18212,7 +18177,7 @@
       <c r="A39" s="0" t="s">
         <v>322</v>
       </c>
-      <c r="B39" s="146" t="n">
+      <c r="B39" s="143" t="n">
         <v>1E-006</v>
       </c>
     </row>
@@ -18236,7 +18201,7 @@
       <c r="A42" s="0" t="s">
         <v>325</v>
       </c>
-      <c r="B42" s="146" t="n">
+      <c r="B42" s="143" t="n">
         <v>1E-005</v>
       </c>
     </row>
@@ -18332,7 +18297,7 @@
       <c r="A54" s="0" t="s">
         <v>337</v>
       </c>
-      <c r="B54" s="146" t="n">
+      <c r="B54" s="143" t="n">
         <v>1E-006</v>
       </c>
     </row>
@@ -18356,7 +18321,7 @@
       <c r="A57" s="0" t="s">
         <v>340</v>
       </c>
-      <c r="B57" s="146" t="n">
+      <c r="B57" s="143" t="n">
         <v>1E-005</v>
       </c>
     </row>
@@ -18420,7 +18385,7 @@
       <c r="A65" s="0" t="s">
         <v>348</v>
       </c>
-      <c r="B65" s="146" t="n">
+      <c r="B65" s="143" t="n">
         <v>8.1921E-011</v>
       </c>
     </row>
@@ -18428,7 +18393,7 @@
       <c r="A66" s="0" t="s">
         <v>349</v>
       </c>
-      <c r="B66" s="146" t="n">
+      <c r="B66" s="143" t="n">
         <v>6.1817E-009</v>
       </c>
     </row>
@@ -18436,7 +18401,7 @@
       <c r="A67" s="0" t="s">
         <v>350</v>
       </c>
-      <c r="B67" s="146" t="n">
+      <c r="B67" s="143" t="n">
         <v>-8.139E-009</v>
       </c>
     </row>
@@ -18444,7 +18409,7 @@
       <c r="A68" s="0" t="s">
         <v>351</v>
       </c>
-      <c r="B68" s="146" t="n">
+      <c r="B68" s="143" t="n">
         <v>4.2612E-009</v>
       </c>
     </row>
@@ -18764,7 +18729,7 @@
       <c r="A108" s="0" t="s">
         <v>391</v>
       </c>
-      <c r="B108" s="146" t="n">
+      <c r="B108" s="143" t="n">
         <v>1E-006</v>
       </c>
     </row>
@@ -18788,7 +18753,7 @@
       <c r="A111" s="0" t="s">
         <v>394</v>
       </c>
-      <c r="B111" s="146" t="n">
+      <c r="B111" s="143" t="n">
         <v>1E-005</v>
       </c>
     </row>
@@ -18884,7 +18849,7 @@
       <c r="A123" s="0" t="s">
         <v>406</v>
       </c>
-      <c r="B123" s="146" t="n">
+      <c r="B123" s="143" t="n">
         <v>1E-006</v>
       </c>
     </row>
@@ -18908,7 +18873,7 @@
       <c r="A126" s="0" t="s">
         <v>409</v>
       </c>
-      <c r="B126" s="146" t="n">
+      <c r="B126" s="143" t="n">
         <v>1E-005</v>
       </c>
     </row>
@@ -19004,7 +18969,7 @@
       <c r="A138" s="0" t="s">
         <v>421</v>
       </c>
-      <c r="B138" s="146" t="n">
+      <c r="B138" s="143" t="n">
         <v>1E-006</v>
       </c>
     </row>
@@ -19028,7 +18993,7 @@
       <c r="A141" s="0" t="s">
         <v>424</v>
       </c>
-      <c r="B141" s="146" t="n">
+      <c r="B141" s="143" t="n">
         <v>1E-005</v>
       </c>
     </row>
@@ -19124,7 +19089,7 @@
       <c r="A153" s="0" t="s">
         <v>436</v>
       </c>
-      <c r="B153" s="146" t="n">
+      <c r="B153" s="143" t="n">
         <v>1E-006</v>
       </c>
     </row>
@@ -19148,7 +19113,7 @@
       <c r="A156" s="0" t="s">
         <v>439</v>
       </c>
-      <c r="B156" s="146" t="n">
+      <c r="B156" s="143" t="n">
         <v>1E-005</v>
       </c>
     </row>
@@ -19212,7 +19177,7 @@
       <c r="A164" s="0" t="s">
         <v>447</v>
       </c>
-      <c r="B164" s="146" t="n">
+      <c r="B164" s="143" t="n">
         <v>1.9024E-008</v>
       </c>
     </row>
@@ -19220,7 +19185,7 @@
       <c r="A165" s="0" t="s">
         <v>448</v>
       </c>
-      <c r="B165" s="146" t="n">
+      <c r="B165" s="143" t="n">
         <v>-9.5679E-009</v>
       </c>
     </row>
@@ -19228,7 +19193,7 @@
       <c r="A166" s="0" t="s">
         <v>449</v>
       </c>
-      <c r="B166" s="146" t="n">
+      <c r="B166" s="143" t="n">
         <v>-1.1631E-009</v>
       </c>
     </row>
@@ -19236,7 +19201,7 @@
       <c r="A167" s="0" t="s">
         <v>450</v>
       </c>
-      <c r="B167" s="146" t="n">
+      <c r="B167" s="143" t="n">
         <v>1.027E-008</v>
       </c>
     </row>
@@ -19372,7 +19337,7 @@
       <c r="A184" s="0" t="s">
         <v>467</v>
       </c>
-      <c r="B184" s="146" t="n">
+      <c r="B184" s="143" t="n">
         <v>2.8833E-008</v>
       </c>
     </row>
@@ -19380,7 +19345,7 @@
       <c r="A185" s="0" t="s">
         <v>468</v>
       </c>
-      <c r="B185" s="146" t="n">
+      <c r="B185" s="143" t="n">
         <v>2.8833E-008</v>
       </c>
     </row>
@@ -19412,7 +19377,7 @@
       <c r="A189" s="0" t="s">
         <v>472</v>
       </c>
-      <c r="B189" s="146" t="n">
+      <c r="B189" s="143" t="n">
         <v>4761600</v>
       </c>
     </row>
@@ -19436,7 +19401,7 @@
       <c r="A192" s="0" t="s">
         <v>475</v>
       </c>
-      <c r="B192" s="146" t="n">
+      <c r="B192" s="143" t="n">
         <v>2.8343E-008</v>
       </c>
     </row>
@@ -19444,7 +19409,7 @@
       <c r="A193" s="0" t="s">
         <v>476</v>
       </c>
-      <c r="B193" s="146" t="n">
+      <c r="B193" s="143" t="n">
         <v>-7.401E-010</v>
       </c>
     </row>
@@ -19452,7 +19417,7 @@
       <c r="A194" s="0" t="s">
         <v>477</v>
       </c>
-      <c r="B194" s="146" t="n">
+      <c r="B194" s="143" t="n">
         <v>-1.4084E-009</v>
       </c>
     </row>
@@ -19460,7 +19425,7 @@
       <c r="A195" s="0" t="s">
         <v>478</v>
       </c>
-      <c r="B195" s="146" t="n">
+      <c r="B195" s="143" t="n">
         <v>2.0325E-008</v>
       </c>
     </row>
@@ -20884,40 +20849,40 @@
       <c r="B337" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C337" s="146" t="n">
+      <c r="C337" s="143" t="n">
         <v>8.3006E-011</v>
       </c>
-      <c r="D337" s="146" t="n">
+      <c r="D337" s="143" t="n">
         <v>8.2839E-011</v>
       </c>
-      <c r="E337" s="146" t="n">
+      <c r="E337" s="143" t="n">
         <v>8.2777E-011</v>
       </c>
-      <c r="F337" s="146" t="n">
+      <c r="F337" s="143" t="n">
         <v>8.1528E-011</v>
       </c>
-      <c r="G337" s="146" t="n">
+      <c r="G337" s="143" t="n">
         <v>8.2662E-011</v>
       </c>
-      <c r="H337" s="146" t="n">
+      <c r="H337" s="143" t="n">
         <v>8.3572E-011</v>
       </c>
-      <c r="I337" s="146" t="n">
+      <c r="I337" s="143" t="n">
         <v>8.489E-011</v>
       </c>
-      <c r="J337" s="146" t="n">
+      <c r="J337" s="143" t="n">
         <v>8.3896E-011</v>
       </c>
-      <c r="K337" s="146" t="n">
+      <c r="K337" s="143" t="n">
         <v>8.2012E-011</v>
       </c>
-      <c r="L337" s="146" t="n">
+      <c r="L337" s="143" t="n">
         <v>8.0897E-011</v>
       </c>
-      <c r="M337" s="146" t="n">
+      <c r="M337" s="143" t="n">
         <v>8.29E-011</v>
       </c>
-      <c r="N337" s="146" t="n">
+      <c r="N337" s="143" t="n">
         <v>8.0797E-011</v>
       </c>
     </row>
@@ -20928,40 +20893,40 @@
       <c r="B338" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C338" s="146" t="n">
+      <c r="C338" s="143" t="n">
         <v>6.3068E-009</v>
       </c>
-      <c r="D338" s="146" t="n">
+      <c r="D338" s="143" t="n">
         <v>6.0737E-009</v>
       </c>
-      <c r="E338" s="146" t="n">
+      <c r="E338" s="143" t="n">
         <v>6.6921E-009</v>
       </c>
-      <c r="F338" s="146" t="n">
+      <c r="F338" s="143" t="n">
         <v>5.7007E-009</v>
       </c>
-      <c r="G338" s="146" t="n">
+      <c r="G338" s="143" t="n">
         <v>5.6393E-009</v>
       </c>
-      <c r="H338" s="146" t="n">
+      <c r="H338" s="143" t="n">
         <v>6.6627E-009</v>
       </c>
-      <c r="I338" s="146" t="n">
+      <c r="I338" s="143" t="n">
         <v>6.6038E-009</v>
       </c>
-      <c r="J338" s="146" t="n">
+      <c r="J338" s="143" t="n">
         <v>5.87E-009</v>
       </c>
-      <c r="K338" s="146" t="n">
+      <c r="K338" s="143" t="n">
         <v>6.1792E-009</v>
       </c>
-      <c r="L338" s="146" t="n">
+      <c r="L338" s="143" t="n">
         <v>5.3276E-009</v>
       </c>
-      <c r="M338" s="146" t="n">
+      <c r="M338" s="143" t="n">
         <v>6.513E-009</v>
       </c>
-      <c r="N338" s="146" t="n">
+      <c r="N338" s="143" t="n">
         <v>5.9829E-009</v>
       </c>
     </row>
@@ -20972,40 +20937,40 @@
       <c r="B339" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C339" s="146" t="n">
+      <c r="C339" s="143" t="n">
         <v>-7.2948E-009</v>
       </c>
-      <c r="D339" s="146" t="n">
+      <c r="D339" s="143" t="n">
         <v>-7.6015E-009</v>
       </c>
-      <c r="E339" s="146" t="n">
+      <c r="E339" s="143" t="n">
         <v>-7.4862E-009</v>
       </c>
-      <c r="F339" s="146" t="n">
+      <c r="F339" s="143" t="n">
         <v>-8.5513E-009</v>
       </c>
-      <c r="G339" s="146" t="n">
+      <c r="G339" s="143" t="n">
         <v>-8.3206E-009</v>
       </c>
-      <c r="H339" s="146" t="n">
+      <c r="H339" s="143" t="n">
         <v>-7.5942E-009</v>
       </c>
-      <c r="I339" s="146" t="n">
+      <c r="I339" s="143" t="n">
         <v>-7.5377E-009</v>
       </c>
-      <c r="J339" s="146" t="n">
+      <c r="J339" s="143" t="n">
         <v>-8.5415E-009</v>
       </c>
-      <c r="K339" s="146" t="n">
+      <c r="K339" s="143" t="n">
         <v>-7.7635E-009</v>
       </c>
-      <c r="L339" s="146" t="n">
+      <c r="L339" s="143" t="n">
         <v>-8.0482E-009</v>
       </c>
-      <c r="M339" s="146" t="n">
+      <c r="M339" s="143" t="n">
         <v>-8.2175E-009</v>
       </c>
-      <c r="N339" s="146" t="n">
+      <c r="N339" s="143" t="n">
         <v>-7.9966E-009</v>
       </c>
     </row>
@@ -21016,40 +20981,40 @@
       <c r="B340" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C340" s="146" t="n">
+      <c r="C340" s="143" t="n">
         <v>4.8625E-009</v>
       </c>
-      <c r="D340" s="146" t="n">
+      <c r="D340" s="143" t="n">
         <v>4.433E-009</v>
       </c>
-      <c r="E340" s="146" t="n">
+      <c r="E340" s="143" t="n">
         <v>3.4611E-009</v>
       </c>
-      <c r="F340" s="146" t="n">
+      <c r="F340" s="143" t="n">
         <v>3.9372E-009</v>
       </c>
-      <c r="G340" s="146" t="n">
+      <c r="G340" s="143" t="n">
         <v>4.8526E-009</v>
       </c>
-      <c r="H340" s="146" t="n">
+      <c r="H340" s="143" t="n">
         <v>4.5041E-009</v>
       </c>
-      <c r="I340" s="146" t="n">
+      <c r="I340" s="143" t="n">
         <v>4.5311E-009</v>
       </c>
-      <c r="J340" s="146" t="n">
+      <c r="J340" s="143" t="n">
         <v>4.2882E-009</v>
       </c>
-      <c r="K340" s="146" t="n">
+      <c r="K340" s="143" t="n">
         <v>4.4551E-009</v>
       </c>
-      <c r="L340" s="146" t="n">
+      <c r="L340" s="143" t="n">
         <v>4.136E-009</v>
       </c>
-      <c r="M340" s="146" t="n">
+      <c r="M340" s="143" t="n">
         <v>3.9078E-009</v>
       </c>
-      <c r="N340" s="146" t="n">
+      <c r="N340" s="143" t="n">
         <v>3.9593E-009</v>
       </c>
     </row>
@@ -21764,40 +21729,40 @@
       <c r="B357" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C357" s="146" t="n">
+      <c r="C357" s="143" t="n">
         <v>2.1231E-008</v>
       </c>
-      <c r="D357" s="146" t="n">
+      <c r="D357" s="143" t="n">
         <v>1.9514E-008</v>
       </c>
-      <c r="E357" s="146" t="n">
+      <c r="E357" s="143" t="n">
         <v>1.8533E-008</v>
       </c>
-      <c r="F357" s="146" t="n">
+      <c r="F357" s="143" t="n">
         <v>2.1231E-008</v>
       </c>
-      <c r="G357" s="146" t="n">
+      <c r="G357" s="143" t="n">
         <v>2.4174E-008</v>
       </c>
-      <c r="H357" s="146" t="n">
+      <c r="H357" s="143" t="n">
         <v>1.9024E-008</v>
       </c>
-      <c r="I357" s="146" t="n">
+      <c r="I357" s="143" t="n">
         <v>2.8588E-008</v>
       </c>
-      <c r="J357" s="146" t="n">
+      <c r="J357" s="143" t="n">
         <v>1.9024E-008</v>
       </c>
-      <c r="K357" s="146" t="n">
+      <c r="K357" s="143" t="n">
         <v>3.2757E-008</v>
       </c>
-      <c r="L357" s="146" t="n">
+      <c r="L357" s="143" t="n">
         <v>3.5455E-008</v>
       </c>
-      <c r="M357" s="146" t="n">
+      <c r="M357" s="143" t="n">
         <v>2.025E-008</v>
       </c>
-      <c r="N357" s="146" t="n">
+      <c r="N357" s="143" t="n">
         <v>2.1231E-008</v>
       </c>
     </row>
@@ -21808,40 +21773,40 @@
       <c r="B358" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C358" s="146" t="n">
+      <c r="C358" s="143" t="n">
         <v>-1.766E-008</v>
       </c>
-      <c r="D358" s="146" t="n">
+      <c r="D358" s="143" t="n">
         <v>-4.4184E-009</v>
       </c>
-      <c r="E358" s="146" t="n">
+      <c r="E358" s="143" t="n">
         <v>-1.1284E-008</v>
       </c>
-      <c r="F358" s="146" t="n">
+      <c r="F358" s="143" t="n">
         <v>-1.1039E-008</v>
       </c>
-      <c r="G358" s="146" t="n">
+      <c r="G358" s="143" t="n">
         <v>-9.5679E-009</v>
       </c>
-      <c r="H358" s="146" t="n">
+      <c r="H358" s="143" t="n">
         <v>-1.1284E-008</v>
       </c>
-      <c r="I358" s="146" t="n">
+      <c r="I358" s="143" t="n">
         <v>-2.2114E-009</v>
       </c>
-      <c r="J358" s="146" t="n">
+      <c r="J358" s="143" t="n">
         <v>-5.3992E-009</v>
       </c>
-      <c r="K358" s="146" t="n">
+      <c r="K358" s="143" t="n">
         <v>9.7642E-010</v>
       </c>
-      <c r="L358" s="146" t="n">
+      <c r="L358" s="143" t="n">
         <v>6.3712E-009</v>
       </c>
-      <c r="M358" s="146" t="n">
+      <c r="M358" s="143" t="n">
         <v>-1.153E-008</v>
       </c>
-      <c r="N358" s="146" t="n">
+      <c r="N358" s="143" t="n">
         <v>-9.8131E-009</v>
       </c>
     </row>
@@ -21852,40 +21817,40 @@
       <c r="B359" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C359" s="146" t="n">
+      <c r="C359" s="143" t="n">
         <v>-9.0112E-009</v>
       </c>
-      <c r="D359" s="146" t="n">
+      <c r="D359" s="143" t="n">
         <v>-4.3514E-009</v>
       </c>
-      <c r="E359" s="146" t="n">
+      <c r="E359" s="143" t="n">
         <v>-6.0682E-009</v>
       </c>
-      <c r="F359" s="146" t="n">
+      <c r="F359" s="143" t="n">
         <v>-9.0112E-009</v>
       </c>
-      <c r="G359" s="146" t="n">
+      <c r="G359" s="143" t="n">
         <v>-4.5967E-009</v>
       </c>
-      <c r="H359" s="146" t="n">
+      <c r="H359" s="143" t="n">
         <v>-1.0483E-008</v>
       </c>
-      <c r="I359" s="146" t="n">
+      <c r="I359" s="143" t="n">
         <v>7.6659E-009</v>
       </c>
-      <c r="J359" s="146" t="n">
+      <c r="J359" s="143" t="n">
         <v>-3.3704E-009</v>
       </c>
-      <c r="K359" s="146" t="n">
+      <c r="K359" s="143" t="n">
         <v>6.6849E-009</v>
       </c>
-      <c r="L359" s="146" t="n">
+      <c r="L359" s="143" t="n">
         <v>5.2134E-009</v>
       </c>
-      <c r="M359" s="146" t="n">
+      <c r="M359" s="143" t="n">
         <v>-1.6536E-009</v>
       </c>
-      <c r="N359" s="146" t="n">
+      <c r="N359" s="143" t="n">
         <v>-5.5777E-009</v>
       </c>
     </row>
@@ -21896,40 +21861,40 @@
       <c r="B360" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C360" s="146" t="n">
+      <c r="C360" s="143" t="n">
         <v>7.8174E-009</v>
       </c>
-      <c r="D360" s="146" t="n">
+      <c r="D360" s="143" t="n">
         <v>2.3513E-008</v>
       </c>
-      <c r="E360" s="146" t="n">
+      <c r="E360" s="143" t="n">
         <v>1.7382E-008</v>
       </c>
-      <c r="F360" s="146" t="n">
+      <c r="F360" s="143" t="n">
         <v>1.1006E-008</v>
       </c>
-      <c r="G360" s="146" t="n">
+      <c r="G360" s="143" t="n">
         <v>1.5665E-008</v>
       </c>
-      <c r="H360" s="146" t="n">
+      <c r="H360" s="143" t="n">
         <v>1.2477E-008</v>
       </c>
-      <c r="I360" s="146" t="n">
+      <c r="I360" s="143" t="n">
         <v>2.057E-008</v>
       </c>
-      <c r="J360" s="146" t="n">
+      <c r="J360" s="143" t="n">
         <v>1.9835E-008</v>
       </c>
-      <c r="K360" s="146" t="n">
+      <c r="K360" s="143" t="n">
         <v>2.5721E-008</v>
       </c>
-      <c r="L360" s="146" t="n">
+      <c r="L360" s="143" t="n">
         <v>2.5475E-008</v>
       </c>
-      <c r="M360" s="146" t="n">
+      <c r="M360" s="143" t="n">
         <v>1.076E-008</v>
       </c>
-      <c r="N360" s="146" t="n">
+      <c r="N360" s="143" t="n">
         <v>1.3213E-008</v>
       </c>
     </row>
@@ -22072,7 +22037,7 @@
       <c r="B364" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C364" s="146" t="n">
+      <c r="C364" s="143" t="n">
         <v>2.8343E-008</v>
       </c>
       <c r="D364" s="0" t="n">
@@ -22116,7 +22081,7 @@
       <c r="B365" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C365" s="146" t="n">
+      <c r="C365" s="143" t="n">
         <v>-7.401E-010</v>
       </c>
       <c r="D365" s="0" t="n">
@@ -22160,7 +22125,7 @@
       <c r="B366" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C366" s="146" t="n">
+      <c r="C366" s="143" t="n">
         <v>-1.4084E-009</v>
       </c>
       <c r="D366" s="0" t="n">
@@ -22204,7 +22169,7 @@
       <c r="B367" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C367" s="146" t="n">
+      <c r="C367" s="143" t="n">
         <v>2.0325E-008</v>
       </c>
       <c r="D367" s="0" t="n">
@@ -23967,10 +23932,10 @@
   <dimension ref="A1:G2383"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A44" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="1" sqref="K56:K58 B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="56.14"/>
@@ -23980,13 +23945,13 @@
       <c r="A1" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B1" s="147" t="s">
+      <c r="B1" s="144" t="s">
         <v>814</v>
       </c>
-      <c r="C1" s="147" t="n">
+      <c r="C1" s="144" t="n">
         <v>350</v>
       </c>
-      <c r="D1" s="147" t="s">
+      <c r="D1" s="144" t="s">
         <v>815</v>
       </c>
     </row>
@@ -23994,10 +23959,10 @@
       <c r="A2" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B2" s="147" t="s">
+      <c r="B2" s="144" t="s">
         <v>816</v>
       </c>
-      <c r="C2" s="147" t="n">
+      <c r="C2" s="144" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -24005,10 +23970,10 @@
       <c r="A3" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="147" t="s">
+      <c r="B3" s="144" t="s">
         <v>817</v>
       </c>
-      <c r="C3" s="147" t="n">
+      <c r="C3" s="144" t="n">
         <v>0.0004</v>
       </c>
     </row>
@@ -24112,7 +24077,7 @@
       <c r="B16" s="0" t="s">
         <v>832</v>
       </c>
-      <c r="C16" s="146" t="n">
+      <c r="C16" s="143" t="n">
         <v>3.71179E-009</v>
       </c>
     </row>
@@ -24120,7 +24085,7 @@
       <c r="B17" s="0" t="s">
         <v>833</v>
       </c>
-      <c r="C17" s="146" t="n">
+      <c r="C17" s="143" t="n">
         <v>3.71272E-009</v>
       </c>
     </row>
@@ -24128,7 +24093,7 @@
       <c r="B18" s="0" t="s">
         <v>834</v>
       </c>
-      <c r="C18" s="146" t="n">
+      <c r="C18" s="143" t="n">
         <v>3.71425E-009</v>
       </c>
     </row>
@@ -24136,7 +24101,7 @@
       <c r="B19" s="0" t="s">
         <v>835</v>
       </c>
-      <c r="C19" s="146" t="n">
+      <c r="C19" s="143" t="n">
         <v>3.71562E-009</v>
       </c>
     </row>
@@ -24624,7 +24589,7 @@
       <c r="B80" s="0" t="s">
         <v>903</v>
       </c>
-      <c r="C80" s="146" t="n">
+      <c r="C80" s="143" t="n">
         <v>1.58855E-007</v>
       </c>
     </row>
@@ -24672,7 +24637,7 @@
       <c r="B86" s="0" t="s">
         <v>909</v>
       </c>
-      <c r="C86" s="146" t="n">
+      <c r="C86" s="143" t="n">
         <v>1.58316E-007</v>
       </c>
     </row>
@@ -24704,7 +24669,7 @@
       <c r="B90" s="0" t="s">
         <v>913</v>
       </c>
-      <c r="C90" s="146" t="n">
+      <c r="C90" s="143" t="n">
         <v>1.57838E-007</v>
       </c>
     </row>
@@ -24792,7 +24757,7 @@
       <c r="B101" s="0" t="s">
         <v>925</v>
       </c>
-      <c r="C101" s="146" t="n">
+      <c r="C101" s="143" t="n">
         <v>2.397E-009</v>
       </c>
     </row>
@@ -24968,7 +24933,7 @@
       <c r="B123" s="0" t="s">
         <v>949</v>
       </c>
-      <c r="C123" s="146" t="n">
+      <c r="C123" s="143" t="n">
         <v>2.37898E-010</v>
       </c>
     </row>
@@ -25032,7 +24997,7 @@
       <c r="B131" s="0" t="s">
         <v>957</v>
       </c>
-      <c r="C131" s="146" t="n">
+      <c r="C131" s="143" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -25048,7 +25013,7 @@
       <c r="B133" s="0" t="s">
         <v>959</v>
       </c>
-      <c r="C133" s="146" t="n">
+      <c r="C133" s="143" t="n">
         <v>1.97895E-005</v>
       </c>
     </row>
@@ -25568,7 +25533,7 @@
       <c r="B198" s="0" t="s">
         <v>1026</v>
       </c>
-      <c r="C198" s="146" t="n">
+      <c r="C198" s="143" t="n">
         <v>2.78422E-007</v>
       </c>
     </row>
@@ -25616,7 +25581,7 @@
       <c r="B204" s="0" t="s">
         <v>1032</v>
       </c>
-      <c r="C204" s="146" t="n">
+      <c r="C204" s="143" t="n">
         <v>2.77565E-007</v>
       </c>
     </row>
@@ -25648,7 +25613,7 @@
       <c r="B208" s="0" t="s">
         <v>1036</v>
       </c>
-      <c r="C208" s="146" t="n">
+      <c r="C208" s="143" t="n">
         <v>2.76716E-007</v>
       </c>
     </row>
@@ -25736,7 +25701,7 @@
       <c r="B219" s="0" t="s">
         <v>1047</v>
       </c>
-      <c r="C219" s="146" t="n">
+      <c r="C219" s="143" t="n">
         <v>5.98328E-009</v>
       </c>
     </row>
@@ -25912,7 +25877,7 @@
       <c r="B241" s="0" t="s">
         <v>1070</v>
       </c>
-      <c r="C241" s="146" t="n">
+      <c r="C241" s="143" t="n">
         <v>4.11728E-010</v>
       </c>
     </row>
@@ -25976,7 +25941,7 @@
       <c r="B249" s="0" t="s">
         <v>1078</v>
       </c>
-      <c r="C249" s="146" t="n">
+      <c r="C249" s="143" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -25992,7 +25957,7 @@
       <c r="B251" s="0" t="s">
         <v>1080</v>
       </c>
-      <c r="C251" s="146" t="n">
+      <c r="C251" s="143" t="n">
         <v>3.46956E-005</v>
       </c>
     </row>
@@ -26512,7 +26477,7 @@
       <c r="B316" s="0" t="s">
         <v>1145</v>
       </c>
-      <c r="C316" s="146" t="n">
+      <c r="C316" s="143" t="n">
         <v>5.45673E-012</v>
       </c>
     </row>
@@ -26560,7 +26525,7 @@
       <c r="B322" s="0" t="s">
         <v>1151</v>
       </c>
-      <c r="C322" s="146" t="n">
+      <c r="C322" s="143" t="n">
         <v>7.71713E-013</v>
       </c>
     </row>
@@ -26592,7 +26557,7 @@
       <c r="B326" s="0" t="s">
         <v>1155</v>
       </c>
-      <c r="C326" s="146" t="n">
+      <c r="C326" s="143" t="n">
         <v>-7.72781E-012</v>
       </c>
     </row>
@@ -26680,7 +26645,7 @@
       <c r="B337" s="0" t="s">
         <v>1166</v>
       </c>
-      <c r="C337" s="146" t="n">
+      <c r="C337" s="143" t="n">
         <v>5.61762E-010</v>
       </c>
     </row>
@@ -26856,7 +26821,7 @@
       <c r="B359" s="0" t="s">
         <v>1189</v>
       </c>
-      <c r="C359" s="146" t="n">
+      <c r="C359" s="143" t="n">
         <v>2.605E-012</v>
       </c>
     </row>
@@ -26920,7 +26885,7 @@
       <c r="B367" s="0" t="s">
         <v>1197</v>
       </c>
-      <c r="C367" s="146" t="n">
+      <c r="C367" s="143" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -26936,7 +26901,7 @@
       <c r="B369" s="0" t="s">
         <v>1199</v>
       </c>
-      <c r="C369" s="146" t="n">
+      <c r="C369" s="143" t="n">
         <v>9.64642E-011</v>
       </c>
     </row>
@@ -27456,7 +27421,7 @@
       <c r="B434" s="0" t="s">
         <v>1264</v>
       </c>
-      <c r="C434" s="146" t="n">
+      <c r="C434" s="143" t="n">
         <v>5.42202E-012</v>
       </c>
     </row>
@@ -27504,7 +27469,7 @@
       <c r="B440" s="0" t="s">
         <v>1270</v>
       </c>
-      <c r="C440" s="146" t="n">
+      <c r="C440" s="143" t="n">
         <v>5.83458E-013</v>
       </c>
     </row>
@@ -27536,7 +27501,7 @@
       <c r="B444" s="0" t="s">
         <v>1274</v>
       </c>
-      <c r="C444" s="146" t="n">
+      <c r="C444" s="143" t="n">
         <v>-5.09224E-012</v>
       </c>
     </row>
@@ -27624,7 +27589,7 @@
       <c r="B455" s="0" t="s">
         <v>1285</v>
       </c>
-      <c r="C455" s="146" t="n">
+      <c r="C455" s="143" t="n">
         <v>2.08783E-010</v>
       </c>
     </row>
@@ -27800,7 +27765,7 @@
       <c r="B477" s="0" t="s">
         <v>1308</v>
       </c>
-      <c r="C477" s="146" t="n">
+      <c r="C477" s="143" t="n">
         <v>2.32565E-012</v>
       </c>
     </row>
@@ -27864,7 +27829,7 @@
       <c r="B485" s="0" t="s">
         <v>1316</v>
       </c>
-      <c r="C485" s="146" t="n">
+      <c r="C485" s="143" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -27880,7 +27845,7 @@
       <c r="B487" s="0" t="s">
         <v>1318</v>
       </c>
-      <c r="C487" s="146" t="n">
+      <c r="C487" s="143" t="n">
         <v>7.29322E-011</v>
       </c>
     </row>
@@ -27968,7 +27933,7 @@
       <c r="B498" s="0" t="s">
         <v>1329</v>
       </c>
-      <c r="C498" s="146" t="n">
+      <c r="C498" s="143" t="n">
         <v>3.71179E-009</v>
       </c>
     </row>
@@ -27976,7 +27941,7 @@
       <c r="B499" s="0" t="s">
         <v>1330</v>
       </c>
-      <c r="C499" s="146" t="n">
+      <c r="C499" s="143" t="n">
         <v>3.71272E-009</v>
       </c>
     </row>
@@ -27984,7 +27949,7 @@
       <c r="B500" s="0" t="s">
         <v>1331</v>
       </c>
-      <c r="C500" s="146" t="n">
+      <c r="C500" s="143" t="n">
         <v>3.71425E-009</v>
       </c>
     </row>
@@ -27992,7 +27957,7 @@
       <c r="B501" s="0" t="s">
         <v>1332</v>
       </c>
-      <c r="C501" s="146" t="n">
+      <c r="C501" s="143" t="n">
         <v>3.71562E-009</v>
       </c>
     </row>
@@ -28560,7 +28525,7 @@
       <c r="B572" s="0" t="s">
         <v>1403</v>
       </c>
-      <c r="C572" s="146" t="n">
+      <c r="C572" s="143" t="n">
         <v>1.19678E-007</v>
       </c>
     </row>
@@ -28608,7 +28573,7 @@
       <c r="B578" s="0" t="s">
         <v>1409</v>
       </c>
-      <c r="C578" s="146" t="n">
+      <c r="C578" s="143" t="n">
         <v>1.19249E-007</v>
       </c>
     </row>
@@ -28640,7 +28605,7 @@
       <c r="B582" s="0" t="s">
         <v>1413</v>
       </c>
-      <c r="C582" s="146" t="n">
+      <c r="C582" s="143" t="n">
         <v>1.18808E-007</v>
       </c>
     </row>
@@ -28728,7 +28693,7 @@
       <c r="B593" s="0" t="s">
         <v>1424</v>
       </c>
-      <c r="C593" s="146" t="n">
+      <c r="C593" s="143" t="n">
         <v>3.58628E-009</v>
       </c>
     </row>
@@ -28904,7 +28869,7 @@
       <c r="B615" s="0" t="s">
         <v>1447</v>
       </c>
-      <c r="C615" s="146" t="n">
+      <c r="C615" s="143" t="n">
         <v>1.9029E-010</v>
       </c>
     </row>
@@ -28968,7 +28933,7 @@
       <c r="B623" s="0" t="s">
         <v>1455</v>
       </c>
-      <c r="C623" s="146" t="n">
+      <c r="C623" s="143" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -28984,7 +28949,7 @@
       <c r="B625" s="0" t="s">
         <v>1457</v>
       </c>
-      <c r="C625" s="146" t="n">
+      <c r="C625" s="143" t="n">
         <v>1.49062E-005</v>
       </c>
     </row>
@@ -29504,7 +29469,7 @@
       <c r="B690" s="0" t="s">
         <v>1522</v>
       </c>
-      <c r="C690" s="146" t="n">
+      <c r="C690" s="143" t="n">
         <v>5.80654E-012</v>
       </c>
     </row>
@@ -29552,7 +29517,7 @@
       <c r="B696" s="0" t="s">
         <v>1528</v>
       </c>
-      <c r="C696" s="146" t="n">
+      <c r="C696" s="143" t="n">
         <v>-1.88255E-013</v>
       </c>
     </row>
@@ -29584,7 +29549,7 @@
       <c r="B700" s="0" t="s">
         <v>1532</v>
       </c>
-      <c r="C700" s="146" t="n">
+      <c r="C700" s="143" t="n">
         <v>-6.71043E-012</v>
       </c>
     </row>
@@ -29672,7 +29637,7 @@
       <c r="B711" s="0" t="s">
         <v>1543</v>
       </c>
-      <c r="C711" s="146" t="n">
+      <c r="C711" s="143" t="n">
         <v>-3.52979E-010</v>
       </c>
     </row>
@@ -29848,7 +29813,7 @@
       <c r="B733" s="0" t="s">
         <v>1566</v>
       </c>
-      <c r="C733" s="146" t="n">
+      <c r="C733" s="143" t="n">
         <v>2.64443E-012</v>
       </c>
     </row>
@@ -29912,7 +29877,7 @@
       <c r="B741" s="0" t="s">
         <v>1574</v>
       </c>
-      <c r="C741" s="146" t="n">
+      <c r="C741" s="143" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -29928,7 +29893,7 @@
       <c r="B743" s="0" t="s">
         <v>1576</v>
       </c>
-      <c r="C743" s="146" t="n">
+      <c r="C743" s="143" t="n">
         <v>-2.35319E-011</v>
       </c>
     </row>
@@ -30484,7 +30449,7 @@
       <c r="B811" s="0" t="s">
         <v>1652</v>
       </c>
-      <c r="C811" s="146" t="n">
+      <c r="C811" s="143" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -31000,7 +30965,7 @@
       <c r="B874" s="0" t="s">
         <v>1717</v>
       </c>
-      <c r="C874" s="146" t="n">
+      <c r="C874" s="143" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -31516,7 +31481,7 @@
       <c r="B937" s="0" t="s">
         <v>1782</v>
       </c>
-      <c r="C937" s="146" t="n">
+      <c r="C937" s="143" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -32032,7 +31997,7 @@
       <c r="B1000" s="0" t="s">
         <v>1847</v>
       </c>
-      <c r="C1000" s="146" t="n">
+      <c r="C1000" s="143" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -32548,7 +32513,7 @@
       <c r="B1063" s="0" t="s">
         <v>1912</v>
       </c>
-      <c r="C1063" s="146" t="n">
+      <c r="C1063" s="143" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -33064,7 +33029,7 @@
       <c r="B1126" s="0" t="s">
         <v>1977</v>
       </c>
-      <c r="C1126" s="146" t="n">
+      <c r="C1126" s="143" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -33580,7 +33545,7 @@
       <c r="B1189" s="0" t="s">
         <v>2042</v>
       </c>
-      <c r="C1189" s="146" t="n">
+      <c r="C1189" s="143" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -34096,7 +34061,7 @@
       <c r="B1252" s="0" t="s">
         <v>2107</v>
       </c>
-      <c r="C1252" s="146" t="n">
+      <c r="C1252" s="143" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -34612,7 +34577,7 @@
       <c r="B1315" s="0" t="s">
         <v>2172</v>
       </c>
-      <c r="C1315" s="146" t="n">
+      <c r="C1315" s="143" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -35128,7 +35093,7 @@
       <c r="B1378" s="0" t="s">
         <v>2237</v>
       </c>
-      <c r="C1378" s="146" t="n">
+      <c r="C1378" s="143" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -35644,7 +35609,7 @@
       <c r="B1441" s="0" t="s">
         <v>2302</v>
       </c>
-      <c r="C1441" s="146" t="n">
+      <c r="C1441" s="143" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -36092,7 +36057,7 @@
       <c r="B1497" s="0" t="s">
         <v>2361</v>
       </c>
-      <c r="C1497" s="146" t="n">
+      <c r="C1497" s="143" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -36718,7 +36683,7 @@
       <c r="B1576" s="0" t="s">
         <v>2445</v>
       </c>
-      <c r="C1576" s="146" t="n">
+      <c r="C1576" s="143" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -36887,7 +36852,7 @@
       <c r="B1596" s="0" t="s">
         <v>2467</v>
       </c>
-      <c r="C1596" s="146" t="n">
+      <c r="C1596" s="143" t="n">
         <v>1000000</v>
       </c>
     </row>
@@ -36895,7 +36860,7 @@
       <c r="B1597" s="0" t="s">
         <v>2468</v>
       </c>
-      <c r="C1597" s="146" t="n">
+      <c r="C1597" s="143" t="n">
         <v>1000000</v>
       </c>
     </row>
@@ -37775,7 +37740,7 @@
       <c r="B1707" s="0" t="s">
         <v>2579</v>
       </c>
-      <c r="C1707" s="146" t="n">
+      <c r="C1707" s="143" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -37791,7 +37756,7 @@
       <c r="B1709" s="0" t="s">
         <v>2581</v>
       </c>
-      <c r="C1709" s="146" t="n">
+      <c r="C1709" s="143" t="n">
         <v>34197800</v>
       </c>
     </row>
@@ -38311,7 +38276,7 @@
       <c r="B1774" s="0" t="s">
         <v>2646</v>
       </c>
-      <c r="C1774" s="146" t="n">
+      <c r="C1774" s="143" t="n">
         <v>12147700</v>
       </c>
     </row>
@@ -38391,7 +38356,7 @@
       <c r="B1784" s="0" t="s">
         <v>2656</v>
       </c>
-      <c r="C1784" s="146" t="n">
+      <c r="C1784" s="143" t="n">
         <v>-7098040</v>
       </c>
     </row>
@@ -38479,7 +38444,7 @@
       <c r="B1795" s="0" t="s">
         <v>2667</v>
       </c>
-      <c r="C1795" s="146" t="n">
+      <c r="C1795" s="143" t="n">
         <v>4465690</v>
       </c>
     </row>
@@ -38655,7 +38620,7 @@
       <c r="B1817" s="0" t="s">
         <v>2690</v>
       </c>
-      <c r="C1817" s="146" t="n">
+      <c r="C1817" s="143" t="n">
         <v>1999640</v>
       </c>
     </row>
@@ -38719,7 +38684,7 @@
       <c r="B1825" s="0" t="s">
         <v>2698</v>
       </c>
-      <c r="C1825" s="146" t="n">
+      <c r="C1825" s="143" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -38735,7 +38700,7 @@
       <c r="B1827" s="0" t="s">
         <v>2700</v>
       </c>
-      <c r="C1827" s="146" t="n">
+      <c r="C1827" s="143" t="n">
         <v>-13532400</v>
       </c>
     </row>
@@ -39338,7 +39303,7 @@
       <c r="B1902" s="0" t="s">
         <v>2777</v>
       </c>
-      <c r="C1902" s="146" t="n">
+      <c r="C1902" s="143" t="n">
         <v>4.37265E-007</v>
       </c>
     </row>
@@ -39386,7 +39351,7 @@
       <c r="B1908" s="0" t="s">
         <v>2783</v>
       </c>
-      <c r="C1908" s="146" t="n">
+      <c r="C1908" s="143" t="n">
         <v>4.35882E-007</v>
       </c>
     </row>
@@ -39418,7 +39383,7 @@
       <c r="B1912" s="0" t="s">
         <v>2787</v>
       </c>
-      <c r="C1912" s="146" t="n">
+      <c r="C1912" s="143" t="n">
         <v>4.34577E-007</v>
       </c>
     </row>
@@ -39506,7 +39471,7 @@
       <c r="B1923" s="0" t="s">
         <v>2798</v>
       </c>
-      <c r="C1923" s="146" t="n">
+      <c r="C1923" s="143" t="n">
         <v>9.15083E-009</v>
       </c>
     </row>
@@ -39682,7 +39647,7 @@
       <c r="B1945" s="0" t="s">
         <v>2821</v>
       </c>
-      <c r="C1945" s="146" t="n">
+      <c r="C1945" s="143" t="n">
         <v>6.45121E-010</v>
       </c>
     </row>
@@ -39746,7 +39711,7 @@
       <c r="B1953" s="0" t="s">
         <v>2829</v>
       </c>
-      <c r="C1953" s="146" t="n">
+      <c r="C1953" s="143" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -39762,7 +39727,7 @@
       <c r="B1955" s="0" t="s">
         <v>2831</v>
       </c>
-      <c r="C1955" s="146" t="n">
+      <c r="C1955" s="143" t="n">
         <v>5.44853E-005</v>
       </c>
     </row>
@@ -40282,7 +40247,7 @@
       <c r="B2020" s="0" t="s">
         <v>2896</v>
       </c>
-      <c r="C2020" s="146" t="n">
+      <c r="C2020" s="143" t="n">
         <v>4.37266E-007</v>
       </c>
     </row>
@@ -40330,7 +40295,7 @@
       <c r="B2026" s="0" t="s">
         <v>2902</v>
       </c>
-      <c r="C2026" s="146" t="n">
+      <c r="C2026" s="143" t="n">
         <v>4.35881E-007</v>
       </c>
     </row>
@@ -40362,7 +40327,7 @@
       <c r="B2030" s="0" t="s">
         <v>2906</v>
       </c>
-      <c r="C2030" s="146" t="n">
+      <c r="C2030" s="143" t="n">
         <v>4.34576E-007</v>
       </c>
     </row>
@@ -40450,7 +40415,7 @@
       <c r="B2041" s="0" t="s">
         <v>2917</v>
       </c>
-      <c r="C2041" s="146" t="n">
+      <c r="C2041" s="143" t="n">
         <v>8.38028E-009</v>
       </c>
     </row>
@@ -40626,7 +40591,7 @@
       <c r="B2063" s="0" t="s">
         <v>2940</v>
       </c>
-      <c r="C2063" s="146" t="n">
+      <c r="C2063" s="143" t="n">
         <v>6.44996E-010</v>
       </c>
     </row>
@@ -40690,7 +40655,7 @@
       <c r="B2071" s="0" t="s">
         <v>2948</v>
       </c>
-      <c r="C2071" s="146" t="n">
+      <c r="C2071" s="143" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -40706,7 +40671,7 @@
       <c r="B2073" s="0" t="s">
         <v>2950</v>
       </c>
-      <c r="C2073" s="146" t="n">
+      <c r="C2073" s="143" t="n">
         <v>5.44851E-005</v>
       </c>
     </row>
@@ -41226,7 +41191,7 @@
       <c r="B2138" s="0" t="s">
         <v>3015</v>
       </c>
-      <c r="C2138" s="146" t="n">
+      <c r="C2138" s="143" t="n">
         <v>1.0545E-011</v>
       </c>
     </row>
@@ -41274,7 +41239,7 @@
       <c r="B2144" s="0" t="s">
         <v>3021</v>
       </c>
-      <c r="C2144" s="146" t="n">
+      <c r="C2144" s="143" t="n">
         <v>1.35517E-012</v>
       </c>
     </row>
@@ -41306,7 +41271,7 @@
       <c r="B2148" s="0" t="s">
         <v>3025</v>
       </c>
-      <c r="C2148" s="146" t="n">
+      <c r="C2148" s="143" t="n">
         <v>-1.06504E-011</v>
       </c>
     </row>
@@ -41394,7 +41359,7 @@
       <c r="B2159" s="0" t="s">
         <v>3036</v>
       </c>
-      <c r="C2159" s="146" t="n">
+      <c r="C2159" s="143" t="n">
         <v>7.70545E-010</v>
       </c>
     </row>
@@ -41570,7 +41535,7 @@
       <c r="B2181" s="0" t="s">
         <v>3059</v>
       </c>
-      <c r="C2181" s="146" t="n">
+      <c r="C2181" s="143" t="n">
         <v>4.1709E-012</v>
       </c>
     </row>
@@ -41634,7 +41599,7 @@
       <c r="B2189" s="0" t="s">
         <v>3067</v>
       </c>
-      <c r="C2189" s="146" t="n">
+      <c r="C2189" s="143" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -41650,7 +41615,7 @@
       <c r="B2191" s="0" t="s">
         <v>3069</v>
       </c>
-      <c r="C2191" s="146" t="n">
+      <c r="C2191" s="143" t="n">
         <v>1.69396E-010</v>
       </c>
     </row>
@@ -42226,7 +42191,7 @@
       <c r="B2263" s="0" t="s">
         <v>3144</v>
       </c>
-      <c r="C2263" s="146" t="n">
+      <c r="C2263" s="143" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -42513,7 +42478,7 @@
       <c r="F2297" s="0" t="s">
         <v>3189</v>
       </c>
-      <c r="G2297" s="148" t="n">
+      <c r="G2297" s="145" t="n">
         <v>41244</v>
       </c>
     </row>
@@ -42605,7 +42570,7 @@
       <c r="B2307" s="0" t="s">
         <v>3203</v>
       </c>
-      <c r="C2307" s="146" t="n">
+      <c r="C2307" s="143" t="n">
         <v>878236000</v>
       </c>
     </row>
@@ -42691,7 +42656,7 @@
       <c r="B2317" s="0" t="s">
         <v>3219</v>
       </c>
-      <c r="C2317" s="146" t="n">
+      <c r="C2317" s="143" t="n">
         <v>32640100000</v>
       </c>
     </row>
@@ -42699,7 +42664,7 @@
       <c r="B2318" s="0" t="s">
         <v>3220</v>
       </c>
-      <c r="C2318" s="146" t="n">
+      <c r="C2318" s="143" t="n">
         <v>33683000000</v>
       </c>
     </row>
@@ -42715,7 +42680,7 @@
       <c r="B2320" s="0" t="s">
         <v>3222</v>
       </c>
-      <c r="C2320" s="146" t="n">
+      <c r="C2320" s="143" t="n">
         <v>30883800</v>
       </c>
     </row>
@@ -42763,7 +42728,7 @@
       <c r="C2326" s="0" t="s">
         <v>3230</v>
       </c>
-      <c r="D2326" s="149" t="n">
+      <c r="D2326" s="146" t="n">
         <v>0.443159722222222</v>
       </c>
     </row>
@@ -42814,7 +42779,7 @@
       <c r="C2332" s="0" t="s">
         <v>3238</v>
       </c>
-      <c r="D2332" s="149" t="n">
+      <c r="D2332" s="146" t="n">
         <v>0.600474537037037</v>
       </c>
     </row>
@@ -42833,7 +42798,7 @@
       <c r="D2334" s="0" t="s">
         <v>3241</v>
       </c>
-      <c r="E2334" s="149" t="n">
+      <c r="E2334" s="146" t="n">
         <v>0.157314814814815</v>
       </c>
     </row>
@@ -42891,7 +42856,7 @@
       <c r="E2339" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="F2339" s="149" t="n">
+      <c r="F2339" s="146" t="n">
         <v>0.596990740740741</v>
       </c>
     </row>
@@ -43363,7 +43328,7 @@
       <c r="E2380" s="0" t="n">
         <v>26</v>
       </c>
-      <c r="F2380" s="149" t="n">
+      <c r="F2380" s="146" t="n">
         <v>0.443159722222222</v>
       </c>
     </row>

</xml_diff>

<commit_message>
start Mn standards on standards spreadsheet
</commit_message>
<xml_diff>
--- a/startup/lookup_table/Modes.xlsx
+++ b/startup/lookup_table/Modes.xlsx
@@ -11767,10 +11767,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
-      <selection pane="bottomRight" activeCell="K56" activeCellId="0" sqref="K56:K58"/>
+      <selection pane="bottomRight" activeCell="D73" activeCellId="0" sqref="D73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.04"/>
@@ -15531,7 +15531,7 @@
   <dimension ref="A1:AMJ31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D28" activeCellId="1" sqref="K56:K58 D28"/>
+      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17105,10 +17105,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G11" activeCellId="1" sqref="K56:K58 G11"/>
+      <selection pane="bottomRight" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33"/>
@@ -17287,10 +17287,10 @@
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="1" sqref="K56:K58 E4"/>
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.36"/>
@@ -17861,10 +17861,10 @@
   <dimension ref="A1:CX484"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="K56:K58 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.26"/>
   </cols>
@@ -23932,10 +23932,10 @@
   <dimension ref="A1:G2383"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A44" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="1" sqref="K56:K58 B4"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="56.14"/>

</xml_diff>

<commit_message>
update lookup table + update change_edge to move m2_lateral
* update dcm_roll position for Si(111) mono
* recalibrate Si(111) mono
* update approximate_pitch
* lims function to toggle lims on and off
* determine m2_lateral position from energy to maintain fixed XAS beam position
* more work on echo_slack
* new offsets for slits i and o, new xafs_ref.outer_position
* fix post plot for find_slot()
</commit_message>
<xml_diff>
--- a/startup/lookup_table/Modes.xlsx
+++ b/startup/lookup_table/Modes.xlsx
@@ -11763,14 +11763,14 @@
   <dimension ref="A1:AMJ66"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="E32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="I30" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
-      <selection pane="bottomRight" activeCell="D73" activeCellId="0" sqref="D73"/>
+      <selection pane="topRight" activeCell="I1" activeCellId="0" sqref="I1"/>
+      <selection pane="bottomLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
+      <selection pane="bottomRight" activeCell="D45" activeCellId="0" sqref="D45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.04"/>
@@ -14738,26 +14738,26 @@
         <v>-55.188</v>
       </c>
       <c r="H54" s="59"/>
-      <c r="I54" s="57" t="n">
-        <v>-23.247</v>
+      <c r="I54" s="60" t="n">
+        <v>-23.853</v>
       </c>
       <c r="J54" s="28" t="n">
         <v>-268324</v>
       </c>
       <c r="K54" s="60" t="n">
-        <v>42.66</v>
+        <v>43.058</v>
       </c>
       <c r="L54" s="28" t="n">
         <v>387964</v>
       </c>
       <c r="M54" s="60" t="n">
-        <v>43.0474</v>
+        <v>43.058</v>
       </c>
       <c r="N54" s="28" t="n">
         <v>394647</v>
       </c>
-      <c r="O54" s="57" t="n">
-        <v>17.066</v>
+      <c r="O54" s="60" t="n">
+        <v>16.963</v>
       </c>
       <c r="P54" s="28" t="n">
         <v>141529</v>
@@ -14878,7 +14878,7 @@
         <v>189</v>
       </c>
       <c r="E56" s="61" t="n">
-        <v>113.887</v>
+        <v>116.887</v>
       </c>
       <c r="F56" s="25" t="n">
         <v>9251952</v>
@@ -14890,25 +14890,25 @@
         <v>4600216</v>
       </c>
       <c r="I56" s="61" t="n">
-        <v>54.059</v>
+        <v>56.009</v>
       </c>
       <c r="J56" s="23" t="n">
         <v>6151303</v>
       </c>
       <c r="K56" s="61" t="n">
-        <v>125.144</v>
+        <v>127.544</v>
       </c>
       <c r="L56" s="23" t="n">
         <v>9901395</v>
       </c>
       <c r="M56" s="61" t="n">
-        <v>124.985</v>
+        <v>127.735</v>
       </c>
       <c r="N56" s="23" t="n">
         <v>9901395</v>
       </c>
       <c r="O56" s="61" t="n">
-        <v>96.516</v>
+        <v>99.466</v>
       </c>
       <c r="P56" s="23" t="n">
         <v>8392750</v>
@@ -14940,7 +14940,7 @@
         <v>192</v>
       </c>
       <c r="E57" s="61" t="n">
-        <v>119.819</v>
+        <v>121.119</v>
       </c>
       <c r="F57" s="32" t="n">
         <v>6972005</v>
@@ -14952,25 +14952,25 @@
         <v>1551088</v>
       </c>
       <c r="I57" s="61" t="n">
-        <v>52.458</v>
+        <v>52.508</v>
       </c>
       <c r="J57" s="32" t="n">
         <v>3351899</v>
       </c>
       <c r="K57" s="61" t="n">
-        <v>130.739</v>
+        <v>131.814</v>
       </c>
       <c r="L57" s="32" t="n">
         <v>7552437</v>
       </c>
       <c r="M57" s="61" t="n">
-        <v>130.33</v>
+        <v>131.98</v>
       </c>
       <c r="N57" s="32" t="n">
         <v>7552437</v>
       </c>
       <c r="O57" s="61" t="n">
-        <v>98.811</v>
+        <v>100.436</v>
       </c>
       <c r="P57" s="32" t="n">
         <v>5879304</v>
@@ -14994,7 +14994,7 @@
         <v>195</v>
       </c>
       <c r="E58" s="61" t="n">
-        <v>119.819</v>
+        <v>121.119</v>
       </c>
       <c r="F58" s="28" t="n">
         <v>5572330</v>
@@ -15006,25 +15006,25 @@
         <v>354340</v>
       </c>
       <c r="I58" s="61" t="n">
-        <v>52.458</v>
+        <v>52.508</v>
       </c>
       <c r="J58" s="32" t="n">
         <v>1952224</v>
       </c>
       <c r="K58" s="61" t="n">
-        <v>130.739</v>
+        <v>131.814</v>
       </c>
       <c r="L58" s="32" t="n">
         <v>6355689</v>
       </c>
       <c r="M58" s="61" t="n">
-        <v>130.33</v>
+        <v>131.98</v>
       </c>
       <c r="N58" s="32" t="n">
         <v>6355689</v>
       </c>
       <c r="O58" s="61" t="n">
-        <v>98.811</v>
+        <v>100.436</v>
       </c>
       <c r="P58" s="66" t="n">
         <v>4479629</v>
@@ -16974,7 +16974,7 @@
       </c>
       <c r="F26" s="104" t="n">
         <f aca="false">'Modes A-F'!I54</f>
-        <v>-23.247</v>
+        <v>-23.853</v>
       </c>
       <c r="G26" s="0"/>
       <c r="H26" s="83" t="s">
@@ -16997,7 +16997,7 @@
       </c>
       <c r="F27" s="104" t="n">
         <f aca="false">'Modes A-F'!K54</f>
-        <v>42.66</v>
+        <v>43.058</v>
       </c>
       <c r="G27" s="0"/>
       <c r="H27" s="0"/>
@@ -17016,7 +17016,7 @@
       </c>
       <c r="F28" s="104" t="n">
         <f aca="false">'Modes A-F'!M54</f>
-        <v>43.0474</v>
+        <v>43.058</v>
       </c>
       <c r="G28" s="0"/>
       <c r="H28" s="0"/>
@@ -17035,7 +17035,7 @@
       </c>
       <c r="F29" s="104" t="n">
         <f aca="false">'Modes A-F'!O54</f>
-        <v>17.066</v>
+        <v>16.963</v>
       </c>
       <c r="G29" s="0"/>
       <c r="H29" s="0"/>
@@ -17108,7 +17108,7 @@
       <selection pane="bottomRight" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33"/>
@@ -17290,7 +17290,7 @@
       <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.36"/>
@@ -17349,11 +17349,11 @@
       </c>
       <c r="G3" s="122" t="n">
         <f aca="false">'Modes A-F'!O54</f>
-        <v>17.066</v>
+        <v>16.963</v>
       </c>
       <c r="H3" s="123" t="n">
         <f aca="false">G3-F3</f>
-        <v>-2.0371189817083</v>
+        <v>-2.1401189817083</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17369,19 +17369,19 @@
       </c>
       <c r="E4" s="104" t="n">
         <f aca="false">'Modes A-F'!K56</f>
-        <v>125.144</v>
+        <v>127.544</v>
       </c>
       <c r="F4" s="104" t="n">
         <f aca="false">E4-B4*TAN(2*(F2-E2)/1000)</f>
-        <v>96.2329132666878</v>
+        <v>98.6329132666878</v>
       </c>
       <c r="G4" s="122" t="n">
         <f aca="false">'Modes A-F'!O56</f>
-        <v>96.516</v>
+        <v>99.466</v>
       </c>
       <c r="H4" s="123" t="n">
         <f aca="false">G4-F4</f>
-        <v>0.283086733312246</v>
+        <v>0.833086733312243</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17398,25 +17398,25 @@
       </c>
       <c r="E5" s="127" t="n">
         <f aca="false">'Modes A-F'!K57</f>
-        <v>130.739</v>
+        <v>131.814</v>
       </c>
       <c r="F5" s="127" t="n">
         <f aca="false">E5-B5*TAN(2*(F2-E2)/1000)</f>
-        <v>98.3629028716503</v>
+        <v>99.4379028716503</v>
       </c>
       <c r="G5" s="128" t="n">
         <f aca="false">'Modes A-F'!O57</f>
-        <v>98.811</v>
+        <v>100.436</v>
       </c>
       <c r="H5" s="123" t="n">
         <f aca="false">G5-F5</f>
-        <v>0.448097128349673</v>
+        <v>0.998097128349684</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H6" s="123" t="n">
         <f aca="false">AVERAGE(H3,H4,H5)</f>
-        <v>-0.435311706682127</v>
+        <v>-0.10297837334879</v>
       </c>
       <c r="I6" s="0" t="s">
         <v>274</v>
@@ -17483,12 +17483,12 @@
       </c>
       <c r="E11" s="123" t="n">
         <f aca="false">'Modes A-F'!E57</f>
-        <v>119.819</v>
+        <v>121.119</v>
       </c>
       <c r="F11" s="123"/>
       <c r="G11" s="132" t="n">
         <f aca="false">E11-B11*TAN(2*(G9-E9)/1000)</f>
-        <v>122.127400030779</v>
+        <v>123.427400030779</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17505,12 +17505,12 @@
       </c>
       <c r="E12" s="133" t="n">
         <f aca="false">'Modes A-F'!E58</f>
-        <v>119.819</v>
+        <v>121.119</v>
       </c>
       <c r="F12" s="133"/>
       <c r="G12" s="134" t="n">
         <f aca="false">E12-B12*TAN(2*(G9-E9)/1000)</f>
-        <v>122.358400033859</v>
+        <v>123.658400033859</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17615,7 +17615,7 @@
       </c>
       <c r="F22" s="138" t="n">
         <f aca="false">'Modes A-F'!I54</f>
-        <v>-23.247</v>
+        <v>-23.853</v>
       </c>
       <c r="G22" s="123" t="n">
         <f aca="false">E10-B22*TAN(2*(G19)/1000)+I17</f>
@@ -17636,15 +17636,15 @@
       </c>
       <c r="E23" s="123" t="n">
         <f aca="false">E11-B23*TAN(2*(E19)/1000)+I17</f>
-        <v>47.0582674801944</v>
+        <v>48.3582674801944</v>
       </c>
       <c r="F23" s="138" t="n">
         <f aca="false">'Modes A-F'!I56</f>
-        <v>54.059</v>
+        <v>56.009</v>
       </c>
       <c r="G23" s="123" t="n">
         <f aca="false">E11-B23*TAN(2*(G19)/1000)+I17</f>
-        <v>52.3588981480704</v>
+        <v>53.6588981480704</v>
       </c>
       <c r="I23" s="119"/>
     </row>
@@ -17662,15 +17662,15 @@
       </c>
       <c r="E24" s="133" t="n">
         <f aca="false">E12-B24*TAN(2*(E19)/1000)+I17</f>
-        <v>38.3378517843995</v>
+        <v>39.6378517843995</v>
       </c>
       <c r="F24" s="139" t="n">
         <f aca="false">'Modes A-F'!I57</f>
-        <v>52.458</v>
+        <v>52.508</v>
       </c>
       <c r="G24" s="140" t="n">
         <f aca="false">E12-B24*TAN(2*(G19)/1000)+I17</f>
-        <v>44.273766090482</v>
+        <v>45.573766090482</v>
       </c>
       <c r="H24" s="125"/>
       <c r="I24" s="141"/>
@@ -17798,7 +17798,7 @@
       </c>
       <c r="E35" s="123" t="n">
         <f aca="false">E11-B35*TAN(2*(E31)/1000)</f>
-        <v>18.1448777773465</v>
+        <v>19.4448777773465</v>
       </c>
       <c r="F35" s="138" t="n">
         <f aca="false">'Modes A-F'!G56</f>
@@ -17806,7 +17806,7 @@
       </c>
       <c r="G35" s="123" t="n">
         <f aca="false">E11-B35*TAN(2*(G31)/1000)+I29</f>
-        <v>23.4457875381681</v>
+        <v>24.7457875381681</v>
       </c>
       <c r="I35" s="119"/>
     </row>
@@ -17824,7 +17824,7 @@
       </c>
       <c r="E36" s="133" t="n">
         <f aca="false">E12-B36*TAN(2*(E31)/1000)</f>
-        <v>5.95917567428903</v>
+        <v>7.25917567428903</v>
       </c>
       <c r="F36" s="139" t="n">
         <f aca="false">'Modes A-F'!G57</f>
@@ -17832,7 +17832,7 @@
       </c>
       <c r="G36" s="133" t="n">
         <f aca="false">E12-B36*TAN(2*(G31)/1000)+I29</f>
-        <v>11.8954025227675</v>
+        <v>13.1954025227675</v>
       </c>
       <c r="H36" s="125"/>
       <c r="I36" s="141"/>
@@ -17864,7 +17864,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.26"/>
   </cols>
@@ -23935,7 +23935,7 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="56.14"/>

</xml_diff>

<commit_message>
lots of beginning of cycle fixes
* new DCM parameters for both monos
* new parameters for approximate_pitch
* use echo_slack in new BMM_common folder
* some qs bug fixes
* fix plotting bug in wafer edge scan
* small improvment to new xanes() plan
* some kafka consumer clean ups
* add primary user for qs
</commit_message>
<xml_diff>
--- a/startup/lookup_table/Modes.xlsx
+++ b/startup/lookup_table/Modes.xlsx
@@ -10818,7 +10818,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="35">
+  <borders count="34">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -10936,15 +10936,6 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="thin">
-        <color rgb="FFCCCCCC"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -11094,7 +11085,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="147">
+  <cellXfs count="146">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -11323,11 +11314,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11336,10 +11327,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11387,15 +11374,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11403,27 +11394,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11435,7 +11422,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="8" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="8" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11443,7 +11430,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11451,12 +11438,16 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -11471,10 +11462,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -11483,11 +11470,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="8" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="8" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11499,15 +11486,15 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11543,7 +11530,79 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="31" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="32" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="32" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11551,87 +11610,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="33" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="31" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="32" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="31" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11651,19 +11638,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="31" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="32" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11763,14 +11750,14 @@
   <dimension ref="A1:AMJ66"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="I30" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="E30" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="I1" activeCellId="0" sqref="I1"/>
+      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
-      <selection pane="bottomRight" activeCell="D45" activeCellId="0" sqref="D45"/>
+      <selection pane="bottomRight" activeCell="E54" activeCellId="0" sqref="E54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.04"/>
@@ -14729,7 +14716,7 @@
         <v>182</v>
       </c>
       <c r="E54" s="57" t="n">
-        <v>31.259</v>
+        <v>32.071</v>
       </c>
       <c r="F54" s="26" t="n">
         <v>276763</v>
@@ -14877,37 +14864,37 @@
       <c r="D56" s="20" t="s">
         <v>189</v>
       </c>
-      <c r="E56" s="61" t="n">
+      <c r="E56" s="57" t="n">
         <v>116.887</v>
       </c>
       <c r="F56" s="25" t="n">
         <v>9251952</v>
       </c>
-      <c r="G56" s="62" t="n">
+      <c r="G56" s="61" t="n">
         <v>24.4104</v>
       </c>
-      <c r="H56" s="63" t="n">
+      <c r="H56" s="62" t="n">
         <v>4600216</v>
       </c>
-      <c r="I56" s="61" t="n">
+      <c r="I56" s="57" t="n">
         <v>56.009</v>
       </c>
       <c r="J56" s="23" t="n">
         <v>6151303</v>
       </c>
-      <c r="K56" s="61" t="n">
+      <c r="K56" s="57" t="n">
         <v>127.544</v>
       </c>
       <c r="L56" s="23" t="n">
         <v>9901395</v>
       </c>
-      <c r="M56" s="61" t="n">
+      <c r="M56" s="57" t="n">
         <v>127.735</v>
       </c>
       <c r="N56" s="23" t="n">
         <v>9901395</v>
       </c>
-      <c r="O56" s="61" t="n">
+      <c r="O56" s="57" t="n">
         <v>99.466</v>
       </c>
       <c r="P56" s="23" t="n">
@@ -14939,37 +14926,37 @@
       <c r="D57" s="0" t="s">
         <v>192</v>
       </c>
-      <c r="E57" s="61" t="n">
+      <c r="E57" s="57" t="n">
         <v>121.119</v>
       </c>
       <c r="F57" s="32" t="n">
         <v>6972005</v>
       </c>
-      <c r="G57" s="64" t="n">
+      <c r="G57" s="63" t="n">
         <v>12.81</v>
       </c>
-      <c r="H57" s="65" t="n">
+      <c r="H57" s="64" t="n">
         <v>1551088</v>
       </c>
-      <c r="I57" s="61" t="n">
+      <c r="I57" s="57" t="n">
         <v>52.508</v>
       </c>
       <c r="J57" s="32" t="n">
         <v>3351899</v>
       </c>
-      <c r="K57" s="61" t="n">
+      <c r="K57" s="57" t="n">
         <v>131.814</v>
       </c>
       <c r="L57" s="32" t="n">
         <v>7552437</v>
       </c>
-      <c r="M57" s="61" t="n">
+      <c r="M57" s="57" t="n">
         <v>131.98</v>
       </c>
       <c r="N57" s="32" t="n">
         <v>7552437</v>
       </c>
-      <c r="O57" s="61" t="n">
+      <c r="O57" s="57" t="n">
         <v>100.436</v>
       </c>
       <c r="P57" s="32" t="n">
@@ -14993,40 +14980,40 @@
       <c r="D58" s="26" t="s">
         <v>195</v>
       </c>
-      <c r="E58" s="61" t="n">
+      <c r="E58" s="57" t="n">
         <v>121.119</v>
       </c>
       <c r="F58" s="28" t="n">
         <v>5572330</v>
       </c>
-      <c r="G58" s="64" t="n">
+      <c r="G58" s="63" t="n">
         <v>12.81</v>
       </c>
-      <c r="H58" s="65" t="n">
+      <c r="H58" s="64" t="n">
         <v>354340</v>
       </c>
-      <c r="I58" s="61" t="n">
+      <c r="I58" s="57" t="n">
         <v>52.508</v>
       </c>
       <c r="J58" s="32" t="n">
         <v>1952224</v>
       </c>
-      <c r="K58" s="61" t="n">
+      <c r="K58" s="57" t="n">
         <v>131.814</v>
       </c>
       <c r="L58" s="32" t="n">
         <v>6355689</v>
       </c>
-      <c r="M58" s="61" t="n">
+      <c r="M58" s="57" t="n">
         <v>131.98</v>
       </c>
       <c r="N58" s="32" t="n">
         <v>6355689</v>
       </c>
-      <c r="O58" s="61" t="n">
+      <c r="O58" s="57" t="n">
         <v>100.436</v>
       </c>
-      <c r="P58" s="66" t="n">
+      <c r="P58" s="65" t="n">
         <v>4479629</v>
       </c>
       <c r="T58" s="27" t="n">
@@ -15052,43 +15039,43 @@
       <c r="D59" s="26" t="s">
         <v>198</v>
       </c>
-      <c r="E59" s="67" t="n">
+      <c r="E59" s="66" t="n">
         <v>-9.0621</v>
       </c>
       <c r="F59" s="28" t="n">
         <v>-242758</v>
       </c>
-      <c r="G59" s="64" t="n">
+      <c r="G59" s="63" t="n">
         <v>-9.0621</v>
       </c>
-      <c r="H59" s="68" t="n">
+      <c r="H59" s="67" t="n">
         <v>-242758</v>
       </c>
-      <c r="I59" s="67" t="n">
+      <c r="I59" s="66" t="n">
         <v>-9.0621</v>
       </c>
       <c r="J59" s="28" t="n">
         <v>-242758</v>
       </c>
-      <c r="K59" s="67" t="n">
+      <c r="K59" s="66" t="n">
         <v>-9.0621</v>
       </c>
       <c r="L59" s="28" t="n">
         <v>-242758</v>
       </c>
-      <c r="M59" s="67" t="n">
+      <c r="M59" s="66" t="n">
         <v>-9.0621</v>
       </c>
       <c r="N59" s="28" t="n">
         <v>-242758</v>
       </c>
-      <c r="O59" s="67" t="n">
+      <c r="O59" s="66" t="n">
         <v>-9.0621</v>
       </c>
       <c r="P59" s="28" t="n">
         <v>-242758</v>
       </c>
-      <c r="T59" s="67" t="n">
+      <c r="T59" s="66" t="n">
         <v>-0.6</v>
       </c>
       <c r="U59" s="28" t="n">
@@ -15106,46 +15093,46 @@
       <c r="D60" s="35" t="s">
         <v>201</v>
       </c>
-      <c r="E60" s="69" t="n">
+      <c r="E60" s="68" t="n">
         <v>15.3898</v>
       </c>
       <c r="F60" s="47" t="n">
         <v>160203</v>
       </c>
-      <c r="G60" s="70" t="n">
+      <c r="G60" s="69" t="n">
         <v>15.3898</v>
       </c>
-      <c r="H60" s="71" t="n">
+      <c r="H60" s="70" t="n">
         <v>160203</v>
       </c>
-      <c r="I60" s="69" t="n">
+      <c r="I60" s="68" t="n">
         <v>15.3898</v>
       </c>
       <c r="J60" s="47" t="n">
         <v>160203</v>
       </c>
-      <c r="K60" s="69" t="n">
+      <c r="K60" s="68" t="n">
         <v>15.3898</v>
       </c>
       <c r="L60" s="47" t="n">
         <v>160203</v>
       </c>
-      <c r="M60" s="69" t="n">
+      <c r="M60" s="68" t="n">
         <v>15.3898</v>
       </c>
       <c r="N60" s="47" t="n">
         <v>160203</v>
       </c>
-      <c r="O60" s="69" t="n">
+      <c r="O60" s="68" t="n">
         <v>15.3898</v>
       </c>
       <c r="P60" s="47" t="n">
         <v>160203</v>
       </c>
-      <c r="Q60" s="72"/>
-      <c r="R60" s="72"/>
-      <c r="S60" s="72"/>
-      <c r="T60" s="69" t="n">
+      <c r="Q60" s="71"/>
+      <c r="R60" s="71"/>
+      <c r="S60" s="71"/>
+      <c r="T60" s="68" t="n">
         <v>33.3721</v>
       </c>
       <c r="U60" s="47" t="n">
@@ -15158,52 +15145,52 @@
       <c r="Z60" s="0"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="73" t="s">
+      <c r="A61" s="72" t="s">
         <v>202</v>
       </c>
-      <c r="B61" s="74" t="s">
+      <c r="B61" s="73" t="s">
         <v>203</v>
       </c>
-      <c r="C61" s="75" t="s">
+      <c r="C61" s="74" t="s">
         <v>204</v>
       </c>
-      <c r="D61" s="75" t="s">
+      <c r="D61" s="74" t="s">
         <v>205</v>
       </c>
-      <c r="E61" s="76" t="n">
-        <v>0</v>
-      </c>
-      <c r="F61" s="77" t="n">
-        <v>0</v>
-      </c>
-      <c r="G61" s="76" t="n">
-        <v>0</v>
-      </c>
-      <c r="H61" s="77" t="n">
-        <v>0</v>
-      </c>
-      <c r="I61" s="76" t="n">
-        <v>0</v>
-      </c>
-      <c r="J61" s="77" t="n">
-        <v>0</v>
-      </c>
-      <c r="K61" s="76" t="n">
-        <v>0</v>
-      </c>
-      <c r="L61" s="77" t="n">
-        <v>0</v>
-      </c>
-      <c r="M61" s="76" t="n">
-        <v>0</v>
-      </c>
-      <c r="N61" s="77" t="n">
-        <v>0</v>
-      </c>
-      <c r="O61" s="76" t="n">
-        <v>0</v>
-      </c>
-      <c r="P61" s="77" t="n">
+      <c r="E61" s="75" t="n">
+        <v>0</v>
+      </c>
+      <c r="F61" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="G61" s="75" t="n">
+        <v>0</v>
+      </c>
+      <c r="H61" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="I61" s="75" t="n">
+        <v>0</v>
+      </c>
+      <c r="J61" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="K61" s="75" t="n">
+        <v>0</v>
+      </c>
+      <c r="L61" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="M61" s="75" t="n">
+        <v>0</v>
+      </c>
+      <c r="N61" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="O61" s="75" t="n">
+        <v>0</v>
+      </c>
+      <c r="P61" s="76" t="n">
         <v>0</v>
       </c>
       <c r="T61" s="30" t="n">
@@ -15214,8 +15201,8 @@
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="73"/>
-      <c r="B62" s="78" t="s">
+      <c r="A62" s="72"/>
+      <c r="B62" s="77" t="s">
         <v>206</v>
       </c>
       <c r="C62" s="0" t="s">
@@ -15268,8 +15255,8 @@
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="73"/>
-      <c r="B63" s="78" t="s">
+      <c r="A63" s="72"/>
+      <c r="B63" s="77" t="s">
         <v>209</v>
       </c>
       <c r="C63" s="0" t="s">
@@ -15322,8 +15309,8 @@
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="73"/>
-      <c r="B64" s="78" t="s">
+      <c r="A64" s="72"/>
+      <c r="B64" s="77" t="s">
         <v>212</v>
       </c>
       <c r="C64" s="0" t="s">
@@ -15376,8 +15363,8 @@
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="73"/>
-      <c r="B65" s="78" t="s">
+      <c r="A65" s="72"/>
+      <c r="B65" s="77" t="s">
         <v>215</v>
       </c>
       <c r="C65" s="0" t="s">
@@ -15430,53 +15417,53 @@
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="73"/>
-      <c r="B66" s="79" t="s">
+      <c r="A66" s="72"/>
+      <c r="B66" s="78" t="s">
         <v>218</v>
       </c>
-      <c r="C66" s="80" t="s">
+      <c r="C66" s="79" t="s">
         <v>219</v>
       </c>
-      <c r="D66" s="80" t="s">
+      <c r="D66" s="79" t="s">
         <v>220</v>
       </c>
-      <c r="E66" s="81" t="n">
-        <v>0</v>
-      </c>
-      <c r="F66" s="82" t="n">
-        <v>0</v>
-      </c>
-      <c r="G66" s="81" t="n">
-        <v>0</v>
-      </c>
-      <c r="H66" s="82" t="n">
-        <v>0</v>
-      </c>
-      <c r="I66" s="81" t="n">
-        <v>0</v>
-      </c>
-      <c r="J66" s="82" t="n">
-        <v>0</v>
-      </c>
-      <c r="K66" s="81" t="n">
-        <v>0</v>
-      </c>
-      <c r="L66" s="82" t="n">
-        <v>0</v>
-      </c>
-      <c r="M66" s="81" t="n">
-        <v>0</v>
-      </c>
-      <c r="N66" s="82" t="n">
-        <v>0</v>
-      </c>
-      <c r="O66" s="81" t="n">
-        <v>0</v>
-      </c>
-      <c r="P66" s="82" t="n">
-        <v>0</v>
-      </c>
-      <c r="T66" s="69" t="n">
+      <c r="E66" s="80" t="n">
+        <v>0</v>
+      </c>
+      <c r="F66" s="81" t="n">
+        <v>0</v>
+      </c>
+      <c r="G66" s="80" t="n">
+        <v>0</v>
+      </c>
+      <c r="H66" s="81" t="n">
+        <v>0</v>
+      </c>
+      <c r="I66" s="80" t="n">
+        <v>0</v>
+      </c>
+      <c r="J66" s="81" t="n">
+        <v>0</v>
+      </c>
+      <c r="K66" s="80" t="n">
+        <v>0</v>
+      </c>
+      <c r="L66" s="81" t="n">
+        <v>0</v>
+      </c>
+      <c r="M66" s="80" t="n">
+        <v>0</v>
+      </c>
+      <c r="N66" s="81" t="n">
+        <v>0</v>
+      </c>
+      <c r="O66" s="80" t="n">
+        <v>0</v>
+      </c>
+      <c r="P66" s="81" t="n">
+        <v>0</v>
+      </c>
+      <c r="T66" s="68" t="n">
         <v>0</v>
       </c>
       <c r="U66" s="47" t="n">
@@ -15536,34 +15523,34 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="83" width="3.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="2" style="83" width="13.26"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="10" style="83" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="82" width="3.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="2" style="82" width="13.26"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="10" style="82" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" s="84" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="83"/>
+    <row r="1" s="83" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="82"/>
       <c r="B1" s="0"/>
       <c r="C1" s="0"/>
       <c r="D1" s="0"/>
       <c r="E1" s="0"/>
-      <c r="F1" s="83"/>
-      <c r="G1" s="83"/>
-      <c r="H1" s="83"/>
-      <c r="I1" s="83"/>
-      <c r="J1" s="83"/>
-      <c r="K1" s="83"/>
-      <c r="L1" s="83"/>
-      <c r="AMJ1" s="83"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
+      <c r="I1" s="82"/>
+      <c r="J1" s="82"/>
+      <c r="K1" s="82"/>
+      <c r="L1" s="82"/>
+      <c r="AMJ1" s="82"/>
     </row>
     <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0"/>
-      <c r="B2" s="85" t="s">
+      <c r="B2" s="84" t="s">
         <v>221</v>
       </c>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
       <c r="F2" s="0"/>
       <c r="G2" s="0"/>
       <c r="H2" s="0"/>
@@ -16584,168 +16571,168 @@
       <c r="AMI2" s="0"/>
       <c r="AMJ2" s="0"/>
     </row>
-    <row r="3" s="90" customFormat="true" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="86"/>
-      <c r="B3" s="87"/>
-      <c r="C3" s="88" t="s">
+    <row r="3" s="89" customFormat="true" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="85"/>
+      <c r="B3" s="86"/>
+      <c r="C3" s="87" t="s">
         <v>222</v>
       </c>
-      <c r="D3" s="88" t="s">
+      <c r="D3" s="87" t="s">
         <v>223</v>
       </c>
-      <c r="E3" s="89" t="s">
+      <c r="E3" s="88" t="s">
         <v>224</v>
       </c>
-      <c r="F3" s="86"/>
-      <c r="G3" s="86"/>
-      <c r="H3" s="86"/>
-      <c r="I3" s="86"/>
-      <c r="J3" s="86"/>
-      <c r="K3" s="86"/>
-      <c r="L3" s="86"/>
-      <c r="AMJ3" s="86"/>
-    </row>
-    <row r="4" s="84" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="83"/>
-      <c r="B4" s="87" t="s">
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="85"/>
+      <c r="AMJ3" s="85"/>
+    </row>
+    <row r="4" s="83" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="82"/>
+      <c r="B4" s="86" t="s">
         <v>225</v>
       </c>
-      <c r="C4" s="83"/>
-      <c r="D4" s="83" t="n">
+      <c r="C4" s="82"/>
+      <c r="D4" s="82" t="n">
         <v>55</v>
       </c>
-      <c r="E4" s="91" t="n">
+      <c r="E4" s="90" t="n">
         <v>55</v>
       </c>
-      <c r="F4" s="83"/>
-      <c r="G4" s="83"/>
-      <c r="H4" s="83"/>
-      <c r="I4" s="83"/>
-      <c r="J4" s="83"/>
-      <c r="K4" s="83"/>
-      <c r="L4" s="83"/>
-      <c r="AMJ4" s="83"/>
-    </row>
-    <row r="5" s="84" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="83"/>
-      <c r="B5" s="87" t="s">
+      <c r="F4" s="82"/>
+      <c r="G4" s="82"/>
+      <c r="H4" s="82"/>
+      <c r="I4" s="82"/>
+      <c r="J4" s="82"/>
+      <c r="K4" s="82"/>
+      <c r="L4" s="82"/>
+      <c r="AMJ4" s="82"/>
+    </row>
+    <row r="5" s="83" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="82"/>
+      <c r="B5" s="86" t="s">
         <v>226</v>
       </c>
-      <c r="C5" s="83" t="s">
+      <c r="C5" s="82" t="s">
         <v>227</v>
       </c>
-      <c r="D5" s="83" t="n">
+      <c r="D5" s="82" t="n">
         <v>-46.5</v>
       </c>
-      <c r="E5" s="91"/>
-      <c r="F5" s="83"/>
-      <c r="G5" s="83"/>
-      <c r="H5" s="83"/>
-      <c r="I5" s="83"/>
-      <c r="J5" s="83"/>
-      <c r="K5" s="83"/>
-      <c r="L5" s="83"/>
-      <c r="AMJ5" s="83"/>
-    </row>
-    <row r="6" s="84" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="83"/>
-      <c r="B6" s="87" t="s">
+      <c r="E5" s="90"/>
+      <c r="F5" s="82"/>
+      <c r="G5" s="82"/>
+      <c r="H5" s="82"/>
+      <c r="I5" s="82"/>
+      <c r="J5" s="82"/>
+      <c r="K5" s="82"/>
+      <c r="L5" s="82"/>
+      <c r="AMJ5" s="82"/>
+    </row>
+    <row r="6" s="83" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="82"/>
+      <c r="B6" s="86" t="s">
         <v>228</v>
       </c>
-      <c r="C6" s="83" t="s">
+      <c r="C6" s="82" t="s">
         <v>229</v>
       </c>
-      <c r="D6" s="83" t="n">
+      <c r="D6" s="82" t="n">
         <v>-20.5</v>
       </c>
-      <c r="E6" s="91"/>
-      <c r="F6" s="83"/>
-      <c r="G6" s="83"/>
-      <c r="H6" s="83"/>
-      <c r="I6" s="83"/>
-      <c r="J6" s="83"/>
-      <c r="K6" s="83"/>
-      <c r="L6" s="83"/>
-      <c r="AMJ6" s="83"/>
-    </row>
-    <row r="7" s="84" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="83"/>
-      <c r="B7" s="87" t="s">
+      <c r="E6" s="90"/>
+      <c r="F6" s="82"/>
+      <c r="G6" s="82"/>
+      <c r="H6" s="82"/>
+      <c r="I6" s="82"/>
+      <c r="J6" s="82"/>
+      <c r="K6" s="82"/>
+      <c r="L6" s="82"/>
+      <c r="AMJ6" s="82"/>
+    </row>
+    <row r="7" s="83" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="82"/>
+      <c r="B7" s="86" t="s">
         <v>230</v>
       </c>
-      <c r="C7" s="83" t="s">
+      <c r="C7" s="82" t="s">
         <v>231</v>
       </c>
-      <c r="D7" s="83" t="n">
+      <c r="D7" s="82" t="n">
         <v>5.5</v>
       </c>
-      <c r="E7" s="91"/>
-      <c r="F7" s="83"/>
-      <c r="G7" s="83"/>
-      <c r="H7" s="83"/>
-      <c r="I7" s="83"/>
-      <c r="J7" s="83"/>
-      <c r="K7" s="83"/>
-      <c r="L7" s="83"/>
-      <c r="AMJ7" s="83"/>
-    </row>
-    <row r="8" s="84" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="83"/>
-      <c r="B8" s="87" t="s">
+      <c r="E7" s="90"/>
+      <c r="F7" s="82"/>
+      <c r="G7" s="82"/>
+      <c r="H7" s="82"/>
+      <c r="I7" s="82"/>
+      <c r="J7" s="82"/>
+      <c r="K7" s="82"/>
+      <c r="L7" s="82"/>
+      <c r="AMJ7" s="82"/>
+    </row>
+    <row r="8" s="83" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="82"/>
+      <c r="B8" s="86" t="s">
         <v>232</v>
       </c>
-      <c r="C8" s="83" t="s">
+      <c r="C8" s="82" t="s">
         <v>233</v>
       </c>
-      <c r="D8" s="83" t="n">
+      <c r="D8" s="82" t="n">
         <v>31</v>
       </c>
-      <c r="E8" s="91"/>
-      <c r="F8" s="83"/>
-      <c r="G8" s="83"/>
-      <c r="H8" s="83"/>
-      <c r="I8" s="83"/>
-      <c r="J8" s="83"/>
-      <c r="K8" s="83"/>
-      <c r="L8" s="83"/>
-      <c r="AMJ8" s="83"/>
-    </row>
-    <row r="9" s="84" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="83"/>
-      <c r="B9" s="87" t="s">
+      <c r="E8" s="90"/>
+      <c r="F8" s="82"/>
+      <c r="G8" s="82"/>
+      <c r="H8" s="82"/>
+      <c r="I8" s="82"/>
+      <c r="J8" s="82"/>
+      <c r="K8" s="82"/>
+      <c r="L8" s="82"/>
+      <c r="AMJ8" s="82"/>
+    </row>
+    <row r="9" s="83" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="82"/>
+      <c r="B9" s="86" t="s">
         <v>234</v>
       </c>
-      <c r="C9" s="83"/>
-      <c r="D9" s="83" t="n">
+      <c r="C9" s="82"/>
+      <c r="D9" s="82" t="n">
         <v>-52.6</v>
       </c>
-      <c r="E9" s="91"/>
-      <c r="F9" s="83"/>
-      <c r="G9" s="83"/>
-      <c r="H9" s="83"/>
-      <c r="I9" s="83"/>
-      <c r="J9" s="83"/>
-      <c r="K9" s="83"/>
-      <c r="L9" s="83"/>
-      <c r="AMJ9" s="83"/>
+      <c r="E9" s="90"/>
+      <c r="F9" s="82"/>
+      <c r="G9" s="82"/>
+      <c r="H9" s="82"/>
+      <c r="I9" s="82"/>
+      <c r="J9" s="82"/>
+      <c r="K9" s="82"/>
+      <c r="L9" s="82"/>
+      <c r="AMJ9" s="82"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="92" t="s">
+      <c r="B10" s="91" t="s">
         <v>235</v>
       </c>
-      <c r="C10" s="93"/>
-      <c r="D10" s="93" t="n">
+      <c r="C10" s="92"/>
+      <c r="D10" s="92" t="n">
         <v>-52</v>
       </c>
-      <c r="E10" s="94"/>
+      <c r="E10" s="93"/>
       <c r="F10" s="0"/>
       <c r="G10" s="0"/>
       <c r="H10" s="0"/>
       <c r="I10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="95"/>
-      <c r="C11" s="96"/>
+      <c r="B11" s="94"/>
+      <c r="C11" s="95"/>
       <c r="D11" s="0"/>
       <c r="E11" s="0"/>
       <c r="F11" s="0"/>
@@ -16754,8 +16741,8 @@
       <c r="I11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="95"/>
-      <c r="C12" s="96"/>
+      <c r="B12" s="94"/>
+      <c r="C12" s="95"/>
       <c r="D12" s="0"/>
       <c r="E12" s="0"/>
       <c r="F12" s="0"/>
@@ -16764,82 +16751,82 @@
       <c r="I12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="97" t="s">
+      <c r="B13" s="96" t="s">
         <v>236</v>
       </c>
-      <c r="C13" s="97"/>
-      <c r="D13" s="97"/>
-      <c r="E13" s="97"/>
+      <c r="C13" s="96"/>
+      <c r="D13" s="96"/>
+      <c r="E13" s="96"/>
       <c r="F13" s="0"/>
       <c r="G13" s="0"/>
       <c r="H13" s="0"/>
       <c r="I13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="98" t="s">
+      <c r="B14" s="97" t="s">
         <v>237</v>
       </c>
-      <c r="C14" s="99" t="s">
+      <c r="C14" s="98" t="s">
         <v>238</v>
       </c>
       <c r="D14" s="0"/>
-      <c r="E14" s="91"/>
+      <c r="E14" s="90"/>
       <c r="F14" s="0"/>
       <c r="G14" s="0"/>
       <c r="H14" s="0"/>
       <c r="I14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="87" t="s">
+      <c r="B15" s="86" t="s">
         <v>225</v>
       </c>
-      <c r="C15" s="83" t="n">
+      <c r="C15" s="82" t="n">
         <v>67</v>
       </c>
       <c r="D15" s="0"/>
-      <c r="E15" s="91"/>
+      <c r="E15" s="90"/>
       <c r="F15" s="0"/>
       <c r="G15" s="0"/>
       <c r="H15" s="0"/>
       <c r="I15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="87" t="s">
+      <c r="B16" s="86" t="s">
         <v>239</v>
       </c>
-      <c r="C16" s="100" t="n">
+      <c r="C16" s="99" t="n">
         <v>-1.5</v>
       </c>
       <c r="D16" s="0"/>
-      <c r="E16" s="91"/>
+      <c r="E16" s="90"/>
       <c r="F16" s="0"/>
       <c r="G16" s="0"/>
       <c r="H16" s="0"/>
       <c r="I16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="87" t="s">
+      <c r="B17" s="86" t="s">
         <v>240</v>
       </c>
-      <c r="C17" s="83" t="n">
+      <c r="C17" s="82" t="n">
         <v>33</v>
       </c>
       <c r="D17" s="0"/>
-      <c r="E17" s="91"/>
+      <c r="E17" s="90"/>
       <c r="F17" s="0"/>
       <c r="G17" s="0"/>
       <c r="H17" s="0"/>
       <c r="I17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="92" t="s">
+      <c r="B18" s="91" t="s">
         <v>241</v>
       </c>
-      <c r="C18" s="93" t="n">
+      <c r="C18" s="92" t="n">
         <v>53</v>
       </c>
-      <c r="D18" s="93"/>
-      <c r="E18" s="94"/>
+      <c r="D18" s="92"/>
+      <c r="E18" s="93"/>
       <c r="F18" s="0"/>
       <c r="G18" s="0"/>
       <c r="H18" s="0"/>
@@ -16866,213 +16853,213 @@
       <c r="I20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="97" t="s">
+      <c r="B21" s="96" t="s">
         <v>176</v>
       </c>
-      <c r="C21" s="97"/>
-      <c r="D21" s="97"/>
-      <c r="E21" s="97"/>
-      <c r="F21" s="97"/>
-      <c r="G21" s="97"/>
-      <c r="H21" s="97"/>
-      <c r="I21" s="97"/>
+      <c r="C21" s="96"/>
+      <c r="D21" s="96"/>
+      <c r="E21" s="96"/>
+      <c r="F21" s="96"/>
+      <c r="G21" s="96"/>
+      <c r="H21" s="96"/>
+      <c r="I21" s="96"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="101" t="s">
+      <c r="B22" s="100" t="s">
         <v>242</v>
       </c>
-      <c r="C22" s="101"/>
-      <c r="D22" s="84"/>
-      <c r="E22" s="95" t="s">
+      <c r="C22" s="100"/>
+      <c r="D22" s="83"/>
+      <c r="E22" s="94" t="s">
         <v>243</v>
       </c>
-      <c r="F22" s="95"/>
-      <c r="G22" s="84"/>
-      <c r="H22" s="102" t="s">
+      <c r="F22" s="94"/>
+      <c r="G22" s="83"/>
+      <c r="H22" s="101" t="s">
         <v>244</v>
       </c>
-      <c r="I22" s="102"/>
+      <c r="I22" s="101"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="98" t="s">
+      <c r="B23" s="97" t="s">
         <v>245</v>
       </c>
-      <c r="C23" s="99" t="s">
+      <c r="C23" s="98" t="s">
         <v>238</v>
       </c>
       <c r="D23" s="0"/>
-      <c r="E23" s="84" t="s">
+      <c r="E23" s="83" t="s">
         <v>245</v>
       </c>
-      <c r="F23" s="99" t="s">
+      <c r="F23" s="98" t="s">
         <v>238</v>
       </c>
       <c r="G23" s="0"/>
-      <c r="H23" s="84" t="s">
+      <c r="H23" s="83" t="s">
         <v>246</v>
       </c>
-      <c r="I23" s="103" t="s">
+      <c r="I23" s="102" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="87" t="s">
+      <c r="B24" s="86" t="s">
         <v>247</v>
       </c>
       <c r="C24" s="0" t="n">
         <v>33</v>
       </c>
       <c r="D24" s="0"/>
-      <c r="E24" s="83" t="s">
+      <c r="E24" s="82" t="s">
         <v>247</v>
       </c>
-      <c r="F24" s="104" t="n">
+      <c r="F24" s="103" t="n">
         <f aca="false">'Modes A-F'!E54</f>
-        <v>31.259</v>
+        <v>32.071</v>
       </c>
       <c r="G24" s="0"/>
-      <c r="H24" s="83" t="s">
+      <c r="H24" s="82" t="s">
         <v>248</v>
       </c>
-      <c r="I24" s="91" t="n">
+      <c r="I24" s="90" t="n">
         <v>40</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="87" t="s">
+      <c r="B25" s="86" t="s">
         <v>249</v>
       </c>
       <c r="C25" s="0" t="n">
         <v>-66.743</v>
       </c>
       <c r="D25" s="0"/>
-      <c r="E25" s="83" t="s">
+      <c r="E25" s="82" t="s">
         <v>249</v>
       </c>
-      <c r="F25" s="104" t="n">
+      <c r="F25" s="103" t="n">
         <f aca="false">'Modes A-F'!G54</f>
         <v>-55.188</v>
       </c>
       <c r="G25" s="0"/>
-      <c r="H25" s="83" t="s">
+      <c r="H25" s="82" t="s">
         <v>250</v>
       </c>
-      <c r="I25" s="91" t="n">
+      <c r="I25" s="90" t="n">
         <v>-17.5</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="87" t="s">
+      <c r="B26" s="86" t="s">
         <v>251</v>
       </c>
       <c r="C26" s="0" t="n">
         <v>-48.1824</v>
       </c>
       <c r="D26" s="0"/>
-      <c r="E26" s="83" t="s">
+      <c r="E26" s="82" t="s">
         <v>251</v>
       </c>
-      <c r="F26" s="104" t="n">
+      <c r="F26" s="103" t="n">
         <f aca="false">'Modes A-F'!I54</f>
         <v>-23.853</v>
       </c>
       <c r="G26" s="0"/>
-      <c r="H26" s="83" t="s">
+      <c r="H26" s="82" t="s">
         <v>252</v>
       </c>
-      <c r="I26" s="91" t="n">
+      <c r="I26" s="90" t="n">
         <v>6.5</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="87" t="s">
+      <c r="B27" s="86" t="s">
         <v>253</v>
       </c>
-      <c r="C27" s="83" t="n">
+      <c r="C27" s="82" t="n">
         <v>27.1</v>
       </c>
       <c r="D27" s="0"/>
-      <c r="E27" s="83" t="s">
+      <c r="E27" s="82" t="s">
         <v>253</v>
       </c>
-      <c r="F27" s="104" t="n">
+      <c r="F27" s="103" t="n">
         <f aca="false">'Modes A-F'!K54</f>
         <v>43.058</v>
       </c>
       <c r="G27" s="0"/>
       <c r="H27" s="0"/>
-      <c r="I27" s="91"/>
+      <c r="I27" s="90"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="87" t="s">
+      <c r="B28" s="86" t="s">
         <v>254</v>
       </c>
-      <c r="C28" s="83" t="n">
+      <c r="C28" s="82" t="n">
         <v>27.1</v>
       </c>
       <c r="D28" s="0"/>
-      <c r="E28" s="83" t="s">
+      <c r="E28" s="82" t="s">
         <v>254</v>
       </c>
-      <c r="F28" s="104" t="n">
+      <c r="F28" s="103" t="n">
         <f aca="false">'Modes A-F'!M54</f>
         <v>43.058</v>
       </c>
       <c r="G28" s="0"/>
       <c r="H28" s="0"/>
-      <c r="I28" s="91"/>
+      <c r="I28" s="90"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="87" t="s">
+      <c r="B29" s="86" t="s">
         <v>255</v>
       </c>
-      <c r="C29" s="83" t="n">
+      <c r="C29" s="82" t="n">
         <v>2.8</v>
       </c>
       <c r="D29" s="0"/>
-      <c r="E29" s="83" t="s">
+      <c r="E29" s="82" t="s">
         <v>255</v>
       </c>
-      <c r="F29" s="104" t="n">
+      <c r="F29" s="103" t="n">
         <f aca="false">'Modes A-F'!O54</f>
         <v>16.963</v>
       </c>
       <c r="G29" s="0"/>
       <c r="H29" s="0"/>
-      <c r="I29" s="91"/>
+      <c r="I29" s="90"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="87" t="s">
+      <c r="B30" s="86" t="s">
         <v>256</v>
       </c>
-      <c r="C30" s="83" t="n">
+      <c r="C30" s="82" t="n">
         <v>15</v>
       </c>
       <c r="D30" s="0"/>
-      <c r="E30" s="83" t="s">
+      <c r="E30" s="82" t="s">
         <v>256</v>
       </c>
-      <c r="F30" s="104" t="n">
+      <c r="F30" s="103" t="n">
         <f aca="false">'Modes A-F'!T54</f>
         <v>53.33</v>
       </c>
       <c r="G30" s="0"/>
       <c r="H30" s="0"/>
-      <c r="I30" s="91"/>
+      <c r="I30" s="90"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="92" t="s">
+      <c r="B31" s="91" t="s">
         <v>248</v>
       </c>
-      <c r="C31" s="93" t="n">
+      <c r="C31" s="92" t="n">
         <v>55</v>
       </c>
-      <c r="D31" s="93"/>
-      <c r="E31" s="93"/>
-      <c r="F31" s="93"/>
-      <c r="G31" s="93"/>
-      <c r="H31" s="93"/>
-      <c r="I31" s="94"/>
+      <c r="D31" s="92"/>
+      <c r="E31" s="92"/>
+      <c r="F31" s="92"/>
+      <c r="G31" s="92"/>
+      <c r="H31" s="92"/>
+      <c r="I31" s="93"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -17108,7 +17095,7 @@
       <selection pane="bottomRight" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33"/>
@@ -17128,14 +17115,14 @@
       <c r="D1" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="105" t="s">
+      <c r="E1" s="104" t="s">
         <v>257</v>
       </c>
-      <c r="F1" s="105"/>
-      <c r="G1" s="106" t="s">
+      <c r="F1" s="104"/>
+      <c r="G1" s="105" t="s">
         <v>258</v>
       </c>
-      <c r="H1" s="106"/>
+      <c r="H1" s="105"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="44" t="s">
@@ -17161,25 +17148,25 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="107" t="s">
+      <c r="B3" s="106" t="s">
         <v>92</v>
       </c>
-      <c r="C3" s="108" t="s">
+      <c r="C3" s="107" t="s">
         <v>93</v>
       </c>
-      <c r="D3" s="108" t="s">
+      <c r="D3" s="107" t="s">
         <v>259</v>
       </c>
-      <c r="E3" s="108" t="n">
+      <c r="E3" s="107" t="n">
         <v>8.77968</v>
       </c>
-      <c r="F3" s="108" t="n">
+      <c r="F3" s="107" t="n">
         <v>-2703</v>
       </c>
-      <c r="G3" s="109" t="n">
+      <c r="G3" s="108" t="n">
         <v>7.16226</v>
       </c>
-      <c r="H3" s="110" t="n">
+      <c r="H3" s="109" t="n">
         <v>-6620</v>
       </c>
     </row>
@@ -17242,11 +17229,11 @@
       <c r="G6" s="1" t="n">
         <v>15.99439325</v>
       </c>
-      <c r="I6" s="111" t="s">
+      <c r="I6" s="110" t="s">
         <v>262</v>
       </c>
-      <c r="J6" s="111"/>
-      <c r="K6" s="111"/>
+      <c r="J6" s="110"/>
+      <c r="K6" s="110"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D7" s="0" t="s">
@@ -17258,9 +17245,9 @@
       <c r="G7" s="1" t="n">
         <v>1.63763854</v>
       </c>
-      <c r="I7" s="111"/>
-      <c r="J7" s="111"/>
-      <c r="K7" s="111"/>
+      <c r="I7" s="110"/>
+      <c r="J7" s="110"/>
+      <c r="K7" s="110"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -17290,7 +17277,7 @@
       <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.36"/>
@@ -17300,26 +17287,26 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="112"/>
-      <c r="B1" s="113"/>
-      <c r="C1" s="113"/>
-      <c r="D1" s="113"/>
-      <c r="E1" s="114" t="s">
+      <c r="A1" s="111"/>
+      <c r="B1" s="112"/>
+      <c r="C1" s="112"/>
+      <c r="D1" s="112"/>
+      <c r="E1" s="113" t="s">
         <v>264</v>
       </c>
-      <c r="F1" s="114" t="s">
+      <c r="F1" s="113" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="115" t="s">
+      <c r="G1" s="114" t="s">
         <v>265</v>
       </c>
-      <c r="H1" s="116" t="s">
+      <c r="H1" s="115" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="117"/>
-      <c r="D2" s="118" t="s">
+      <c r="A2" s="116"/>
+      <c r="D2" s="117" t="s">
         <v>267</v>
       </c>
       <c r="E2" s="0" t="n">
@@ -17328,93 +17315,93 @@
       <c r="F2" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="G2" s="119"/>
+      <c r="G2" s="118"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="120" t="s">
+      <c r="A3" s="119" t="s">
         <v>268</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>9002</v>
       </c>
-      <c r="D3" s="118" t="s">
+      <c r="D3" s="117" t="s">
         <v>269</v>
       </c>
-      <c r="E3" s="121" t="n">
+      <c r="E3" s="120" t="n">
         <v>46.1092</v>
       </c>
-      <c r="F3" s="104" t="n">
+      <c r="F3" s="103" t="n">
         <f aca="false">E3-B3*TAN(2*(F2-E2)/1000)</f>
         <v>19.1031189817083</v>
       </c>
-      <c r="G3" s="122" t="n">
+      <c r="G3" s="121" t="n">
         <f aca="false">'Modes A-F'!O54</f>
         <v>16.963</v>
       </c>
-      <c r="H3" s="123" t="n">
+      <c r="H3" s="122" t="n">
         <f aca="false">G3-F3</f>
         <v>-2.1401189817083</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="120" t="s">
+      <c r="A4" s="119" t="s">
         <v>270</v>
       </c>
       <c r="B4" s="0" t="n">
         <f aca="false">B3+635</f>
         <v>9637</v>
       </c>
-      <c r="D4" s="118" t="s">
+      <c r="D4" s="117" t="s">
         <v>271</v>
       </c>
-      <c r="E4" s="104" t="n">
+      <c r="E4" s="103" t="n">
         <f aca="false">'Modes A-F'!K56</f>
         <v>127.544</v>
       </c>
-      <c r="F4" s="104" t="n">
+      <c r="F4" s="103" t="n">
         <f aca="false">E4-B4*TAN(2*(F2-E2)/1000)</f>
         <v>98.6329132666878</v>
       </c>
-      <c r="G4" s="122" t="n">
+      <c r="G4" s="121" t="n">
         <f aca="false">'Modes A-F'!O56</f>
         <v>99.466</v>
       </c>
-      <c r="H4" s="123" t="n">
+      <c r="H4" s="122" t="n">
         <f aca="false">G4-F4</f>
         <v>0.833086733312243</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="124" t="s">
+      <c r="A5" s="123" t="s">
         <v>272</v>
       </c>
-      <c r="B5" s="125" t="n">
+      <c r="B5" s="124" t="n">
         <f aca="false">B3+1790</f>
         <v>10792</v>
       </c>
-      <c r="C5" s="125"/>
-      <c r="D5" s="126" t="s">
+      <c r="C5" s="124"/>
+      <c r="D5" s="125" t="s">
         <v>273</v>
       </c>
-      <c r="E5" s="127" t="n">
+      <c r="E5" s="126" t="n">
         <f aca="false">'Modes A-F'!K57</f>
         <v>131.814</v>
       </c>
-      <c r="F5" s="127" t="n">
+      <c r="F5" s="126" t="n">
         <f aca="false">E5-B5*TAN(2*(F2-E2)/1000)</f>
         <v>99.4379028716503</v>
       </c>
-      <c r="G5" s="128" t="n">
+      <c r="G5" s="127" t="n">
         <f aca="false">'Modes A-F'!O57</f>
         <v>100.436</v>
       </c>
-      <c r="H5" s="123" t="n">
+      <c r="H5" s="122" t="n">
         <f aca="false">G5-F5</f>
         <v>0.998097128349684</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H6" s="123" t="n">
+      <c r="H6" s="122" t="n">
         <f aca="false">AVERAGE(H3,H4,H5)</f>
         <v>-0.10297837334879</v>
       </c>
@@ -17423,419 +17410,419 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="129" t="s">
+      <c r="A8" s="128" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="129"/>
-      <c r="C8" s="129"/>
-      <c r="D8" s="113"/>
-      <c r="E8" s="113"/>
-      <c r="F8" s="130" t="s">
+      <c r="B8" s="128"/>
+      <c r="C8" s="128"/>
+      <c r="D8" s="112"/>
+      <c r="E8" s="112"/>
+      <c r="F8" s="129" t="s">
         <v>275</v>
       </c>
-      <c r="G8" s="131" t="n">
+      <c r="G8" s="130" t="n">
         <v>-0.1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="117"/>
-      <c r="D9" s="118" t="s">
+      <c r="A9" s="116"/>
+      <c r="D9" s="117" t="s">
         <v>267</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>3.5</v>
       </c>
-      <c r="G9" s="119" t="n">
+      <c r="G9" s="118" t="n">
         <f aca="false">E9+G8</f>
         <v>3.4</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="120" t="s">
+      <c r="A10" s="119" t="s">
         <v>276</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>10907</v>
       </c>
-      <c r="D10" s="118" t="s">
+      <c r="D10" s="117" t="s">
         <v>269</v>
       </c>
-      <c r="E10" s="123" t="n">
+      <c r="E10" s="122" t="n">
         <f aca="false">'Modes A-F'!E54</f>
-        <v>31.259</v>
-      </c>
-      <c r="F10" s="123"/>
-      <c r="G10" s="132" t="n">
+        <v>32.071</v>
+      </c>
+      <c r="F10" s="122"/>
+      <c r="G10" s="131" t="n">
         <f aca="false">E10-B10*TAN(2*(G9-E9)/1000)</f>
-        <v>33.4404000290853</v>
+        <v>34.2524000290853</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="120" t="s">
+      <c r="A11" s="119" t="s">
         <v>277</v>
       </c>
       <c r="B11" s="0" t="n">
         <f aca="false">B10+635</f>
         <v>11542</v>
       </c>
-      <c r="D11" s="118" t="s">
+      <c r="D11" s="117" t="s">
         <v>271</v>
       </c>
-      <c r="E11" s="123" t="n">
+      <c r="E11" s="122" t="n">
         <f aca="false">'Modes A-F'!E57</f>
         <v>121.119</v>
       </c>
-      <c r="F11" s="123"/>
-      <c r="G11" s="132" t="n">
+      <c r="F11" s="122"/>
+      <c r="G11" s="131" t="n">
         <f aca="false">E11-B11*TAN(2*(G9-E9)/1000)</f>
         <v>123.427400030779</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="124" t="s">
+      <c r="A12" s="123" t="s">
         <v>278</v>
       </c>
-      <c r="B12" s="125" t="n">
+      <c r="B12" s="124" t="n">
         <f aca="false">B10+1790</f>
         <v>12697</v>
       </c>
-      <c r="C12" s="125"/>
-      <c r="D12" s="126" t="s">
+      <c r="C12" s="124"/>
+      <c r="D12" s="125" t="s">
         <v>273</v>
       </c>
-      <c r="E12" s="133" t="n">
+      <c r="E12" s="132" t="n">
         <f aca="false">'Modes A-F'!E58</f>
         <v>121.119</v>
       </c>
-      <c r="F12" s="133"/>
-      <c r="G12" s="134" t="n">
+      <c r="F12" s="132"/>
+      <c r="G12" s="133" t="n">
         <f aca="false">E12-B12*TAN(2*(G9-E9)/1000)</f>
         <v>123.658400033859</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="129" t="s">
+      <c r="A16" s="128" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="129"/>
-      <c r="C16" s="129"/>
-      <c r="D16" s="113"/>
-      <c r="E16" s="113"/>
-      <c r="F16" s="130" t="s">
+      <c r="B16" s="128"/>
+      <c r="C16" s="128"/>
+      <c r="D16" s="112"/>
+      <c r="E16" s="112"/>
+      <c r="F16" s="129" t="s">
         <v>275</v>
       </c>
-      <c r="G16" s="113" t="n">
+      <c r="G16" s="112" t="n">
         <v>0.275</v>
       </c>
-      <c r="H16" s="113"/>
-      <c r="I16" s="131"/>
+      <c r="H16" s="112"/>
+      <c r="I16" s="130"/>
     </row>
     <row r="17" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="117"/>
-      <c r="D17" s="118" t="s">
+      <c r="A17" s="116"/>
+      <c r="D17" s="117" t="s">
         <v>267</v>
       </c>
       <c r="E17" s="0" t="n">
         <v>3.225</v>
       </c>
-      <c r="G17" s="72" t="n">
+      <c r="G17" s="71" t="n">
         <f aca="false">E17+G16</f>
         <v>3.5</v>
       </c>
-      <c r="H17" s="61" t="s">
+      <c r="H17" s="57" t="s">
         <v>279</v>
       </c>
-      <c r="I17" s="119" t="n">
+      <c r="I17" s="118" t="n">
         <f aca="false">B18*TAN(2*(E9-G17)/1000)</f>
         <v>0</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="120" t="s">
+      <c r="A18" s="119" t="s">
         <v>280</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>1908</v>
       </c>
-      <c r="D18" s="118" t="s">
+      <c r="D18" s="117" t="s">
         <v>281</v>
       </c>
       <c r="E18" s="0" t="n">
         <v>-7.25</v>
       </c>
-      <c r="G18" s="135" t="n">
+      <c r="G18" s="134" t="n">
         <f aca="false">E18+B18*TAN(2*(G17-E17)/1000)</f>
         <v>-6.20059989418549</v>
       </c>
-      <c r="I18" s="119"/>
+      <c r="I18" s="118"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="117"/>
-      <c r="D19" s="118" t="s">
+      <c r="A19" s="116"/>
+      <c r="D19" s="117" t="s">
         <v>282</v>
       </c>
       <c r="E19" s="0" t="n">
         <f aca="false">3.5 + (3.5-E17)</f>
         <v>3.775</v>
       </c>
-      <c r="G19" s="72" t="n">
+      <c r="G19" s="71" t="n">
         <f aca="false">E19-G16</f>
         <v>3.5</v>
       </c>
-      <c r="I19" s="119"/>
+      <c r="I19" s="118"/>
     </row>
     <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="117"/>
-      <c r="D20" s="118"/>
-      <c r="G20" s="136" t="s">
+      <c r="A20" s="116"/>
+      <c r="D20" s="117"/>
+      <c r="G20" s="135" t="s">
         <v>283</v>
       </c>
-      <c r="I20" s="119"/>
+      <c r="I20" s="118"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="117"/>
-      <c r="F21" s="137" t="s">
+      <c r="A21" s="116"/>
+      <c r="F21" s="136" t="s">
         <v>265</v>
       </c>
-      <c r="I21" s="119"/>
+      <c r="I21" s="118"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="120" t="s">
+      <c r="A22" s="119" t="s">
         <v>268</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>9002</v>
       </c>
-      <c r="D22" s="118" t="s">
+      <c r="D22" s="117" t="s">
         <v>269</v>
       </c>
-      <c r="E22" s="123" t="n">
+      <c r="E22" s="122" t="n">
         <f aca="false">E10-B22*TAN(2*(E19)/1000)+I17</f>
-        <v>-36.7073914229833</v>
-      </c>
-      <c r="F22" s="138" t="n">
+        <v>-35.8953914229833</v>
+      </c>
+      <c r="F22" s="137" t="n">
         <f aca="false">'Modes A-F'!I54</f>
         <v>-23.853</v>
       </c>
-      <c r="G22" s="123" t="n">
+      <c r="G22" s="122" t="n">
         <f aca="false">E10-B22*TAN(2*(G19)/1000)+I17</f>
-        <v>-31.75602924884</v>
-      </c>
-      <c r="I22" s="119"/>
+        <v>-30.94402924884</v>
+      </c>
+      <c r="I22" s="118"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="120" t="s">
+      <c r="A23" s="119" t="s">
         <v>270</v>
       </c>
       <c r="B23" s="0" t="n">
         <f aca="false">B22+635</f>
         <v>9637</v>
       </c>
-      <c r="D23" s="118" t="s">
+      <c r="D23" s="117" t="s">
         <v>271</v>
       </c>
-      <c r="E23" s="123" t="n">
+      <c r="E23" s="122" t="n">
         <f aca="false">E11-B23*TAN(2*(E19)/1000)+I17</f>
         <v>48.3582674801944</v>
       </c>
-      <c r="F23" s="138" t="n">
+      <c r="F23" s="137" t="n">
         <f aca="false">'Modes A-F'!I56</f>
         <v>56.009</v>
       </c>
-      <c r="G23" s="123" t="n">
+      <c r="G23" s="122" t="n">
         <f aca="false">E11-B23*TAN(2*(G19)/1000)+I17</f>
         <v>53.6588981480704</v>
       </c>
-      <c r="I23" s="119"/>
+      <c r="I23" s="118"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="124" t="s">
+      <c r="A24" s="123" t="s">
         <v>272</v>
       </c>
-      <c r="B24" s="125" t="n">
+      <c r="B24" s="124" t="n">
         <f aca="false">B22+1790</f>
         <v>10792</v>
       </c>
-      <c r="C24" s="125"/>
-      <c r="D24" s="126" t="s">
+      <c r="C24" s="124"/>
+      <c r="D24" s="125" t="s">
         <v>273</v>
       </c>
-      <c r="E24" s="133" t="n">
+      <c r="E24" s="132" t="n">
         <f aca="false">E12-B24*TAN(2*(E19)/1000)+I17</f>
         <v>39.6378517843995</v>
       </c>
-      <c r="F24" s="139" t="n">
+      <c r="F24" s="138" t="n">
         <f aca="false">'Modes A-F'!I57</f>
         <v>52.508</v>
       </c>
-      <c r="G24" s="140" t="n">
+      <c r="G24" s="139" t="n">
         <f aca="false">E12-B24*TAN(2*(G19)/1000)+I17</f>
         <v>45.573766090482</v>
       </c>
-      <c r="H24" s="125"/>
-      <c r="I24" s="141"/>
+      <c r="H24" s="124"/>
+      <c r="I24" s="140"/>
     </row>
     <row r="28" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="142" t="s">
+      <c r="A28" s="141" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="142"/>
-      <c r="C28" s="142"/>
-      <c r="D28" s="113"/>
-      <c r="E28" s="113"/>
-      <c r="F28" s="130" t="s">
+      <c r="B28" s="141"/>
+      <c r="C28" s="141"/>
+      <c r="D28" s="112"/>
+      <c r="E28" s="112"/>
+      <c r="F28" s="129" t="s">
         <v>275</v>
       </c>
-      <c r="G28" s="113" t="n">
+      <c r="G28" s="112" t="n">
         <v>0.275</v>
       </c>
-      <c r="H28" s="113"/>
-      <c r="I28" s="131"/>
+      <c r="H28" s="112"/>
+      <c r="I28" s="130"/>
     </row>
     <row r="29" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="117"/>
-      <c r="D29" s="118" t="s">
+      <c r="A29" s="116"/>
+      <c r="D29" s="117" t="s">
         <v>267</v>
       </c>
       <c r="E29" s="0" t="n">
         <v>3.225</v>
       </c>
-      <c r="G29" s="72" t="n">
+      <c r="G29" s="71" t="n">
         <f aca="false">E29+G28</f>
         <v>3.5</v>
       </c>
-      <c r="H29" s="61" t="s">
+      <c r="H29" s="57" t="s">
         <v>279</v>
       </c>
-      <c r="I29" s="119" t="n">
+      <c r="I29" s="118" t="n">
         <f aca="false">B30*TAN(2*(E9-G29)/1000)</f>
         <v>0</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="120" t="s">
+      <c r="A30" s="119" t="s">
         <v>280</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>1908</v>
       </c>
-      <c r="D30" s="118" t="s">
+      <c r="D30" s="117" t="s">
         <v>281</v>
       </c>
       <c r="E30" s="0" t="n">
         <v>-6.583</v>
       </c>
-      <c r="G30" s="135" t="n">
+      <c r="G30" s="134" t="n">
         <f aca="false">E30+B30*TAN(2*(G29-E29)/1000)</f>
         <v>-5.53359989418549</v>
       </c>
-      <c r="I30" s="119"/>
+      <c r="I30" s="118"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="117"/>
-      <c r="D31" s="118" t="s">
+      <c r="A31" s="116"/>
+      <c r="D31" s="117" t="s">
         <v>282</v>
       </c>
       <c r="E31" s="0" t="n">
         <f aca="false">5+(3.5-E29)</f>
         <v>5.275</v>
       </c>
-      <c r="G31" s="72" t="n">
+      <c r="G31" s="71" t="n">
         <f aca="false">E31-G28</f>
         <v>5</v>
       </c>
-      <c r="I31" s="119"/>
+      <c r="I31" s="118"/>
     </row>
     <row r="32" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="117"/>
-      <c r="D32" s="118"/>
-      <c r="G32" s="136" t="s">
+      <c r="A32" s="116"/>
+      <c r="D32" s="117"/>
+      <c r="G32" s="135" t="s">
         <v>283</v>
       </c>
-      <c r="I32" s="119"/>
+      <c r="I32" s="118"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="117"/>
-      <c r="F33" s="137" t="s">
+      <c r="A33" s="116"/>
+      <c r="F33" s="136" t="s">
         <v>265</v>
       </c>
-      <c r="I33" s="119"/>
+      <c r="I33" s="118"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="120" t="s">
+      <c r="A34" s="119" t="s">
         <v>268</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>9002</v>
       </c>
-      <c r="D34" s="118" t="s">
+      <c r="D34" s="117" t="s">
         <v>269</v>
       </c>
-      <c r="E34" s="123" t="n">
+      <c r="E34" s="122" t="n">
         <f aca="false">E10-B34*TAN(2*(E31)/1000)</f>
-        <v>-63.7156236638297</v>
-      </c>
-      <c r="F34" s="138" t="n">
+        <v>-62.9036236638297</v>
+      </c>
+      <c r="F34" s="137" t="n">
         <f aca="false">'Modes A-F'!G54</f>
         <v>-55.188</v>
       </c>
-      <c r="G34" s="123" t="n">
+      <c r="G34" s="122" t="n">
         <f aca="false">E10-B34*TAN(2*(G31)/1000)+I29</f>
-        <v>-58.7640007866982</v>
-      </c>
-      <c r="I34" s="119"/>
+        <v>-57.9520007866982</v>
+      </c>
+      <c r="I34" s="118"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="120" t="s">
+      <c r="A35" s="119" t="s">
         <v>270</v>
       </c>
       <c r="B35" s="0" t="n">
         <f aca="false">B34+635</f>
         <v>9637</v>
       </c>
-      <c r="D35" s="118" t="s">
+      <c r="D35" s="117" t="s">
         <v>271</v>
       </c>
-      <c r="E35" s="123" t="n">
+      <c r="E35" s="122" t="n">
         <f aca="false">E11-B35*TAN(2*(E31)/1000)</f>
         <v>19.4448777773465</v>
       </c>
-      <c r="F35" s="138" t="n">
+      <c r="F35" s="137" t="n">
         <f aca="false">'Modes A-F'!G56</f>
         <v>24.4104</v>
       </c>
-      <c r="G35" s="123" t="n">
+      <c r="G35" s="122" t="n">
         <f aca="false">E11-B35*TAN(2*(G31)/1000)+I29</f>
         <v>24.7457875381681</v>
       </c>
-      <c r="I35" s="119"/>
+      <c r="I35" s="118"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="124" t="s">
+      <c r="A36" s="123" t="s">
         <v>272</v>
       </c>
-      <c r="B36" s="125" t="n">
+      <c r="B36" s="124" t="n">
         <f aca="false">B34+1790</f>
         <v>10792</v>
       </c>
-      <c r="C36" s="125"/>
-      <c r="D36" s="126" t="s">
+      <c r="C36" s="124"/>
+      <c r="D36" s="125" t="s">
         <v>273</v>
       </c>
-      <c r="E36" s="133" t="n">
+      <c r="E36" s="132" t="n">
         <f aca="false">E12-B36*TAN(2*(E31)/1000)</f>
         <v>7.25917567428903</v>
       </c>
-      <c r="F36" s="139" t="n">
+      <c r="F36" s="138" t="n">
         <f aca="false">'Modes A-F'!G57</f>
         <v>12.81</v>
       </c>
-      <c r="G36" s="133" t="n">
+      <c r="G36" s="132" t="n">
         <f aca="false">E12-B36*TAN(2*(G31)/1000)+I29</f>
         <v>13.1954025227675</v>
       </c>
-      <c r="H36" s="125"/>
-      <c r="I36" s="141"/>
+      <c r="H36" s="124"/>
+      <c r="I36" s="140"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -17864,7 +17851,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.26"/>
   </cols>
@@ -17937,7 +17924,7 @@
       <c r="A9" s="0" t="s">
         <v>292</v>
       </c>
-      <c r="B9" s="143" t="n">
+      <c r="B9" s="142" t="n">
         <v>1E-006</v>
       </c>
     </row>
@@ -17961,7 +17948,7 @@
       <c r="A12" s="0" t="s">
         <v>295</v>
       </c>
-      <c r="B12" s="143" t="n">
+      <c r="B12" s="142" t="n">
         <v>1E-005</v>
       </c>
     </row>
@@ -18057,7 +18044,7 @@
       <c r="A24" s="0" t="s">
         <v>307</v>
       </c>
-      <c r="B24" s="143" t="n">
+      <c r="B24" s="142" t="n">
         <v>1E-006</v>
       </c>
     </row>
@@ -18081,7 +18068,7 @@
       <c r="A27" s="0" t="s">
         <v>310</v>
       </c>
-      <c r="B27" s="143" t="n">
+      <c r="B27" s="142" t="n">
         <v>1E-005</v>
       </c>
     </row>
@@ -18177,7 +18164,7 @@
       <c r="A39" s="0" t="s">
         <v>322</v>
       </c>
-      <c r="B39" s="143" t="n">
+      <c r="B39" s="142" t="n">
         <v>1E-006</v>
       </c>
     </row>
@@ -18201,7 +18188,7 @@
       <c r="A42" s="0" t="s">
         <v>325</v>
       </c>
-      <c r="B42" s="143" t="n">
+      <c r="B42" s="142" t="n">
         <v>1E-005</v>
       </c>
     </row>
@@ -18297,7 +18284,7 @@
       <c r="A54" s="0" t="s">
         <v>337</v>
       </c>
-      <c r="B54" s="143" t="n">
+      <c r="B54" s="142" t="n">
         <v>1E-006</v>
       </c>
     </row>
@@ -18321,7 +18308,7 @@
       <c r="A57" s="0" t="s">
         <v>340</v>
       </c>
-      <c r="B57" s="143" t="n">
+      <c r="B57" s="142" t="n">
         <v>1E-005</v>
       </c>
     </row>
@@ -18385,7 +18372,7 @@
       <c r="A65" s="0" t="s">
         <v>348</v>
       </c>
-      <c r="B65" s="143" t="n">
+      <c r="B65" s="142" t="n">
         <v>8.1921E-011</v>
       </c>
     </row>
@@ -18393,7 +18380,7 @@
       <c r="A66" s="0" t="s">
         <v>349</v>
       </c>
-      <c r="B66" s="143" t="n">
+      <c r="B66" s="142" t="n">
         <v>6.1817E-009</v>
       </c>
     </row>
@@ -18401,7 +18388,7 @@
       <c r="A67" s="0" t="s">
         <v>350</v>
       </c>
-      <c r="B67" s="143" t="n">
+      <c r="B67" s="142" t="n">
         <v>-8.139E-009</v>
       </c>
     </row>
@@ -18409,7 +18396,7 @@
       <c r="A68" s="0" t="s">
         <v>351</v>
       </c>
-      <c r="B68" s="143" t="n">
+      <c r="B68" s="142" t="n">
         <v>4.2612E-009</v>
       </c>
     </row>
@@ -18729,7 +18716,7 @@
       <c r="A108" s="0" t="s">
         <v>391</v>
       </c>
-      <c r="B108" s="143" t="n">
+      <c r="B108" s="142" t="n">
         <v>1E-006</v>
       </c>
     </row>
@@ -18753,7 +18740,7 @@
       <c r="A111" s="0" t="s">
         <v>394</v>
       </c>
-      <c r="B111" s="143" t="n">
+      <c r="B111" s="142" t="n">
         <v>1E-005</v>
       </c>
     </row>
@@ -18849,7 +18836,7 @@
       <c r="A123" s="0" t="s">
         <v>406</v>
       </c>
-      <c r="B123" s="143" t="n">
+      <c r="B123" s="142" t="n">
         <v>1E-006</v>
       </c>
     </row>
@@ -18873,7 +18860,7 @@
       <c r="A126" s="0" t="s">
         <v>409</v>
       </c>
-      <c r="B126" s="143" t="n">
+      <c r="B126" s="142" t="n">
         <v>1E-005</v>
       </c>
     </row>
@@ -18969,7 +18956,7 @@
       <c r="A138" s="0" t="s">
         <v>421</v>
       </c>
-      <c r="B138" s="143" t="n">
+      <c r="B138" s="142" t="n">
         <v>1E-006</v>
       </c>
     </row>
@@ -18993,7 +18980,7 @@
       <c r="A141" s="0" t="s">
         <v>424</v>
       </c>
-      <c r="B141" s="143" t="n">
+      <c r="B141" s="142" t="n">
         <v>1E-005</v>
       </c>
     </row>
@@ -19089,7 +19076,7 @@
       <c r="A153" s="0" t="s">
         <v>436</v>
       </c>
-      <c r="B153" s="143" t="n">
+      <c r="B153" s="142" t="n">
         <v>1E-006</v>
       </c>
     </row>
@@ -19113,7 +19100,7 @@
       <c r="A156" s="0" t="s">
         <v>439</v>
       </c>
-      <c r="B156" s="143" t="n">
+      <c r="B156" s="142" t="n">
         <v>1E-005</v>
       </c>
     </row>
@@ -19177,7 +19164,7 @@
       <c r="A164" s="0" t="s">
         <v>447</v>
       </c>
-      <c r="B164" s="143" t="n">
+      <c r="B164" s="142" t="n">
         <v>1.9024E-008</v>
       </c>
     </row>
@@ -19185,7 +19172,7 @@
       <c r="A165" s="0" t="s">
         <v>448</v>
       </c>
-      <c r="B165" s="143" t="n">
+      <c r="B165" s="142" t="n">
         <v>-9.5679E-009</v>
       </c>
     </row>
@@ -19193,7 +19180,7 @@
       <c r="A166" s="0" t="s">
         <v>449</v>
       </c>
-      <c r="B166" s="143" t="n">
+      <c r="B166" s="142" t="n">
         <v>-1.1631E-009</v>
       </c>
     </row>
@@ -19201,7 +19188,7 @@
       <c r="A167" s="0" t="s">
         <v>450</v>
       </c>
-      <c r="B167" s="143" t="n">
+      <c r="B167" s="142" t="n">
         <v>1.027E-008</v>
       </c>
     </row>
@@ -19337,7 +19324,7 @@
       <c r="A184" s="0" t="s">
         <v>467</v>
       </c>
-      <c r="B184" s="143" t="n">
+      <c r="B184" s="142" t="n">
         <v>2.8833E-008</v>
       </c>
     </row>
@@ -19345,7 +19332,7 @@
       <c r="A185" s="0" t="s">
         <v>468</v>
       </c>
-      <c r="B185" s="143" t="n">
+      <c r="B185" s="142" t="n">
         <v>2.8833E-008</v>
       </c>
     </row>
@@ -19377,7 +19364,7 @@
       <c r="A189" s="0" t="s">
         <v>472</v>
       </c>
-      <c r="B189" s="143" t="n">
+      <c r="B189" s="142" t="n">
         <v>4761600</v>
       </c>
     </row>
@@ -19401,7 +19388,7 @@
       <c r="A192" s="0" t="s">
         <v>475</v>
       </c>
-      <c r="B192" s="143" t="n">
+      <c r="B192" s="142" t="n">
         <v>2.8343E-008</v>
       </c>
     </row>
@@ -19409,7 +19396,7 @@
       <c r="A193" s="0" t="s">
         <v>476</v>
       </c>
-      <c r="B193" s="143" t="n">
+      <c r="B193" s="142" t="n">
         <v>-7.401E-010</v>
       </c>
     </row>
@@ -19417,7 +19404,7 @@
       <c r="A194" s="0" t="s">
         <v>477</v>
       </c>
-      <c r="B194" s="143" t="n">
+      <c r="B194" s="142" t="n">
         <v>-1.4084E-009</v>
       </c>
     </row>
@@ -19425,7 +19412,7 @@
       <c r="A195" s="0" t="s">
         <v>478</v>
       </c>
-      <c r="B195" s="143" t="n">
+      <c r="B195" s="142" t="n">
         <v>2.0325E-008</v>
       </c>
     </row>
@@ -20849,40 +20836,40 @@
       <c r="B337" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C337" s="143" t="n">
+      <c r="C337" s="142" t="n">
         <v>8.3006E-011</v>
       </c>
-      <c r="D337" s="143" t="n">
+      <c r="D337" s="142" t="n">
         <v>8.2839E-011</v>
       </c>
-      <c r="E337" s="143" t="n">
+      <c r="E337" s="142" t="n">
         <v>8.2777E-011</v>
       </c>
-      <c r="F337" s="143" t="n">
+      <c r="F337" s="142" t="n">
         <v>8.1528E-011</v>
       </c>
-      <c r="G337" s="143" t="n">
+      <c r="G337" s="142" t="n">
         <v>8.2662E-011</v>
       </c>
-      <c r="H337" s="143" t="n">
+      <c r="H337" s="142" t="n">
         <v>8.3572E-011</v>
       </c>
-      <c r="I337" s="143" t="n">
+      <c r="I337" s="142" t="n">
         <v>8.489E-011</v>
       </c>
-      <c r="J337" s="143" t="n">
+      <c r="J337" s="142" t="n">
         <v>8.3896E-011</v>
       </c>
-      <c r="K337" s="143" t="n">
+      <c r="K337" s="142" t="n">
         <v>8.2012E-011</v>
       </c>
-      <c r="L337" s="143" t="n">
+      <c r="L337" s="142" t="n">
         <v>8.0897E-011</v>
       </c>
-      <c r="M337" s="143" t="n">
+      <c r="M337" s="142" t="n">
         <v>8.29E-011</v>
       </c>
-      <c r="N337" s="143" t="n">
+      <c r="N337" s="142" t="n">
         <v>8.0797E-011</v>
       </c>
     </row>
@@ -20893,40 +20880,40 @@
       <c r="B338" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C338" s="143" t="n">
+      <c r="C338" s="142" t="n">
         <v>6.3068E-009</v>
       </c>
-      <c r="D338" s="143" t="n">
+      <c r="D338" s="142" t="n">
         <v>6.0737E-009</v>
       </c>
-      <c r="E338" s="143" t="n">
+      <c r="E338" s="142" t="n">
         <v>6.6921E-009</v>
       </c>
-      <c r="F338" s="143" t="n">
+      <c r="F338" s="142" t="n">
         <v>5.7007E-009</v>
       </c>
-      <c r="G338" s="143" t="n">
+      <c r="G338" s="142" t="n">
         <v>5.6393E-009</v>
       </c>
-      <c r="H338" s="143" t="n">
+      <c r="H338" s="142" t="n">
         <v>6.6627E-009</v>
       </c>
-      <c r="I338" s="143" t="n">
+      <c r="I338" s="142" t="n">
         <v>6.6038E-009</v>
       </c>
-      <c r="J338" s="143" t="n">
+      <c r="J338" s="142" t="n">
         <v>5.87E-009</v>
       </c>
-      <c r="K338" s="143" t="n">
+      <c r="K338" s="142" t="n">
         <v>6.1792E-009</v>
       </c>
-      <c r="L338" s="143" t="n">
+      <c r="L338" s="142" t="n">
         <v>5.3276E-009</v>
       </c>
-      <c r="M338" s="143" t="n">
+      <c r="M338" s="142" t="n">
         <v>6.513E-009</v>
       </c>
-      <c r="N338" s="143" t="n">
+      <c r="N338" s="142" t="n">
         <v>5.9829E-009</v>
       </c>
     </row>
@@ -20937,40 +20924,40 @@
       <c r="B339" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C339" s="143" t="n">
+      <c r="C339" s="142" t="n">
         <v>-7.2948E-009</v>
       </c>
-      <c r="D339" s="143" t="n">
+      <c r="D339" s="142" t="n">
         <v>-7.6015E-009</v>
       </c>
-      <c r="E339" s="143" t="n">
+      <c r="E339" s="142" t="n">
         <v>-7.4862E-009</v>
       </c>
-      <c r="F339" s="143" t="n">
+      <c r="F339" s="142" t="n">
         <v>-8.5513E-009</v>
       </c>
-      <c r="G339" s="143" t="n">
+      <c r="G339" s="142" t="n">
         <v>-8.3206E-009</v>
       </c>
-      <c r="H339" s="143" t="n">
+      <c r="H339" s="142" t="n">
         <v>-7.5942E-009</v>
       </c>
-      <c r="I339" s="143" t="n">
+      <c r="I339" s="142" t="n">
         <v>-7.5377E-009</v>
       </c>
-      <c r="J339" s="143" t="n">
+      <c r="J339" s="142" t="n">
         <v>-8.5415E-009</v>
       </c>
-      <c r="K339" s="143" t="n">
+      <c r="K339" s="142" t="n">
         <v>-7.7635E-009</v>
       </c>
-      <c r="L339" s="143" t="n">
+      <c r="L339" s="142" t="n">
         <v>-8.0482E-009</v>
       </c>
-      <c r="M339" s="143" t="n">
+      <c r="M339" s="142" t="n">
         <v>-8.2175E-009</v>
       </c>
-      <c r="N339" s="143" t="n">
+      <c r="N339" s="142" t="n">
         <v>-7.9966E-009</v>
       </c>
     </row>
@@ -20981,40 +20968,40 @@
       <c r="B340" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C340" s="143" t="n">
+      <c r="C340" s="142" t="n">
         <v>4.8625E-009</v>
       </c>
-      <c r="D340" s="143" t="n">
+      <c r="D340" s="142" t="n">
         <v>4.433E-009</v>
       </c>
-      <c r="E340" s="143" t="n">
+      <c r="E340" s="142" t="n">
         <v>3.4611E-009</v>
       </c>
-      <c r="F340" s="143" t="n">
+      <c r="F340" s="142" t="n">
         <v>3.9372E-009</v>
       </c>
-      <c r="G340" s="143" t="n">
+      <c r="G340" s="142" t="n">
         <v>4.8526E-009</v>
       </c>
-      <c r="H340" s="143" t="n">
+      <c r="H340" s="142" t="n">
         <v>4.5041E-009</v>
       </c>
-      <c r="I340" s="143" t="n">
+      <c r="I340" s="142" t="n">
         <v>4.5311E-009</v>
       </c>
-      <c r="J340" s="143" t="n">
+      <c r="J340" s="142" t="n">
         <v>4.2882E-009</v>
       </c>
-      <c r="K340" s="143" t="n">
+      <c r="K340" s="142" t="n">
         <v>4.4551E-009</v>
       </c>
-      <c r="L340" s="143" t="n">
+      <c r="L340" s="142" t="n">
         <v>4.136E-009</v>
       </c>
-      <c r="M340" s="143" t="n">
+      <c r="M340" s="142" t="n">
         <v>3.9078E-009</v>
       </c>
-      <c r="N340" s="143" t="n">
+      <c r="N340" s="142" t="n">
         <v>3.9593E-009</v>
       </c>
     </row>
@@ -21729,40 +21716,40 @@
       <c r="B357" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C357" s="143" t="n">
+      <c r="C357" s="142" t="n">
         <v>2.1231E-008</v>
       </c>
-      <c r="D357" s="143" t="n">
+      <c r="D357" s="142" t="n">
         <v>1.9514E-008</v>
       </c>
-      <c r="E357" s="143" t="n">
+      <c r="E357" s="142" t="n">
         <v>1.8533E-008</v>
       </c>
-      <c r="F357" s="143" t="n">
+      <c r="F357" s="142" t="n">
         <v>2.1231E-008</v>
       </c>
-      <c r="G357" s="143" t="n">
+      <c r="G357" s="142" t="n">
         <v>2.4174E-008</v>
       </c>
-      <c r="H357" s="143" t="n">
+      <c r="H357" s="142" t="n">
         <v>1.9024E-008</v>
       </c>
-      <c r="I357" s="143" t="n">
+      <c r="I357" s="142" t="n">
         <v>2.8588E-008</v>
       </c>
-      <c r="J357" s="143" t="n">
+      <c r="J357" s="142" t="n">
         <v>1.9024E-008</v>
       </c>
-      <c r="K357" s="143" t="n">
+      <c r="K357" s="142" t="n">
         <v>3.2757E-008</v>
       </c>
-      <c r="L357" s="143" t="n">
+      <c r="L357" s="142" t="n">
         <v>3.5455E-008</v>
       </c>
-      <c r="M357" s="143" t="n">
+      <c r="M357" s="142" t="n">
         <v>2.025E-008</v>
       </c>
-      <c r="N357" s="143" t="n">
+      <c r="N357" s="142" t="n">
         <v>2.1231E-008</v>
       </c>
     </row>
@@ -21773,40 +21760,40 @@
       <c r="B358" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C358" s="143" t="n">
+      <c r="C358" s="142" t="n">
         <v>-1.766E-008</v>
       </c>
-      <c r="D358" s="143" t="n">
+      <c r="D358" s="142" t="n">
         <v>-4.4184E-009</v>
       </c>
-      <c r="E358" s="143" t="n">
+      <c r="E358" s="142" t="n">
         <v>-1.1284E-008</v>
       </c>
-      <c r="F358" s="143" t="n">
+      <c r="F358" s="142" t="n">
         <v>-1.1039E-008</v>
       </c>
-      <c r="G358" s="143" t="n">
+      <c r="G358" s="142" t="n">
         <v>-9.5679E-009</v>
       </c>
-      <c r="H358" s="143" t="n">
+      <c r="H358" s="142" t="n">
         <v>-1.1284E-008</v>
       </c>
-      <c r="I358" s="143" t="n">
+      <c r="I358" s="142" t="n">
         <v>-2.2114E-009</v>
       </c>
-      <c r="J358" s="143" t="n">
+      <c r="J358" s="142" t="n">
         <v>-5.3992E-009</v>
       </c>
-      <c r="K358" s="143" t="n">
+      <c r="K358" s="142" t="n">
         <v>9.7642E-010</v>
       </c>
-      <c r="L358" s="143" t="n">
+      <c r="L358" s="142" t="n">
         <v>6.3712E-009</v>
       </c>
-      <c r="M358" s="143" t="n">
+      <c r="M358" s="142" t="n">
         <v>-1.153E-008</v>
       </c>
-      <c r="N358" s="143" t="n">
+      <c r="N358" s="142" t="n">
         <v>-9.8131E-009</v>
       </c>
     </row>
@@ -21817,40 +21804,40 @@
       <c r="B359" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C359" s="143" t="n">
+      <c r="C359" s="142" t="n">
         <v>-9.0112E-009</v>
       </c>
-      <c r="D359" s="143" t="n">
+      <c r="D359" s="142" t="n">
         <v>-4.3514E-009</v>
       </c>
-      <c r="E359" s="143" t="n">
+      <c r="E359" s="142" t="n">
         <v>-6.0682E-009</v>
       </c>
-      <c r="F359" s="143" t="n">
+      <c r="F359" s="142" t="n">
         <v>-9.0112E-009</v>
       </c>
-      <c r="G359" s="143" t="n">
+      <c r="G359" s="142" t="n">
         <v>-4.5967E-009</v>
       </c>
-      <c r="H359" s="143" t="n">
+      <c r="H359" s="142" t="n">
         <v>-1.0483E-008</v>
       </c>
-      <c r="I359" s="143" t="n">
+      <c r="I359" s="142" t="n">
         <v>7.6659E-009</v>
       </c>
-      <c r="J359" s="143" t="n">
+      <c r="J359" s="142" t="n">
         <v>-3.3704E-009</v>
       </c>
-      <c r="K359" s="143" t="n">
+      <c r="K359" s="142" t="n">
         <v>6.6849E-009</v>
       </c>
-      <c r="L359" s="143" t="n">
+      <c r="L359" s="142" t="n">
         <v>5.2134E-009</v>
       </c>
-      <c r="M359" s="143" t="n">
+      <c r="M359" s="142" t="n">
         <v>-1.6536E-009</v>
       </c>
-      <c r="N359" s="143" t="n">
+      <c r="N359" s="142" t="n">
         <v>-5.5777E-009</v>
       </c>
     </row>
@@ -21861,40 +21848,40 @@
       <c r="B360" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C360" s="143" t="n">
+      <c r="C360" s="142" t="n">
         <v>7.8174E-009</v>
       </c>
-      <c r="D360" s="143" t="n">
+      <c r="D360" s="142" t="n">
         <v>2.3513E-008</v>
       </c>
-      <c r="E360" s="143" t="n">
+      <c r="E360" s="142" t="n">
         <v>1.7382E-008</v>
       </c>
-      <c r="F360" s="143" t="n">
+      <c r="F360" s="142" t="n">
         <v>1.1006E-008</v>
       </c>
-      <c r="G360" s="143" t="n">
+      <c r="G360" s="142" t="n">
         <v>1.5665E-008</v>
       </c>
-      <c r="H360" s="143" t="n">
+      <c r="H360" s="142" t="n">
         <v>1.2477E-008</v>
       </c>
-      <c r="I360" s="143" t="n">
+      <c r="I360" s="142" t="n">
         <v>2.057E-008</v>
       </c>
-      <c r="J360" s="143" t="n">
+      <c r="J360" s="142" t="n">
         <v>1.9835E-008</v>
       </c>
-      <c r="K360" s="143" t="n">
+      <c r="K360" s="142" t="n">
         <v>2.5721E-008</v>
       </c>
-      <c r="L360" s="143" t="n">
+      <c r="L360" s="142" t="n">
         <v>2.5475E-008</v>
       </c>
-      <c r="M360" s="143" t="n">
+      <c r="M360" s="142" t="n">
         <v>1.076E-008</v>
       </c>
-      <c r="N360" s="143" t="n">
+      <c r="N360" s="142" t="n">
         <v>1.3213E-008</v>
       </c>
     </row>
@@ -22037,7 +22024,7 @@
       <c r="B364" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C364" s="143" t="n">
+      <c r="C364" s="142" t="n">
         <v>2.8343E-008</v>
       </c>
       <c r="D364" s="0" t="n">
@@ -22081,7 +22068,7 @@
       <c r="B365" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C365" s="143" t="n">
+      <c r="C365" s="142" t="n">
         <v>-7.401E-010</v>
       </c>
       <c r="D365" s="0" t="n">
@@ -22125,7 +22112,7 @@
       <c r="B366" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C366" s="143" t="n">
+      <c r="C366" s="142" t="n">
         <v>-1.4084E-009</v>
       </c>
       <c r="D366" s="0" t="n">
@@ -22169,7 +22156,7 @@
       <c r="B367" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C367" s="143" t="n">
+      <c r="C367" s="142" t="n">
         <v>2.0325E-008</v>
       </c>
       <c r="D367" s="0" t="n">
@@ -23935,7 +23922,7 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="56.14"/>
@@ -23945,13 +23932,13 @@
       <c r="A1" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B1" s="144" t="s">
+      <c r="B1" s="143" t="s">
         <v>814</v>
       </c>
-      <c r="C1" s="144" t="n">
+      <c r="C1" s="143" t="n">
         <v>350</v>
       </c>
-      <c r="D1" s="144" t="s">
+      <c r="D1" s="143" t="s">
         <v>815</v>
       </c>
     </row>
@@ -23959,10 +23946,10 @@
       <c r="A2" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B2" s="144" t="s">
+      <c r="B2" s="143" t="s">
         <v>816</v>
       </c>
-      <c r="C2" s="144" t="n">
+      <c r="C2" s="143" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -23970,10 +23957,10 @@
       <c r="A3" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="144" t="s">
+      <c r="B3" s="143" t="s">
         <v>817</v>
       </c>
-      <c r="C3" s="144" t="n">
+      <c r="C3" s="143" t="n">
         <v>0.0004</v>
       </c>
     </row>
@@ -24077,7 +24064,7 @@
       <c r="B16" s="0" t="s">
         <v>832</v>
       </c>
-      <c r="C16" s="143" t="n">
+      <c r="C16" s="142" t="n">
         <v>3.71179E-009</v>
       </c>
     </row>
@@ -24085,7 +24072,7 @@
       <c r="B17" s="0" t="s">
         <v>833</v>
       </c>
-      <c r="C17" s="143" t="n">
+      <c r="C17" s="142" t="n">
         <v>3.71272E-009</v>
       </c>
     </row>
@@ -24093,7 +24080,7 @@
       <c r="B18" s="0" t="s">
         <v>834</v>
       </c>
-      <c r="C18" s="143" t="n">
+      <c r="C18" s="142" t="n">
         <v>3.71425E-009</v>
       </c>
     </row>
@@ -24101,7 +24088,7 @@
       <c r="B19" s="0" t="s">
         <v>835</v>
       </c>
-      <c r="C19" s="143" t="n">
+      <c r="C19" s="142" t="n">
         <v>3.71562E-009</v>
       </c>
     </row>
@@ -24589,7 +24576,7 @@
       <c r="B80" s="0" t="s">
         <v>903</v>
       </c>
-      <c r="C80" s="143" t="n">
+      <c r="C80" s="142" t="n">
         <v>1.58855E-007</v>
       </c>
     </row>
@@ -24637,7 +24624,7 @@
       <c r="B86" s="0" t="s">
         <v>909</v>
       </c>
-      <c r="C86" s="143" t="n">
+      <c r="C86" s="142" t="n">
         <v>1.58316E-007</v>
       </c>
     </row>
@@ -24669,7 +24656,7 @@
       <c r="B90" s="0" t="s">
         <v>913</v>
       </c>
-      <c r="C90" s="143" t="n">
+      <c r="C90" s="142" t="n">
         <v>1.57838E-007</v>
       </c>
     </row>
@@ -24757,7 +24744,7 @@
       <c r="B101" s="0" t="s">
         <v>925</v>
       </c>
-      <c r="C101" s="143" t="n">
+      <c r="C101" s="142" t="n">
         <v>2.397E-009</v>
       </c>
     </row>
@@ -24933,7 +24920,7 @@
       <c r="B123" s="0" t="s">
         <v>949</v>
       </c>
-      <c r="C123" s="143" t="n">
+      <c r="C123" s="142" t="n">
         <v>2.37898E-010</v>
       </c>
     </row>
@@ -24997,7 +24984,7 @@
       <c r="B131" s="0" t="s">
         <v>957</v>
       </c>
-      <c r="C131" s="143" t="n">
+      <c r="C131" s="142" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -25013,7 +25000,7 @@
       <c r="B133" s="0" t="s">
         <v>959</v>
       </c>
-      <c r="C133" s="143" t="n">
+      <c r="C133" s="142" t="n">
         <v>1.97895E-005</v>
       </c>
     </row>
@@ -25533,7 +25520,7 @@
       <c r="B198" s="0" t="s">
         <v>1026</v>
       </c>
-      <c r="C198" s="143" t="n">
+      <c r="C198" s="142" t="n">
         <v>2.78422E-007</v>
       </c>
     </row>
@@ -25581,7 +25568,7 @@
       <c r="B204" s="0" t="s">
         <v>1032</v>
       </c>
-      <c r="C204" s="143" t="n">
+      <c r="C204" s="142" t="n">
         <v>2.77565E-007</v>
       </c>
     </row>
@@ -25613,7 +25600,7 @@
       <c r="B208" s="0" t="s">
         <v>1036</v>
       </c>
-      <c r="C208" s="143" t="n">
+      <c r="C208" s="142" t="n">
         <v>2.76716E-007</v>
       </c>
     </row>
@@ -25701,7 +25688,7 @@
       <c r="B219" s="0" t="s">
         <v>1047</v>
       </c>
-      <c r="C219" s="143" t="n">
+      <c r="C219" s="142" t="n">
         <v>5.98328E-009</v>
       </c>
     </row>
@@ -25877,7 +25864,7 @@
       <c r="B241" s="0" t="s">
         <v>1070</v>
       </c>
-      <c r="C241" s="143" t="n">
+      <c r="C241" s="142" t="n">
         <v>4.11728E-010</v>
       </c>
     </row>
@@ -25941,7 +25928,7 @@
       <c r="B249" s="0" t="s">
         <v>1078</v>
       </c>
-      <c r="C249" s="143" t="n">
+      <c r="C249" s="142" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -25957,7 +25944,7 @@
       <c r="B251" s="0" t="s">
         <v>1080</v>
       </c>
-      <c r="C251" s="143" t="n">
+      <c r="C251" s="142" t="n">
         <v>3.46956E-005</v>
       </c>
     </row>
@@ -26477,7 +26464,7 @@
       <c r="B316" s="0" t="s">
         <v>1145</v>
       </c>
-      <c r="C316" s="143" t="n">
+      <c r="C316" s="142" t="n">
         <v>5.45673E-012</v>
       </c>
     </row>
@@ -26525,7 +26512,7 @@
       <c r="B322" s="0" t="s">
         <v>1151</v>
       </c>
-      <c r="C322" s="143" t="n">
+      <c r="C322" s="142" t="n">
         <v>7.71713E-013</v>
       </c>
     </row>
@@ -26557,7 +26544,7 @@
       <c r="B326" s="0" t="s">
         <v>1155</v>
       </c>
-      <c r="C326" s="143" t="n">
+      <c r="C326" s="142" t="n">
         <v>-7.72781E-012</v>
       </c>
     </row>
@@ -26645,7 +26632,7 @@
       <c r="B337" s="0" t="s">
         <v>1166</v>
       </c>
-      <c r="C337" s="143" t="n">
+      <c r="C337" s="142" t="n">
         <v>5.61762E-010</v>
       </c>
     </row>
@@ -26821,7 +26808,7 @@
       <c r="B359" s="0" t="s">
         <v>1189</v>
       </c>
-      <c r="C359" s="143" t="n">
+      <c r="C359" s="142" t="n">
         <v>2.605E-012</v>
       </c>
     </row>
@@ -26885,7 +26872,7 @@
       <c r="B367" s="0" t="s">
         <v>1197</v>
       </c>
-      <c r="C367" s="143" t="n">
+      <c r="C367" s="142" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -26901,7 +26888,7 @@
       <c r="B369" s="0" t="s">
         <v>1199</v>
       </c>
-      <c r="C369" s="143" t="n">
+      <c r="C369" s="142" t="n">
         <v>9.64642E-011</v>
       </c>
     </row>
@@ -27421,7 +27408,7 @@
       <c r="B434" s="0" t="s">
         <v>1264</v>
       </c>
-      <c r="C434" s="143" t="n">
+      <c r="C434" s="142" t="n">
         <v>5.42202E-012</v>
       </c>
     </row>
@@ -27469,7 +27456,7 @@
       <c r="B440" s="0" t="s">
         <v>1270</v>
       </c>
-      <c r="C440" s="143" t="n">
+      <c r="C440" s="142" t="n">
         <v>5.83458E-013</v>
       </c>
     </row>
@@ -27501,7 +27488,7 @@
       <c r="B444" s="0" t="s">
         <v>1274</v>
       </c>
-      <c r="C444" s="143" t="n">
+      <c r="C444" s="142" t="n">
         <v>-5.09224E-012</v>
       </c>
     </row>
@@ -27589,7 +27576,7 @@
       <c r="B455" s="0" t="s">
         <v>1285</v>
       </c>
-      <c r="C455" s="143" t="n">
+      <c r="C455" s="142" t="n">
         <v>2.08783E-010</v>
       </c>
     </row>
@@ -27765,7 +27752,7 @@
       <c r="B477" s="0" t="s">
         <v>1308</v>
       </c>
-      <c r="C477" s="143" t="n">
+      <c r="C477" s="142" t="n">
         <v>2.32565E-012</v>
       </c>
     </row>
@@ -27829,7 +27816,7 @@
       <c r="B485" s="0" t="s">
         <v>1316</v>
       </c>
-      <c r="C485" s="143" t="n">
+      <c r="C485" s="142" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -27845,7 +27832,7 @@
       <c r="B487" s="0" t="s">
         <v>1318</v>
       </c>
-      <c r="C487" s="143" t="n">
+      <c r="C487" s="142" t="n">
         <v>7.29322E-011</v>
       </c>
     </row>
@@ -27933,7 +27920,7 @@
       <c r="B498" s="0" t="s">
         <v>1329</v>
       </c>
-      <c r="C498" s="143" t="n">
+      <c r="C498" s="142" t="n">
         <v>3.71179E-009</v>
       </c>
     </row>
@@ -27941,7 +27928,7 @@
       <c r="B499" s="0" t="s">
         <v>1330</v>
       </c>
-      <c r="C499" s="143" t="n">
+      <c r="C499" s="142" t="n">
         <v>3.71272E-009</v>
       </c>
     </row>
@@ -27949,7 +27936,7 @@
       <c r="B500" s="0" t="s">
         <v>1331</v>
       </c>
-      <c r="C500" s="143" t="n">
+      <c r="C500" s="142" t="n">
         <v>3.71425E-009</v>
       </c>
     </row>
@@ -27957,7 +27944,7 @@
       <c r="B501" s="0" t="s">
         <v>1332</v>
       </c>
-      <c r="C501" s="143" t="n">
+      <c r="C501" s="142" t="n">
         <v>3.71562E-009</v>
       </c>
     </row>
@@ -28525,7 +28512,7 @@
       <c r="B572" s="0" t="s">
         <v>1403</v>
       </c>
-      <c r="C572" s="143" t="n">
+      <c r="C572" s="142" t="n">
         <v>1.19678E-007</v>
       </c>
     </row>
@@ -28573,7 +28560,7 @@
       <c r="B578" s="0" t="s">
         <v>1409</v>
       </c>
-      <c r="C578" s="143" t="n">
+      <c r="C578" s="142" t="n">
         <v>1.19249E-007</v>
       </c>
     </row>
@@ -28605,7 +28592,7 @@
       <c r="B582" s="0" t="s">
         <v>1413</v>
       </c>
-      <c r="C582" s="143" t="n">
+      <c r="C582" s="142" t="n">
         <v>1.18808E-007</v>
       </c>
     </row>
@@ -28693,7 +28680,7 @@
       <c r="B593" s="0" t="s">
         <v>1424</v>
       </c>
-      <c r="C593" s="143" t="n">
+      <c r="C593" s="142" t="n">
         <v>3.58628E-009</v>
       </c>
     </row>
@@ -28869,7 +28856,7 @@
       <c r="B615" s="0" t="s">
         <v>1447</v>
       </c>
-      <c r="C615" s="143" t="n">
+      <c r="C615" s="142" t="n">
         <v>1.9029E-010</v>
       </c>
     </row>
@@ -28933,7 +28920,7 @@
       <c r="B623" s="0" t="s">
         <v>1455</v>
       </c>
-      <c r="C623" s="143" t="n">
+      <c r="C623" s="142" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -28949,7 +28936,7 @@
       <c r="B625" s="0" t="s">
         <v>1457</v>
       </c>
-      <c r="C625" s="143" t="n">
+      <c r="C625" s="142" t="n">
         <v>1.49062E-005</v>
       </c>
     </row>
@@ -29469,7 +29456,7 @@
       <c r="B690" s="0" t="s">
         <v>1522</v>
       </c>
-      <c r="C690" s="143" t="n">
+      <c r="C690" s="142" t="n">
         <v>5.80654E-012</v>
       </c>
     </row>
@@ -29517,7 +29504,7 @@
       <c r="B696" s="0" t="s">
         <v>1528</v>
       </c>
-      <c r="C696" s="143" t="n">
+      <c r="C696" s="142" t="n">
         <v>-1.88255E-013</v>
       </c>
     </row>
@@ -29549,7 +29536,7 @@
       <c r="B700" s="0" t="s">
         <v>1532</v>
       </c>
-      <c r="C700" s="143" t="n">
+      <c r="C700" s="142" t="n">
         <v>-6.71043E-012</v>
       </c>
     </row>
@@ -29637,7 +29624,7 @@
       <c r="B711" s="0" t="s">
         <v>1543</v>
       </c>
-      <c r="C711" s="143" t="n">
+      <c r="C711" s="142" t="n">
         <v>-3.52979E-010</v>
       </c>
     </row>
@@ -29813,7 +29800,7 @@
       <c r="B733" s="0" t="s">
         <v>1566</v>
       </c>
-      <c r="C733" s="143" t="n">
+      <c r="C733" s="142" t="n">
         <v>2.64443E-012</v>
       </c>
     </row>
@@ -29877,7 +29864,7 @@
       <c r="B741" s="0" t="s">
         <v>1574</v>
       </c>
-      <c r="C741" s="143" t="n">
+      <c r="C741" s="142" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -29893,7 +29880,7 @@
       <c r="B743" s="0" t="s">
         <v>1576</v>
       </c>
-      <c r="C743" s="143" t="n">
+      <c r="C743" s="142" t="n">
         <v>-2.35319E-011</v>
       </c>
     </row>
@@ -30449,7 +30436,7 @@
       <c r="B811" s="0" t="s">
         <v>1652</v>
       </c>
-      <c r="C811" s="143" t="n">
+      <c r="C811" s="142" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -30965,7 +30952,7 @@
       <c r="B874" s="0" t="s">
         <v>1717</v>
       </c>
-      <c r="C874" s="143" t="n">
+      <c r="C874" s="142" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -31481,7 +31468,7 @@
       <c r="B937" s="0" t="s">
         <v>1782</v>
       </c>
-      <c r="C937" s="143" t="n">
+      <c r="C937" s="142" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -31997,7 +31984,7 @@
       <c r="B1000" s="0" t="s">
         <v>1847</v>
       </c>
-      <c r="C1000" s="143" t="n">
+      <c r="C1000" s="142" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -32513,7 +32500,7 @@
       <c r="B1063" s="0" t="s">
         <v>1912</v>
       </c>
-      <c r="C1063" s="143" t="n">
+      <c r="C1063" s="142" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -33029,7 +33016,7 @@
       <c r="B1126" s="0" t="s">
         <v>1977</v>
       </c>
-      <c r="C1126" s="143" t="n">
+      <c r="C1126" s="142" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -33545,7 +33532,7 @@
       <c r="B1189" s="0" t="s">
         <v>2042</v>
       </c>
-      <c r="C1189" s="143" t="n">
+      <c r="C1189" s="142" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -34061,7 +34048,7 @@
       <c r="B1252" s="0" t="s">
         <v>2107</v>
       </c>
-      <c r="C1252" s="143" t="n">
+      <c r="C1252" s="142" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -34577,7 +34564,7 @@
       <c r="B1315" s="0" t="s">
         <v>2172</v>
       </c>
-      <c r="C1315" s="143" t="n">
+      <c r="C1315" s="142" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -35093,7 +35080,7 @@
       <c r="B1378" s="0" t="s">
         <v>2237</v>
       </c>
-      <c r="C1378" s="143" t="n">
+      <c r="C1378" s="142" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -35609,7 +35596,7 @@
       <c r="B1441" s="0" t="s">
         <v>2302</v>
       </c>
-      <c r="C1441" s="143" t="n">
+      <c r="C1441" s="142" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -36057,7 +36044,7 @@
       <c r="B1497" s="0" t="s">
         <v>2361</v>
       </c>
-      <c r="C1497" s="143" t="n">
+      <c r="C1497" s="142" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -36683,7 +36670,7 @@
       <c r="B1576" s="0" t="s">
         <v>2445</v>
       </c>
-      <c r="C1576" s="143" t="n">
+      <c r="C1576" s="142" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -36852,7 +36839,7 @@
       <c r="B1596" s="0" t="s">
         <v>2467</v>
       </c>
-      <c r="C1596" s="143" t="n">
+      <c r="C1596" s="142" t="n">
         <v>1000000</v>
       </c>
     </row>
@@ -36860,7 +36847,7 @@
       <c r="B1597" s="0" t="s">
         <v>2468</v>
       </c>
-      <c r="C1597" s="143" t="n">
+      <c r="C1597" s="142" t="n">
         <v>1000000</v>
       </c>
     </row>
@@ -37740,7 +37727,7 @@
       <c r="B1707" s="0" t="s">
         <v>2579</v>
       </c>
-      <c r="C1707" s="143" t="n">
+      <c r="C1707" s="142" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -37756,7 +37743,7 @@
       <c r="B1709" s="0" t="s">
         <v>2581</v>
       </c>
-      <c r="C1709" s="143" t="n">
+      <c r="C1709" s="142" t="n">
         <v>34197800</v>
       </c>
     </row>
@@ -38276,7 +38263,7 @@
       <c r="B1774" s="0" t="s">
         <v>2646</v>
       </c>
-      <c r="C1774" s="143" t="n">
+      <c r="C1774" s="142" t="n">
         <v>12147700</v>
       </c>
     </row>
@@ -38356,7 +38343,7 @@
       <c r="B1784" s="0" t="s">
         <v>2656</v>
       </c>
-      <c r="C1784" s="143" t="n">
+      <c r="C1784" s="142" t="n">
         <v>-7098040</v>
       </c>
     </row>
@@ -38444,7 +38431,7 @@
       <c r="B1795" s="0" t="s">
         <v>2667</v>
       </c>
-      <c r="C1795" s="143" t="n">
+      <c r="C1795" s="142" t="n">
         <v>4465690</v>
       </c>
     </row>
@@ -38620,7 +38607,7 @@
       <c r="B1817" s="0" t="s">
         <v>2690</v>
       </c>
-      <c r="C1817" s="143" t="n">
+      <c r="C1817" s="142" t="n">
         <v>1999640</v>
       </c>
     </row>
@@ -38684,7 +38671,7 @@
       <c r="B1825" s="0" t="s">
         <v>2698</v>
       </c>
-      <c r="C1825" s="143" t="n">
+      <c r="C1825" s="142" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -38700,7 +38687,7 @@
       <c r="B1827" s="0" t="s">
         <v>2700</v>
       </c>
-      <c r="C1827" s="143" t="n">
+      <c r="C1827" s="142" t="n">
         <v>-13532400</v>
       </c>
     </row>
@@ -39303,7 +39290,7 @@
       <c r="B1902" s="0" t="s">
         <v>2777</v>
       </c>
-      <c r="C1902" s="143" t="n">
+      <c r="C1902" s="142" t="n">
         <v>4.37265E-007</v>
       </c>
     </row>
@@ -39351,7 +39338,7 @@
       <c r="B1908" s="0" t="s">
         <v>2783</v>
       </c>
-      <c r="C1908" s="143" t="n">
+      <c r="C1908" s="142" t="n">
         <v>4.35882E-007</v>
       </c>
     </row>
@@ -39383,7 +39370,7 @@
       <c r="B1912" s="0" t="s">
         <v>2787</v>
       </c>
-      <c r="C1912" s="143" t="n">
+      <c r="C1912" s="142" t="n">
         <v>4.34577E-007</v>
       </c>
     </row>
@@ -39471,7 +39458,7 @@
       <c r="B1923" s="0" t="s">
         <v>2798</v>
       </c>
-      <c r="C1923" s="143" t="n">
+      <c r="C1923" s="142" t="n">
         <v>9.15083E-009</v>
       </c>
     </row>
@@ -39647,7 +39634,7 @@
       <c r="B1945" s="0" t="s">
         <v>2821</v>
       </c>
-      <c r="C1945" s="143" t="n">
+      <c r="C1945" s="142" t="n">
         <v>6.45121E-010</v>
       </c>
     </row>
@@ -39711,7 +39698,7 @@
       <c r="B1953" s="0" t="s">
         <v>2829</v>
       </c>
-      <c r="C1953" s="143" t="n">
+      <c r="C1953" s="142" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -39727,7 +39714,7 @@
       <c r="B1955" s="0" t="s">
         <v>2831</v>
       </c>
-      <c r="C1955" s="143" t="n">
+      <c r="C1955" s="142" t="n">
         <v>5.44853E-005</v>
       </c>
     </row>
@@ -40247,7 +40234,7 @@
       <c r="B2020" s="0" t="s">
         <v>2896</v>
       </c>
-      <c r="C2020" s="143" t="n">
+      <c r="C2020" s="142" t="n">
         <v>4.37266E-007</v>
       </c>
     </row>
@@ -40295,7 +40282,7 @@
       <c r="B2026" s="0" t="s">
         <v>2902</v>
       </c>
-      <c r="C2026" s="143" t="n">
+      <c r="C2026" s="142" t="n">
         <v>4.35881E-007</v>
       </c>
     </row>
@@ -40327,7 +40314,7 @@
       <c r="B2030" s="0" t="s">
         <v>2906</v>
       </c>
-      <c r="C2030" s="143" t="n">
+      <c r="C2030" s="142" t="n">
         <v>4.34576E-007</v>
       </c>
     </row>
@@ -40415,7 +40402,7 @@
       <c r="B2041" s="0" t="s">
         <v>2917</v>
       </c>
-      <c r="C2041" s="143" t="n">
+      <c r="C2041" s="142" t="n">
         <v>8.38028E-009</v>
       </c>
     </row>
@@ -40591,7 +40578,7 @@
       <c r="B2063" s="0" t="s">
         <v>2940</v>
       </c>
-      <c r="C2063" s="143" t="n">
+      <c r="C2063" s="142" t="n">
         <v>6.44996E-010</v>
       </c>
     </row>
@@ -40655,7 +40642,7 @@
       <c r="B2071" s="0" t="s">
         <v>2948</v>
       </c>
-      <c r="C2071" s="143" t="n">
+      <c r="C2071" s="142" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -40671,7 +40658,7 @@
       <c r="B2073" s="0" t="s">
         <v>2950</v>
       </c>
-      <c r="C2073" s="143" t="n">
+      <c r="C2073" s="142" t="n">
         <v>5.44851E-005</v>
       </c>
     </row>
@@ -41191,7 +41178,7 @@
       <c r="B2138" s="0" t="s">
         <v>3015</v>
       </c>
-      <c r="C2138" s="143" t="n">
+      <c r="C2138" s="142" t="n">
         <v>1.0545E-011</v>
       </c>
     </row>
@@ -41239,7 +41226,7 @@
       <c r="B2144" s="0" t="s">
         <v>3021</v>
       </c>
-      <c r="C2144" s="143" t="n">
+      <c r="C2144" s="142" t="n">
         <v>1.35517E-012</v>
       </c>
     </row>
@@ -41271,7 +41258,7 @@
       <c r="B2148" s="0" t="s">
         <v>3025</v>
       </c>
-      <c r="C2148" s="143" t="n">
+      <c r="C2148" s="142" t="n">
         <v>-1.06504E-011</v>
       </c>
     </row>
@@ -41359,7 +41346,7 @@
       <c r="B2159" s="0" t="s">
         <v>3036</v>
       </c>
-      <c r="C2159" s="143" t="n">
+      <c r="C2159" s="142" t="n">
         <v>7.70545E-010</v>
       </c>
     </row>
@@ -41535,7 +41522,7 @@
       <c r="B2181" s="0" t="s">
         <v>3059</v>
       </c>
-      <c r="C2181" s="143" t="n">
+      <c r="C2181" s="142" t="n">
         <v>4.1709E-012</v>
       </c>
     </row>
@@ -41599,7 +41586,7 @@
       <c r="B2189" s="0" t="s">
         <v>3067</v>
       </c>
-      <c r="C2189" s="143" t="n">
+      <c r="C2189" s="142" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -41615,7 +41602,7 @@
       <c r="B2191" s="0" t="s">
         <v>3069</v>
       </c>
-      <c r="C2191" s="143" t="n">
+      <c r="C2191" s="142" t="n">
         <v>1.69396E-010</v>
       </c>
     </row>
@@ -42191,7 +42178,7 @@
       <c r="B2263" s="0" t="s">
         <v>3144</v>
       </c>
-      <c r="C2263" s="143" t="n">
+      <c r="C2263" s="142" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -42478,7 +42465,7 @@
       <c r="F2297" s="0" t="s">
         <v>3189</v>
       </c>
-      <c r="G2297" s="145" t="n">
+      <c r="G2297" s="144" t="n">
         <v>41244</v>
       </c>
     </row>
@@ -42570,7 +42557,7 @@
       <c r="B2307" s="0" t="s">
         <v>3203</v>
       </c>
-      <c r="C2307" s="143" t="n">
+      <c r="C2307" s="142" t="n">
         <v>878236000</v>
       </c>
     </row>
@@ -42656,7 +42643,7 @@
       <c r="B2317" s="0" t="s">
         <v>3219</v>
       </c>
-      <c r="C2317" s="143" t="n">
+      <c r="C2317" s="142" t="n">
         <v>32640100000</v>
       </c>
     </row>
@@ -42664,7 +42651,7 @@
       <c r="B2318" s="0" t="s">
         <v>3220</v>
       </c>
-      <c r="C2318" s="143" t="n">
+      <c r="C2318" s="142" t="n">
         <v>33683000000</v>
       </c>
     </row>
@@ -42680,7 +42667,7 @@
       <c r="B2320" s="0" t="s">
         <v>3222</v>
       </c>
-      <c r="C2320" s="143" t="n">
+      <c r="C2320" s="142" t="n">
         <v>30883800</v>
       </c>
     </row>
@@ -42728,7 +42715,7 @@
       <c r="C2326" s="0" t="s">
         <v>3230</v>
       </c>
-      <c r="D2326" s="146" t="n">
+      <c r="D2326" s="145" t="n">
         <v>0.443159722222222</v>
       </c>
     </row>
@@ -42779,7 +42766,7 @@
       <c r="C2332" s="0" t="s">
         <v>3238</v>
       </c>
-      <c r="D2332" s="146" t="n">
+      <c r="D2332" s="145" t="n">
         <v>0.600474537037037</v>
       </c>
     </row>
@@ -42798,7 +42785,7 @@
       <c r="D2334" s="0" t="s">
         <v>3241</v>
       </c>
-      <c r="E2334" s="146" t="n">
+      <c r="E2334" s="145" t="n">
         <v>0.157314814814815</v>
       </c>
     </row>
@@ -42856,7 +42843,7 @@
       <c r="E2339" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="F2339" s="146" t="n">
+      <c r="F2339" s="145" t="n">
         <v>0.596990740740741</v>
       </c>
     </row>
@@ -43328,7 +43315,7 @@
       <c r="E2380" s="0" t="n">
         <v>26</v>
       </c>
-      <c r="F2380" s="146" t="n">
+      <c r="F2380" s="145" t="n">
         <v>0.443159722222222</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated look up table
</commit_message>
<xml_diff>
--- a/startup/lookup_table/Modes.xlsx
+++ b/startup/lookup_table/Modes.xlsx
@@ -11750,14 +11750,14 @@
   <dimension ref="A1:AMJ66"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="E30" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="E17" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
-      <selection pane="bottomRight" activeCell="E54" activeCellId="0" sqref="E54"/>
+      <selection pane="bottomLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+      <selection pane="bottomRight" activeCell="I58" activeCellId="0" sqref="I58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.04"/>
@@ -14716,7 +14716,7 @@
         <v>182</v>
       </c>
       <c r="E54" s="57" t="n">
-        <v>32.071</v>
+        <v>32.673</v>
       </c>
       <c r="F54" s="26" t="n">
         <v>276763</v>
@@ -14726,19 +14726,19 @@
       </c>
       <c r="H54" s="59"/>
       <c r="I54" s="60" t="n">
-        <v>-23.853</v>
+        <v>-24.656</v>
       </c>
       <c r="J54" s="28" t="n">
         <v>-268324</v>
       </c>
       <c r="K54" s="60" t="n">
-        <v>43.058</v>
+        <v>43.602</v>
       </c>
       <c r="L54" s="28" t="n">
         <v>387964</v>
       </c>
       <c r="M54" s="60" t="n">
-        <v>43.058</v>
+        <v>43.602</v>
       </c>
       <c r="N54" s="28" t="n">
         <v>394647</v>
@@ -14865,7 +14865,7 @@
         <v>189</v>
       </c>
       <c r="E56" s="57" t="n">
-        <v>116.887</v>
+        <v>116.501</v>
       </c>
       <c r="F56" s="25" t="n">
         <v>9251952</v>
@@ -14877,25 +14877,25 @@
         <v>4600216</v>
       </c>
       <c r="I56" s="57" t="n">
-        <v>56.009</v>
+        <v>54.346</v>
       </c>
       <c r="J56" s="23" t="n">
         <v>6151303</v>
       </c>
       <c r="K56" s="57" t="n">
-        <v>127.544</v>
+        <v>126.993</v>
       </c>
       <c r="L56" s="23" t="n">
         <v>9901395</v>
       </c>
       <c r="M56" s="57" t="n">
-        <v>127.735</v>
+        <v>127.056</v>
       </c>
       <c r="N56" s="23" t="n">
         <v>9901395</v>
       </c>
       <c r="O56" s="57" t="n">
-        <v>99.466</v>
+        <v>99.133</v>
       </c>
       <c r="P56" s="23" t="n">
         <v>8392750</v>
@@ -14927,7 +14927,7 @@
         <v>192</v>
       </c>
       <c r="E57" s="57" t="n">
-        <v>121.119</v>
+        <v>122.433</v>
       </c>
       <c r="F57" s="32" t="n">
         <v>6972005</v>
@@ -14939,25 +14939,25 @@
         <v>1551088</v>
       </c>
       <c r="I57" s="57" t="n">
-        <v>52.508</v>
+        <v>52.245</v>
       </c>
       <c r="J57" s="32" t="n">
         <v>3351899</v>
       </c>
       <c r="K57" s="57" t="n">
-        <v>131.814</v>
+        <v>132.648</v>
       </c>
       <c r="L57" s="32" t="n">
         <v>7552437</v>
       </c>
       <c r="M57" s="57" t="n">
-        <v>131.98</v>
+        <v>132.701</v>
       </c>
       <c r="N57" s="32" t="n">
         <v>7552437</v>
       </c>
       <c r="O57" s="57" t="n">
-        <v>100.436</v>
+        <v>101.303</v>
       </c>
       <c r="P57" s="32" t="n">
         <v>5879304</v>
@@ -14981,7 +14981,7 @@
         <v>195</v>
       </c>
       <c r="E58" s="57" t="n">
-        <v>121.119</v>
+        <v>122.433</v>
       </c>
       <c r="F58" s="28" t="n">
         <v>5572330</v>
@@ -14993,25 +14993,25 @@
         <v>354340</v>
       </c>
       <c r="I58" s="57" t="n">
-        <v>52.508</v>
+        <v>52.245</v>
       </c>
       <c r="J58" s="32" t="n">
         <v>1952224</v>
       </c>
       <c r="K58" s="57" t="n">
-        <v>131.814</v>
+        <v>132.648</v>
       </c>
       <c r="L58" s="32" t="n">
         <v>6355689</v>
       </c>
       <c r="M58" s="57" t="n">
-        <v>131.98</v>
+        <v>132.701</v>
       </c>
       <c r="N58" s="32" t="n">
         <v>6355689</v>
       </c>
       <c r="O58" s="57" t="n">
-        <v>100.436</v>
+        <v>101.303</v>
       </c>
       <c r="P58" s="65" t="n">
         <v>4479629</v>
@@ -15518,7 +15518,7 @@
   <dimension ref="A1:AMJ31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
+      <selection pane="topLeft" activeCell="D28" activeCellId="1" sqref="I58 D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16915,7 +16915,7 @@
       </c>
       <c r="F24" s="103" t="n">
         <f aca="false">'Modes A-F'!E54</f>
-        <v>32.071</v>
+        <v>32.673</v>
       </c>
       <c r="G24" s="0"/>
       <c r="H24" s="82" t="s">
@@ -16961,7 +16961,7 @@
       </c>
       <c r="F26" s="103" t="n">
         <f aca="false">'Modes A-F'!I54</f>
-        <v>-23.853</v>
+        <v>-24.656</v>
       </c>
       <c r="G26" s="0"/>
       <c r="H26" s="82" t="s">
@@ -16984,7 +16984,7 @@
       </c>
       <c r="F27" s="103" t="n">
         <f aca="false">'Modes A-F'!K54</f>
-        <v>43.058</v>
+        <v>43.602</v>
       </c>
       <c r="G27" s="0"/>
       <c r="H27" s="0"/>
@@ -17003,7 +17003,7 @@
       </c>
       <c r="F28" s="103" t="n">
         <f aca="false">'Modes A-F'!M54</f>
-        <v>43.058</v>
+        <v>43.602</v>
       </c>
       <c r="G28" s="0"/>
       <c r="H28" s="0"/>
@@ -17092,10 +17092,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G11" activeCellId="0" sqref="G11"/>
+      <selection pane="bottomRight" activeCell="G11" activeCellId="1" sqref="I58 G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33"/>
@@ -17274,10 +17274,10 @@
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+      <selection pane="topLeft" activeCell="E4" activeCellId="1" sqref="I58 E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.36"/>
@@ -17356,19 +17356,19 @@
       </c>
       <c r="E4" s="103" t="n">
         <f aca="false">'Modes A-F'!K56</f>
-        <v>127.544</v>
+        <v>126.993</v>
       </c>
       <c r="F4" s="103" t="n">
         <f aca="false">E4-B4*TAN(2*(F2-E2)/1000)</f>
-        <v>98.6329132666878</v>
+        <v>98.0819132666877</v>
       </c>
       <c r="G4" s="121" t="n">
         <f aca="false">'Modes A-F'!O56</f>
-        <v>99.466</v>
+        <v>99.133</v>
       </c>
       <c r="H4" s="122" t="n">
         <f aca="false">G4-F4</f>
-        <v>0.833086733312243</v>
+        <v>1.05108673331225</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17385,25 +17385,25 @@
       </c>
       <c r="E5" s="126" t="n">
         <f aca="false">'Modes A-F'!K57</f>
-        <v>131.814</v>
+        <v>132.648</v>
       </c>
       <c r="F5" s="126" t="n">
         <f aca="false">E5-B5*TAN(2*(F2-E2)/1000)</f>
-        <v>99.4379028716503</v>
+        <v>100.27190287165</v>
       </c>
       <c r="G5" s="127" t="n">
         <f aca="false">'Modes A-F'!O57</f>
-        <v>100.436</v>
+        <v>101.303</v>
       </c>
       <c r="H5" s="122" t="n">
         <f aca="false">G5-F5</f>
-        <v>0.998097128349684</v>
+        <v>1.03109712834967</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H6" s="122" t="n">
         <f aca="false">AVERAGE(H3,H4,H5)</f>
-        <v>-0.10297837334879</v>
+        <v>-0.0193117066821276</v>
       </c>
       <c r="I6" s="0" t="s">
         <v>274</v>
@@ -17449,12 +17449,12 @@
       </c>
       <c r="E10" s="122" t="n">
         <f aca="false">'Modes A-F'!E54</f>
-        <v>32.071</v>
+        <v>32.673</v>
       </c>
       <c r="F10" s="122"/>
       <c r="G10" s="131" t="n">
         <f aca="false">E10-B10*TAN(2*(G9-E9)/1000)</f>
-        <v>34.2524000290853</v>
+        <v>34.8544000290853</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17470,12 +17470,12 @@
       </c>
       <c r="E11" s="122" t="n">
         <f aca="false">'Modes A-F'!E57</f>
-        <v>121.119</v>
+        <v>122.433</v>
       </c>
       <c r="F11" s="122"/>
       <c r="G11" s="131" t="n">
         <f aca="false">E11-B11*TAN(2*(G9-E9)/1000)</f>
-        <v>123.427400030779</v>
+        <v>124.741400030779</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17492,12 +17492,12 @@
       </c>
       <c r="E12" s="132" t="n">
         <f aca="false">'Modes A-F'!E58</f>
-        <v>121.119</v>
+        <v>122.433</v>
       </c>
       <c r="F12" s="132"/>
       <c r="G12" s="133" t="n">
         <f aca="false">E12-B12*TAN(2*(G9-E9)/1000)</f>
-        <v>123.658400033859</v>
+        <v>124.972400033859</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17598,15 +17598,15 @@
       </c>
       <c r="E22" s="122" t="n">
         <f aca="false">E10-B22*TAN(2*(E19)/1000)+I17</f>
-        <v>-35.8953914229833</v>
+        <v>-35.2933914229833</v>
       </c>
       <c r="F22" s="137" t="n">
         <f aca="false">'Modes A-F'!I54</f>
-        <v>-23.853</v>
+        <v>-24.656</v>
       </c>
       <c r="G22" s="122" t="n">
         <f aca="false">E10-B22*TAN(2*(G19)/1000)+I17</f>
-        <v>-30.94402924884</v>
+        <v>-30.3420292488399</v>
       </c>
       <c r="I22" s="118"/>
     </row>
@@ -17623,15 +17623,15 @@
       </c>
       <c r="E23" s="122" t="n">
         <f aca="false">E11-B23*TAN(2*(E19)/1000)+I17</f>
-        <v>48.3582674801944</v>
+        <v>49.6722674801944</v>
       </c>
       <c r="F23" s="137" t="n">
         <f aca="false">'Modes A-F'!I56</f>
-        <v>56.009</v>
+        <v>54.346</v>
       </c>
       <c r="G23" s="122" t="n">
         <f aca="false">E11-B23*TAN(2*(G19)/1000)+I17</f>
-        <v>53.6588981480704</v>
+        <v>54.9728981480704</v>
       </c>
       <c r="I23" s="118"/>
     </row>
@@ -17649,15 +17649,15 @@
       </c>
       <c r="E24" s="132" t="n">
         <f aca="false">E12-B24*TAN(2*(E19)/1000)+I17</f>
-        <v>39.6378517843995</v>
+        <v>40.9518517843995</v>
       </c>
       <c r="F24" s="138" t="n">
         <f aca="false">'Modes A-F'!I57</f>
-        <v>52.508</v>
+        <v>52.245</v>
       </c>
       <c r="G24" s="139" t="n">
         <f aca="false">E12-B24*TAN(2*(G19)/1000)+I17</f>
-        <v>45.573766090482</v>
+        <v>46.887766090482</v>
       </c>
       <c r="H24" s="124"/>
       <c r="I24" s="140"/>
@@ -17760,7 +17760,7 @@
       </c>
       <c r="E34" s="122" t="n">
         <f aca="false">E10-B34*TAN(2*(E31)/1000)</f>
-        <v>-62.9036236638297</v>
+        <v>-62.3016236638297</v>
       </c>
       <c r="F34" s="137" t="n">
         <f aca="false">'Modes A-F'!G54</f>
@@ -17768,7 +17768,7 @@
       </c>
       <c r="G34" s="122" t="n">
         <f aca="false">E10-B34*TAN(2*(G31)/1000)+I29</f>
-        <v>-57.9520007866982</v>
+        <v>-57.3500007866982</v>
       </c>
       <c r="I34" s="118"/>
     </row>
@@ -17785,7 +17785,7 @@
       </c>
       <c r="E35" s="122" t="n">
         <f aca="false">E11-B35*TAN(2*(E31)/1000)</f>
-        <v>19.4448777773465</v>
+        <v>20.7588777773465</v>
       </c>
       <c r="F35" s="137" t="n">
         <f aca="false">'Modes A-F'!G56</f>
@@ -17793,7 +17793,7 @@
       </c>
       <c r="G35" s="122" t="n">
         <f aca="false">E11-B35*TAN(2*(G31)/1000)+I29</f>
-        <v>24.7457875381681</v>
+        <v>26.0597875381681</v>
       </c>
       <c r="I35" s="118"/>
     </row>
@@ -17811,7 +17811,7 @@
       </c>
       <c r="E36" s="132" t="n">
         <f aca="false">E12-B36*TAN(2*(E31)/1000)</f>
-        <v>7.25917567428903</v>
+        <v>8.57317567428903</v>
       </c>
       <c r="F36" s="138" t="n">
         <f aca="false">'Modes A-F'!G57</f>
@@ -17819,7 +17819,7 @@
       </c>
       <c r="G36" s="132" t="n">
         <f aca="false">E12-B36*TAN(2*(G31)/1000)+I29</f>
-        <v>13.1954025227675</v>
+        <v>14.5094025227675</v>
       </c>
       <c r="H36" s="124"/>
       <c r="I36" s="140"/>
@@ -17848,10 +17848,10 @@
   <dimension ref="A1:CX484"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="I58 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.26"/>
   </cols>
@@ -23919,10 +23919,10 @@
   <dimension ref="A1:G2383"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A44" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="1" sqref="I58 B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="56.14"/>

</xml_diff>

<commit_message>
add to .gitignore, remove unneeded file, update Mode spreadsheet
</commit_message>
<xml_diff>
--- a/startup/lookup_table/Modes.xlsx
+++ b/startup/lookup_table/Modes.xlsx
@@ -11750,14 +11750,14 @@
   <dimension ref="A1:AMJ66"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="I35" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="E35" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="I1" activeCellId="0" sqref="I1"/>
+      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
-      <selection pane="bottomRight" activeCell="L55" activeCellId="0" sqref="L55"/>
+      <selection pane="bottomRight" activeCell="E54" activeCellId="0" sqref="E54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.04"/>
@@ -14716,7 +14716,7 @@
         <v>182</v>
       </c>
       <c r="E54" s="57" t="n">
-        <v>32.673</v>
+        <v>32.92</v>
       </c>
       <c r="F54" s="26" t="n">
         <v>276763</v>
@@ -16915,7 +16915,7 @@
       </c>
       <c r="F24" s="103" t="n">
         <f aca="false">'Modes A-F'!E54</f>
-        <v>32.673</v>
+        <v>32.92</v>
       </c>
       <c r="G24" s="0"/>
       <c r="H24" s="82" t="s">
@@ -17095,7 +17095,7 @@
       <selection pane="bottomRight" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33"/>
@@ -17277,7 +17277,7 @@
       <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.36"/>
@@ -17449,12 +17449,12 @@
       </c>
       <c r="E10" s="122" t="n">
         <f aca="false">'Modes A-F'!E54</f>
-        <v>32.673</v>
+        <v>32.92</v>
       </c>
       <c r="F10" s="122"/>
       <c r="G10" s="131" t="n">
         <f aca="false">E10-B10*TAN(2*(G9-E9)/1000)</f>
-        <v>34.8544000290853</v>
+        <v>35.1014000290853</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17598,7 +17598,7 @@
       </c>
       <c r="E22" s="122" t="n">
         <f aca="false">E10-B22*TAN(2*(E19)/1000)+I17</f>
-        <v>-35.2933914229833</v>
+        <v>-35.0463914229833</v>
       </c>
       <c r="F22" s="137" t="n">
         <f aca="false">'Modes A-F'!I54</f>
@@ -17606,7 +17606,7 @@
       </c>
       <c r="G22" s="122" t="n">
         <f aca="false">E10-B22*TAN(2*(G19)/1000)+I17</f>
-        <v>-30.3420292488399</v>
+        <v>-30.0950292488399</v>
       </c>
       <c r="I22" s="118"/>
     </row>
@@ -17760,7 +17760,7 @@
       </c>
       <c r="E34" s="122" t="n">
         <f aca="false">E10-B34*TAN(2*(E31)/1000)</f>
-        <v>-62.3016236638297</v>
+        <v>-62.0546236638297</v>
       </c>
       <c r="F34" s="137" t="n">
         <f aca="false">'Modes A-F'!G54</f>
@@ -17768,7 +17768,7 @@
       </c>
       <c r="G34" s="122" t="n">
         <f aca="false">E10-B34*TAN(2*(G31)/1000)+I29</f>
-        <v>-57.3500007866982</v>
+        <v>-57.1030007866982</v>
       </c>
       <c r="I34" s="118"/>
     </row>
@@ -17851,7 +17851,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.26"/>
   </cols>
@@ -23922,7 +23922,7 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="56.14"/>

</xml_diff>

<commit_message>
new calibration for 111 and 311, work on new IC integration
* try to deal better with DM3 amplifier faults
* simplify class inheritance in BMM/dwelltime
* shorter sleeps in recovery in modes.py
* attempt to avoid a common CLI mistake made by BR when callibrating mono
* define ION_CHAMBERS global and use it everywhere
* clean up detector configuration
* new xafs_ref positions
* fix column labels in xdi.py using ION_CHAMBERS
* live plot of I0 is not nanoamps (rather than nanoamp-seconds)
</commit_message>
<xml_diff>
--- a/startup/lookup_table/Modes.xlsx
+++ b/startup/lookup_table/Modes.xlsx
@@ -11750,14 +11750,14 @@
   <dimension ref="A1:AMJ66"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="E35" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="I14" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
-      <selection pane="bottomRight" activeCell="E54" activeCellId="0" sqref="E54"/>
+      <selection pane="topRight" activeCell="I1" activeCellId="0" sqref="I1"/>
+      <selection pane="bottomLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+      <selection pane="bottomRight" activeCell="U46" activeCellId="0" sqref="U46:U47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.04"/>
@@ -14204,10 +14204,10 @@
         <v>-86467</v>
       </c>
       <c r="T46" s="31" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="U46" s="32" t="n">
-        <v>132229</v>
+        <v>73535</v>
       </c>
     </row>
     <row r="47" s="35" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14261,10 +14261,10 @@
       <c r="R47" s="26"/>
       <c r="S47" s="26"/>
       <c r="T47" s="38" t="n">
-        <v>15.0002</v>
+        <v>8</v>
       </c>
       <c r="U47" s="45" t="n">
-        <v>114420</v>
+        <v>33084</v>
       </c>
       <c r="V47" s="0"/>
       <c r="W47" s="0"/>
@@ -15518,7 +15518,7 @@
   <dimension ref="A1:AMJ31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
+      <selection pane="topLeft" activeCell="D28" activeCellId="1" sqref="U46:U47 D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17092,10 +17092,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G11" activeCellId="0" sqref="G11"/>
+      <selection pane="bottomRight" activeCell="G11" activeCellId="1" sqref="U46:U47 G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33"/>
@@ -17274,15 +17274,14 @@
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+      <selection pane="topLeft" activeCell="E4" activeCellId="1" sqref="U46:U47 E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.18"/>
   </cols>
   <sheetData>
@@ -17848,10 +17847,10 @@
   <dimension ref="A1:CX484"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="U46:U47 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.26"/>
   </cols>
@@ -23919,10 +23918,10 @@
   <dimension ref="A1:G2383"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A44" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="1" sqref="U46:U47 B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="56.14"/>

</xml_diff>

<commit_message>
* update Modes.xlsx and calibration of both monos
also:
+ correct shape of new usbcam2
+ fully resolved files for kafka args in DossierTools cameras
+ uncomment usbcam2
+ fix several folder/workspace confusions
+ s/close_last_plot/close_plots in macros
+ adjustable slit height in rocking curve
+ screen position of live triplot for new, larger monitors
+ bmm_live XRF plot, check for "XDI" in startdoc
</commit_message>
<xml_diff>
--- a/startup/lookup_table/Modes.xlsx
+++ b/startup/lookup_table/Modes.xlsx
@@ -10783,6 +10783,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFD7"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor rgb="FFFFFFD7"/>
       </patternFill>
@@ -10791,12 +10797,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF3333"/>
         <bgColor rgb="FFFF6600"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFD7"/>
-        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
     <fill>
@@ -11314,19 +11314,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11750,14 +11750,14 @@
   <dimension ref="A1:AMJ66"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="G26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="E32" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
-      <selection pane="bottomRight" activeCell="K58" activeCellId="0" sqref="K58"/>
+      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
+      <selection pane="bottomRight" activeCell="E54" activeCellId="0" sqref="E54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.01953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.04"/>
@@ -14716,7 +14716,7 @@
         <v>182</v>
       </c>
       <c r="E54" s="57" t="n">
-        <v>32.92</v>
+        <v>36.018</v>
       </c>
       <c r="F54" s="26" t="n">
         <v>276763</v>
@@ -14725,32 +14725,32 @@
         <v>-55.188</v>
       </c>
       <c r="H54" s="59"/>
-      <c r="I54" s="60" t="n">
-        <v>-24.656</v>
+      <c r="I54" s="57" t="n">
+        <v>-22.645</v>
       </c>
       <c r="J54" s="28" t="n">
         <v>-268324</v>
       </c>
-      <c r="K54" s="60" t="n">
-        <v>43.404</v>
+      <c r="K54" s="57" t="n">
+        <v>45.66</v>
       </c>
       <c r="L54" s="28" t="n">
         <v>387964</v>
       </c>
-      <c r="M54" s="60" t="n">
-        <v>43.404</v>
+      <c r="M54" s="57" t="n">
+        <v>45.712</v>
       </c>
       <c r="N54" s="28" t="n">
         <v>394647</v>
       </c>
-      <c r="O54" s="60" t="n">
-        <v>16.963</v>
+      <c r="O54" s="57" t="n">
+        <v>19.46</v>
       </c>
       <c r="P54" s="28" t="n">
         <v>141529</v>
       </c>
-      <c r="T54" s="60" t="n">
-        <v>54.774</v>
+      <c r="T54" s="57" t="n">
+        <v>55.974</v>
       </c>
       <c r="U54" s="28" t="n">
         <v>497477</v>
@@ -14864,8 +14864,8 @@
       <c r="D56" s="20" t="s">
         <v>189</v>
       </c>
-      <c r="E56" s="57" t="n">
-        <v>116.501</v>
+      <c r="E56" s="60" t="n">
+        <v>118.101</v>
       </c>
       <c r="F56" s="25" t="n">
         <v>9251952</v>
@@ -14876,26 +14876,26 @@
       <c r="H56" s="62" t="n">
         <v>4600216</v>
       </c>
-      <c r="I56" s="57" t="n">
-        <v>54.346</v>
+      <c r="I56" s="60" t="n">
+        <v>53.596</v>
       </c>
       <c r="J56" s="23" t="n">
         <v>6151303</v>
       </c>
-      <c r="K56" s="57" t="n">
-        <v>126.3</v>
+      <c r="K56" s="60" t="n">
+        <v>126.5</v>
       </c>
       <c r="L56" s="23" t="n">
         <v>9901395</v>
       </c>
-      <c r="M56" s="57" t="n">
-        <v>127.056</v>
+      <c r="M56" s="60" t="n">
+        <v>126.584</v>
       </c>
       <c r="N56" s="23" t="n">
         <v>9901395</v>
       </c>
-      <c r="O56" s="57" t="n">
-        <v>99.133</v>
+      <c r="O56" s="60" t="n">
+        <v>98.835</v>
       </c>
       <c r="P56" s="23" t="n">
         <v>8392750</v>
@@ -14926,8 +14926,8 @@
       <c r="D57" s="0" t="s">
         <v>192</v>
       </c>
-      <c r="E57" s="57" t="n">
-        <v>122.433</v>
+      <c r="E57" s="60" t="n">
+        <v>128.533</v>
       </c>
       <c r="F57" s="32" t="n">
         <v>6972005</v>
@@ -14938,26 +14938,26 @@
       <c r="H57" s="64" t="n">
         <v>1551088</v>
       </c>
-      <c r="I57" s="57" t="n">
-        <v>52.245</v>
+      <c r="I57" s="60" t="n">
+        <v>51.995</v>
       </c>
       <c r="J57" s="32" t="n">
         <v>3351899</v>
       </c>
-      <c r="K57" s="57" t="n">
-        <v>133.398</v>
+      <c r="K57" s="60" t="n">
+        <v>133.6</v>
       </c>
       <c r="L57" s="32" t="n">
         <v>7552437</v>
       </c>
-      <c r="M57" s="57" t="n">
-        <v>132.701</v>
+      <c r="M57" s="60" t="n">
+        <v>133.016</v>
       </c>
       <c r="N57" s="32" t="n">
         <v>7552437</v>
       </c>
-      <c r="O57" s="57" t="n">
-        <v>101.303</v>
+      <c r="O57" s="60" t="n">
+        <v>105.267</v>
       </c>
       <c r="P57" s="32" t="n">
         <v>5879304</v>
@@ -14980,8 +14980,8 @@
       <c r="D58" s="26" t="s">
         <v>195</v>
       </c>
-      <c r="E58" s="57" t="n">
-        <v>122.433</v>
+      <c r="E58" s="60" t="n">
+        <v>128.533</v>
       </c>
       <c r="F58" s="28" t="n">
         <v>5572330</v>
@@ -14992,26 +14992,26 @@
       <c r="H58" s="64" t="n">
         <v>354340</v>
       </c>
-      <c r="I58" s="57" t="n">
-        <v>52.245</v>
+      <c r="I58" s="60" t="n">
+        <v>51.995</v>
       </c>
       <c r="J58" s="32" t="n">
         <v>1952224</v>
       </c>
-      <c r="K58" s="57" t="n">
-        <v>133.398</v>
+      <c r="K58" s="60" t="n">
+        <v>133.6</v>
       </c>
       <c r="L58" s="32" t="n">
         <v>6355689</v>
       </c>
-      <c r="M58" s="57" t="n">
-        <v>132.701</v>
+      <c r="M58" s="60" t="n">
+        <v>133.016</v>
       </c>
       <c r="N58" s="32" t="n">
         <v>6355689</v>
       </c>
-      <c r="O58" s="57" t="n">
-        <v>101.303</v>
+      <c r="O58" s="60" t="n">
+        <v>105.267</v>
       </c>
       <c r="P58" s="65" t="n">
         <v>4479629</v>
@@ -15518,7 +15518,7 @@
   <dimension ref="A1:AMJ31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D28" activeCellId="1" sqref="K58 D28"/>
+      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16915,7 +16915,7 @@
       </c>
       <c r="F24" s="103" t="n">
         <f aca="false">'Modes A-F'!E54</f>
-        <v>32.92</v>
+        <v>36.018</v>
       </c>
       <c r="G24" s="0"/>
       <c r="H24" s="82" t="s">
@@ -16961,7 +16961,7 @@
       </c>
       <c r="F26" s="103" t="n">
         <f aca="false">'Modes A-F'!I54</f>
-        <v>-24.656</v>
+        <v>-22.645</v>
       </c>
       <c r="G26" s="0"/>
       <c r="H26" s="82" t="s">
@@ -16984,7 +16984,7 @@
       </c>
       <c r="F27" s="103" t="n">
         <f aca="false">'Modes A-F'!K54</f>
-        <v>43.404</v>
+        <v>45.66</v>
       </c>
       <c r="G27" s="0"/>
       <c r="H27" s="0"/>
@@ -17003,7 +17003,7 @@
       </c>
       <c r="F28" s="103" t="n">
         <f aca="false">'Modes A-F'!M54</f>
-        <v>43.404</v>
+        <v>45.712</v>
       </c>
       <c r="G28" s="0"/>
       <c r="H28" s="0"/>
@@ -17022,7 +17022,7 @@
       </c>
       <c r="F29" s="103" t="n">
         <f aca="false">'Modes A-F'!O54</f>
-        <v>16.963</v>
+        <v>19.46</v>
       </c>
       <c r="G29" s="0"/>
       <c r="H29" s="0"/>
@@ -17041,7 +17041,7 @@
       </c>
       <c r="F30" s="103" t="n">
         <f aca="false">'Modes A-F'!T54</f>
-        <v>54.774</v>
+        <v>55.974</v>
       </c>
       <c r="G30" s="0"/>
       <c r="H30" s="0"/>
@@ -17092,10 +17092,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G11" activeCellId="1" sqref="K58 G11"/>
+      <selection pane="bottomRight" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33"/>
@@ -17276,10 +17276,10 @@
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="1" sqref="K58 E4"/>
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="11.96"/>
@@ -17340,11 +17340,11 @@
       </c>
       <c r="G3" s="121" t="n">
         <f aca="false">'Modes A-F'!O54</f>
-        <v>16.963</v>
+        <v>19.46</v>
       </c>
       <c r="H3" s="122" t="n">
         <f aca="false">G3-F3</f>
-        <v>-2.1401189817083</v>
+        <v>0.356881018291702</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17360,19 +17360,19 @@
       </c>
       <c r="E4" s="103" t="n">
         <f aca="false">'Modes A-F'!K56</f>
-        <v>126.3</v>
+        <v>126.5</v>
       </c>
       <c r="F4" s="103" t="n">
         <f aca="false">E4-B4*TAN(2*(F2-E2)/1000)</f>
-        <v>97.3889132666877</v>
+        <v>97.5889132666878</v>
       </c>
       <c r="G4" s="121" t="n">
         <f aca="false">'Modes A-F'!O56</f>
-        <v>99.133</v>
+        <v>98.835</v>
       </c>
       <c r="H4" s="122" t="n">
         <f aca="false">G4-F4</f>
-        <v>1.74408673331224</v>
+        <v>1.24608673331224</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17389,25 +17389,25 @@
       </c>
       <c r="E5" s="126" t="n">
         <f aca="false">'Modes A-F'!K57</f>
-        <v>133.398</v>
+        <v>133.6</v>
       </c>
       <c r="F5" s="126" t="n">
         <f aca="false">E5-B5*TAN(2*(F2-E2)/1000)</f>
-        <v>101.02190287165</v>
+        <v>101.22390287165</v>
       </c>
       <c r="G5" s="127" t="n">
         <f aca="false">'Modes A-F'!O57</f>
-        <v>101.303</v>
+        <v>105.267</v>
       </c>
       <c r="H5" s="122" t="n">
         <f aca="false">G5-F5</f>
-        <v>0.281097128349671</v>
+        <v>4.04309712834967</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H6" s="122" t="n">
         <f aca="false">AVERAGE(H3,H4,H5)</f>
-        <v>-0.0383117066821283</v>
+        <v>1.8820216266512</v>
       </c>
       <c r="I6" s="0" t="s">
         <v>274</v>
@@ -17453,12 +17453,12 @@
       </c>
       <c r="E10" s="122" t="n">
         <f aca="false">'Modes A-F'!E54</f>
-        <v>32.92</v>
+        <v>36.018</v>
       </c>
       <c r="F10" s="122"/>
       <c r="G10" s="131" t="n">
         <f aca="false">E10-B10*TAN(2*(G9-E9)/1000)</f>
-        <v>35.1014000290853</v>
+        <v>38.1994000290853</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17474,12 +17474,12 @@
       </c>
       <c r="E11" s="122" t="n">
         <f aca="false">'Modes A-F'!E57</f>
-        <v>122.433</v>
+        <v>128.533</v>
       </c>
       <c r="F11" s="122"/>
       <c r="G11" s="131" t="n">
         <f aca="false">E11-B11*TAN(2*(G9-E9)/1000)</f>
-        <v>124.741400030779</v>
+        <v>130.841400030779</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17496,12 +17496,12 @@
       </c>
       <c r="E12" s="132" t="n">
         <f aca="false">'Modes A-F'!E58</f>
-        <v>122.433</v>
+        <v>128.533</v>
       </c>
       <c r="F12" s="132"/>
       <c r="G12" s="133" t="n">
         <f aca="false">E12-B12*TAN(2*(G9-E9)/1000)</f>
-        <v>124.972400033859</v>
+        <v>131.072400033859</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17533,7 +17533,7 @@
         <f aca="false">E17+G16</f>
         <v>3.5</v>
       </c>
-      <c r="H17" s="57" t="s">
+      <c r="H17" s="60" t="s">
         <v>279</v>
       </c>
       <c r="I17" s="118" t="n">
@@ -17602,15 +17602,15 @@
       </c>
       <c r="E22" s="122" t="n">
         <f aca="false">E10-B22*TAN(2*(E19)/1000)+I17</f>
-        <v>-35.0463914229833</v>
+        <v>-31.9483914229833</v>
       </c>
       <c r="F22" s="137" t="n">
         <f aca="false">'Modes A-F'!I54</f>
-        <v>-24.656</v>
+        <v>-22.645</v>
       </c>
       <c r="G22" s="122" t="n">
         <f aca="false">E10-B22*TAN(2*(G19)/1000)+I17</f>
-        <v>-30.0950292488399</v>
+        <v>-26.9970292488399</v>
       </c>
       <c r="I22" s="118"/>
     </row>
@@ -17627,15 +17627,15 @@
       </c>
       <c r="E23" s="122" t="n">
         <f aca="false">E11-B23*TAN(2*(E19)/1000)+I17</f>
-        <v>49.6722674801944</v>
+        <v>55.7722674801944</v>
       </c>
       <c r="F23" s="137" t="n">
         <f aca="false">'Modes A-F'!I56</f>
-        <v>54.346</v>
+        <v>53.596</v>
       </c>
       <c r="G23" s="122" t="n">
         <f aca="false">E11-B23*TAN(2*(G19)/1000)+I17</f>
-        <v>54.9728981480704</v>
+        <v>61.0728981480704</v>
       </c>
       <c r="I23" s="118"/>
     </row>
@@ -17653,15 +17653,15 @@
       </c>
       <c r="E24" s="132" t="n">
         <f aca="false">E12-B24*TAN(2*(E19)/1000)+I17</f>
-        <v>40.9518517843995</v>
+        <v>47.0518517843995</v>
       </c>
       <c r="F24" s="138" t="n">
         <f aca="false">'Modes A-F'!I57</f>
-        <v>52.245</v>
+        <v>51.995</v>
       </c>
       <c r="G24" s="139" t="n">
         <f aca="false">E12-B24*TAN(2*(G19)/1000)+I17</f>
-        <v>46.887766090482</v>
+        <v>52.987766090482</v>
       </c>
       <c r="H24" s="124"/>
       <c r="I24" s="140"/>
@@ -17695,7 +17695,7 @@
         <f aca="false">E29+G28</f>
         <v>3.5</v>
       </c>
-      <c r="H29" s="57" t="s">
+      <c r="H29" s="60" t="s">
         <v>279</v>
       </c>
       <c r="I29" s="118" t="n">
@@ -17764,7 +17764,7 @@
       </c>
       <c r="E34" s="122" t="n">
         <f aca="false">E10-B34*TAN(2*(E31)/1000)</f>
-        <v>-62.0546236638297</v>
+        <v>-58.9566236638297</v>
       </c>
       <c r="F34" s="137" t="n">
         <f aca="false">'Modes A-F'!G54</f>
@@ -17772,7 +17772,7 @@
       </c>
       <c r="G34" s="122" t="n">
         <f aca="false">E10-B34*TAN(2*(G31)/1000)+I29</f>
-        <v>-57.1030007866982</v>
+        <v>-54.0050007866982</v>
       </c>
       <c r="I34" s="118"/>
     </row>
@@ -17789,7 +17789,7 @@
       </c>
       <c r="E35" s="122" t="n">
         <f aca="false">E11-B35*TAN(2*(E31)/1000)</f>
-        <v>20.7588777773465</v>
+        <v>26.8588777773465</v>
       </c>
       <c r="F35" s="137" t="n">
         <f aca="false">'Modes A-F'!G56</f>
@@ -17797,7 +17797,7 @@
       </c>
       <c r="G35" s="122" t="n">
         <f aca="false">E11-B35*TAN(2*(G31)/1000)+I29</f>
-        <v>26.0597875381681</v>
+        <v>32.1597875381681</v>
       </c>
       <c r="I35" s="118"/>
     </row>
@@ -17815,7 +17815,7 @@
       </c>
       <c r="E36" s="132" t="n">
         <f aca="false">E12-B36*TAN(2*(E31)/1000)</f>
-        <v>8.57317567428903</v>
+        <v>14.673175674289</v>
       </c>
       <c r="F36" s="138" t="n">
         <f aca="false">'Modes A-F'!G57</f>
@@ -17823,7 +17823,7 @@
       </c>
       <c r="G36" s="132" t="n">
         <f aca="false">E12-B36*TAN(2*(G31)/1000)+I29</f>
-        <v>14.5094025227675</v>
+        <v>20.6094025227675</v>
       </c>
       <c r="H36" s="124"/>
       <c r="I36" s="140"/>
@@ -17852,10 +17852,10 @@
   <dimension ref="A1:CX484"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="K58 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="102" min="2" style="0" width="11.96"/>
@@ -23924,10 +23924,10 @@
   <dimension ref="A1:G2383"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A44" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="1" sqref="K58 B4"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="56.14"/>

</xml_diff>

<commit_message>
working on electron yield
+ fixed kafka_message
+ fixed raster dossier bug
</commit_message>
<xml_diff>
--- a/startup/lookup_table/Modes.xlsx
+++ b/startup/lookup_table/Modes.xlsx
@@ -11750,14 +11750,14 @@
   <dimension ref="A1:AMJ66"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="M32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="E32" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="M1" activeCellId="0" sqref="M1"/>
+      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
-      <selection pane="bottomRight" activeCell="T54" activeCellId="0" sqref="T54"/>
+      <selection pane="bottomRight" activeCell="E58" activeCellId="0" sqref="E58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.0546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.04"/>
@@ -14927,7 +14927,7 @@
         <v>192</v>
       </c>
       <c r="E57" s="60" t="n">
-        <v>128.533</v>
+        <v>125.533</v>
       </c>
       <c r="F57" s="32" t="n">
         <v>6972005</v>
@@ -14981,7 +14981,7 @@
         <v>195</v>
       </c>
       <c r="E58" s="60" t="n">
-        <v>128.533</v>
+        <v>125.533</v>
       </c>
       <c r="F58" s="28" t="n">
         <v>5572330</v>
@@ -15518,7 +15518,7 @@
   <dimension ref="A1:AMJ31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
+      <selection pane="topLeft" activeCell="C27" activeCellId="1" sqref="E58 C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17092,10 +17092,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G11" activeCellId="0" sqref="G11"/>
+      <selection pane="bottomRight" activeCell="G11" activeCellId="1" sqref="E58 G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33"/>
@@ -17276,10 +17276,10 @@
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+      <selection pane="topLeft" activeCell="E4" activeCellId="1" sqref="E58 E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="11.96"/>
@@ -17474,12 +17474,12 @@
       </c>
       <c r="E11" s="122" t="n">
         <f aca="false">'Modes A-F'!E57</f>
-        <v>128.533</v>
+        <v>125.533</v>
       </c>
       <c r="F11" s="122"/>
       <c r="G11" s="131" t="n">
         <f aca="false">E11-B11*TAN(2*(G9-E9)/1000)</f>
-        <v>130.841400030779</v>
+        <v>127.841400030779</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17496,12 +17496,12 @@
       </c>
       <c r="E12" s="132" t="n">
         <f aca="false">'Modes A-F'!E58</f>
-        <v>128.533</v>
+        <v>125.533</v>
       </c>
       <c r="F12" s="132"/>
       <c r="G12" s="133" t="n">
         <f aca="false">E12-B12*TAN(2*(G9-E9)/1000)</f>
-        <v>131.072400033859</v>
+        <v>128.072400033859</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17627,7 +17627,7 @@
       </c>
       <c r="E23" s="122" t="n">
         <f aca="false">E11-B23*TAN(2*(E19)/1000)+I17</f>
-        <v>55.7722674801944</v>
+        <v>52.7722674801944</v>
       </c>
       <c r="F23" s="137" t="n">
         <f aca="false">'Modes A-F'!I56</f>
@@ -17635,7 +17635,7 @@
       </c>
       <c r="G23" s="122" t="n">
         <f aca="false">E11-B23*TAN(2*(G19)/1000)+I17</f>
-        <v>61.0728981480704</v>
+        <v>58.0728981480704</v>
       </c>
       <c r="I23" s="118"/>
     </row>
@@ -17653,7 +17653,7 @@
       </c>
       <c r="E24" s="132" t="n">
         <f aca="false">E12-B24*TAN(2*(E19)/1000)+I17</f>
-        <v>47.0518517843995</v>
+        <v>44.0518517843995</v>
       </c>
       <c r="F24" s="138" t="n">
         <f aca="false">'Modes A-F'!I57</f>
@@ -17661,7 +17661,7 @@
       </c>
       <c r="G24" s="139" t="n">
         <f aca="false">E12-B24*TAN(2*(G19)/1000)+I17</f>
-        <v>52.987766090482</v>
+        <v>49.987766090482</v>
       </c>
       <c r="H24" s="124"/>
       <c r="I24" s="140"/>
@@ -17789,7 +17789,7 @@
       </c>
       <c r="E35" s="122" t="n">
         <f aca="false">E11-B35*TAN(2*(E31)/1000)</f>
-        <v>26.8588777773465</v>
+        <v>23.8588777773465</v>
       </c>
       <c r="F35" s="137" t="n">
         <f aca="false">'Modes A-F'!G56</f>
@@ -17797,7 +17797,7 @@
       </c>
       <c r="G35" s="122" t="n">
         <f aca="false">E11-B35*TAN(2*(G31)/1000)+I29</f>
-        <v>32.1597875381681</v>
+        <v>29.1597875381681</v>
       </c>
       <c r="I35" s="118"/>
     </row>
@@ -17815,7 +17815,7 @@
       </c>
       <c r="E36" s="132" t="n">
         <f aca="false">E12-B36*TAN(2*(E31)/1000)</f>
-        <v>14.673175674289</v>
+        <v>11.673175674289</v>
       </c>
       <c r="F36" s="138" t="n">
         <f aca="false">'Modes A-F'!G57</f>
@@ -17823,7 +17823,7 @@
       </c>
       <c r="G36" s="132" t="n">
         <f aca="false">E12-B36*TAN(2*(G31)/1000)+I29</f>
-        <v>20.6094025227675</v>
+        <v>17.6094025227675</v>
       </c>
       <c r="H36" s="124"/>
       <c r="I36" s="140"/>
@@ -17852,10 +17852,10 @@
   <dimension ref="A1:CX484"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="E58 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="102" min="2" style="0" width="11.96"/>
@@ -23924,10 +23924,10 @@
   <dimension ref="A1:G2383"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A44" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="1" sqref="E58 B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="56.14"/>

</xml_diff>

<commit_message>
a lot of Dante work
+ xafs_det --> xafs_detx throughout
+ try to fix missing messagelog
</commit_message>
<xml_diff>
--- a/startup/lookup_table/Modes.xlsx
+++ b/startup/lookup_table/Modes.xlsx
@@ -11750,14 +11750,14 @@
   <dimension ref="A1:AMJ66"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="E32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="E35" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
-      <selection pane="bottomRight" activeCell="T58" activeCellId="0" sqref="T58"/>
+      <selection pane="bottomLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
+      <selection pane="bottomRight" activeCell="K55" activeCellId="0" sqref="K55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.07421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.09375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.04"/>
@@ -14716,7 +14716,7 @@
         <v>182</v>
       </c>
       <c r="E54" s="57" t="n">
-        <v>36.018</v>
+        <v>36.215</v>
       </c>
       <c r="F54" s="26" t="n">
         <v>276763</v>
@@ -14732,13 +14732,13 @@
         <v>-268324</v>
       </c>
       <c r="K54" s="57" t="n">
-        <v>45.66</v>
+        <v>45.363</v>
       </c>
       <c r="L54" s="28" t="n">
         <v>387964</v>
       </c>
       <c r="M54" s="57" t="n">
-        <v>45.712</v>
+        <v>45.4622</v>
       </c>
       <c r="N54" s="28" t="n">
         <v>394647</v>
@@ -14865,7 +14865,7 @@
         <v>189</v>
       </c>
       <c r="E56" s="60" t="n">
-        <v>118.101</v>
+        <v>119.35</v>
       </c>
       <c r="F56" s="25" t="n">
         <v>9251952</v>
@@ -14877,25 +14877,25 @@
         <v>4600216</v>
       </c>
       <c r="I56" s="60" t="n">
-        <v>53.596</v>
+        <v>55</v>
       </c>
       <c r="J56" s="23" t="n">
         <v>6151303</v>
       </c>
       <c r="K56" s="60" t="n">
-        <v>126.5</v>
+        <v>128.1</v>
       </c>
       <c r="L56" s="23" t="n">
         <v>9901395</v>
       </c>
       <c r="M56" s="60" t="n">
-        <v>126.584</v>
+        <v>128</v>
       </c>
       <c r="N56" s="23" t="n">
         <v>9901395</v>
       </c>
       <c r="O56" s="60" t="n">
-        <v>98.835</v>
+        <v>98.9</v>
       </c>
       <c r="P56" s="23" t="n">
         <v>8392750</v>
@@ -14927,7 +14927,7 @@
         <v>192</v>
       </c>
       <c r="E57" s="60" t="n">
-        <v>125.533</v>
+        <v>124.933</v>
       </c>
       <c r="F57" s="32" t="n">
         <v>6972005</v>
@@ -14939,7 +14939,7 @@
         <v>1551088</v>
       </c>
       <c r="I57" s="60" t="n">
-        <v>51.995</v>
+        <v>52.545</v>
       </c>
       <c r="J57" s="32" t="n">
         <v>3351899</v>
@@ -14951,13 +14951,13 @@
         <v>7552437</v>
       </c>
       <c r="M57" s="60" t="n">
-        <v>133.016</v>
+        <v>133.6</v>
       </c>
       <c r="N57" s="32" t="n">
         <v>7552437</v>
       </c>
       <c r="O57" s="60" t="n">
-        <v>105.267</v>
+        <v>101.167</v>
       </c>
       <c r="P57" s="32" t="n">
         <v>5879304</v>
@@ -14981,7 +14981,7 @@
         <v>195</v>
       </c>
       <c r="E58" s="60" t="n">
-        <v>125.533</v>
+        <v>124.933</v>
       </c>
       <c r="F58" s="28" t="n">
         <v>5572330</v>
@@ -14993,7 +14993,7 @@
         <v>354340</v>
       </c>
       <c r="I58" s="60" t="n">
-        <v>51.995</v>
+        <v>52.545</v>
       </c>
       <c r="J58" s="32" t="n">
         <v>1952224</v>
@@ -15005,13 +15005,13 @@
         <v>6355689</v>
       </c>
       <c r="M58" s="60" t="n">
-        <v>133.016</v>
+        <v>133.6</v>
       </c>
       <c r="N58" s="32" t="n">
         <v>6355689</v>
       </c>
       <c r="O58" s="60" t="n">
-        <v>105.267</v>
+        <v>101.167</v>
       </c>
       <c r="P58" s="65" t="n">
         <v>4479629</v>
@@ -15518,7 +15518,7 @@
   <dimension ref="A1:AMJ31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C27" activeCellId="1" sqref="T58 C27"/>
+      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16915,7 +16915,7 @@
       </c>
       <c r="F24" s="103" t="n">
         <f aca="false">'Modes A-F'!E54</f>
-        <v>36.018</v>
+        <v>36.215</v>
       </c>
       <c r="G24" s="0"/>
       <c r="H24" s="82" t="s">
@@ -16984,7 +16984,7 @@
       </c>
       <c r="F27" s="103" t="n">
         <f aca="false">'Modes A-F'!K54</f>
-        <v>45.66</v>
+        <v>45.363</v>
       </c>
       <c r="G27" s="0"/>
       <c r="H27" s="0"/>
@@ -17003,7 +17003,7 @@
       </c>
       <c r="F28" s="103" t="n">
         <f aca="false">'Modes A-F'!M54</f>
-        <v>45.712</v>
+        <v>45.4622</v>
       </c>
       <c r="G28" s="0"/>
       <c r="H28" s="0"/>
@@ -17092,10 +17092,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G11" activeCellId="1" sqref="T58 G11"/>
+      <selection pane="bottomRight" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33"/>
@@ -17276,10 +17276,10 @@
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="1" sqref="T58 E4"/>
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="11.96"/>
@@ -17360,19 +17360,19 @@
       </c>
       <c r="E4" s="103" t="n">
         <f aca="false">'Modes A-F'!K56</f>
-        <v>126.5</v>
+        <v>128.1</v>
       </c>
       <c r="F4" s="103" t="n">
         <f aca="false">E4-B4*TAN(2*(F2-E2)/1000)</f>
-        <v>97.5889132666878</v>
+        <v>99.1889132666877</v>
       </c>
       <c r="G4" s="121" t="n">
         <f aca="false">'Modes A-F'!O56</f>
-        <v>98.835</v>
+        <v>98.9</v>
       </c>
       <c r="H4" s="122" t="n">
         <f aca="false">G4-F4</f>
-        <v>1.24608673331224</v>
+        <v>-0.288913266687743</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17397,17 +17397,17 @@
       </c>
       <c r="G5" s="127" t="n">
         <f aca="false">'Modes A-F'!O57</f>
-        <v>105.267</v>
+        <v>101.167</v>
       </c>
       <c r="H5" s="122" t="n">
         <f aca="false">G5-F5</f>
-        <v>4.04309712834967</v>
+        <v>-0.0569028716503226</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H6" s="122" t="n">
         <f aca="false">AVERAGE(H3,H4,H5)</f>
-        <v>1.8820216266512</v>
+        <v>0.00368829331787882</v>
       </c>
       <c r="I6" s="0" t="s">
         <v>274</v>
@@ -17453,12 +17453,12 @@
       </c>
       <c r="E10" s="122" t="n">
         <f aca="false">'Modes A-F'!E54</f>
-        <v>36.018</v>
+        <v>36.215</v>
       </c>
       <c r="F10" s="122"/>
       <c r="G10" s="131" t="n">
         <f aca="false">E10-B10*TAN(2*(G9-E9)/1000)</f>
-        <v>38.1994000290853</v>
+        <v>38.3964000290853</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17474,12 +17474,12 @@
       </c>
       <c r="E11" s="122" t="n">
         <f aca="false">'Modes A-F'!E57</f>
-        <v>125.533</v>
+        <v>124.933</v>
       </c>
       <c r="F11" s="122"/>
       <c r="G11" s="131" t="n">
         <f aca="false">E11-B11*TAN(2*(G9-E9)/1000)</f>
-        <v>127.841400030779</v>
+        <v>127.241400030779</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17496,12 +17496,12 @@
       </c>
       <c r="E12" s="132" t="n">
         <f aca="false">'Modes A-F'!E58</f>
-        <v>125.533</v>
+        <v>124.933</v>
       </c>
       <c r="F12" s="132"/>
       <c r="G12" s="133" t="n">
         <f aca="false">E12-B12*TAN(2*(G9-E9)/1000)</f>
-        <v>128.072400033859</v>
+        <v>127.472400033859</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17602,7 +17602,7 @@
       </c>
       <c r="E22" s="122" t="n">
         <f aca="false">E10-B22*TAN(2*(E19)/1000)+I17</f>
-        <v>-31.9483914229833</v>
+        <v>-31.7513914229833</v>
       </c>
       <c r="F22" s="137" t="n">
         <f aca="false">'Modes A-F'!I54</f>
@@ -17610,7 +17610,7 @@
       </c>
       <c r="G22" s="122" t="n">
         <f aca="false">E10-B22*TAN(2*(G19)/1000)+I17</f>
-        <v>-26.9970292488399</v>
+        <v>-26.8000292488399</v>
       </c>
       <c r="I22" s="118"/>
     </row>
@@ -17627,15 +17627,15 @@
       </c>
       <c r="E23" s="122" t="n">
         <f aca="false">E11-B23*TAN(2*(E19)/1000)+I17</f>
-        <v>52.7722674801944</v>
+        <v>52.1722674801944</v>
       </c>
       <c r="F23" s="137" t="n">
         <f aca="false">'Modes A-F'!I56</f>
-        <v>53.596</v>
+        <v>55</v>
       </c>
       <c r="G23" s="122" t="n">
         <f aca="false">E11-B23*TAN(2*(G19)/1000)+I17</f>
-        <v>58.0728981480704</v>
+        <v>57.4728981480704</v>
       </c>
       <c r="I23" s="118"/>
     </row>
@@ -17653,15 +17653,15 @@
       </c>
       <c r="E24" s="132" t="n">
         <f aca="false">E12-B24*TAN(2*(E19)/1000)+I17</f>
-        <v>44.0518517843995</v>
+        <v>43.4518517843995</v>
       </c>
       <c r="F24" s="138" t="n">
         <f aca="false">'Modes A-F'!I57</f>
-        <v>51.995</v>
+        <v>52.545</v>
       </c>
       <c r="G24" s="139" t="n">
         <f aca="false">E12-B24*TAN(2*(G19)/1000)+I17</f>
-        <v>49.987766090482</v>
+        <v>49.387766090482</v>
       </c>
       <c r="H24" s="124"/>
       <c r="I24" s="140"/>
@@ -17764,7 +17764,7 @@
       </c>
       <c r="E34" s="122" t="n">
         <f aca="false">E10-B34*TAN(2*(E31)/1000)</f>
-        <v>-58.9566236638297</v>
+        <v>-58.7596236638297</v>
       </c>
       <c r="F34" s="137" t="n">
         <f aca="false">'Modes A-F'!G54</f>
@@ -17772,7 +17772,7 @@
       </c>
       <c r="G34" s="122" t="n">
         <f aca="false">E10-B34*TAN(2*(G31)/1000)+I29</f>
-        <v>-54.0050007866982</v>
+        <v>-53.8080007866982</v>
       </c>
       <c r="I34" s="118"/>
     </row>
@@ -17789,7 +17789,7 @@
       </c>
       <c r="E35" s="122" t="n">
         <f aca="false">E11-B35*TAN(2*(E31)/1000)</f>
-        <v>23.8588777773465</v>
+        <v>23.2588777773465</v>
       </c>
       <c r="F35" s="137" t="n">
         <f aca="false">'Modes A-F'!G56</f>
@@ -17797,7 +17797,7 @@
       </c>
       <c r="G35" s="122" t="n">
         <f aca="false">E11-B35*TAN(2*(G31)/1000)+I29</f>
-        <v>29.1597875381681</v>
+        <v>28.5597875381681</v>
       </c>
       <c r="I35" s="118"/>
     </row>
@@ -17815,7 +17815,7 @@
       </c>
       <c r="E36" s="132" t="n">
         <f aca="false">E12-B36*TAN(2*(E31)/1000)</f>
-        <v>11.673175674289</v>
+        <v>11.073175674289</v>
       </c>
       <c r="F36" s="138" t="n">
         <f aca="false">'Modes A-F'!G57</f>
@@ -17823,7 +17823,7 @@
       </c>
       <c r="G36" s="132" t="n">
         <f aca="false">E12-B36*TAN(2*(G31)/1000)+I29</f>
-        <v>17.6094025227675</v>
+        <v>17.0094025227675</v>
       </c>
       <c r="H36" s="124"/>
       <c r="I36" s="140"/>
@@ -17852,10 +17852,10 @@
   <dimension ref="A1:CX484"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="T58 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="102" min="2" style="0" width="11.96"/>
@@ -23924,10 +23924,10 @@
   <dimension ref="A1:G2383"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A44" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="1" sqref="T58 B4"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="56.14"/>

</xml_diff>

<commit_message>
stuff fixed during operations
+ agent improvements forMS/BMM experiment
+ made wiggle_bct work correctly
+ smaller lakeshore temperature deadband
+ start working on NSLS2 Slack channels
+ small macrobuilder changes
+ WITH_RADIOLOGICAL config parameter for use with Tc, U, etc
+ explicit lakeshore ramp_rate
+ flail around with telemetry
+ fix xrfat()
</commit_message>
<xml_diff>
--- a/startup/lookup_table/Modes.xlsx
+++ b/startup/lookup_table/Modes.xlsx
@@ -11754,10 +11754,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
-      <selection pane="bottomRight" activeCell="K55" activeCellId="0" sqref="K55"/>
+      <selection pane="bottomRight" activeCell="C73" activeCellId="0" sqref="C73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.09375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.04"/>
@@ -17095,7 +17095,7 @@
       <selection pane="bottomRight" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33"/>
@@ -17279,7 +17279,7 @@
       <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="11.96"/>
@@ -17855,7 +17855,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="102" min="2" style="0" width="11.96"/>
@@ -23927,7 +23927,7 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="56.14"/>

</xml_diff>

<commit_message>
replace slit_height with mirror pitch adjustment in change_edge()
also:

+ put startup dir in INI
+ try to wiggle_bct more effectively
+ wrote mirror_pitch special linescan
+ make slits=False and mirror=True the default in change_edge
+ comment out slits=False message
+ fine tune report multiplexing to restenct INI config booleans for nsls2 and bmm slacks
+ add check for bmmbot token in secrets location
+ begin work on a post and pin method for bmmbot
</commit_message>
<xml_diff>
--- a/startup/lookup_table/Modes.xlsx
+++ b/startup/lookup_table/Modes.xlsx
@@ -108,6 +108,19 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Rh/Pt stripe</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E54" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Position determined at Pt L3 edge</t>
         </r>
       </text>
     </comment>
@@ -223,6 +236,19 @@
         </r>
       </text>
     </comment>
+    <comment ref="I54" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Position set at Fe K edge</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="K24" authorId="0">
       <text>
         <r>
@@ -285,6 +311,19 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Rh/Pt stripe</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K54" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Position determined at Pt L3 edge</t>
         </r>
       </text>
     </comment>
@@ -353,6 +392,18 @@
         </r>
       </text>
     </comment>
+    <comment ref="M54" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Position determined at Pt L3 edge</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="O24" authorId="0">
       <text>
         <r>
@@ -415,6 +466,18 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Bare Si</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O54" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Position determined at Cr K edge</t>
         </r>
       </text>
     </comment>
@@ -10633,7 +10696,7 @@
     <numFmt numFmtId="170" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="171" formatCode="hh:mm:ss"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="20">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -10689,6 +10752,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -11414,87 +11482,87 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="8" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="12" fillId="8" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="8" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="8" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11502,27 +11570,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11538,7 +11606,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="32" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="32" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11598,7 +11666,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11626,7 +11694,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11650,7 +11718,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11750,14 +11818,14 @@
   <dimension ref="A1:AMJ66"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="E35" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="E26" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
-      <selection pane="bottomRight" activeCell="C73" activeCellId="0" sqref="C73"/>
+      <selection pane="bottomLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
+      <selection pane="bottomRight" activeCell="I43" activeCellId="0" sqref="I43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.12109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.04"/>
@@ -14716,7 +14784,7 @@
         <v>182</v>
       </c>
       <c r="E54" s="57" t="n">
-        <v>36.215</v>
+        <v>36.67</v>
       </c>
       <c r="F54" s="26" t="n">
         <v>276763</v>
@@ -14726,25 +14794,25 @@
       </c>
       <c r="H54" s="59"/>
       <c r="I54" s="57" t="n">
-        <v>-22.645</v>
+        <v>-23.297</v>
       </c>
       <c r="J54" s="28" t="n">
         <v>-268324</v>
       </c>
       <c r="K54" s="57" t="n">
-        <v>45.363</v>
+        <v>45.406</v>
       </c>
       <c r="L54" s="28" t="n">
         <v>387964</v>
       </c>
       <c r="M54" s="57" t="n">
-        <v>45.4622</v>
+        <v>45.406</v>
       </c>
       <c r="N54" s="28" t="n">
         <v>394647</v>
       </c>
       <c r="O54" s="57" t="n">
-        <v>19.46</v>
+        <v>19.322</v>
       </c>
       <c r="P54" s="28" t="n">
         <v>141529</v>
@@ -14889,7 +14957,7 @@
         <v>9901395</v>
       </c>
       <c r="M56" s="60" t="n">
-        <v>128</v>
+        <v>128.1</v>
       </c>
       <c r="N56" s="23" t="n">
         <v>9901395</v>
@@ -16915,7 +16983,7 @@
       </c>
       <c r="F24" s="103" t="n">
         <f aca="false">'Modes A-F'!E54</f>
-        <v>36.215</v>
+        <v>36.67</v>
       </c>
       <c r="G24" s="0"/>
       <c r="H24" s="82" t="s">
@@ -16961,7 +17029,7 @@
       </c>
       <c r="F26" s="103" t="n">
         <f aca="false">'Modes A-F'!I54</f>
-        <v>-22.645</v>
+        <v>-23.297</v>
       </c>
       <c r="G26" s="0"/>
       <c r="H26" s="82" t="s">
@@ -16984,7 +17052,7 @@
       </c>
       <c r="F27" s="103" t="n">
         <f aca="false">'Modes A-F'!K54</f>
-        <v>45.363</v>
+        <v>45.406</v>
       </c>
       <c r="G27" s="0"/>
       <c r="H27" s="0"/>
@@ -17003,7 +17071,7 @@
       </c>
       <c r="F28" s="103" t="n">
         <f aca="false">'Modes A-F'!M54</f>
-        <v>45.4622</v>
+        <v>45.406</v>
       </c>
       <c r="G28" s="0"/>
       <c r="H28" s="0"/>
@@ -17022,7 +17090,7 @@
       </c>
       <c r="F29" s="103" t="n">
         <f aca="false">'Modes A-F'!O54</f>
-        <v>19.46</v>
+        <v>19.322</v>
       </c>
       <c r="G29" s="0"/>
       <c r="H29" s="0"/>
@@ -17095,7 +17163,7 @@
       <selection pane="bottomRight" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33"/>
@@ -17279,7 +17347,7 @@
       <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="11.96"/>
@@ -17340,11 +17408,11 @@
       </c>
       <c r="G3" s="121" t="n">
         <f aca="false">'Modes A-F'!O54</f>
-        <v>19.46</v>
+        <v>19.322</v>
       </c>
       <c r="H3" s="122" t="n">
         <f aca="false">G3-F3</f>
-        <v>0.356881018291702</v>
+        <v>0.2188810182917</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17407,7 +17475,7 @@
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H6" s="122" t="n">
         <f aca="false">AVERAGE(H3,H4,H5)</f>
-        <v>0.00368829331787882</v>
+        <v>-0.0423117066821218</v>
       </c>
       <c r="I6" s="0" t="s">
         <v>274</v>
@@ -17453,12 +17521,12 @@
       </c>
       <c r="E10" s="122" t="n">
         <f aca="false">'Modes A-F'!E54</f>
-        <v>36.215</v>
+        <v>36.67</v>
       </c>
       <c r="F10" s="122"/>
       <c r="G10" s="131" t="n">
         <f aca="false">E10-B10*TAN(2*(G9-E9)/1000)</f>
-        <v>38.3964000290853</v>
+        <v>38.8514000290853</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17602,15 +17670,15 @@
       </c>
       <c r="E22" s="122" t="n">
         <f aca="false">E10-B22*TAN(2*(E19)/1000)+I17</f>
-        <v>-31.7513914229833</v>
+        <v>-31.2963914229833</v>
       </c>
       <c r="F22" s="137" t="n">
         <f aca="false">'Modes A-F'!I54</f>
-        <v>-22.645</v>
+        <v>-23.297</v>
       </c>
       <c r="G22" s="122" t="n">
         <f aca="false">E10-B22*TAN(2*(G19)/1000)+I17</f>
-        <v>-26.8000292488399</v>
+        <v>-26.3450292488399</v>
       </c>
       <c r="I22" s="118"/>
     </row>
@@ -17764,7 +17832,7 @@
       </c>
       <c r="E34" s="122" t="n">
         <f aca="false">E10-B34*TAN(2*(E31)/1000)</f>
-        <v>-58.7596236638297</v>
+        <v>-58.3046236638297</v>
       </c>
       <c r="F34" s="137" t="n">
         <f aca="false">'Modes A-F'!G54</f>
@@ -17772,7 +17840,7 @@
       </c>
       <c r="G34" s="122" t="n">
         <f aca="false">E10-B34*TAN(2*(G31)/1000)+I29</f>
-        <v>-53.8080007866982</v>
+        <v>-53.3530007866982</v>
       </c>
       <c r="I34" s="118"/>
     </row>
@@ -17855,7 +17923,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="102" min="2" style="0" width="11.96"/>
@@ -23927,7 +23995,7 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="56.14"/>

</xml_diff>

<commit_message>
better delivery of focused beam, much closer in different modes
also:
+ fixed a bug writing resonant refl. XDI files
+ quick_change alternative to change_edge
+ added no_slits argument to change_edge
+ add a retry loop to ga pitch scan analysis step
+ add some sleeps to ga auto_align so analysis can be seen briefly
+ add hcenter special linescan type
+ use ROI and ROISTATS in pilatus
+ hint pilatus signals sensibly
+ post and pin introduction to slack convo channel
+ begin work on resonant reflectivity automation
+ experimental measure_multiple_rois
+ chat method in bmmbot
</commit_message>
<xml_diff>
--- a/startup/lookup_table/Modes.xlsx
+++ b/startup/lookup_table/Modes.xlsx
@@ -40,6 +40,19 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Blocks beam around 31.5</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A56" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Positions found at Pt L3 (A, D, E), Fe K (C), Cr K (F) edges using slits mounted approx above jacks</t>
         </r>
       </text>
     </comment>
@@ -399,6 +412,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Position determined at Pt L3 edge</t>
         </r>
@@ -476,6 +490,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Position determined at Cr K edge</t>
         </r>
@@ -10696,7 +10711,7 @@
     <numFmt numFmtId="170" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="171" formatCode="hh:mm:ss"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="19">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -10752,11 +10767,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -11482,87 +11492,87 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="8" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="8" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="8" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="8" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11570,27 +11580,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11606,7 +11616,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="32" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="32" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11666,7 +11676,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11694,7 +11704,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11718,7 +11728,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11818,14 +11828,14 @@
   <dimension ref="A1:AMJ66"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="E26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="I26" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topRight" activeCell="I1" activeCellId="0" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
-      <selection pane="bottomRight" activeCell="I43" activeCellId="0" sqref="I43"/>
+      <selection pane="bottomRight" activeCell="T54" activeCellId="0" sqref="T54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.12109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.04"/>
@@ -14818,7 +14828,7 @@
         <v>141529</v>
       </c>
       <c r="T54" s="57" t="n">
-        <v>57.95</v>
+        <v>58.501</v>
       </c>
       <c r="U54" s="28" t="n">
         <v>497477</v>
@@ -14933,7 +14943,7 @@
         <v>189</v>
       </c>
       <c r="E56" s="60" t="n">
-        <v>119.35</v>
+        <v>120.604</v>
       </c>
       <c r="F56" s="25" t="n">
         <v>9251952</v>
@@ -14945,25 +14955,25 @@
         <v>4600216</v>
       </c>
       <c r="I56" s="60" t="n">
-        <v>55</v>
+        <v>55.463</v>
       </c>
       <c r="J56" s="23" t="n">
         <v>6151303</v>
       </c>
       <c r="K56" s="60" t="n">
-        <v>128.1</v>
+        <v>128.866</v>
       </c>
       <c r="L56" s="23" t="n">
         <v>9901395</v>
       </c>
       <c r="M56" s="60" t="n">
-        <v>128.1</v>
+        <v>128.866</v>
       </c>
       <c r="N56" s="23" t="n">
         <v>9901395</v>
       </c>
       <c r="O56" s="60" t="n">
-        <v>98.9</v>
+        <v>100.725</v>
       </c>
       <c r="P56" s="23" t="n">
         <v>8392750</v>
@@ -14995,7 +15005,7 @@
         <v>192</v>
       </c>
       <c r="E57" s="60" t="n">
-        <v>124.933</v>
+        <v>127.083</v>
       </c>
       <c r="F57" s="32" t="n">
         <v>6972005</v>
@@ -15007,25 +15017,25 @@
         <v>1551088</v>
       </c>
       <c r="I57" s="60" t="n">
-        <v>52.545</v>
+        <v>53.637</v>
       </c>
       <c r="J57" s="32" t="n">
         <v>3351899</v>
       </c>
       <c r="K57" s="60" t="n">
-        <v>133.6</v>
+        <v>135.05</v>
       </c>
       <c r="L57" s="32" t="n">
         <v>7552437</v>
       </c>
       <c r="M57" s="60" t="n">
-        <v>133.6</v>
+        <v>135.05</v>
       </c>
       <c r="N57" s="32" t="n">
         <v>7552437</v>
       </c>
       <c r="O57" s="60" t="n">
-        <v>101.167</v>
+        <v>103.567</v>
       </c>
       <c r="P57" s="32" t="n">
         <v>5879304</v>
@@ -15049,7 +15059,7 @@
         <v>195</v>
       </c>
       <c r="E58" s="60" t="n">
-        <v>124.933</v>
+        <v>127.083</v>
       </c>
       <c r="F58" s="28" t="n">
         <v>5572330</v>
@@ -15061,25 +15071,25 @@
         <v>354340</v>
       </c>
       <c r="I58" s="60" t="n">
-        <v>52.545</v>
+        <v>53.637</v>
       </c>
       <c r="J58" s="32" t="n">
         <v>1952224</v>
       </c>
       <c r="K58" s="60" t="n">
-        <v>133.6</v>
+        <v>135.05</v>
       </c>
       <c r="L58" s="32" t="n">
         <v>6355689</v>
       </c>
       <c r="M58" s="60" t="n">
-        <v>133.6</v>
+        <v>135.05</v>
       </c>
       <c r="N58" s="32" t="n">
         <v>6355689</v>
       </c>
       <c r="O58" s="60" t="n">
-        <v>101.167</v>
+        <v>103.567</v>
       </c>
       <c r="P58" s="65" t="n">
         <v>4479629</v>
@@ -17109,7 +17119,7 @@
       </c>
       <c r="F30" s="103" t="n">
         <f aca="false">'Modes A-F'!T54</f>
-        <v>57.95</v>
+        <v>58.501</v>
       </c>
       <c r="G30" s="0"/>
       <c r="H30" s="0"/>
@@ -17163,7 +17173,7 @@
       <selection pane="bottomRight" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33"/>
@@ -17347,7 +17357,7 @@
       <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="11.96"/>
@@ -17428,19 +17438,19 @@
       </c>
       <c r="E4" s="103" t="n">
         <f aca="false">'Modes A-F'!K56</f>
-        <v>128.1</v>
+        <v>128.866</v>
       </c>
       <c r="F4" s="103" t="n">
         <f aca="false">E4-B4*TAN(2*(F2-E2)/1000)</f>
-        <v>99.1889132666877</v>
+        <v>99.9549132666878</v>
       </c>
       <c r="G4" s="121" t="n">
         <f aca="false">'Modes A-F'!O56</f>
-        <v>98.9</v>
+        <v>100.725</v>
       </c>
       <c r="H4" s="122" t="n">
         <f aca="false">G4-F4</f>
-        <v>-0.288913266687743</v>
+        <v>0.770086733312226</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17457,25 +17467,25 @@
       </c>
       <c r="E5" s="126" t="n">
         <f aca="false">'Modes A-F'!K57</f>
-        <v>133.6</v>
+        <v>135.05</v>
       </c>
       <c r="F5" s="126" t="n">
         <f aca="false">E5-B5*TAN(2*(F2-E2)/1000)</f>
-        <v>101.22390287165</v>
+        <v>102.67390287165</v>
       </c>
       <c r="G5" s="127" t="n">
         <f aca="false">'Modes A-F'!O57</f>
-        <v>101.167</v>
+        <v>103.567</v>
       </c>
       <c r="H5" s="122" t="n">
         <f aca="false">G5-F5</f>
-        <v>-0.0569028716503226</v>
+        <v>0.893097128349652</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H6" s="122" t="n">
         <f aca="false">AVERAGE(H3,H4,H5)</f>
-        <v>-0.0423117066821218</v>
+        <v>0.627354959984526</v>
       </c>
       <c r="I6" s="0" t="s">
         <v>274</v>
@@ -17542,12 +17552,12 @@
       </c>
       <c r="E11" s="122" t="n">
         <f aca="false">'Modes A-F'!E57</f>
-        <v>124.933</v>
+        <v>127.083</v>
       </c>
       <c r="F11" s="122"/>
       <c r="G11" s="131" t="n">
         <f aca="false">E11-B11*TAN(2*(G9-E9)/1000)</f>
-        <v>127.241400030779</v>
+        <v>129.391400030779</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17564,12 +17574,12 @@
       </c>
       <c r="E12" s="132" t="n">
         <f aca="false">'Modes A-F'!E58</f>
-        <v>124.933</v>
+        <v>127.083</v>
       </c>
       <c r="F12" s="132"/>
       <c r="G12" s="133" t="n">
         <f aca="false">E12-B12*TAN(2*(G9-E9)/1000)</f>
-        <v>127.472400033859</v>
+        <v>129.622400033859</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17695,15 +17705,15 @@
       </c>
       <c r="E23" s="122" t="n">
         <f aca="false">E11-B23*TAN(2*(E19)/1000)+I17</f>
-        <v>52.1722674801944</v>
+        <v>54.3222674801944</v>
       </c>
       <c r="F23" s="137" t="n">
         <f aca="false">'Modes A-F'!I56</f>
-        <v>55</v>
+        <v>55.463</v>
       </c>
       <c r="G23" s="122" t="n">
         <f aca="false">E11-B23*TAN(2*(G19)/1000)+I17</f>
-        <v>57.4728981480704</v>
+        <v>59.6228981480704</v>
       </c>
       <c r="I23" s="118"/>
     </row>
@@ -17721,15 +17731,15 @@
       </c>
       <c r="E24" s="132" t="n">
         <f aca="false">E12-B24*TAN(2*(E19)/1000)+I17</f>
-        <v>43.4518517843995</v>
+        <v>45.6018517843995</v>
       </c>
       <c r="F24" s="138" t="n">
         <f aca="false">'Modes A-F'!I57</f>
-        <v>52.545</v>
+        <v>53.637</v>
       </c>
       <c r="G24" s="139" t="n">
         <f aca="false">E12-B24*TAN(2*(G19)/1000)+I17</f>
-        <v>49.387766090482</v>
+        <v>51.537766090482</v>
       </c>
       <c r="H24" s="124"/>
       <c r="I24" s="140"/>
@@ -17857,7 +17867,7 @@
       </c>
       <c r="E35" s="122" t="n">
         <f aca="false">E11-B35*TAN(2*(E31)/1000)</f>
-        <v>23.2588777773465</v>
+        <v>25.4088777773465</v>
       </c>
       <c r="F35" s="137" t="n">
         <f aca="false">'Modes A-F'!G56</f>
@@ -17865,7 +17875,7 @@
       </c>
       <c r="G35" s="122" t="n">
         <f aca="false">E11-B35*TAN(2*(G31)/1000)+I29</f>
-        <v>28.5597875381681</v>
+        <v>30.7097875381681</v>
       </c>
       <c r="I35" s="118"/>
     </row>
@@ -17883,7 +17893,7 @@
       </c>
       <c r="E36" s="132" t="n">
         <f aca="false">E12-B36*TAN(2*(E31)/1000)</f>
-        <v>11.073175674289</v>
+        <v>13.223175674289</v>
       </c>
       <c r="F36" s="138" t="n">
         <f aca="false">'Modes A-F'!G57</f>
@@ -17891,7 +17901,7 @@
       </c>
       <c r="G36" s="132" t="n">
         <f aca="false">E12-B36*TAN(2*(G31)/1000)+I29</f>
-        <v>17.0094025227675</v>
+        <v>19.1594025227675</v>
       </c>
       <c r="H36" s="124"/>
       <c r="I36" s="140"/>
@@ -17923,7 +17933,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="102" min="2" style="0" width="11.96"/>
@@ -23995,7 +24005,7 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="56.14"/>

</xml_diff>